<commit_message>
Added thank you notes written here
</commit_message>
<xml_diff>
--- a/Guest_List_Invited.xlsx
+++ b/Guest_List_Invited.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="253">
   <si>
     <t xml:space="preserve">Priority </t>
   </si>
@@ -766,6 +766,18 @@
   </si>
   <si>
     <t>12442 Old Meridian, Apartment 01-106, Carmel, IN 46032</t>
+  </si>
+  <si>
+    <t>Towels and kitchen stuff from BB&amp;B</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>$200 for candlelight dinner on beach</t>
+  </si>
+  <si>
+    <t>$120 for waterfall cycling adventure</t>
   </si>
 </sst>
 </file>
@@ -1192,7 +1204,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1202,9 +1214,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA211"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P79" sqref="P79"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W39" sqref="W39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1226,6 +1238,7 @@
     <col min="20" max="20" width="10.85546875" customWidth="1"/>
     <col min="21" max="21" width="11" customWidth="1"/>
     <col min="22" max="22" width="11.85546875" customWidth="1"/>
+    <col min="23" max="23" width="12.85546875" customWidth="1"/>
     <col min="24" max="25" width="0" hidden="1" customWidth="1"/>
     <col min="26" max="26" width="13.85546875" hidden="1" customWidth="1"/>
     <col min="27" max="27" width="10" bestFit="1" customWidth="1"/>
@@ -1275,7 +1288,7 @@
       </c>
       <c r="R2" s="14">
         <f>D3+G3*(1+Z4/100)</f>
-        <v>163.76023290668545</v>
+        <v>163.70329265657784</v>
       </c>
       <c r="S2" t="s">
         <v>221</v>
@@ -1299,34 +1312,34 @@
       </c>
       <c r="D3" s="19">
         <f>SUM(E6:E129)</f>
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3">
         <f>SUM(J6:J173)</f>
-        <v>132.39999999999992</v>
+        <v>133.39999999999995</v>
       </c>
       <c r="G3">
         <f>SUM(O6:O129)</f>
-        <v>108.39999999999989</v>
+        <v>103.39999999999991</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
       <c r="P3" s="12">
         <f>G3+D3</f>
-        <v>132.39999999999989</v>
+        <v>133.39999999999992</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>225</v>
       </c>
       <c r="R3" s="14">
         <f>D3+G3*(1-Z4/100)</f>
-        <v>101.03976709331434</v>
+        <v>103.09670734342197</v>
       </c>
       <c r="S3" s="13">
         <f>SUM(X6:X129)/COUNT(X6:X11,X14:X41,X45:X50,X53:X59,X62:X85,X88:X113,X116:X124,X127:X129)</f>
-        <v>0.13761467889908258</v>
+        <v>0.1743119266055046</v>
       </c>
       <c r="T3" s="10"/>
       <c r="U3" s="10"/>
@@ -1402,7 +1415,7 @@
       </c>
       <c r="Z4" s="10">
         <f>STDEV(Y6:Y129)</f>
-        <v>28.930104157459017</v>
+        <v>29.306859435762057</v>
       </c>
       <c r="AA4" s="10" t="s">
         <v>247</v>
@@ -3249,6 +3262,9 @@
       <c r="U34" t="s">
         <v>153</v>
       </c>
+      <c r="W34" t="s">
+        <v>251</v>
+      </c>
       <c r="X34">
         <f t="shared" si="10"/>
         <v>1</v>
@@ -3507,6 +3523,9 @@
       </c>
       <c r="U38" t="s">
         <v>153</v>
+      </c>
+      <c r="W38" t="s">
+        <v>252</v>
       </c>
       <c r="X38">
         <f t="shared" si="10"/>
@@ -4786,7 +4805,7 @@
       <c r="B61" s="17"/>
       <c r="D61">
         <f>SUM(J62:J84)</f>
-        <v>29.199999999999989</v>
+        <v>29.399999999999991</v>
       </c>
       <c r="J61">
         <f t="shared" si="9"/>
@@ -5834,6 +5853,9 @@
       <c r="D77">
         <v>1</v>
       </c>
+      <c r="E77">
+        <v>1</v>
+      </c>
       <c r="F77">
         <v>3</v>
       </c>
@@ -5845,15 +5867,15 @@
       </c>
       <c r="J77">
         <f t="shared" si="20"/>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="K77">
         <f t="shared" si="15"/>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="L77">
         <f t="shared" si="16"/>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="M77">
         <f t="shared" si="17"/>
@@ -5865,7 +5887,7 @@
       </c>
       <c r="O77">
         <f t="shared" si="14"/>
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="P77" t="s">
         <v>159</v>
@@ -5878,11 +5900,11 @@
       </c>
       <c r="X77">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="Y77">
+        <v>1</v>
+      </c>
+      <c r="Y77" t="str">
         <f t="shared" si="19"/>
-        <v>90</v>
+        <v/>
       </c>
     </row>
     <row r="78" spans="1:25">
@@ -6077,7 +6099,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="81" spans="1:25">
+    <row r="81" spans="1:27">
       <c r="A81" t="s">
         <v>68</v>
       </c>
@@ -6090,6 +6112,9 @@
       <c r="D81">
         <v>1</v>
       </c>
+      <c r="E81">
+        <v>1</v>
+      </c>
       <c r="F81">
         <v>3</v>
       </c>
@@ -6101,15 +6126,15 @@
       </c>
       <c r="J81">
         <f t="shared" si="20"/>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="K81">
         <f t="shared" si="15"/>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="L81">
         <f t="shared" si="16"/>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="M81">
         <f t="shared" si="17"/>
@@ -6121,7 +6146,7 @@
       </c>
       <c r="O81">
         <f t="shared" si="14"/>
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="P81" t="s">
         <v>118</v>
@@ -6134,14 +6159,14 @@
       </c>
       <c r="X81">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="Y81">
+        <v>1</v>
+      </c>
+      <c r="Y81" t="str">
         <f t="shared" si="19"/>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="82" spans="1:25">
+        <v/>
+      </c>
+    </row>
+    <row r="82" spans="1:27">
       <c r="A82" t="s">
         <v>172</v>
       </c>
@@ -6205,7 +6230,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="83" spans="1:25">
+    <row r="83" spans="1:27">
       <c r="A83" t="s">
         <v>227</v>
       </c>
@@ -6272,7 +6297,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="84" spans="1:25">
+    <row r="84" spans="1:27">
       <c r="A84" t="s">
         <v>71</v>
       </c>
@@ -6336,7 +6361,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="85" spans="1:25">
+    <row r="85" spans="1:27">
       <c r="A85" t="s">
         <v>228</v>
       </c>
@@ -6400,7 +6425,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="86" spans="1:25">
+    <row r="86" spans="1:27">
       <c r="B86" s="6"/>
       <c r="J86">
         <f t="shared" si="20"/>
@@ -6431,14 +6456,14 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="1:25">
+    <row r="87" spans="1:27">
       <c r="A87" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B87" s="17"/>
       <c r="D87">
         <f>SUM(J88:J102)</f>
-        <v>19.399999999999999</v>
+        <v>19.8</v>
       </c>
       <c r="J87">
         <f t="shared" si="20"/>
@@ -6469,7 +6494,7 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="1:25">
+    <row r="88" spans="1:27">
       <c r="A88" s="2" t="s">
         <v>83</v>
       </c>
@@ -6533,7 +6558,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="89" spans="1:25">
+    <row r="89" spans="1:27">
       <c r="A89" t="s">
         <v>77</v>
       </c>
@@ -6597,7 +6622,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="90" spans="1:25">
+    <row r="90" spans="1:27">
       <c r="A90" t="s">
         <v>137</v>
       </c>
@@ -6661,7 +6686,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="91" spans="1:25">
+    <row r="91" spans="1:27">
       <c r="A91" t="s">
         <v>78</v>
       </c>
@@ -6725,7 +6750,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="92" spans="1:25">
+    <row r="92" spans="1:27">
       <c r="A92" t="s">
         <v>79</v>
       </c>
@@ -6780,6 +6805,9 @@
       <c r="U92" t="s">
         <v>153</v>
       </c>
+      <c r="W92" t="s">
+        <v>249</v>
+      </c>
       <c r="X92">
         <f t="shared" si="24"/>
         <v>0</v>
@@ -6788,8 +6816,11 @@
         <f t="shared" si="19"/>
         <v>80</v>
       </c>
-    </row>
-    <row r="93" spans="1:25">
+      <c r="AA92" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="93" spans="1:27">
       <c r="A93" t="s">
         <v>160</v>
       </c>
@@ -6802,6 +6833,9 @@
       <c r="D93">
         <v>1</v>
       </c>
+      <c r="E93">
+        <v>2</v>
+      </c>
       <c r="F93">
         <v>4</v>
       </c>
@@ -6813,19 +6847,19 @@
       </c>
       <c r="J93">
         <f t="shared" si="20"/>
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="K93">
         <f t="shared" si="21"/>
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="L93">
         <f t="shared" si="22"/>
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="M93">
         <f t="shared" si="23"/>
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="N93">
         <f t="shared" si="18"/>
@@ -6833,7 +6867,7 @@
       </c>
       <c r="O93">
         <f t="shared" si="14"/>
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="P93" t="s">
         <v>149</v>
@@ -6846,14 +6880,14 @@
       </c>
       <c r="X93">
         <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="Y93">
+        <v>1</v>
+      </c>
+      <c r="Y93" t="str">
         <f t="shared" si="19"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="94" spans="1:25">
+        <v/>
+      </c>
+    </row>
+    <row r="94" spans="1:27">
       <c r="A94" t="s">
         <v>157</v>
       </c>
@@ -6917,7 +6951,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="95" spans="1:25">
+    <row r="95" spans="1:27">
       <c r="A95" t="s">
         <v>161</v>
       </c>
@@ -6981,7 +7015,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="96" spans="1:25">
+    <row r="96" spans="1:27">
       <c r="A96" t="s">
         <v>123</v>
       </c>
@@ -7769,6 +7803,9 @@
       <c r="D109">
         <v>1</v>
       </c>
+      <c r="E109">
+        <v>2</v>
+      </c>
       <c r="F109">
         <v>3</v>
       </c>
@@ -7780,7 +7817,7 @@
       </c>
       <c r="J109">
         <f t="shared" si="20"/>
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="N109">
         <f t="shared" si="18"/>
@@ -7788,7 +7825,7 @@
       </c>
       <c r="O109">
         <f t="shared" si="14"/>
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="P109" t="s">
         <v>97</v>
@@ -7801,11 +7838,11 @@
       </c>
       <c r="X109">
         <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="Y109">
+        <v>1</v>
+      </c>
+      <c r="Y109" t="str">
         <f t="shared" si="19"/>
-        <v>80</v>
+        <v/>
       </c>
     </row>
     <row r="110" spans="1:25">

</xml_diff>

<commit_message>
Updated if we sent thank you notes to people
</commit_message>
<xml_diff>
--- a/Guest_List_Invited.xlsx
+++ b/Guest_List_Invited.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="253">
   <si>
     <t xml:space="preserve">Priority </t>
   </si>
@@ -1204,7 +1204,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1216,7 +1216,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W39" sqref="W39"/>
+      <selection pane="bottomLeft" activeCell="AA39" sqref="AA39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3140,7 +3140,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:25">
+    <row r="33" spans="1:27">
       <c r="A33" s="2" t="s">
         <v>26</v>
       </c>
@@ -3204,7 +3204,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:25">
+    <row r="34" spans="1:27">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
@@ -3273,8 +3273,11 @@
         <f t="shared" si="7"/>
         <v/>
       </c>
-    </row>
-    <row r="35" spans="1:25">
+      <c r="AA34" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
@@ -3338,7 +3341,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:25">
+    <row r="36" spans="1:27">
       <c r="A36" s="2" t="s">
         <v>40</v>
       </c>
@@ -3402,7 +3405,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:25">
+    <row r="37" spans="1:27">
       <c r="A37" s="2" t="s">
         <v>41</v>
       </c>
@@ -3466,7 +3469,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:25">
+    <row r="38" spans="1:27">
       <c r="A38" s="2" t="s">
         <v>42</v>
       </c>
@@ -3535,8 +3538,11 @@
         <f t="shared" si="7"/>
         <v/>
       </c>
-    </row>
-    <row r="39" spans="1:25">
+      <c r="AA38" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27">
       <c r="A39" s="2" t="s">
         <v>43</v>
       </c>
@@ -3600,7 +3606,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:25">
+    <row r="40" spans="1:27">
       <c r="A40" s="2" t="s">
         <v>44</v>
       </c>
@@ -3664,7 +3670,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:25">
+    <row r="41" spans="1:27">
       <c r="A41" t="s">
         <v>103</v>
       </c>
@@ -3728,7 +3734,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:25">
+    <row r="42" spans="1:27">
       <c r="A42" s="2"/>
       <c r="B42" s="7"/>
       <c r="D42">
@@ -3764,7 +3770,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:25">
+    <row r="43" spans="1:27">
       <c r="B43" s="6"/>
       <c r="C43" s="1"/>
       <c r="D43">
@@ -3800,7 +3806,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:25">
+    <row r="44" spans="1:27">
       <c r="A44" s="1" t="s">
         <v>27</v>
       </c>
@@ -3838,7 +3844,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:25">
+    <row r="45" spans="1:27">
       <c r="A45" t="s">
         <v>28</v>
       </c>
@@ -3902,7 +3908,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="1:25">
+    <row r="46" spans="1:27">
       <c r="A46" t="s">
         <v>29</v>
       </c>
@@ -3966,7 +3972,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:25">
+    <row r="47" spans="1:27">
       <c r="A47" t="s">
         <v>30</v>
       </c>
@@ -4030,7 +4036,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:25">
+    <row r="48" spans="1:27">
       <c r="A48" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
added DJ to count
</commit_message>
<xml_diff>
--- a/Guest_List_Invited.xlsx
+++ b/Guest_List_Invited.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\logan\Documents\GitHub\Farrell_Garrett_Wedding\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2178637-0B36-4806-9E8C-71658C9A4F80}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="171027"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="254">
   <si>
     <t xml:space="preserve">Priority </t>
   </si>
@@ -778,16 +784,19 @@
   </si>
   <si>
     <t xml:space="preserve">Aja and Phillip </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DJ </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1204,22 +1213,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E86" sqref="E86"/>
+      <pane ySplit="4" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.85546875" customWidth="1"/>
     <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
@@ -1244,7 +1253,7 @@
     <col min="27" max="27" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15" customHeight="1">
+    <row r="1" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5">
         <v>4</v>
       </c>
@@ -1264,7 +1273,7 @@
       <c r="U1" s="10"/>
       <c r="V1" s="10"/>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>3</v>
       </c>
@@ -1288,7 +1297,7 @@
       </c>
       <c r="R2" s="14">
         <f>D3+G3*(1+Z4/100)</f>
-        <v>151.65239805127794</v>
+        <v>152.65239805127794</v>
       </c>
       <c r="S2" t="s">
         <v>220</v>
@@ -1302,7 +1311,7 @@
         <v>28.53908325175902</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1311,8 +1320,8 @@
         <v>89</v>
       </c>
       <c r="D3" s="19">
-        <f>SUM(E6:E129)</f>
-        <v>51</v>
+        <f>SUM(E6:E130)</f>
+        <v>52</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3">
@@ -1320,7 +1329,7 @@
         <v>128.79999999999995</v>
       </c>
       <c r="G3">
-        <f>SUM(O6:O129)</f>
+        <f>SUM(O6:O130)</f>
         <v>77.799999999999983</v>
       </c>
       <c r="H3" s="11"/>
@@ -1328,14 +1337,14 @@
       <c r="J3" s="11"/>
       <c r="P3" s="12">
         <f>G3+D3</f>
-        <v>128.79999999999998</v>
+        <v>129.79999999999998</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>224</v>
       </c>
       <c r="R3" s="14">
         <f>D3+G3*(1-Z4/100)</f>
-        <v>105.94760194872201</v>
+        <v>106.94760194872201</v>
       </c>
       <c r="S3" s="13">
         <f>SUM(X6:X129)/COUNT(X6:X11,X14:X41,X45:X50,X53:X59,X62:X85,X88:X113,X116:X124,X127:X129)</f>
@@ -1351,7 +1360,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="4" spans="1:27" s="10" customFormat="1" ht="31.5" customHeight="1">
+    <row r="4" spans="1:27" s="10" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -1421,7 +1430,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="5" spans="1:27">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1431,7 +1440,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:27">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1498,7 +1507,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:27">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1565,7 +1574,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:27">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1632,7 +1641,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:27">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1699,7 +1708,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1766,7 +1775,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:27">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -1835,7 +1844,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:27">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
       <c r="C12" s="1"/>
       <c r="D12">
@@ -1871,7 +1880,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:27">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -1909,7 +1918,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:27">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
@@ -1973,7 +1982,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:27">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -2037,7 +2046,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:27">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
@@ -2104,7 +2113,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
@@ -2168,7 +2177,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
@@ -2232,7 +2241,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>190</v>
       </c>
@@ -2299,7 +2308,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -2366,7 +2375,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
@@ -2430,7 +2439,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
@@ -2494,7 +2503,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>233</v>
       </c>
@@ -2561,7 +2570,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>17</v>
       </c>
@@ -2625,7 +2634,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>18</v>
       </c>
@@ -2692,7 +2701,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>19</v>
       </c>
@@ -2756,7 +2765,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>20</v>
       </c>
@@ -2820,7 +2829,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>21</v>
       </c>
@@ -2884,7 +2893,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>22</v>
       </c>
@@ -2951,7 +2960,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>23</v>
       </c>
@@ -3015,7 +3024,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>24</v>
       </c>
@@ -3079,7 +3088,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>25</v>
       </c>
@@ -3143,7 +3152,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:27">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>26</v>
       </c>
@@ -3207,7 +3216,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:27">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
@@ -3280,7 +3289,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="35" spans="1:27">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
@@ -3344,7 +3353,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:27">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>40</v>
       </c>
@@ -3408,7 +3417,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:27">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>41</v>
       </c>
@@ -3472,7 +3481,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:27">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>42</v>
       </c>
@@ -3545,7 +3554,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="39" spans="1:27">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>43</v>
       </c>
@@ -3612,7 +3621,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:27">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>44</v>
       </c>
@@ -3679,7 +3688,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:27">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>102</v>
       </c>
@@ -3743,7 +3752,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:27">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="7"/>
       <c r="D42">
@@ -3779,7 +3788,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:27">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B43" s="6"/>
       <c r="C43" s="1"/>
       <c r="D43">
@@ -3815,7 +3824,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:27">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>27</v>
       </c>
@@ -3853,7 +3862,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:27">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>28</v>
       </c>
@@ -3920,7 +3929,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:27">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>29</v>
       </c>
@@ -3984,7 +3993,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:27">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>30</v>
       </c>
@@ -4048,7 +4057,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:27">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>31</v>
       </c>
@@ -4115,7 +4124,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>32</v>
       </c>
@@ -4182,7 +4191,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:25">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>234</v>
       </c>
@@ -4251,7 +4260,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="1:25">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B51" s="6"/>
       <c r="J51">
         <f t="shared" si="9"/>
@@ -4282,7 +4291,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:25">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>49</v>
       </c>
@@ -4320,7 +4329,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:25">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>48</v>
       </c>
@@ -4391,7 +4400,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:25">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>51</v>
       </c>
@@ -4458,7 +4467,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:25">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>50</v>
       </c>
@@ -4529,7 +4538,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:25">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>79</v>
       </c>
@@ -4596,7 +4605,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:25">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>52</v>
       </c>
@@ -4666,7 +4675,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:25">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>53</v>
       </c>
@@ -4733,7 +4742,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:25">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>54</v>
       </c>
@@ -4800,7 +4809,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:25">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B60" s="6"/>
       <c r="J60">
         <f t="shared" si="9"/>
@@ -4831,7 +4840,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:25">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>47</v>
       </c>
@@ -4869,7 +4878,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:25">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>225</v>
       </c>
@@ -4937,7 +4946,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="63" spans="1:25">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>55</v>
       </c>
@@ -5005,7 +5014,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="64" spans="1:25">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>56</v>
       </c>
@@ -5075,7 +5084,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="1:25">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>58</v>
       </c>
@@ -5143,7 +5152,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="66" spans="1:25">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>169</v>
       </c>
@@ -5211,7 +5220,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="67" spans="1:25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>193</v>
       </c>
@@ -5267,7 +5276,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:25">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>59</v>
       </c>
@@ -5335,7 +5344,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="69" spans="1:25">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>60</v>
       </c>
@@ -5403,7 +5412,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="70" spans="1:25">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>61</v>
       </c>
@@ -5474,7 +5483,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:25">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>62</v>
       </c>
@@ -5544,7 +5553,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:25">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>63</v>
       </c>
@@ -5614,7 +5623,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:25">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>64</v>
       </c>
@@ -5681,7 +5690,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:25">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>65</v>
       </c>
@@ -5745,7 +5754,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="75" spans="1:25">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>66</v>
       </c>
@@ -5809,7 +5818,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="76" spans="1:25">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>67</v>
       </c>
@@ -5879,7 +5888,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:25">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>168</v>
       </c>
@@ -5946,7 +5955,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:25">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>69</v>
       </c>
@@ -6010,7 +6019,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="79" spans="1:25">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>129</v>
       </c>
@@ -6074,7 +6083,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="80" spans="1:25">
+    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>70</v>
       </c>
@@ -6138,7 +6147,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="81" spans="1:27">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>68</v>
       </c>
@@ -6205,7 +6214,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:27">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>171</v>
       </c>
@@ -6269,7 +6278,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="83" spans="1:27">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>226</v>
       </c>
@@ -6336,7 +6345,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="84" spans="1:27">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>252</v>
       </c>
@@ -6400,7 +6409,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="85" spans="1:27">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>227</v>
       </c>
@@ -6464,7 +6473,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="86" spans="1:27">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B86" s="6"/>
       <c r="J86">
         <f t="shared" si="20"/>
@@ -6495,7 +6504,7 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="1:27">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>75</v>
       </c>
@@ -6533,7 +6542,7 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="1:27">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>82</v>
       </c>
@@ -6600,7 +6609,7 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="1:27">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>76</v>
       </c>
@@ -6667,7 +6676,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="1:27">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>136</v>
       </c>
@@ -6731,7 +6740,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="91" spans="1:27">
+    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>77</v>
       </c>
@@ -6798,7 +6807,7 @@
         <v/>
       </c>
     </row>
-    <row r="92" spans="1:27">
+    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>78</v>
       </c>
@@ -6868,7 +6877,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="93" spans="1:27">
+    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>159</v>
       </c>
@@ -6935,7 +6944,7 @@
         <v/>
       </c>
     </row>
-    <row r="94" spans="1:27">
+    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>156</v>
       </c>
@@ -7002,7 +7011,7 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="1:27">
+    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>160</v>
       </c>
@@ -7069,7 +7078,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="1:27">
+    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>122</v>
       </c>
@@ -7133,7 +7142,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="97" spans="1:25">
+    <row r="97" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>137</v>
       </c>
@@ -7197,7 +7206,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="98" spans="1:25">
+    <row r="98" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>80</v>
       </c>
@@ -7261,7 +7270,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="99" spans="1:25">
+    <row r="99" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>161</v>
       </c>
@@ -7325,7 +7334,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="100" spans="1:25">
+    <row r="100" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>149</v>
       </c>
@@ -7389,7 +7398,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="101" spans="1:25">
+    <row r="101" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>81</v>
       </c>
@@ -7453,7 +7462,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="102" spans="1:25">
+    <row r="102" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>153</v>
       </c>
@@ -7517,7 +7526,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="103" spans="1:25">
+    <row r="103" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>154</v>
       </c>
@@ -7581,7 +7590,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="104" spans="1:25">
+    <row r="104" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>232</v>
       </c>
@@ -7636,7 +7645,7 @@
         <v/>
       </c>
     </row>
-    <row r="105" spans="1:25">
+    <row r="105" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>120</v>
       </c>
@@ -7688,7 +7697,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="106" spans="1:25">
+    <row r="106" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>162</v>
       </c>
@@ -7743,7 +7752,7 @@
         <v/>
       </c>
     </row>
-    <row r="107" spans="1:25">
+    <row r="107" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>163</v>
       </c>
@@ -7795,7 +7804,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="108" spans="1:25">
+    <row r="108" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>84</v>
       </c>
@@ -7850,7 +7859,7 @@
         <v/>
       </c>
     </row>
-    <row r="109" spans="1:25">
+    <row r="109" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>230</v>
       </c>
@@ -7905,7 +7914,7 @@
         <v/>
       </c>
     </row>
-    <row r="110" spans="1:25">
+    <row r="110" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>229</v>
       </c>
@@ -7969,7 +7978,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="111" spans="1:25">
+    <row r="111" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>231</v>
       </c>
@@ -8033,7 +8042,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="112" spans="1:25">
+    <row r="112" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>83</v>
       </c>
@@ -8097,7 +8106,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="113" spans="1:25">
+    <row r="113" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>228</v>
       </c>
@@ -8161,7 +8170,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="114" spans="1:25">
+    <row r="114" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B114" s="6"/>
       <c r="D114">
         <f t="shared" ref="D114:D115" si="29">IF(F114=4, 1,0)</f>
@@ -8196,7 +8205,7 @@
         <v/>
       </c>
     </row>
-    <row r="115" spans="1:25">
+    <row r="115" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>85</v>
       </c>
@@ -8234,7 +8243,7 @@
         <v/>
       </c>
     </row>
-    <row r="116" spans="1:25">
+    <row r="116" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>235</v>
       </c>
@@ -8298,7 +8307,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="117" spans="1:25">
+    <row r="117" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>86</v>
       </c>
@@ -8362,7 +8371,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="118" spans="1:25">
+    <row r="118" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>236</v>
       </c>
@@ -8426,7 +8435,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="119" spans="1:25">
+    <row r="119" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>87</v>
       </c>
@@ -8490,7 +8499,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="120" spans="1:25">
+    <row r="120" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>88</v>
       </c>
@@ -8554,7 +8563,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="121" spans="1:25">
+    <row r="121" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>237</v>
       </c>
@@ -8618,7 +8627,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="122" spans="1:25">
+    <row r="122" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>238</v>
       </c>
@@ -8682,7 +8691,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="123" spans="1:25">
+    <row r="123" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>239</v>
       </c>
@@ -8746,7 +8755,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="124" spans="1:25">
+    <row r="124" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>240</v>
       </c>
@@ -8807,7 +8816,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="125" spans="1:25">
+    <row r="125" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B125" s="6"/>
       <c r="J125">
         <f t="shared" si="20"/>
@@ -8826,7 +8835,7 @@
         <v/>
       </c>
     </row>
-    <row r="126" spans="1:25">
+    <row r="126" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>210</v>
       </c>
@@ -8844,7 +8853,7 @@
         <v/>
       </c>
     </row>
-    <row r="127" spans="1:25">
+    <row r="127" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>211</v>
       </c>
@@ -8878,7 +8887,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="128" spans="1:25">
+    <row r="128" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>212</v>
       </c>
@@ -8912,7 +8921,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="129" spans="1:25">
+    <row r="129" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>213</v>
       </c>
@@ -8946,250 +8955,268 @@
         <v>100</v>
       </c>
     </row>
-    <row r="130" spans="1:25">
+    <row r="130" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>253</v>
+      </c>
       <c r="B130" s="6"/>
-    </row>
-    <row r="131" spans="1:25">
+      <c r="C130">
+        <v>1</v>
+      </c>
+      <c r="D130">
+        <v>1</v>
+      </c>
+      <c r="E130">
+        <v>1</v>
+      </c>
+      <c r="G130">
+        <v>1</v>
+      </c>
+      <c r="I130">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="131" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B131" s="6"/>
     </row>
-    <row r="132" spans="1:25">
+    <row r="132" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B132" s="6"/>
     </row>
-    <row r="133" spans="1:25">
+    <row r="133" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B133" s="6"/>
     </row>
-    <row r="134" spans="1:25">
+    <row r="134" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B134" s="6"/>
     </row>
-    <row r="135" spans="1:25">
+    <row r="135" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B135" s="6"/>
     </row>
-    <row r="136" spans="1:25">
+    <row r="136" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B136" s="6"/>
     </row>
-    <row r="137" spans="1:25">
+    <row r="137" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B137" s="6"/>
     </row>
-    <row r="138" spans="1:25">
+    <row r="138" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B138" s="6"/>
     </row>
-    <row r="139" spans="1:25">
+    <row r="139" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B139" s="6"/>
     </row>
-    <row r="140" spans="1:25">
+    <row r="140" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B140" s="6"/>
     </row>
-    <row r="141" spans="1:25">
+    <row r="141" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B141" s="6"/>
     </row>
-    <row r="142" spans="1:25">
+    <row r="142" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B142" s="6"/>
     </row>
-    <row r="143" spans="1:25">
+    <row r="143" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B143" s="6"/>
     </row>
-    <row r="144" spans="1:25">
+    <row r="144" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B144" s="6"/>
     </row>
-    <row r="145" spans="2:2">
+    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B145" s="6"/>
     </row>
-    <row r="146" spans="2:2">
+    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B146" s="6"/>
     </row>
-    <row r="147" spans="2:2">
+    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B147" s="6"/>
     </row>
-    <row r="148" spans="2:2">
+    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B148" s="6"/>
     </row>
-    <row r="149" spans="2:2">
+    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B149" s="6"/>
     </row>
-    <row r="150" spans="2:2">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B150" s="6"/>
     </row>
-    <row r="151" spans="2:2">
+    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B151" s="6"/>
     </row>
-    <row r="152" spans="2:2">
+    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B152" s="6"/>
     </row>
-    <row r="153" spans="2:2">
+    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B153" s="6"/>
     </row>
-    <row r="154" spans="2:2">
+    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B154" s="6"/>
     </row>
-    <row r="155" spans="2:2">
+    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B155" s="6"/>
     </row>
-    <row r="156" spans="2:2">
+    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B156" s="6"/>
     </row>
-    <row r="157" spans="2:2">
+    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B157" s="6"/>
     </row>
-    <row r="158" spans="2:2">
+    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B158" s="6"/>
     </row>
-    <row r="159" spans="2:2">
+    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B159" s="6"/>
     </row>
-    <row r="160" spans="2:2">
+    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B160" s="6"/>
     </row>
-    <row r="161" spans="2:2">
+    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B161" s="6"/>
     </row>
-    <row r="162" spans="2:2">
+    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B162" s="6"/>
     </row>
-    <row r="163" spans="2:2">
+    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B163" s="6"/>
     </row>
-    <row r="164" spans="2:2">
+    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B164" s="6"/>
     </row>
-    <row r="165" spans="2:2">
+    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B165" s="6"/>
     </row>
-    <row r="166" spans="2:2">
+    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B166" s="6"/>
     </row>
-    <row r="167" spans="2:2">
+    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B167" s="6"/>
     </row>
-    <row r="168" spans="2:2">
+    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B168" s="6"/>
     </row>
-    <row r="169" spans="2:2">
+    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B169" s="6"/>
     </row>
-    <row r="170" spans="2:2">
+    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B170" s="6"/>
     </row>
-    <row r="171" spans="2:2">
+    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B171" s="6"/>
     </row>
-    <row r="172" spans="2:2">
+    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B172" s="6"/>
     </row>
-    <row r="173" spans="2:2">
+    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B173" s="6"/>
     </row>
-    <row r="174" spans="2:2">
+    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B174" s="6"/>
     </row>
-    <row r="175" spans="2:2">
+    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B175" s="6"/>
     </row>
-    <row r="176" spans="2:2">
+    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B176" s="6"/>
     </row>
-    <row r="177" spans="2:2">
+    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B177" s="6"/>
     </row>
-    <row r="178" spans="2:2">
+    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B178" s="6"/>
     </row>
-    <row r="179" spans="2:2">
+    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B179" s="6"/>
     </row>
-    <row r="180" spans="2:2">
+    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B180" s="6"/>
     </row>
-    <row r="181" spans="2:2">
+    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B181" s="6"/>
     </row>
-    <row r="182" spans="2:2">
+    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B182" s="6"/>
     </row>
-    <row r="183" spans="2:2">
+    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B183" s="6"/>
     </row>
-    <row r="184" spans="2:2">
+    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B184" s="6"/>
     </row>
-    <row r="185" spans="2:2">
+    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B185" s="6"/>
     </row>
-    <row r="186" spans="2:2">
+    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B186" s="6"/>
     </row>
-    <row r="187" spans="2:2">
+    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B187" s="6"/>
     </row>
-    <row r="188" spans="2:2">
+    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B188" s="6"/>
     </row>
-    <row r="189" spans="2:2">
+    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B189" s="6"/>
     </row>
-    <row r="190" spans="2:2">
+    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B190" s="6"/>
     </row>
-    <row r="191" spans="2:2">
+    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B191" s="6"/>
     </row>
-    <row r="192" spans="2:2">
+    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B192" s="6"/>
     </row>
-    <row r="193" spans="2:2">
+    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B193" s="6"/>
     </row>
-    <row r="194" spans="2:2">
+    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B194" s="6"/>
     </row>
-    <row r="195" spans="2:2">
+    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B195" s="6"/>
     </row>
-    <row r="196" spans="2:2">
+    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B196" s="6"/>
     </row>
-    <row r="197" spans="2:2">
+    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B197" s="6"/>
     </row>
-    <row r="198" spans="2:2">
+    <row r="198" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B198" s="6"/>
     </row>
-    <row r="199" spans="2:2">
+    <row r="199" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B199" s="6"/>
     </row>
-    <row r="200" spans="2:2">
+    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B200" s="6"/>
     </row>
-    <row r="201" spans="2:2">
+    <row r="201" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B201" s="6"/>
     </row>
-    <row r="202" spans="2:2">
+    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B202" s="6"/>
     </row>
-    <row r="203" spans="2:2">
+    <row r="203" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B203" s="6"/>
     </row>
-    <row r="204" spans="2:2">
+    <row r="204" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B204" s="6"/>
     </row>
-    <row r="205" spans="2:2">
+    <row r="205" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B205" s="6"/>
     </row>
-    <row r="206" spans="2:2">
+    <row r="206" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B206" s="6"/>
     </row>
-    <row r="207" spans="2:2">
+    <row r="207" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B207" s="6"/>
     </row>
-    <row r="208" spans="2:2">
+    <row r="208" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B208" s="6"/>
     </row>
-    <row r="209" spans="2:2">
+    <row r="209" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B209" s="6"/>
     </row>
-    <row r="210" spans="2:2">
+    <row r="210" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B210" s="6"/>
     </row>
-    <row r="211" spans="2:2">
+    <row r="211" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B211" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added haluska guest, changed colors
</commit_message>
<xml_diff>
--- a/Guest_List_Invited.xlsx
+++ b/Guest_List_Invited.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\logan\Documents\GitHub\Farrell_Garrett_Wedding\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA04181F-D130-4636-967E-73ED81F08E05}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="171027"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="261">
   <si>
     <t xml:space="preserve">Priority </t>
   </si>
@@ -198,9 +204,6 @@
     <t>Mi-Sun Bae</t>
   </si>
   <si>
-    <t>Michael Haluska</t>
-  </si>
-  <si>
     <t>Gary Jordan and Liz Roti-Roti</t>
   </si>
   <si>
@@ -799,16 +802,22 @@
   </si>
   <si>
     <t xml:space="preserve">Dutch Oven </t>
+  </si>
+  <si>
+    <t>Michael Haluska and Kelly Regimbal</t>
+  </si>
+  <si>
+    <t>both chicken</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -937,11 +946,95 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="14">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF7C80"/>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1225,22 +1318,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA211"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AC211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1:E1"/>
+      <pane ySplit="4" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.85546875" customWidth="1"/>
     <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
@@ -1265,54 +1358,54 @@
     <col min="27" max="27" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15" customHeight="1">
+    <row r="1" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5">
         <v>4</v>
       </c>
       <c r="B1" s="15"/>
       <c r="D1" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E1" s="20"/>
       <c r="F1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G1">
         <f>SUM(G6:G11,G14:G41,G45:G50,G53:G59,G62:G85,G88:G113,G116:G124,G127:G129)</f>
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="T1" s="10"/>
       <c r="U1" s="10"/>
       <c r="V1" s="10"/>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>3</v>
       </c>
       <c r="B2" s="6"/>
       <c r="D2" s="19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E2" s="19"/>
       <c r="G2" s="19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H2" s="19"/>
       <c r="I2" s="19"/>
       <c r="J2" s="11"/>
       <c r="K2" s="11"/>
       <c r="P2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="Q2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="R2" s="14">
         <f>D3+G3*(1+Z4/100)</f>
-        <v>148.14746094485622</v>
+        <v>149.13321355274704</v>
       </c>
       <c r="S2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T2" s="10"/>
       <c r="U2" s="10"/>
@@ -1323,44 +1416,44 @@
         <v>28.53908325175902</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D3" s="19">
         <f>SUM(E6:E129)</f>
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3">
         <f>SUM(J6:J173)</f>
-        <v>128.59999999999997</v>
+        <v>129.89999999999998</v>
       </c>
       <c r="G3">
         <f>SUM(O6:O129)</f>
-        <v>68.599999999999966</v>
+        <v>66.899999999999977</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
       <c r="P3" s="12">
         <f>G3+D3</f>
-        <v>128.59999999999997</v>
+        <v>129.89999999999998</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="R3" s="14">
         <f>D3+G3*(1-Z4/100)</f>
-        <v>109.05253905514371</v>
+        <v>110.66678644725292</v>
       </c>
       <c r="S3" s="13">
         <f>SUM(X6:X129)/COUNT(X6:X11,X14:X41,X45:X50,X53:X59,X62:X85,X88:X113,X116:X124,X127:X129)</f>
-        <v>0.42201834862385323</v>
+        <v>0.44036697247706424</v>
       </c>
       <c r="T3" s="10"/>
       <c r="U3" s="10"/>
@@ -1369,10 +1462,10 @@
         <v>34</v>
       </c>
       <c r="Z3" s="10" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" s="10" customFormat="1" ht="31.5" customHeight="1">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="10" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -1381,37 +1474,37 @@
         <v>33</v>
       </c>
       <c r="D4" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="N4" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>217</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="L4" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>90</v>
-      </c>
       <c r="O4" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P4" s="10" t="s">
         <v>2</v>
@@ -1420,29 +1513,29 @@
         <v>3</v>
       </c>
       <c r="T4" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="U4" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="U4" s="10" t="s">
+      <c r="V4" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="V4" s="10" t="s">
-        <v>127</v>
-      </c>
       <c r="W4" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="Y4" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Z4" s="10">
         <f>STDEV(Y6:Y129)</f>
-        <v>28.494841027487261</v>
+        <v>28.749198135645848</v>
       </c>
       <c r="AA4" s="10" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1452,7 +1545,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:27">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1502,13 +1595,13 @@
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="T6">
         <v>1</v>
       </c>
       <c r="U6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X6">
         <f t="shared" ref="X6:X11" si="1">IF(ISNUMBER(E6),1,0)</f>
@@ -1519,7 +1612,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:27">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1569,13 +1662,13 @@
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="T7">
         <v>1</v>
       </c>
       <c r="U7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X7">
         <f t="shared" si="1"/>
@@ -1586,7 +1679,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:27">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1636,13 +1729,13 @@
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="T8">
         <v>1</v>
       </c>
       <c r="U8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X8">
         <f t="shared" si="1"/>
@@ -1653,7 +1746,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:27">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1703,13 +1796,13 @@
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="T9">
         <v>1</v>
       </c>
       <c r="U9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X9">
         <f t="shared" si="1"/>
@@ -1720,7 +1813,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1770,13 +1863,13 @@
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="T10">
         <v>1</v>
       </c>
       <c r="U10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X10">
         <f t="shared" si="1"/>
@@ -1787,7 +1880,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:27">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -1837,7 +1930,7 @@
         <v>0</v>
       </c>
       <c r="P11" s="18" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="Q11" s="8"/>
       <c r="R11" s="8"/>
@@ -1845,7 +1938,7 @@
         <v>1</v>
       </c>
       <c r="U11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X11">
         <f t="shared" si="1"/>
@@ -1856,7 +1949,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:27">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
       <c r="C12" s="1"/>
       <c r="D12">
@@ -1891,8 +1984,15 @@
         <f t="shared" si="7"/>
         <v/>
       </c>
-    </row>
-    <row r="13" spans="1:27">
+      <c r="AB12">
+        <v>1</v>
+      </c>
+      <c r="AC12" t="b">
+        <f>AND(IF(AB12&gt;0,1,0),ISNUMBER(AB12))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -1930,7 +2030,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:27">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
@@ -1977,13 +2077,13 @@
         <v>1</v>
       </c>
       <c r="P14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="T14">
         <v>1</v>
       </c>
       <c r="U14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X14">
         <f t="shared" ref="X14:X40" si="10">IF(ISNUMBER(E14),1,0)</f>
@@ -1994,7 +2094,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:27">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -2041,13 +2141,13 @@
         <v>1</v>
       </c>
       <c r="P15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="T15">
         <v>1</v>
       </c>
       <c r="U15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X15">
         <f t="shared" si="10"/>
@@ -2058,7 +2158,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:27">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
@@ -2105,7 +2205,7 @@
         <v>1</v>
       </c>
       <c r="P16" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Q16" s="7"/>
       <c r="R16" s="7"/>
@@ -2114,7 +2214,7 @@
         <v>1</v>
       </c>
       <c r="U16" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X16">
         <f t="shared" si="10"/>
@@ -2125,7 +2225,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:27">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
@@ -2172,13 +2272,13 @@
         <v>0.5</v>
       </c>
       <c r="P17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="T17">
         <v>1</v>
       </c>
       <c r="U17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X17">
         <f t="shared" si="10"/>
@@ -2189,7 +2289,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:27">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
@@ -2236,13 +2336,13 @@
         <v>1</v>
       </c>
       <c r="P18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="T18">
         <v>1</v>
       </c>
       <c r="U18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X18">
         <f t="shared" si="10"/>
@@ -2253,9 +2353,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:27">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B19" s="7">
         <v>12</v>
@@ -2300,7 +2400,7 @@
         <v>0.5</v>
       </c>
       <c r="P19" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="Q19" s="6"/>
       <c r="R19" s="6"/>
@@ -2309,7 +2409,7 @@
         <v>1</v>
       </c>
       <c r="U19" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X19">
         <f t="shared" si="10"/>
@@ -2320,7 +2420,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:27">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -2367,7 +2467,7 @@
         <v>0.5</v>
       </c>
       <c r="P20" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
@@ -2376,7 +2476,7 @@
         <v>1</v>
       </c>
       <c r="U20" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X20">
         <f t="shared" si="10"/>
@@ -2387,7 +2487,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:27">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
@@ -2434,13 +2534,13 @@
         <v>1</v>
       </c>
       <c r="P21" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="T21">
         <v>1</v>
       </c>
       <c r="U21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X21">
         <f t="shared" si="10"/>
@@ -2451,7 +2551,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:27">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
@@ -2498,13 +2598,13 @@
         <v>1</v>
       </c>
       <c r="P22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="T22">
         <v>1</v>
       </c>
       <c r="U22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X22">
         <f t="shared" si="10"/>
@@ -2515,9 +2615,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:27">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B23" s="7">
         <v>16</v>
@@ -2562,7 +2662,7 @@
         <v>0.5</v>
       </c>
       <c r="P23" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
@@ -2571,7 +2671,7 @@
         <v>1</v>
       </c>
       <c r="U23" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X23">
         <f t="shared" si="10"/>
@@ -2582,7 +2682,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:27">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>17</v>
       </c>
@@ -2632,19 +2732,19 @@
         <v>0</v>
       </c>
       <c r="P24" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="S24" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="T24">
         <v>1</v>
       </c>
       <c r="U24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="W24" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="X24">
         <f t="shared" si="10"/>
@@ -2655,10 +2755,10 @@
         <v/>
       </c>
       <c r="AA24" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="25" spans="1:27">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>18</v>
       </c>
@@ -2708,16 +2808,16 @@
         <v>0</v>
       </c>
       <c r="P25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="T25">
         <v>1</v>
       </c>
       <c r="U25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="W25" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="X25">
         <f t="shared" si="10"/>
@@ -2728,10 +2828,10 @@
         <v/>
       </c>
       <c r="AA25" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="26" spans="1:27">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>19</v>
       </c>
@@ -2778,13 +2878,13 @@
         <v>0.5</v>
       </c>
       <c r="P26" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="T26">
         <v>1</v>
       </c>
       <c r="U26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X26">
         <f t="shared" si="10"/>
@@ -2795,7 +2895,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:27">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>20</v>
       </c>
@@ -2845,13 +2945,13 @@
         <v>0</v>
       </c>
       <c r="P27" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="T27">
         <v>1</v>
       </c>
       <c r="U27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X27">
         <f t="shared" si="10"/>
@@ -2862,7 +2962,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:27">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>21</v>
       </c>
@@ -2912,13 +3012,13 @@
         <v>0</v>
       </c>
       <c r="P28" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="T28">
         <v>1</v>
       </c>
       <c r="U28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X28">
         <f t="shared" si="10"/>
@@ -2929,7 +3029,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:27">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>22</v>
       </c>
@@ -2979,13 +3079,13 @@
         <v>0</v>
       </c>
       <c r="P29" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="T29">
         <v>1</v>
       </c>
       <c r="U29" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X29">
         <f t="shared" si="10"/>
@@ -2996,7 +3096,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:27">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>23</v>
       </c>
@@ -3043,13 +3143,13 @@
         <v>0.5</v>
       </c>
       <c r="P30" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="T30">
         <v>1</v>
       </c>
       <c r="U30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X30">
         <f t="shared" si="10"/>
@@ -3060,7 +3160,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:27">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>24</v>
       </c>
@@ -3107,13 +3207,13 @@
         <v>0.5</v>
       </c>
       <c r="P31" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="T31">
         <v>1</v>
       </c>
       <c r="U31" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X31">
         <f t="shared" si="10"/>
@@ -3124,7 +3224,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:27">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>25</v>
       </c>
@@ -3171,13 +3271,13 @@
         <v>0.5</v>
       </c>
       <c r="P32" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="T32">
         <v>1</v>
       </c>
       <c r="U32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X32">
         <f t="shared" si="10"/>
@@ -3188,7 +3288,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:27">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>26</v>
       </c>
@@ -3235,13 +3335,13 @@
         <v>0.5</v>
       </c>
       <c r="P33" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="T33">
         <v>1</v>
       </c>
       <c r="U33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X33">
         <f t="shared" si="10"/>
@@ -3252,7 +3352,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:27">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
@@ -3302,16 +3402,16 @@
         <v>0</v>
       </c>
       <c r="P34" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="T34">
         <v>1</v>
       </c>
       <c r="U34" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="W34" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="X34">
         <f t="shared" si="10"/>
@@ -3322,10 +3422,10 @@
         <v/>
       </c>
       <c r="AA34" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="35" spans="1:27">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
@@ -3372,13 +3472,13 @@
         <v>2</v>
       </c>
       <c r="P35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="T35">
         <v>1</v>
       </c>
       <c r="U35" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X35">
         <f t="shared" si="10"/>
@@ -3389,7 +3489,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:27">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>40</v>
       </c>
@@ -3436,13 +3536,13 @@
         <v>1</v>
       </c>
       <c r="P36" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="T36">
         <v>1</v>
       </c>
       <c r="U36" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X36">
         <f t="shared" si="10"/>
@@ -3453,7 +3553,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:27">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>41</v>
       </c>
@@ -3500,13 +3600,13 @@
         <v>1</v>
       </c>
       <c r="P37" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="T37">
         <v>1</v>
       </c>
       <c r="U37" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X37">
         <f t="shared" si="10"/>
@@ -3517,7 +3617,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:27">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>42</v>
       </c>
@@ -3567,16 +3667,16 @@
         <v>0</v>
       </c>
       <c r="P38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="T38">
         <v>1</v>
       </c>
       <c r="U38" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="W38" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="X38">
         <f t="shared" si="10"/>
@@ -3587,10 +3687,10 @@
         <v/>
       </c>
       <c r="AA38" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="39" spans="1:27">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>43</v>
       </c>
@@ -3640,13 +3740,13 @@
         <v>0</v>
       </c>
       <c r="P39" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="T39">
         <v>1</v>
       </c>
       <c r="U39" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X39">
         <f t="shared" si="10"/>
@@ -3657,7 +3757,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:27">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>44</v>
       </c>
@@ -3707,16 +3807,16 @@
         <v>0</v>
       </c>
       <c r="P40" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="S40" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="T40">
         <v>1</v>
       </c>
       <c r="U40" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X40">
         <f t="shared" si="10"/>
@@ -3727,9 +3827,9 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:27">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B41" s="7">
         <v>34</v>
@@ -3774,13 +3874,13 @@
         <v>0.5</v>
       </c>
       <c r="P41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="T41">
         <v>1</v>
       </c>
       <c r="U41" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X41">
         <f>IF(ISNUMBER(E41),1,0)</f>
@@ -3791,7 +3891,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:27">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="7"/>
       <c r="D42">
@@ -3827,7 +3927,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:27">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B43" s="6"/>
       <c r="C43" s="1"/>
       <c r="D43">
@@ -3863,7 +3963,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:27">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>27</v>
       </c>
@@ -3901,7 +4001,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:27">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>28</v>
       </c>
@@ -3951,19 +4051,19 @@
         <v>0</v>
       </c>
       <c r="P45" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="S45" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="T45">
         <v>1</v>
       </c>
       <c r="U45" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="W45" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="X45">
         <f t="shared" ref="X45:X50" si="11">IF(ISNUMBER(E45),1,0)</f>
@@ -3974,10 +4074,10 @@
         <v/>
       </c>
       <c r="AA45" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="46" spans="1:27">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>29</v>
       </c>
@@ -4024,13 +4124,13 @@
         <v>0.4</v>
       </c>
       <c r="P46" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="T46">
         <v>1</v>
       </c>
       <c r="U46" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X46">
         <f t="shared" si="11"/>
@@ -4041,7 +4141,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:27">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>30</v>
       </c>
@@ -4091,13 +4191,13 @@
         <v>0</v>
       </c>
       <c r="P47" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="T47">
         <v>1</v>
       </c>
       <c r="U47" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X47">
         <f t="shared" si="11"/>
@@ -4108,7 +4208,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:27">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>31</v>
       </c>
@@ -4155,7 +4255,7 @@
         <v>0.2</v>
       </c>
       <c r="P48" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="S48" t="s">
         <v>45</v>
@@ -4164,7 +4264,7 @@
         <v>1</v>
       </c>
       <c r="U48" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X48">
         <f t="shared" si="11"/>
@@ -4175,7 +4275,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:25">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>32</v>
       </c>
@@ -4225,7 +4325,7 @@
         <v>0</v>
       </c>
       <c r="P49" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="S49" t="s">
         <v>45</v>
@@ -4234,7 +4334,7 @@
         <v>1</v>
       </c>
       <c r="U49" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X49">
         <f t="shared" si="11"/>
@@ -4245,9 +4345,9 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:25">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B50" s="6">
         <v>40</v>
@@ -4292,7 +4392,7 @@
         <v>0.5</v>
       </c>
       <c r="P50" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Q50" s="6"/>
       <c r="R50" s="6"/>
@@ -4303,7 +4403,7 @@
         <v>1</v>
       </c>
       <c r="U50" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X50">
         <f t="shared" si="11"/>
@@ -4313,8 +4413,11 @@
         <f t="shared" si="7"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="51" spans="1:25">
+      <c r="AC50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B51" s="6"/>
       <c r="J51">
         <f t="shared" si="9"/>
@@ -4345,7 +4448,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:25">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>49</v>
       </c>
@@ -4383,7 +4486,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:25">
+    <row r="53" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>48</v>
       </c>
@@ -4433,7 +4536,7 @@
         <v>0</v>
       </c>
       <c r="P53" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Q53" s="6"/>
       <c r="R53" s="6"/>
@@ -4442,7 +4545,7 @@
         <v>1</v>
       </c>
       <c r="U53" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="V53" s="6"/>
       <c r="X53">
@@ -4454,7 +4557,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:25">
+    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>51</v>
       </c>
@@ -4501,7 +4604,7 @@
         <v>2</v>
       </c>
       <c r="P54" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Q54" s="6"/>
       <c r="R54" s="6"/>
@@ -4510,7 +4613,7 @@
         <v>1</v>
       </c>
       <c r="U54" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X54">
         <f t="shared" si="12"/>
@@ -4521,7 +4624,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:25">
+    <row r="55" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>50</v>
       </c>
@@ -4571,7 +4674,7 @@
         <v>0</v>
       </c>
       <c r="P55" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="Q55" s="6"/>
       <c r="R55" s="6"/>
@@ -4580,7 +4683,7 @@
         <v>1</v>
       </c>
       <c r="U55" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="V55" s="6"/>
       <c r="X55">
@@ -4592,9 +4695,9 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:25">
+    <row r="56" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B56" s="6">
         <v>44</v>
@@ -4642,13 +4745,13 @@
         <v>0</v>
       </c>
       <c r="P56" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="T56">
         <v>1</v>
       </c>
       <c r="U56" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X56">
         <f t="shared" si="12"/>
@@ -4659,7 +4762,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:25">
+    <row r="57" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>52</v>
       </c>
@@ -4709,16 +4812,16 @@
         <v>0</v>
       </c>
       <c r="P57" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="T57">
         <v>1</v>
       </c>
       <c r="U57" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="V57" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X57">
         <f t="shared" si="12"/>
@@ -4729,7 +4832,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:25">
+    <row r="58" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>53</v>
       </c>
@@ -4779,16 +4882,16 @@
         <v>0</v>
       </c>
       <c r="P58" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="S58" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="T58">
         <v>1</v>
       </c>
       <c r="U58" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X58">
         <f t="shared" si="12"/>
@@ -4799,7 +4902,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:25">
+    <row r="59" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>54</v>
       </c>
@@ -4849,13 +4952,13 @@
         <v>0</v>
       </c>
       <c r="P59" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="T59">
         <v>1</v>
       </c>
       <c r="U59" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X59">
         <f t="shared" si="12"/>
@@ -4866,7 +4969,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:25">
+    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B60" s="6"/>
       <c r="J60">
         <f t="shared" si="9"/>
@@ -4897,14 +5000,14 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:25">
+    <row r="61" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B61" s="17"/>
       <c r="D61">
         <f>SUM(J62:J84)</f>
-        <v>28.999999999999993</v>
+        <v>30.099999999999991</v>
       </c>
       <c r="J61">
         <f t="shared" si="9"/>
@@ -4935,9 +5038,9 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:25">
+    <row r="62" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B62" s="6">
         <v>48</v>
@@ -4982,7 +5085,7 @@
         <v>1.8</v>
       </c>
       <c r="P62" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="Q62" s="6"/>
       <c r="R62" s="6"/>
@@ -4991,7 +5094,7 @@
         <v>1</v>
       </c>
       <c r="U62" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="V62" s="6"/>
       <c r="X62">
@@ -5003,7 +5106,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="63" spans="1:25">
+    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>55</v>
       </c>
@@ -5050,7 +5153,7 @@
         <v>1.8</v>
       </c>
       <c r="P63" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q63" s="6"/>
       <c r="R63" s="6"/>
@@ -5059,7 +5162,7 @@
         <v>1</v>
       </c>
       <c r="U63" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="V63" s="6"/>
       <c r="X63">
@@ -5071,7 +5174,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="64" spans="1:25">
+    <row r="64" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>56</v>
       </c>
@@ -5118,18 +5221,18 @@
         <v>0.9</v>
       </c>
       <c r="P64" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q64" s="6"/>
       <c r="R64" s="6"/>
       <c r="S64" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="T64" s="6">
         <v>1</v>
       </c>
       <c r="U64" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="V64" s="6"/>
       <c r="X64">
@@ -5141,7 +5244,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="1:25">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>57</v>
       </c>
@@ -5188,7 +5291,7 @@
         <v>0.9</v>
       </c>
       <c r="P65" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Q65" s="6"/>
       <c r="R65" s="6"/>
@@ -5197,7 +5300,7 @@
         <v>1</v>
       </c>
       <c r="U65" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="V65" s="6"/>
       <c r="X65">
@@ -5209,9 +5312,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="66" spans="1:25">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B66" s="6">
         <v>52</v>
@@ -5259,7 +5362,7 @@
         <v>0</v>
       </c>
       <c r="P66" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Q66" s="6"/>
       <c r="R66" s="6"/>
@@ -5268,7 +5371,7 @@
         <v>1</v>
       </c>
       <c r="U66" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="V66" s="6"/>
       <c r="X66">
@@ -5280,9 +5383,9 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B67" s="6">
         <v>53</v>
@@ -5315,18 +5418,18 @@
         <v>0</v>
       </c>
       <c r="P67" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Q67" s="6"/>
       <c r="R67" s="6"/>
       <c r="S67" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="T67" s="6">
         <v>1</v>
       </c>
       <c r="U67" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="V67" s="6"/>
       <c r="X67">
@@ -5338,7 +5441,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:25">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>58</v>
       </c>
@@ -5385,7 +5488,7 @@
         <v>0.9</v>
       </c>
       <c r="P68" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q68" s="6"/>
       <c r="R68" s="6"/>
@@ -5394,7 +5497,7 @@
         <v>1</v>
       </c>
       <c r="U68" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="V68" s="6"/>
       <c r="X68">
@@ -5406,9 +5509,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="69" spans="1:25">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>59</v>
+        <v>259</v>
       </c>
       <c r="B69" s="6">
         <v>55</v>
@@ -5419,64 +5522,69 @@
       <c r="D69">
         <v>1</v>
       </c>
+      <c r="E69">
+        <v>2</v>
+      </c>
       <c r="F69">
         <v>4</v>
       </c>
       <c r="G69">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I69">
         <v>90</v>
       </c>
       <c r="J69">
         <f t="shared" si="9"/>
-        <v>0.9</v>
+        <v>2</v>
       </c>
       <c r="K69">
         <f t="shared" si="2"/>
-        <v>0.9</v>
+        <v>2</v>
       </c>
       <c r="L69">
         <f t="shared" si="3"/>
-        <v>0.9</v>
+        <v>2</v>
       </c>
       <c r="M69">
         <f t="shared" si="4"/>
-        <v>0.9</v>
+        <v>2</v>
       </c>
       <c r="N69">
         <f t="shared" si="5"/>
-        <v>0.9</v>
+        <v>1.8</v>
       </c>
       <c r="O69">
         <f t="shared" ref="O69:O121" si="14">IF(ISNUMBER(E69), 0, J69)</f>
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="P69" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Q69" s="6"/>
       <c r="R69" s="6"/>
-      <c r="S69" s="6"/>
+      <c r="S69" s="6" t="s">
+        <v>260</v>
+      </c>
       <c r="T69" s="6">
         <v>1</v>
       </c>
       <c r="U69" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="V69" s="6"/>
       <c r="X69">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="Y69">
+        <v>1</v>
+      </c>
+      <c r="Y69" t="str">
         <f t="shared" si="7"/>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="70" spans="1:25">
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B70" s="6">
         <v>56</v>
@@ -5524,7 +5632,7 @@
         <v>0</v>
       </c>
       <c r="P70" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q70" s="6"/>
       <c r="R70" s="6"/>
@@ -5533,7 +5641,7 @@
         <v>1</v>
       </c>
       <c r="U70" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="V70" s="6"/>
       <c r="X70">
@@ -5545,9 +5653,9 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:25">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B71" s="6">
         <v>57</v>
@@ -5595,16 +5703,16 @@
         <v>0</v>
       </c>
       <c r="P71" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="T71">
         <v>1</v>
       </c>
       <c r="U71" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="V71" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X71">
         <f t="shared" si="13"/>
@@ -5615,9 +5723,9 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:25">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B72" s="6">
         <v>58</v>
@@ -5665,16 +5773,16 @@
         <v>0</v>
       </c>
       <c r="P72" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="T72">
         <v>1</v>
       </c>
       <c r="U72" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="V72" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X72">
         <f t="shared" si="13"/>
@@ -5685,9 +5793,9 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:25">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B73" s="6">
         <v>59</v>
@@ -5735,13 +5843,13 @@
         <v>0</v>
       </c>
       <c r="P73" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="T73">
         <v>1</v>
       </c>
       <c r="U73" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X73">
         <f t="shared" si="13"/>
@@ -5752,9 +5860,9 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:25">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B74" s="6">
         <v>60</v>
@@ -5799,13 +5907,13 @@
         <v>0.9</v>
       </c>
       <c r="P74" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="T74">
         <v>1</v>
       </c>
       <c r="U74" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X74">
         <f t="shared" si="13"/>
@@ -5816,9 +5924,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="75" spans="1:25">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B75" s="6">
         <v>61</v>
@@ -5863,13 +5971,13 @@
         <v>0.9</v>
       </c>
       <c r="P75" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="T75">
         <v>1</v>
       </c>
       <c r="U75" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X75">
         <f t="shared" si="13"/>
@@ -5880,9 +5988,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="76" spans="1:25">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B76" s="6">
         <v>62</v>
@@ -5930,16 +6038,16 @@
         <v>0</v>
       </c>
       <c r="P76" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="T76">
         <v>1</v>
       </c>
       <c r="U76" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="V76" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X76">
         <f t="shared" si="13"/>
@@ -5950,9 +6058,9 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:25">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B77" s="6">
         <v>63</v>
@@ -6000,13 +6108,13 @@
         <v>0</v>
       </c>
       <c r="P77" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="T77">
         <v>1</v>
       </c>
       <c r="U77" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X77">
         <f t="shared" si="13"/>
@@ -6017,9 +6125,9 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:25">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B78" s="6">
         <v>64</v>
@@ -6064,13 +6172,13 @@
         <v>0.9</v>
       </c>
       <c r="P78" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T78">
         <v>1</v>
       </c>
       <c r="U78" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X78">
         <f t="shared" si="13"/>
@@ -6081,9 +6189,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="79" spans="1:25">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B79" s="6">
         <v>65</v>
@@ -6128,13 +6236,13 @@
         <v>0.9</v>
       </c>
       <c r="P79" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T79">
         <v>1</v>
       </c>
       <c r="U79" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X79">
         <f t="shared" si="13"/>
@@ -6145,9 +6253,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="80" spans="1:25">
+    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B80" s="6">
         <v>66</v>
@@ -6192,13 +6300,13 @@
         <v>0.9</v>
       </c>
       <c r="P80" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="T80">
         <v>1</v>
       </c>
       <c r="U80" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X80">
         <f t="shared" si="13"/>
@@ -6209,9 +6317,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="81" spans="1:27">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B81" s="6">
         <v>67</v>
@@ -6259,13 +6367,13 @@
         <v>0</v>
       </c>
       <c r="P81" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="T81" s="6">
         <v>1</v>
       </c>
       <c r="U81" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X81">
         <f t="shared" si="13"/>
@@ -6276,9 +6384,9 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:27">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B82" s="6">
         <v>68</v>
@@ -6323,13 +6431,13 @@
         <v>0.9</v>
       </c>
       <c r="P82" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="T82">
         <v>1</v>
       </c>
       <c r="U82" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X82">
         <f t="shared" si="13"/>
@@ -6340,9 +6448,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="83" spans="1:27">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B83" s="6">
         <v>69</v>
@@ -6387,7 +6495,7 @@
         <v>0.9</v>
       </c>
       <c r="P83" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Q83" s="6"/>
       <c r="R83" s="6"/>
@@ -6396,7 +6504,7 @@
         <v>1</v>
       </c>
       <c r="U83" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X83">
         <f t="shared" si="13"/>
@@ -6407,9 +6515,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="84" spans="1:27">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B84" s="6">
         <v>70</v>
@@ -6454,13 +6562,13 @@
         <v>0.5</v>
       </c>
       <c r="P84" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="T84">
         <v>1</v>
       </c>
       <c r="U84" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X84">
         <f t="shared" si="13"/>
@@ -6471,9 +6579,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="85" spans="1:27">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B85" s="6">
         <v>71</v>
@@ -6518,13 +6626,13 @@
         <v>1.8</v>
       </c>
       <c r="P85" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T85">
         <v>1</v>
       </c>
       <c r="U85" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X85">
         <f t="shared" si="13"/>
@@ -6535,7 +6643,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="86" spans="1:27">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B86" s="6"/>
       <c r="J86">
         <f t="shared" si="20"/>
@@ -6566,9 +6674,9 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="1:27">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B87" s="17"/>
       <c r="D87">
@@ -6604,9 +6712,9 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="1:27">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B88" s="7">
         <v>72</v>
@@ -6654,13 +6762,13 @@
         <v>0</v>
       </c>
       <c r="P88" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="T88">
         <v>1</v>
       </c>
       <c r="U88" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X88">
         <f t="shared" ref="X88:X113" si="24">IF(ISNUMBER(E88),1,0)</f>
@@ -6671,9 +6779,9 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="1:27">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B89" s="7">
         <v>73</v>
@@ -6721,13 +6829,13 @@
         <v>0</v>
       </c>
       <c r="P89" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="T89">
         <v>1</v>
       </c>
       <c r="U89" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X89">
         <f t="shared" si="24"/>
@@ -6738,9 +6846,9 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="1:27">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B90" s="7">
         <v>74</v>
@@ -6785,13 +6893,13 @@
         <v>1.6</v>
       </c>
       <c r="P90" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="T90">
         <v>1</v>
       </c>
       <c r="U90" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X90">
         <f t="shared" si="24"/>
@@ -6802,9 +6910,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="91" spans="1:27">
+    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B91" s="7">
         <v>75</v>
@@ -6852,13 +6960,13 @@
         <v>0</v>
       </c>
       <c r="P91" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="T91">
         <v>1</v>
       </c>
       <c r="U91" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X91">
         <f t="shared" si="24"/>
@@ -6869,9 +6977,9 @@
         <v/>
       </c>
     </row>
-    <row r="92" spans="1:27">
+    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B92" s="7">
         <v>76</v>
@@ -6916,16 +7024,16 @@
         <v>1.6</v>
       </c>
       <c r="P92" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="T92">
         <v>1</v>
       </c>
       <c r="U92" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="W92" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="X92">
         <f t="shared" si="24"/>
@@ -6936,12 +7044,12 @@
         <v>80</v>
       </c>
       <c r="AA92" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="93" spans="1:27">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B93" s="7">
         <v>77</v>
@@ -6989,13 +7097,13 @@
         <v>0</v>
       </c>
       <c r="P93" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="T93">
         <v>1</v>
       </c>
       <c r="U93" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X93">
         <f t="shared" si="24"/>
@@ -7006,9 +7114,9 @@
         <v/>
       </c>
     </row>
-    <row r="94" spans="1:27">
+    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B94" s="7">
         <v>78</v>
@@ -7056,13 +7164,13 @@
         <v>0</v>
       </c>
       <c r="P94" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="T94">
         <v>1</v>
       </c>
       <c r="U94" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X94">
         <f t="shared" si="24"/>
@@ -7073,9 +7181,9 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="1:27">
+    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B95" s="7">
         <v>79</v>
@@ -7123,13 +7231,13 @@
         <v>0</v>
       </c>
       <c r="P95" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="T95">
         <v>1</v>
       </c>
       <c r="U95" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X95">
         <f t="shared" si="24"/>
@@ -7140,9 +7248,9 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="1:27">
+    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B96" s="7">
         <v>80</v>
@@ -7187,13 +7295,13 @@
         <v>1</v>
       </c>
       <c r="P96" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="T96">
         <v>1</v>
       </c>
       <c r="U96" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X96">
         <f t="shared" si="24"/>
@@ -7204,9 +7312,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="97" spans="1:25">
+    <row r="97" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B97" s="7">
         <v>81</v>
@@ -7251,13 +7359,13 @@
         <v>0.5</v>
       </c>
       <c r="P97" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="T97">
         <v>1</v>
       </c>
       <c r="U97" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X97">
         <f t="shared" si="24"/>
@@ -7268,9 +7376,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="98" spans="1:25">
+    <row r="98" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B98" s="7">
         <v>82</v>
@@ -7318,13 +7426,13 @@
         <v>0</v>
       </c>
       <c r="P98" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="T98">
         <v>1</v>
       </c>
       <c r="U98" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X98">
         <f t="shared" si="24"/>
@@ -7335,9 +7443,9 @@
         <v/>
       </c>
     </row>
-    <row r="99" spans="1:25">
+    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B99" s="7">
         <v>83</v>
@@ -7385,16 +7493,16 @@
         <v>0</v>
       </c>
       <c r="P99" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="T99">
         <v>1</v>
       </c>
       <c r="U99" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="W99" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="X99">
         <f t="shared" si="24"/>
@@ -7404,10 +7512,13 @@
         <f t="shared" si="19"/>
         <v/>
       </c>
-    </row>
-    <row r="100" spans="1:25">
+      <c r="AA99" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B100" s="7">
         <v>84</v>
@@ -7452,13 +7563,13 @@
         <v>0.9</v>
       </c>
       <c r="P100" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="T100">
         <v>1</v>
       </c>
       <c r="U100" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X100">
         <f t="shared" si="24"/>
@@ -7469,9 +7580,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="101" spans="1:25">
+    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B101" s="7">
         <v>85</v>
@@ -7516,13 +7627,13 @@
         <v>0.8</v>
       </c>
       <c r="P101" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="T101">
         <v>1</v>
       </c>
       <c r="U101" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X101">
         <f t="shared" si="24"/>
@@ -7533,9 +7644,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="102" spans="1:25">
+    <row r="102" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B102" s="7">
         <v>86</v>
@@ -7580,13 +7691,13 @@
         <v>1.6</v>
       </c>
       <c r="P102" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="T102">
         <v>1</v>
       </c>
       <c r="U102" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X102">
         <f t="shared" si="24"/>
@@ -7597,9 +7708,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="103" spans="1:25">
+    <row r="103" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B103" s="7">
         <v>87</v>
@@ -7647,13 +7758,13 @@
         <v>0</v>
       </c>
       <c r="P103" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T103">
         <v>1</v>
       </c>
       <c r="U103" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X103">
         <f t="shared" si="24"/>
@@ -7664,9 +7775,9 @@
         <v/>
       </c>
     </row>
-    <row r="104" spans="1:25">
+    <row r="104" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B104" s="7">
         <v>88</v>
@@ -7702,16 +7813,16 @@
         <v>0</v>
       </c>
       <c r="P104" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="S104" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="T104">
         <v>1</v>
       </c>
       <c r="U104" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X104">
         <f t="shared" si="24"/>
@@ -7722,9 +7833,9 @@
         <v/>
       </c>
     </row>
-    <row r="105" spans="1:25">
+    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B105" s="7">
         <v>89</v>
@@ -7757,13 +7868,13 @@
         <v>1.6</v>
       </c>
       <c r="P105" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="T105">
         <v>1</v>
       </c>
       <c r="U105" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X105">
         <f t="shared" si="24"/>
@@ -7774,9 +7885,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="106" spans="1:25">
+    <row r="106" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B106" s="7">
         <v>90</v>
@@ -7812,13 +7923,13 @@
         <v>0</v>
       </c>
       <c r="P106" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="T106">
         <v>1</v>
       </c>
       <c r="U106" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X106">
         <f t="shared" si="24"/>
@@ -7829,9 +7940,9 @@
         <v/>
       </c>
     </row>
-    <row r="107" spans="1:25">
+    <row r="107" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B107" s="7">
         <v>91</v>
@@ -7864,13 +7975,13 @@
         <v>1</v>
       </c>
       <c r="P107" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="T107">
         <v>1</v>
       </c>
       <c r="U107" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X107">
         <f t="shared" si="24"/>
@@ -7881,9 +7992,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="108" spans="1:25">
+    <row r="108" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B108" s="7">
         <v>92</v>
@@ -7919,13 +8030,13 @@
         <v>0</v>
       </c>
       <c r="P108" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="T108">
         <v>1</v>
       </c>
       <c r="U108" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X108">
         <f t="shared" si="24"/>
@@ -7936,9 +8047,9 @@
         <v/>
       </c>
     </row>
-    <row r="109" spans="1:25">
+    <row r="109" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B109" s="7">
         <v>93</v>
@@ -7974,13 +8085,13 @@
         <v>0</v>
       </c>
       <c r="P109" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="T109">
         <v>1</v>
       </c>
       <c r="U109" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X109">
         <f t="shared" si="24"/>
@@ -7991,9 +8102,9 @@
         <v/>
       </c>
     </row>
-    <row r="110" spans="1:25">
+    <row r="110" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B110" s="7">
         <v>94</v>
@@ -8004,6 +8115,9 @@
       <c r="D110">
         <v>1</v>
       </c>
+      <c r="E110">
+        <v>1</v>
+      </c>
       <c r="F110">
         <v>4</v>
       </c>
@@ -8015,19 +8129,19 @@
       </c>
       <c r="J110">
         <f t="shared" si="20"/>
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="K110">
         <f t="shared" si="21"/>
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="L110">
         <f t="shared" si="22"/>
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="M110">
         <f t="shared" si="23"/>
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="N110">
         <f t="shared" ref="N110:N124" si="25">IF(D110=1,G110*I110/100,0)</f>
@@ -8035,29 +8149,29 @@
       </c>
       <c r="O110">
         <f t="shared" si="14"/>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="P110" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="T110">
         <v>1</v>
       </c>
       <c r="U110" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X110">
         <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="Y110">
+        <v>1</v>
+      </c>
+      <c r="Y110" t="str">
         <f t="shared" si="19"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="111" spans="1:25">
+        <v/>
+      </c>
+    </row>
+    <row r="111" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B111" s="7">
         <v>95</v>
@@ -8102,13 +8216,13 @@
         <v>1.6</v>
       </c>
       <c r="P111" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="T111">
         <v>1</v>
       </c>
       <c r="U111" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X111">
         <f t="shared" si="24"/>
@@ -8119,9 +8233,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="112" spans="1:25">
+    <row r="112" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B112" s="7">
         <v>96</v>
@@ -8166,13 +8280,13 @@
         <v>1.6</v>
       </c>
       <c r="P112" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="T112">
         <v>1</v>
       </c>
       <c r="U112" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X112">
         <f t="shared" si="24"/>
@@ -8183,9 +8297,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="113" spans="1:25">
+    <row r="113" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B113" s="7">
         <v>97</v>
@@ -8230,13 +8344,13 @@
         <v>0.8</v>
       </c>
       <c r="P113" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="T113">
         <v>1</v>
       </c>
       <c r="U113" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X113">
         <f t="shared" si="24"/>
@@ -8247,7 +8361,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="114" spans="1:25">
+    <row r="114" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B114" s="6"/>
       <c r="D114">
         <f t="shared" ref="D114:D115" si="29">IF(F114=4, 1,0)</f>
@@ -8282,9 +8396,9 @@
         <v/>
       </c>
     </row>
-    <row r="115" spans="1:25">
+    <row r="115" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B115" s="17"/>
       <c r="D115">
@@ -8320,9 +8434,9 @@
         <v/>
       </c>
     </row>
-    <row r="116" spans="1:25">
+    <row r="116" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B116" s="6">
         <v>98</v>
@@ -8367,13 +8481,13 @@
         <v>1</v>
       </c>
       <c r="P116" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="T116">
         <v>1</v>
       </c>
       <c r="U116" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X116">
         <f t="shared" ref="X116:X124" si="33">IF(ISNUMBER(E116),1,0)</f>
@@ -8384,9 +8498,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="117" spans="1:25">
+    <row r="117" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B117" s="6">
         <v>99</v>
@@ -8431,13 +8545,13 @@
         <v>1.6</v>
       </c>
       <c r="P117" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T117">
         <v>1</v>
       </c>
       <c r="U117" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X117">
         <f t="shared" si="33"/>
@@ -8448,9 +8562,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="118" spans="1:25">
+    <row r="118" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B118" s="6">
         <v>100</v>
@@ -8495,13 +8609,13 @@
         <v>1.8</v>
       </c>
       <c r="P118" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="T118">
         <v>1</v>
       </c>
       <c r="U118" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X118">
         <f t="shared" si="33"/>
@@ -8512,9 +8626,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="119" spans="1:25">
+    <row r="119" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B119" s="6">
         <v>101</v>
@@ -8559,13 +8673,13 @@
         <v>1.8</v>
       </c>
       <c r="P119" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="T119">
         <v>1</v>
       </c>
       <c r="U119" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X119">
         <f t="shared" si="33"/>
@@ -8576,9 +8690,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="120" spans="1:25">
+    <row r="120" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B120" s="6">
         <v>102</v>
@@ -8623,13 +8737,13 @@
         <v>1.8</v>
       </c>
       <c r="P120" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="T120">
         <v>1</v>
       </c>
       <c r="U120" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X120">
         <f t="shared" si="33"/>
@@ -8640,9 +8754,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="121" spans="1:25">
+    <row r="121" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B121" s="6">
         <v>103</v>
@@ -8687,13 +8801,13 @@
         <v>1.8</v>
       </c>
       <c r="P121" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="T121">
         <v>1</v>
       </c>
       <c r="U121" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X121">
         <f t="shared" si="33"/>
@@ -8704,9 +8818,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="122" spans="1:25">
+    <row r="122" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B122" s="6">
         <v>104</v>
@@ -8751,13 +8865,13 @@
         <v>0.9</v>
       </c>
       <c r="P122" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="T122">
         <v>1</v>
       </c>
       <c r="U122" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X122">
         <f t="shared" si="33"/>
@@ -8768,9 +8882,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="123" spans="1:25">
+    <row r="123" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B123" s="6">
         <v>105</v>
@@ -8815,13 +8929,13 @@
         <v>1.8</v>
       </c>
       <c r="P123" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="T123">
         <v>1</v>
       </c>
       <c r="U123" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X123">
         <f t="shared" si="33"/>
@@ -8832,9 +8946,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="124" spans="1:25">
+    <row r="124" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B124" s="6">
         <v>106</v>
@@ -8882,7 +8996,7 @@
         <v>1</v>
       </c>
       <c r="U124" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X124">
         <f t="shared" si="33"/>
@@ -8893,7 +9007,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="125" spans="1:25">
+    <row r="125" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B125" s="6"/>
       <c r="J125">
         <f t="shared" si="20"/>
@@ -8912,9 +9026,9 @@
         <v/>
       </c>
     </row>
-    <row r="126" spans="1:25">
+    <row r="126" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B126" s="17"/>
       <c r="J126">
@@ -8930,9 +9044,9 @@
         <v/>
       </c>
     </row>
-    <row r="127" spans="1:25">
+    <row r="127" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B127" s="6"/>
       <c r="C127">
@@ -8964,9 +9078,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="128" spans="1:25">
+    <row r="128" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B128" s="6"/>
       <c r="C128">
@@ -8998,9 +9112,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="129" spans="1:25">
+    <row r="129" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B129" s="6"/>
       <c r="C129">
@@ -9032,250 +9146,250 @@
         <v>100</v>
       </c>
     </row>
-    <row r="130" spans="1:25">
+    <row r="130" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B130" s="6"/>
     </row>
-    <row r="131" spans="1:25">
+    <row r="131" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B131" s="6"/>
     </row>
-    <row r="132" spans="1:25">
+    <row r="132" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B132" s="6"/>
     </row>
-    <row r="133" spans="1:25">
+    <row r="133" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B133" s="6"/>
     </row>
-    <row r="134" spans="1:25">
+    <row r="134" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B134" s="6"/>
     </row>
-    <row r="135" spans="1:25">
+    <row r="135" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B135" s="6"/>
     </row>
-    <row r="136" spans="1:25">
+    <row r="136" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B136" s="6"/>
     </row>
-    <row r="137" spans="1:25">
+    <row r="137" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B137" s="6"/>
     </row>
-    <row r="138" spans="1:25">
+    <row r="138" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B138" s="6"/>
     </row>
-    <row r="139" spans="1:25">
+    <row r="139" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B139" s="6"/>
     </row>
-    <row r="140" spans="1:25">
+    <row r="140" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B140" s="6"/>
     </row>
-    <row r="141" spans="1:25">
+    <row r="141" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B141" s="6"/>
     </row>
-    <row r="142" spans="1:25">
+    <row r="142" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B142" s="6"/>
     </row>
-    <row r="143" spans="1:25">
+    <row r="143" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B143" s="6"/>
     </row>
-    <row r="144" spans="1:25">
+    <row r="144" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B144" s="6"/>
     </row>
-    <row r="145" spans="2:2">
+    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B145" s="6"/>
     </row>
-    <row r="146" spans="2:2">
+    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B146" s="6"/>
     </row>
-    <row r="147" spans="2:2">
+    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B147" s="6"/>
     </row>
-    <row r="148" spans="2:2">
+    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B148" s="6"/>
     </row>
-    <row r="149" spans="2:2">
+    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B149" s="6"/>
     </row>
-    <row r="150" spans="2:2">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B150" s="6"/>
     </row>
-    <row r="151" spans="2:2">
+    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B151" s="6"/>
     </row>
-    <row r="152" spans="2:2">
+    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B152" s="6"/>
     </row>
-    <row r="153" spans="2:2">
+    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B153" s="6"/>
     </row>
-    <row r="154" spans="2:2">
+    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B154" s="6"/>
     </row>
-    <row r="155" spans="2:2">
+    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B155" s="6"/>
     </row>
-    <row r="156" spans="2:2">
+    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B156" s="6"/>
     </row>
-    <row r="157" spans="2:2">
+    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B157" s="6"/>
     </row>
-    <row r="158" spans="2:2">
+    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B158" s="6"/>
     </row>
-    <row r="159" spans="2:2">
+    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B159" s="6"/>
     </row>
-    <row r="160" spans="2:2">
+    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B160" s="6"/>
     </row>
-    <row r="161" spans="2:2">
+    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B161" s="6"/>
     </row>
-    <row r="162" spans="2:2">
+    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B162" s="6"/>
     </row>
-    <row r="163" spans="2:2">
+    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B163" s="6"/>
     </row>
-    <row r="164" spans="2:2">
+    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B164" s="6"/>
     </row>
-    <row r="165" spans="2:2">
+    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B165" s="6"/>
     </row>
-    <row r="166" spans="2:2">
+    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B166" s="6"/>
     </row>
-    <row r="167" spans="2:2">
+    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B167" s="6"/>
     </row>
-    <row r="168" spans="2:2">
+    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B168" s="6"/>
     </row>
-    <row r="169" spans="2:2">
+    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B169" s="6"/>
     </row>
-    <row r="170" spans="2:2">
+    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B170" s="6"/>
     </row>
-    <row r="171" spans="2:2">
+    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B171" s="6"/>
     </row>
-    <row r="172" spans="2:2">
+    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B172" s="6"/>
     </row>
-    <row r="173" spans="2:2">
+    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B173" s="6"/>
     </row>
-    <row r="174" spans="2:2">
+    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B174" s="6"/>
     </row>
-    <row r="175" spans="2:2">
+    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B175" s="6"/>
     </row>
-    <row r="176" spans="2:2">
+    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B176" s="6"/>
     </row>
-    <row r="177" spans="2:2">
+    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B177" s="6"/>
     </row>
-    <row r="178" spans="2:2">
+    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B178" s="6"/>
     </row>
-    <row r="179" spans="2:2">
+    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B179" s="6"/>
     </row>
-    <row r="180" spans="2:2">
+    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B180" s="6"/>
     </row>
-    <row r="181" spans="2:2">
+    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B181" s="6"/>
     </row>
-    <row r="182" spans="2:2">
+    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B182" s="6"/>
     </row>
-    <row r="183" spans="2:2">
+    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B183" s="6"/>
     </row>
-    <row r="184" spans="2:2">
+    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B184" s="6"/>
     </row>
-    <row r="185" spans="2:2">
+    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B185" s="6"/>
     </row>
-    <row r="186" spans="2:2">
+    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B186" s="6"/>
     </row>
-    <row r="187" spans="2:2">
+    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B187" s="6"/>
     </row>
-    <row r="188" spans="2:2">
+    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B188" s="6"/>
     </row>
-    <row r="189" spans="2:2">
+    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B189" s="6"/>
     </row>
-    <row r="190" spans="2:2">
+    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B190" s="6"/>
     </row>
-    <row r="191" spans="2:2">
+    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B191" s="6"/>
     </row>
-    <row r="192" spans="2:2">
+    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B192" s="6"/>
     </row>
-    <row r="193" spans="2:2">
+    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B193" s="6"/>
     </row>
-    <row r="194" spans="2:2">
+    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B194" s="6"/>
     </row>
-    <row r="195" spans="2:2">
+    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B195" s="6"/>
     </row>
-    <row r="196" spans="2:2">
+    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B196" s="6"/>
     </row>
-    <row r="197" spans="2:2">
+    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B197" s="6"/>
     </row>
-    <row r="198" spans="2:2">
+    <row r="198" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B198" s="6"/>
     </row>
-    <row r="199" spans="2:2">
+    <row r="199" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B199" s="6"/>
     </row>
-    <row r="200" spans="2:2">
+    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B200" s="6"/>
     </row>
-    <row r="201" spans="2:2">
+    <row r="201" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B201" s="6"/>
     </row>
-    <row r="202" spans="2:2">
+    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B202" s="6"/>
     </row>
-    <row r="203" spans="2:2">
+    <row r="203" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B203" s="6"/>
     </row>
-    <row r="204" spans="2:2">
+    <row r="204" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B204" s="6"/>
     </row>
-    <row r="205" spans="2:2">
+    <row r="205" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B205" s="6"/>
     </row>
-    <row r="206" spans="2:2">
+    <row r="206" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B206" s="6"/>
     </row>
-    <row r="207" spans="2:2">
+    <row r="207" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B207" s="6"/>
     </row>
-    <row r="208" spans="2:2">
+    <row r="208" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B208" s="6"/>
     </row>
-    <row r="209" spans="2:2">
+    <row r="209" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B209" s="6"/>
     </row>
-    <row r="210" spans="2:2">
+    <row r="210" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B210" s="6"/>
     </row>
-    <row r="211" spans="2:2">
+    <row r="211" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B211" s="6"/>
     </row>
   </sheetData>
@@ -9286,8 +9400,8 @@
     <mergeCell ref="G2:I2"/>
   </mergeCells>
   <conditionalFormatting sqref="A6:A11 A53:A59 A45:A50 A116:A124 A88:A113 A62:A85 A14:A41 B212:B1048576 A127:A1048576 A3:A4">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>ISNUMBER(E3)</formula>
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>IF(E3&gt;0,1,0)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>ISBLANK($E3)</formula>

</xml_diff>

<commit_message>
Wishful thinking that we would actually get RSVPs...
</commit_message>
<xml_diff>
--- a/Guest_List_Invited.xlsx
+++ b/Guest_List_Invited.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\logan\Documents\GitHub\Farrell_Garrett_Wedding\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA04181F-D130-4636-967E-73ED81F08E05}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -654,9 +648,6 @@
     <t xml:space="preserve">additional mouths </t>
   </si>
   <si>
-    <t>Seth and Wife</t>
-  </si>
-  <si>
     <t>Fr. Phil</t>
   </si>
   <si>
@@ -808,16 +799,19 @@
   </si>
   <si>
     <t>both chicken</t>
+  </si>
+  <si>
+    <t>Seth and Allison Saldivar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -946,91 +940,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -1318,22 +1228,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E50" sqref="E50"/>
+      <pane ySplit="4" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A129" sqref="A129"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35.85546875" customWidth="1"/>
     <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
@@ -1358,7 +1268,7 @@
     <col min="27" max="27" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" ht="15" customHeight="1">
       <c r="A1" s="5">
         <v>4</v>
       </c>
@@ -1378,34 +1288,34 @@
       <c r="U1" s="10"/>
       <c r="V1" s="10"/>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29">
       <c r="A2" s="4">
         <v>3</v>
       </c>
       <c r="B2" s="6"/>
       <c r="D2" s="19" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E2" s="19"/>
       <c r="G2" s="19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H2" s="19"/>
       <c r="I2" s="19"/>
       <c r="J2" s="11"/>
       <c r="K2" s="11"/>
       <c r="P2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="Q2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="R2" s="14">
         <f>D3+G3*(1+Z4/100)</f>
-        <v>149.13321355274704</v>
+        <v>147.34253001816853</v>
       </c>
       <c r="S2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="T2" s="10"/>
       <c r="U2" s="10"/>
@@ -1416,7 +1326,7 @@
         <v>28.53908325175902</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1426,34 +1336,34 @@
       </c>
       <c r="D3" s="19">
         <f>SUM(E6:E129)</f>
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3">
         <f>SUM(J6:J173)</f>
-        <v>129.89999999999998</v>
+        <v>129.99999999999997</v>
       </c>
       <c r="G3">
         <f>SUM(O6:O129)</f>
-        <v>66.899999999999977</v>
+        <v>60.999999999999972</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
       <c r="P3" s="12">
         <f>G3+D3</f>
-        <v>129.89999999999998</v>
+        <v>129.99999999999997</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="R3" s="14">
         <f>D3+G3*(1-Z4/100)</f>
-        <v>110.66678644725292</v>
+        <v>112.65746998183141</v>
       </c>
       <c r="S3" s="13">
         <f>SUM(X6:X129)/COUNT(X6:X11,X14:X41,X45:X50,X53:X59,X62:X85,X88:X113,X116:X124,X127:X129)</f>
-        <v>0.44036697247706424</v>
+        <v>0.47706422018348627</v>
       </c>
       <c r="T3" s="10"/>
       <c r="U3" s="10"/>
@@ -1462,10 +1372,10 @@
         <v>34</v>
       </c>
       <c r="Z3" s="10" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" s="10" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="10" customFormat="1" ht="31.5" customHeight="1">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -1477,7 +1387,7 @@
         <v>88</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>0</v>
@@ -1489,7 +1399,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K4" s="10" t="s">
         <v>69</v>
@@ -1504,7 +1414,7 @@
         <v>89</v>
       </c>
       <c r="O4" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="P4" s="10" t="s">
         <v>2</v>
@@ -1522,20 +1432,20 @@
         <v>126</v>
       </c>
       <c r="W4" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="Y4" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="Z4" s="10">
         <f>STDEV(Y6:Y129)</f>
-        <v>28.749198135645848</v>
+        <v>28.43037707896486</v>
       </c>
       <c r="AA4" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1545,7 +1455,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1612,7 +1522,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1679,7 +1589,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1746,7 +1656,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1813,7 +1723,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1880,7 +1790,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -1930,7 +1840,7 @@
         <v>0</v>
       </c>
       <c r="P11" s="18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="Q11" s="8"/>
       <c r="R11" s="8"/>
@@ -1949,7 +1859,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29">
       <c r="B12" s="6"/>
       <c r="C12" s="1"/>
       <c r="D12">
@@ -1992,7 +1902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -2030,7 +1940,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
@@ -2094,7 +2004,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -2158,7 +2068,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
@@ -2225,7 +2135,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27">
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
@@ -2289,7 +2199,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27">
       <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
@@ -2353,7 +2263,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27">
       <c r="A19" s="2" t="s">
         <v>188</v>
       </c>
@@ -2420,7 +2330,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -2487,7 +2397,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27">
       <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
@@ -2551,7 +2461,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27">
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
@@ -2615,9 +2525,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27">
       <c r="A23" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B23" s="7">
         <v>16</v>
@@ -2682,7 +2592,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27">
       <c r="A24" s="2" t="s">
         <v>17</v>
       </c>
@@ -2735,7 +2645,7 @@
         <v>193</v>
       </c>
       <c r="S24" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="T24">
         <v>1</v>
@@ -2744,7 +2654,7 @@
         <v>150</v>
       </c>
       <c r="W24" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="X24">
         <f t="shared" si="10"/>
@@ -2755,10 +2665,10 @@
         <v/>
       </c>
       <c r="AA24" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27">
       <c r="A25" s="2" t="s">
         <v>18</v>
       </c>
@@ -2817,7 +2727,7 @@
         <v>150</v>
       </c>
       <c r="W25" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="X25">
         <f t="shared" si="10"/>
@@ -2828,10 +2738,10 @@
         <v/>
       </c>
       <c r="AA25" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27">
       <c r="A26" s="2" t="s">
         <v>19</v>
       </c>
@@ -2895,7 +2805,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27">
       <c r="A27" s="2" t="s">
         <v>20</v>
       </c>
@@ -2962,7 +2872,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27">
       <c r="A28" s="2" t="s">
         <v>21</v>
       </c>
@@ -3029,7 +2939,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27">
       <c r="A29" s="2" t="s">
         <v>22</v>
       </c>
@@ -3096,7 +3006,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27">
       <c r="A30" s="2" t="s">
         <v>23</v>
       </c>
@@ -3160,7 +3070,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27">
       <c r="A31" s="2" t="s">
         <v>24</v>
       </c>
@@ -3224,7 +3134,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27">
       <c r="A32" s="2" t="s">
         <v>25</v>
       </c>
@@ -3288,7 +3198,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27">
       <c r="A33" s="2" t="s">
         <v>26</v>
       </c>
@@ -3352,7 +3262,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
@@ -3411,7 +3321,7 @@
         <v>150</v>
       </c>
       <c r="W34" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="X34">
         <f t="shared" si="10"/>
@@ -3422,10 +3332,10 @@
         <v/>
       </c>
       <c r="AA34" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
@@ -3489,7 +3399,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27">
       <c r="A36" s="2" t="s">
         <v>40</v>
       </c>
@@ -3553,7 +3463,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27">
       <c r="A37" s="2" t="s">
         <v>41</v>
       </c>
@@ -3617,7 +3527,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27">
       <c r="A38" s="2" t="s">
         <v>42</v>
       </c>
@@ -3676,7 +3586,7 @@
         <v>150</v>
       </c>
       <c r="W38" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="X38">
         <f t="shared" si="10"/>
@@ -3687,10 +3597,10 @@
         <v/>
       </c>
       <c r="AA38" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27">
       <c r="A39" s="2" t="s">
         <v>43</v>
       </c>
@@ -3757,7 +3667,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27">
       <c r="A40" s="2" t="s">
         <v>44</v>
       </c>
@@ -3807,10 +3717,10 @@
         <v>0</v>
       </c>
       <c r="P40" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="S40" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="T40">
         <v>1</v>
@@ -3827,7 +3737,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27">
       <c r="A41" t="s">
         <v>100</v>
       </c>
@@ -3891,7 +3801,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27">
       <c r="A42" s="2"/>
       <c r="B42" s="7"/>
       <c r="D42">
@@ -3927,7 +3837,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27">
       <c r="B43" s="6"/>
       <c r="C43" s="1"/>
       <c r="D43">
@@ -3963,7 +3873,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27">
       <c r="A44" s="1" t="s">
         <v>27</v>
       </c>
@@ -4001,7 +3911,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27">
       <c r="A45" t="s">
         <v>28</v>
       </c>
@@ -4054,7 +3964,7 @@
         <v>183</v>
       </c>
       <c r="S45" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="T45">
         <v>1</v>
@@ -4063,7 +3973,7 @@
         <v>150</v>
       </c>
       <c r="W45" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="X45">
         <f t="shared" ref="X45:X50" si="11">IF(ISNUMBER(E45),1,0)</f>
@@ -4074,10 +3984,10 @@
         <v/>
       </c>
       <c r="AA45" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27">
       <c r="A46" t="s">
         <v>29</v>
       </c>
@@ -4141,7 +4051,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27">
       <c r="A47" t="s">
         <v>30</v>
       </c>
@@ -4208,7 +4118,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27">
       <c r="A48" t="s">
         <v>31</v>
       </c>
@@ -4275,7 +4185,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:29">
       <c r="A49" t="s">
         <v>32</v>
       </c>
@@ -4345,9 +4255,9 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:29">
       <c r="A50" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B50" s="6">
         <v>40</v>
@@ -4417,7 +4327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:29">
       <c r="B51" s="6"/>
       <c r="J51">
         <f t="shared" si="9"/>
@@ -4448,7 +4358,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:29">
       <c r="A52" s="1" t="s">
         <v>49</v>
       </c>
@@ -4486,7 +4396,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:29">
       <c r="A53" t="s">
         <v>48</v>
       </c>
@@ -4557,7 +4467,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:29">
       <c r="A54" t="s">
         <v>51</v>
       </c>
@@ -4624,7 +4534,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:29">
       <c r="A55" t="s">
         <v>50</v>
       </c>
@@ -4695,7 +4605,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:29">
       <c r="A56" t="s">
         <v>77</v>
       </c>
@@ -4762,7 +4672,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:29">
       <c r="A57" t="s">
         <v>52</v>
       </c>
@@ -4832,7 +4742,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:29">
       <c r="A58" t="s">
         <v>53</v>
       </c>
@@ -4885,7 +4795,7 @@
         <v>119</v>
       </c>
       <c r="S58" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="T58">
         <v>1</v>
@@ -4902,7 +4812,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:29">
       <c r="A59" t="s">
         <v>54</v>
       </c>
@@ -4952,7 +4862,7 @@
         <v>0</v>
       </c>
       <c r="P59" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="T59">
         <v>1</v>
@@ -4969,7 +4879,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:29">
       <c r="B60" s="6"/>
       <c r="J60">
         <f t="shared" si="9"/>
@@ -5000,14 +4910,14 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:29">
       <c r="A61" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B61" s="17"/>
       <c r="D61">
         <f>SUM(J62:J84)</f>
-        <v>30.099999999999991</v>
+        <v>30.199999999999992</v>
       </c>
       <c r="J61">
         <f t="shared" si="9"/>
@@ -5038,9 +4948,9 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:29">
       <c r="A62" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B62" s="6">
         <v>48</v>
@@ -5085,7 +4995,7 @@
         <v>1.8</v>
       </c>
       <c r="P62" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="Q62" s="6"/>
       <c r="R62" s="6"/>
@@ -5106,7 +5016,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:29">
       <c r="A63" t="s">
         <v>55</v>
       </c>
@@ -5174,7 +5084,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:29">
       <c r="A64" t="s">
         <v>56</v>
       </c>
@@ -5226,7 +5136,7 @@
       <c r="Q64" s="6"/>
       <c r="R64" s="6"/>
       <c r="S64" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="T64" s="6">
         <v>1</v>
@@ -5244,7 +5154,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:25">
       <c r="A65" t="s">
         <v>57</v>
       </c>
@@ -5312,7 +5222,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:25">
       <c r="A66" t="s">
         <v>167</v>
       </c>
@@ -5383,7 +5293,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:25">
       <c r="A67" t="s">
         <v>191</v>
       </c>
@@ -5423,7 +5333,7 @@
       <c r="Q67" s="6"/>
       <c r="R67" s="6"/>
       <c r="S67" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="T67" s="6">
         <v>1</v>
@@ -5441,7 +5351,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:25">
       <c r="A68" t="s">
         <v>58</v>
       </c>
@@ -5509,9 +5419,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:25">
       <c r="A69" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B69" s="6">
         <v>55</v>
@@ -5564,7 +5474,7 @@
       <c r="Q69" s="6"/>
       <c r="R69" s="6"/>
       <c r="S69" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="T69" s="6">
         <v>1</v>
@@ -5582,7 +5492,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:25">
       <c r="A70" t="s">
         <v>59</v>
       </c>
@@ -5653,7 +5563,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:25">
       <c r="A71" t="s">
         <v>60</v>
       </c>
@@ -5723,7 +5633,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:25">
       <c r="A72" t="s">
         <v>61</v>
       </c>
@@ -5793,7 +5703,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:25">
       <c r="A73" t="s">
         <v>62</v>
       </c>
@@ -5860,7 +5770,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:25">
       <c r="A74" t="s">
         <v>63</v>
       </c>
@@ -5924,7 +5834,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:25">
       <c r="A75" t="s">
         <v>64</v>
       </c>
@@ -5988,7 +5898,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:25">
       <c r="A76" t="s">
         <v>65</v>
       </c>
@@ -6058,7 +5968,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:25">
       <c r="A77" t="s">
         <v>166</v>
       </c>
@@ -6125,7 +6035,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:25">
       <c r="A78" t="s">
         <v>67</v>
       </c>
@@ -6189,7 +6099,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:25">
       <c r="A79" t="s">
         <v>127</v>
       </c>
@@ -6202,6 +6112,9 @@
       <c r="D79">
         <v>1</v>
       </c>
+      <c r="E79">
+        <v>1</v>
+      </c>
       <c r="F79">
         <v>4</v>
       </c>
@@ -6213,19 +6126,19 @@
       </c>
       <c r="J79">
         <f t="shared" si="20"/>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="K79">
         <f t="shared" si="15"/>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="L79">
         <f t="shared" si="16"/>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="M79">
         <f t="shared" si="17"/>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="N79">
         <f t="shared" si="18"/>
@@ -6233,7 +6146,7 @@
       </c>
       <c r="O79">
         <f t="shared" si="14"/>
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="P79" t="s">
         <v>112</v>
@@ -6246,14 +6159,14 @@
       </c>
       <c r="X79">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="Y79">
+        <v>1</v>
+      </c>
+      <c r="Y79" t="str">
         <f t="shared" si="19"/>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="80" spans="1:25">
       <c r="A80" t="s">
         <v>68</v>
       </c>
@@ -6317,7 +6230,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:27">
       <c r="A81" t="s">
         <v>66</v>
       </c>
@@ -6384,7 +6297,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:27">
       <c r="A82" t="s">
         <v>169</v>
       </c>
@@ -6448,9 +6361,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:27">
       <c r="A83" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B83" s="6">
         <v>69</v>
@@ -6515,9 +6428,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:27">
       <c r="A84" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B84" s="6">
         <v>70</v>
@@ -6579,9 +6492,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:27">
       <c r="A85" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B85" s="6">
         <v>71</v>
@@ -6643,7 +6556,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:27">
       <c r="B86" s="6"/>
       <c r="J86">
         <f t="shared" si="20"/>
@@ -6674,7 +6587,7 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:27">
       <c r="A87" s="1" t="s">
         <v>73</v>
       </c>
@@ -6712,7 +6625,7 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:27">
       <c r="A88" s="2" t="s">
         <v>80</v>
       </c>
@@ -6779,7 +6692,7 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:27">
       <c r="A89" t="s">
         <v>74</v>
       </c>
@@ -6846,7 +6759,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:27">
       <c r="A90" t="s">
         <v>134</v>
       </c>
@@ -6910,7 +6823,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:27">
       <c r="A91" t="s">
         <v>75</v>
       </c>
@@ -6977,7 +6890,7 @@
         <v/>
       </c>
     </row>
-    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:27">
       <c r="A92" t="s">
         <v>76</v>
       </c>
@@ -7033,7 +6946,7 @@
         <v>150</v>
       </c>
       <c r="W92" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="X92">
         <f t="shared" si="24"/>
@@ -7044,10 +6957,10 @@
         <v>80</v>
       </c>
       <c r="AA92" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="93" spans="1:27">
       <c r="A93" t="s">
         <v>157</v>
       </c>
@@ -7114,7 +7027,7 @@
         <v/>
       </c>
     </row>
-    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:27">
       <c r="A94" t="s">
         <v>154</v>
       </c>
@@ -7181,7 +7094,7 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:27">
       <c r="A95" t="s">
         <v>158</v>
       </c>
@@ -7248,7 +7161,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:27">
       <c r="A96" t="s">
         <v>120</v>
       </c>
@@ -7312,7 +7225,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="97" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:27">
       <c r="A97" t="s">
         <v>135</v>
       </c>
@@ -7376,7 +7289,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="98" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:27">
       <c r="A98" t="s">
         <v>78</v>
       </c>
@@ -7443,7 +7356,7 @@
         <v/>
       </c>
     </row>
-    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:27">
       <c r="A99" t="s">
         <v>159</v>
       </c>
@@ -7502,7 +7415,7 @@
         <v>150</v>
       </c>
       <c r="W99" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="X99">
         <f t="shared" si="24"/>
@@ -7513,10 +7426,10 @@
         <v/>
       </c>
       <c r="AA99" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="100" spans="1:27">
       <c r="A100" t="s">
         <v>147</v>
       </c>
@@ -7580,7 +7493,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:27">
       <c r="A101" t="s">
         <v>79</v>
       </c>
@@ -7644,7 +7557,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="102" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:27">
       <c r="A102" t="s">
         <v>151</v>
       </c>
@@ -7708,7 +7621,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="103" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:27">
       <c r="A103" t="s">
         <v>152</v>
       </c>
@@ -7775,9 +7688,9 @@
         <v/>
       </c>
     </row>
-    <row r="104" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:27">
       <c r="A104" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B104" s="7">
         <v>88</v>
@@ -7816,7 +7729,7 @@
         <v>116</v>
       </c>
       <c r="S104" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="T104">
         <v>1</v>
@@ -7833,7 +7746,7 @@
         <v/>
       </c>
     </row>
-    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:27">
       <c r="A105" t="s">
         <v>118</v>
       </c>
@@ -7885,7 +7798,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="106" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:27">
       <c r="A106" t="s">
         <v>160</v>
       </c>
@@ -7940,7 +7853,7 @@
         <v/>
       </c>
     </row>
-    <row r="107" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:27">
       <c r="A107" t="s">
         <v>161</v>
       </c>
@@ -7992,7 +7905,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="108" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:27">
       <c r="A108" t="s">
         <v>82</v>
       </c>
@@ -8047,9 +7960,9 @@
         <v/>
       </c>
     </row>
-    <row r="109" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:27">
       <c r="A109" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B109" s="7">
         <v>93</v>
@@ -8102,9 +8015,9 @@
         <v/>
       </c>
     </row>
-    <row r="110" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:27">
       <c r="A110" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B110" s="7">
         <v>94</v>
@@ -8169,9 +8082,9 @@
         <v/>
       </c>
     </row>
-    <row r="111" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:27">
       <c r="A111" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B111" s="7">
         <v>95</v>
@@ -8233,7 +8146,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="112" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:27">
       <c r="A112" t="s">
         <v>81</v>
       </c>
@@ -8297,9 +8210,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="113" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:25">
       <c r="A113" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B113" s="7">
         <v>97</v>
@@ -8361,7 +8274,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="114" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:25">
       <c r="B114" s="6"/>
       <c r="D114">
         <f t="shared" ref="D114:D115" si="29">IF(F114=4, 1,0)</f>
@@ -8396,7 +8309,7 @@
         <v/>
       </c>
     </row>
-    <row r="115" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:25">
       <c r="A115" s="1" t="s">
         <v>83</v>
       </c>
@@ -8434,9 +8347,9 @@
         <v/>
       </c>
     </row>
-    <row r="116" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:25">
       <c r="A116" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B116" s="6">
         <v>98</v>
@@ -8498,7 +8411,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="117" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:25">
       <c r="A117" t="s">
         <v>84</v>
       </c>
@@ -8562,9 +8475,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="118" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:25">
       <c r="A118" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B118" s="6">
         <v>100</v>
@@ -8626,7 +8539,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="119" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:25">
       <c r="A119" t="s">
         <v>85</v>
       </c>
@@ -8690,7 +8603,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="120" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:25">
       <c r="A120" t="s">
         <v>86</v>
       </c>
@@ -8754,9 +8667,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="121" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:25">
       <c r="A121" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B121" s="6">
         <v>103</v>
@@ -8818,9 +8731,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="122" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:25">
       <c r="A122" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B122" s="6">
         <v>104</v>
@@ -8865,7 +8778,7 @@
         <v>0.9</v>
       </c>
       <c r="P122" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="T122">
         <v>1</v>
@@ -8882,9 +8795,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="123" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:25">
       <c r="A123" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B123" s="6">
         <v>105</v>
@@ -8946,9 +8859,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="124" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:25">
       <c r="A124" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B124" s="6">
         <v>106</v>
@@ -9007,7 +8920,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="125" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:25">
       <c r="B125" s="6"/>
       <c r="J125">
         <f t="shared" si="20"/>
@@ -9026,7 +8939,7 @@
         <v/>
       </c>
     </row>
-    <row r="126" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:25">
       <c r="A126" s="1" t="s">
         <v>208</v>
       </c>
@@ -9044,9 +8957,9 @@
         <v/>
       </c>
     </row>
-    <row r="127" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:25">
       <c r="A127" t="s">
-        <v>209</v>
+        <v>260</v>
       </c>
       <c r="B127" s="6"/>
       <c r="C127">
@@ -9055,6 +8968,9 @@
       <c r="D127">
         <v>1</v>
       </c>
+      <c r="E127">
+        <v>2</v>
+      </c>
       <c r="G127">
         <v>2</v>
       </c>
@@ -9067,20 +8983,20 @@
       </c>
       <c r="O127">
         <f t="shared" si="34"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X127">
         <f>IF(ISNUMBER(E127),1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Y127">
+        <v>1</v>
+      </c>
+      <c r="Y127" t="str">
         <f t="shared" si="19"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="128" spans="1:25" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="128" spans="1:25">
       <c r="A128" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B128" s="6"/>
       <c r="C128">
@@ -9089,6 +9005,9 @@
       <c r="D128">
         <v>1</v>
       </c>
+      <c r="E128">
+        <v>1</v>
+      </c>
       <c r="G128">
         <v>1</v>
       </c>
@@ -9101,20 +9020,20 @@
       </c>
       <c r="O128">
         <f t="shared" si="34"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X128">
         <f>IF(ISNUMBER(E128),1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Y128">
+        <v>1</v>
+      </c>
+      <c r="Y128" t="str">
         <f t="shared" si="19"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="129" spans="1:25" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="129" spans="1:25">
       <c r="A129" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B129" s="6"/>
       <c r="C129">
@@ -9123,6 +9042,9 @@
       <c r="D129">
         <v>1</v>
       </c>
+      <c r="E129">
+        <v>2</v>
+      </c>
       <c r="G129">
         <v>2</v>
       </c>
@@ -9135,261 +9057,261 @@
       </c>
       <c r="O129">
         <f t="shared" si="34"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X129">
         <f>IF(ISNUMBER(E129),1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Y129">
+        <v>1</v>
+      </c>
+      <c r="Y129" t="str">
         <f t="shared" si="19"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="130" spans="1:25" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="130" spans="1:25">
       <c r="B130" s="6"/>
     </row>
-    <row r="131" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:25">
       <c r="B131" s="6"/>
     </row>
-    <row r="132" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:25">
       <c r="B132" s="6"/>
     </row>
-    <row r="133" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:25">
       <c r="B133" s="6"/>
     </row>
-    <row r="134" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:25">
       <c r="B134" s="6"/>
     </row>
-    <row r="135" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:25">
       <c r="B135" s="6"/>
     </row>
-    <row r="136" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:25">
       <c r="B136" s="6"/>
     </row>
-    <row r="137" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:25">
       <c r="B137" s="6"/>
     </row>
-    <row r="138" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:25">
       <c r="B138" s="6"/>
     </row>
-    <row r="139" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:25">
       <c r="B139" s="6"/>
     </row>
-    <row r="140" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:25">
       <c r="B140" s="6"/>
     </row>
-    <row r="141" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:25">
       <c r="B141" s="6"/>
     </row>
-    <row r="142" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:25">
       <c r="B142" s="6"/>
     </row>
-    <row r="143" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:25">
       <c r="B143" s="6"/>
     </row>
-    <row r="144" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:25">
       <c r="B144" s="6"/>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:2">
       <c r="B145" s="6"/>
     </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:2">
       <c r="B146" s="6"/>
     </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:2">
       <c r="B147" s="6"/>
     </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:2">
       <c r="B148" s="6"/>
     </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:2">
       <c r="B149" s="6"/>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:2">
       <c r="B150" s="6"/>
     </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:2">
       <c r="B151" s="6"/>
     </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:2">
       <c r="B152" s="6"/>
     </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:2">
       <c r="B153" s="6"/>
     </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:2">
       <c r="B154" s="6"/>
     </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:2">
       <c r="B155" s="6"/>
     </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:2">
       <c r="B156" s="6"/>
     </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:2">
       <c r="B157" s="6"/>
     </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:2">
       <c r="B158" s="6"/>
     </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:2">
       <c r="B159" s="6"/>
     </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:2">
       <c r="B160" s="6"/>
     </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:2">
       <c r="B161" s="6"/>
     </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:2">
       <c r="B162" s="6"/>
     </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:2">
       <c r="B163" s="6"/>
     </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:2">
       <c r="B164" s="6"/>
     </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:2">
       <c r="B165" s="6"/>
     </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:2">
       <c r="B166" s="6"/>
     </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:2">
       <c r="B167" s="6"/>
     </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:2">
       <c r="B168" s="6"/>
     </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:2">
       <c r="B169" s="6"/>
     </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:2">
       <c r="B170" s="6"/>
     </row>
-    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:2">
       <c r="B171" s="6"/>
     </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:2">
       <c r="B172" s="6"/>
     </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:2">
       <c r="B173" s="6"/>
     </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:2">
       <c r="B174" s="6"/>
     </row>
-    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:2">
       <c r="B175" s="6"/>
     </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:2">
       <c r="B176" s="6"/>
     </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:2">
       <c r="B177" s="6"/>
     </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:2">
       <c r="B178" s="6"/>
     </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:2">
       <c r="B179" s="6"/>
     </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:2">
       <c r="B180" s="6"/>
     </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:2">
       <c r="B181" s="6"/>
     </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:2">
       <c r="B182" s="6"/>
     </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:2">
       <c r="B183" s="6"/>
     </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:2">
       <c r="B184" s="6"/>
     </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:2">
       <c r="B185" s="6"/>
     </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:2">
       <c r="B186" s="6"/>
     </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:2">
       <c r="B187" s="6"/>
     </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:2">
       <c r="B188" s="6"/>
     </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:2">
       <c r="B189" s="6"/>
     </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:2">
       <c r="B190" s="6"/>
     </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:2">
       <c r="B191" s="6"/>
     </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:2">
       <c r="B192" s="6"/>
     </row>
-    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:2">
       <c r="B193" s="6"/>
     </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:2">
       <c r="B194" s="6"/>
     </row>
-    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:2">
       <c r="B195" s="6"/>
     </row>
-    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:2">
       <c r="B196" s="6"/>
     </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:2">
       <c r="B197" s="6"/>
     </row>
-    <row r="198" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:2">
       <c r="B198" s="6"/>
     </row>
-    <row r="199" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:2">
       <c r="B199" s="6"/>
     </row>
-    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:2">
       <c r="B200" s="6"/>
     </row>
-    <row r="201" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:2">
       <c r="B201" s="6"/>
     </row>
-    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:2">
       <c r="B202" s="6"/>
     </row>
-    <row r="203" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:2">
       <c r="B203" s="6"/>
     </row>
-    <row r="204" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:2">
       <c r="B204" s="6"/>
     </row>
-    <row r="205" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:2">
       <c r="B205" s="6"/>
     </row>
-    <row r="206" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:2">
       <c r="B206" s="6"/>
     </row>
-    <row r="207" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:2">
       <c r="B207" s="6"/>
     </row>
-    <row r="208" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:2">
       <c r="B208" s="6"/>
     </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:2">
       <c r="B209" s="6"/>
     </row>
-    <row r="210" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:2">
       <c r="B210" s="6"/>
     </row>
-    <row r="211" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:2">
       <c r="B211" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated guest, added DJ
</commit_message>
<xml_diff>
--- a/Guest_List_Invited.xlsx
+++ b/Guest_List_Invited.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\logan\Documents\GitHub\Farrell_Garrett_Wedding\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5E1E13-F4A1-46FE-86CD-C7394323C1CA}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="171027"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="263">
   <si>
     <t xml:space="preserve">Priority </t>
   </si>
@@ -802,16 +808,22 @@
   </si>
   <si>
     <t>Seth and Allison Saldivar</t>
+  </si>
+  <si>
+    <t>DJ</t>
+  </si>
+  <si>
+    <t>chicken for both</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1228,22 +1240,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A129" sqref="A129"/>
+      <pane ySplit="4" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P119" sqref="P119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.85546875" customWidth="1"/>
     <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
@@ -1268,7 +1280,7 @@
     <col min="27" max="27" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15" customHeight="1">
+    <row r="1" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5">
         <v>4</v>
       </c>
@@ -1288,7 +1300,7 @@
       <c r="U1" s="10"/>
       <c r="V1" s="10"/>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>3</v>
       </c>
@@ -1312,7 +1324,7 @@
       </c>
       <c r="R2" s="14">
         <f>D3+G3*(1+Z4/100)</f>
-        <v>147.34253001816853</v>
+        <v>147.05123214886862</v>
       </c>
       <c r="S2" t="s">
         <v>217</v>
@@ -1326,7 +1338,7 @@
         <v>28.53908325175902</v>
       </c>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1336,34 +1348,34 @@
       </c>
       <c r="D3" s="19">
         <f>SUM(E6:E129)</f>
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3">
         <f>SUM(J6:J173)</f>
-        <v>129.99999999999997</v>
+        <v>131.19999999999999</v>
       </c>
       <c r="G3">
         <f>SUM(O6:O129)</f>
-        <v>60.999999999999972</v>
+        <v>59.199999999999974</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
       <c r="P3" s="12">
         <f>G3+D3</f>
-        <v>129.99999999999997</v>
+        <v>130.19999999999999</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>221</v>
       </c>
       <c r="R3" s="14">
         <f>D3+G3*(1-Z4/100)</f>
-        <v>112.65746998183141</v>
+        <v>113.3487678511313</v>
       </c>
       <c r="S3" s="13">
         <f>SUM(X6:X129)/COUNT(X6:X11,X14:X41,X45:X50,X53:X59,X62:X85,X88:X113,X116:X124,X127:X129)</f>
-        <v>0.47706422018348627</v>
+        <v>0.48623853211009177</v>
       </c>
       <c r="T3" s="10"/>
       <c r="U3" s="10"/>
@@ -1375,7 +1387,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="4" spans="1:29" s="10" customFormat="1" ht="31.5" customHeight="1">
+    <row r="4" spans="1:29" s="10" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -1439,13 +1451,13 @@
       </c>
       <c r="Z4" s="10">
         <f>STDEV(Y6:Y129)</f>
-        <v>28.43037707896486</v>
+        <v>28.464919170386263</v>
       </c>
       <c r="AA4" s="10" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="5" spans="1:29">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1455,7 +1467,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1522,7 +1534,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1589,7 +1601,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1656,7 +1668,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:29">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1723,7 +1735,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:29">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1790,7 +1802,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:29">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -1859,7 +1871,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:29">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
       <c r="C12" s="1"/>
       <c r="D12">
@@ -1902,7 +1914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:29">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -1940,7 +1952,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:29">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
@@ -2004,7 +2016,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:29">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -2068,7 +2080,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:29">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
@@ -2135,7 +2147,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:27">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
@@ -2199,7 +2211,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:27">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
@@ -2263,7 +2275,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:27">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>188</v>
       </c>
@@ -2330,7 +2342,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:27">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -2397,7 +2409,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:27">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
@@ -2461,7 +2473,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:27">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
@@ -2525,7 +2537,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:27">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>230</v>
       </c>
@@ -2592,7 +2604,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:27">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>17</v>
       </c>
@@ -2668,7 +2680,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="25" spans="1:27">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>18</v>
       </c>
@@ -2741,7 +2753,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="26" spans="1:27">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>19</v>
       </c>
@@ -2805,7 +2817,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:27">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>20</v>
       </c>
@@ -2872,7 +2884,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:27">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>21</v>
       </c>
@@ -2939,7 +2951,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:27">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>22</v>
       </c>
@@ -3006,7 +3018,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:27">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>23</v>
       </c>
@@ -3070,7 +3082,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:27">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>24</v>
       </c>
@@ -3134,7 +3146,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:27">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>25</v>
       </c>
@@ -3198,7 +3210,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:27">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>26</v>
       </c>
@@ -3262,7 +3274,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:27">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
@@ -3335,7 +3347,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="35" spans="1:27">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
@@ -3399,7 +3411,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:27">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>40</v>
       </c>
@@ -3463,7 +3475,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:27">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>41</v>
       </c>
@@ -3527,7 +3539,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:27">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>42</v>
       </c>
@@ -3600,7 +3612,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="39" spans="1:27">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>43</v>
       </c>
@@ -3667,7 +3679,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:27">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>44</v>
       </c>
@@ -3737,7 +3749,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:27">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>100</v>
       </c>
@@ -3801,7 +3813,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:27">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="7"/>
       <c r="D42">
@@ -3837,7 +3849,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:27">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B43" s="6"/>
       <c r="C43" s="1"/>
       <c r="D43">
@@ -3873,7 +3885,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:27">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>27</v>
       </c>
@@ -3911,7 +3923,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:27">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>28</v>
       </c>
@@ -3987,7 +3999,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="46" spans="1:27">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>29</v>
       </c>
@@ -4051,7 +4063,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:27">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>30</v>
       </c>
@@ -4118,7 +4130,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:27">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>31</v>
       </c>
@@ -4185,7 +4197,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:29">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>32</v>
       </c>
@@ -4255,7 +4267,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:29">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>231</v>
       </c>
@@ -4327,7 +4339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:29">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B51" s="6"/>
       <c r="J51">
         <f t="shared" si="9"/>
@@ -4358,7 +4370,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:29">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>49</v>
       </c>
@@ -4396,7 +4408,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:29">
+    <row r="53" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>48</v>
       </c>
@@ -4467,7 +4479,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:29">
+    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>51</v>
       </c>
@@ -4534,7 +4546,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:29">
+    <row r="55" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>50</v>
       </c>
@@ -4605,7 +4617,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:29">
+    <row r="56" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>77</v>
       </c>
@@ -4672,7 +4684,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:29">
+    <row r="57" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>52</v>
       </c>
@@ -4742,7 +4754,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:29">
+    <row r="58" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>53</v>
       </c>
@@ -4812,7 +4824,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:29">
+    <row r="59" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>54</v>
       </c>
@@ -4879,7 +4891,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:29">
+    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B60" s="6"/>
       <c r="J60">
         <f t="shared" si="9"/>
@@ -4910,7 +4922,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:29">
+    <row r="61" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>47</v>
       </c>
@@ -4948,7 +4960,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:29">
+    <row r="62" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>222</v>
       </c>
@@ -5016,7 +5028,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="63" spans="1:29">
+    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>55</v>
       </c>
@@ -5084,7 +5096,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="64" spans="1:29">
+    <row r="64" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>56</v>
       </c>
@@ -5154,7 +5166,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="1:25">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>57</v>
       </c>
@@ -5222,7 +5234,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="66" spans="1:25">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>167</v>
       </c>
@@ -5293,7 +5305,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>191</v>
       </c>
@@ -5351,7 +5363,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:25">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>58</v>
       </c>
@@ -5419,7 +5431,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="69" spans="1:25">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>258</v>
       </c>
@@ -5492,7 +5504,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:25">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>59</v>
       </c>
@@ -5559,11 +5571,11 @@
         <v>1</v>
       </c>
       <c r="Y70" t="str">
-        <f t="shared" ref="Y70:Y129" si="19">IF(ISNUMBER(E70),"",IF(ISNUMBER(I70),I70,""))</f>
+        <f t="shared" ref="Y70:Y130" si="19">IF(ISNUMBER(E70),"",IF(ISNUMBER(I70),I70,""))</f>
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:25">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>60</v>
       </c>
@@ -5633,7 +5645,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:25">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>61</v>
       </c>
@@ -5703,7 +5715,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:25">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>62</v>
       </c>
@@ -5770,7 +5782,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:25">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>63</v>
       </c>
@@ -5834,7 +5846,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="75" spans="1:25">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>64</v>
       </c>
@@ -5898,7 +5910,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="76" spans="1:25">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>65</v>
       </c>
@@ -5968,7 +5980,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:25">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>166</v>
       </c>
@@ -6035,7 +6047,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:25">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>67</v>
       </c>
@@ -6099,7 +6111,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="79" spans="1:25">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>127</v>
       </c>
@@ -6166,7 +6178,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="1:25">
+    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>68</v>
       </c>
@@ -6230,7 +6242,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="81" spans="1:27">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>66</v>
       </c>
@@ -6297,7 +6309,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:27">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>169</v>
       </c>
@@ -6361,7 +6373,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="83" spans="1:27">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>223</v>
       </c>
@@ -6428,7 +6440,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="84" spans="1:27">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>249</v>
       </c>
@@ -6492,7 +6504,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="85" spans="1:27">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>224</v>
       </c>
@@ -6556,7 +6568,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="86" spans="1:27">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B86" s="6"/>
       <c r="J86">
         <f t="shared" si="20"/>
@@ -6587,7 +6599,7 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="1:27">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>73</v>
       </c>
@@ -6625,7 +6637,7 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="1:27">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>80</v>
       </c>
@@ -6692,7 +6704,7 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="1:27">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>74</v>
       </c>
@@ -6759,7 +6771,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="1:27">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>134</v>
       </c>
@@ -6823,7 +6835,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="91" spans="1:27">
+    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>75</v>
       </c>
@@ -6890,7 +6902,7 @@
         <v/>
       </c>
     </row>
-    <row r="92" spans="1:27">
+    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>76</v>
       </c>
@@ -6960,7 +6972,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="93" spans="1:27">
+    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>157</v>
       </c>
@@ -7027,7 +7039,7 @@
         <v/>
       </c>
     </row>
-    <row r="94" spans="1:27">
+    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>154</v>
       </c>
@@ -7094,7 +7106,7 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="1:27">
+    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>158</v>
       </c>
@@ -7161,7 +7173,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="1:27">
+    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>120</v>
       </c>
@@ -7225,7 +7237,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="97" spans="1:27">
+    <row r="97" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>135</v>
       </c>
@@ -7289,7 +7301,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="98" spans="1:27">
+    <row r="98" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>78</v>
       </c>
@@ -7356,7 +7368,7 @@
         <v/>
       </c>
     </row>
-    <row r="99" spans="1:27">
+    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>159</v>
       </c>
@@ -7429,7 +7441,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="100" spans="1:27">
+    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>147</v>
       </c>
@@ -7493,7 +7505,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="101" spans="1:27">
+    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>79</v>
       </c>
@@ -7557,7 +7569,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="102" spans="1:27">
+    <row r="102" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>151</v>
       </c>
@@ -7621,7 +7633,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="103" spans="1:27">
+    <row r="103" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>152</v>
       </c>
@@ -7688,7 +7700,7 @@
         <v/>
       </c>
     </row>
-    <row r="104" spans="1:27">
+    <row r="104" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>229</v>
       </c>
@@ -7746,7 +7758,7 @@
         <v/>
       </c>
     </row>
-    <row r="105" spans="1:27">
+    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>118</v>
       </c>
@@ -7798,7 +7810,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="106" spans="1:27">
+    <row r="106" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>160</v>
       </c>
@@ -7853,7 +7865,7 @@
         <v/>
       </c>
     </row>
-    <row r="107" spans="1:27">
+    <row r="107" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>161</v>
       </c>
@@ -7905,7 +7917,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="108" spans="1:27">
+    <row r="108" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>82</v>
       </c>
@@ -7960,7 +7972,7 @@
         <v/>
       </c>
     </row>
-    <row r="109" spans="1:27">
+    <row r="109" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>227</v>
       </c>
@@ -8015,7 +8027,7 @@
         <v/>
       </c>
     </row>
-    <row r="110" spans="1:27">
+    <row r="110" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>226</v>
       </c>
@@ -8082,7 +8094,7 @@
         <v/>
       </c>
     </row>
-    <row r="111" spans="1:27">
+    <row r="111" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>228</v>
       </c>
@@ -8146,7 +8158,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="112" spans="1:27">
+    <row r="112" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>81</v>
       </c>
@@ -8210,7 +8222,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="113" spans="1:25">
+    <row r="113" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>225</v>
       </c>
@@ -8274,7 +8286,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="114" spans="1:25">
+    <row r="114" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B114" s="6"/>
       <c r="D114">
         <f t="shared" ref="D114:D115" si="29">IF(F114=4, 1,0)</f>
@@ -8309,7 +8321,7 @@
         <v/>
       </c>
     </row>
-    <row r="115" spans="1:25">
+    <row r="115" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>83</v>
       </c>
@@ -8347,7 +8359,7 @@
         <v/>
       </c>
     </row>
-    <row r="116" spans="1:25">
+    <row r="116" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>232</v>
       </c>
@@ -8411,7 +8423,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="117" spans="1:25">
+    <row r="117" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>84</v>
       </c>
@@ -8475,7 +8487,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="118" spans="1:25">
+    <row r="118" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>233</v>
       </c>
@@ -8539,7 +8551,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="119" spans="1:25">
+    <row r="119" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>85</v>
       </c>
@@ -8603,7 +8615,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="120" spans="1:25">
+    <row r="120" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>86</v>
       </c>
@@ -8667,7 +8679,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="121" spans="1:25">
+    <row r="121" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>234</v>
       </c>
@@ -8731,7 +8743,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="122" spans="1:25">
+    <row r="122" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>235</v>
       </c>
@@ -8774,7 +8786,7 @@
         <v>0.9</v>
       </c>
       <c r="O122">
-        <f t="shared" ref="O122:O129" si="34">IF(ISNUMBER(E122), 0, J122)</f>
+        <f t="shared" ref="O122:O130" si="34">IF(ISNUMBER(E122), 0, J122)</f>
         <v>0.9</v>
       </c>
       <c r="P122" t="s">
@@ -8795,7 +8807,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="123" spans="1:25">
+    <row r="123" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>236</v>
       </c>
@@ -8859,7 +8871,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="124" spans="1:25">
+    <row r="124" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>237</v>
       </c>
@@ -8872,6 +8884,9 @@
       <c r="D124">
         <v>1</v>
       </c>
+      <c r="E124">
+        <v>2</v>
+      </c>
       <c r="F124">
         <v>2</v>
       </c>
@@ -8883,11 +8898,11 @@
       </c>
       <c r="J124">
         <f t="shared" si="20"/>
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="K124">
         <f t="shared" si="30"/>
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="L124">
         <f t="shared" si="31"/>
@@ -8903,7 +8918,10 @@
       </c>
       <c r="O124">
         <f t="shared" si="34"/>
-        <v>1.8</v>
+        <v>0</v>
+      </c>
+      <c r="S124" t="s">
+        <v>262</v>
       </c>
       <c r="T124">
         <v>1</v>
@@ -8913,14 +8931,14 @@
       </c>
       <c r="X124">
         <f t="shared" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="Y124">
+        <v>1</v>
+      </c>
+      <c r="Y124" t="str">
         <f t="shared" si="19"/>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="125" spans="1:25">
+        <v/>
+      </c>
+    </row>
+    <row r="125" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B125" s="6"/>
       <c r="J125">
         <f t="shared" si="20"/>
@@ -8939,7 +8957,7 @@
         <v/>
       </c>
     </row>
-    <row r="126" spans="1:25">
+    <row r="126" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>208</v>
       </c>
@@ -8957,7 +8975,7 @@
         <v/>
       </c>
     </row>
-    <row r="127" spans="1:25">
+    <row r="127" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>260</v>
       </c>
@@ -8978,7 +8996,7 @@
         <v>100</v>
       </c>
       <c r="J127">
-        <f t="shared" ref="J127:J129" si="35">IF(ISNUMBER(E127), E127, I127*G127/100)</f>
+        <f t="shared" ref="J127:J130" si="35">IF(ISNUMBER(E127), E127, I127*G127/100)</f>
         <v>2</v>
       </c>
       <c r="O127">
@@ -8994,7 +9012,7 @@
         <v/>
       </c>
     </row>
-    <row r="128" spans="1:25">
+    <row r="128" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>209</v>
       </c>
@@ -9031,7 +9049,7 @@
         <v/>
       </c>
     </row>
-    <row r="129" spans="1:25">
+    <row r="129" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>210</v>
       </c>
@@ -9068,250 +9086,280 @@
         <v/>
       </c>
     </row>
-    <row r="130" spans="1:25">
+    <row r="130" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>261</v>
+      </c>
       <c r="B130" s="6"/>
-    </row>
-    <row r="131" spans="1:25">
+      <c r="C130">
+        <v>1</v>
+      </c>
+      <c r="D130">
+        <v>1</v>
+      </c>
+      <c r="E130">
+        <v>1</v>
+      </c>
+      <c r="G130">
+        <v>1</v>
+      </c>
+      <c r="I130">
+        <v>100</v>
+      </c>
+      <c r="J130">
+        <f t="shared" si="35"/>
+        <v>1</v>
+      </c>
+      <c r="O130">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="Y130" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="131" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B131" s="6"/>
     </row>
-    <row r="132" spans="1:25">
+    <row r="132" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B132" s="6"/>
     </row>
-    <row r="133" spans="1:25">
+    <row r="133" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B133" s="6"/>
     </row>
-    <row r="134" spans="1:25">
+    <row r="134" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B134" s="6"/>
     </row>
-    <row r="135" spans="1:25">
+    <row r="135" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B135" s="6"/>
     </row>
-    <row r="136" spans="1:25">
+    <row r="136" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B136" s="6"/>
     </row>
-    <row r="137" spans="1:25">
+    <row r="137" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B137" s="6"/>
     </row>
-    <row r="138" spans="1:25">
+    <row r="138" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B138" s="6"/>
     </row>
-    <row r="139" spans="1:25">
+    <row r="139" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B139" s="6"/>
     </row>
-    <row r="140" spans="1:25">
+    <row r="140" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B140" s="6"/>
     </row>
-    <row r="141" spans="1:25">
+    <row r="141" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B141" s="6"/>
     </row>
-    <row r="142" spans="1:25">
+    <row r="142" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B142" s="6"/>
     </row>
-    <row r="143" spans="1:25">
+    <row r="143" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B143" s="6"/>
     </row>
-    <row r="144" spans="1:25">
+    <row r="144" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B144" s="6"/>
     </row>
-    <row r="145" spans="2:2">
+    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B145" s="6"/>
     </row>
-    <row r="146" spans="2:2">
+    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B146" s="6"/>
     </row>
-    <row r="147" spans="2:2">
+    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B147" s="6"/>
     </row>
-    <row r="148" spans="2:2">
+    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B148" s="6"/>
     </row>
-    <row r="149" spans="2:2">
+    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B149" s="6"/>
     </row>
-    <row r="150" spans="2:2">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B150" s="6"/>
     </row>
-    <row r="151" spans="2:2">
+    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B151" s="6"/>
     </row>
-    <row r="152" spans="2:2">
+    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B152" s="6"/>
     </row>
-    <row r="153" spans="2:2">
+    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B153" s="6"/>
     </row>
-    <row r="154" spans="2:2">
+    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B154" s="6"/>
     </row>
-    <row r="155" spans="2:2">
+    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B155" s="6"/>
     </row>
-    <row r="156" spans="2:2">
+    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B156" s="6"/>
     </row>
-    <row r="157" spans="2:2">
+    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B157" s="6"/>
     </row>
-    <row r="158" spans="2:2">
+    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B158" s="6"/>
     </row>
-    <row r="159" spans="2:2">
+    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B159" s="6"/>
     </row>
-    <row r="160" spans="2:2">
+    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B160" s="6"/>
     </row>
-    <row r="161" spans="2:2">
+    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B161" s="6"/>
     </row>
-    <row r="162" spans="2:2">
+    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B162" s="6"/>
     </row>
-    <row r="163" spans="2:2">
+    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B163" s="6"/>
     </row>
-    <row r="164" spans="2:2">
+    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B164" s="6"/>
     </row>
-    <row r="165" spans="2:2">
+    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B165" s="6"/>
     </row>
-    <row r="166" spans="2:2">
+    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B166" s="6"/>
     </row>
-    <row r="167" spans="2:2">
+    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B167" s="6"/>
     </row>
-    <row r="168" spans="2:2">
+    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B168" s="6"/>
     </row>
-    <row r="169" spans="2:2">
+    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B169" s="6"/>
     </row>
-    <row r="170" spans="2:2">
+    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B170" s="6"/>
     </row>
-    <row r="171" spans="2:2">
+    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B171" s="6"/>
     </row>
-    <row r="172" spans="2:2">
+    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B172" s="6"/>
     </row>
-    <row r="173" spans="2:2">
+    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B173" s="6"/>
     </row>
-    <row r="174" spans="2:2">
+    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B174" s="6"/>
     </row>
-    <row r="175" spans="2:2">
+    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B175" s="6"/>
     </row>
-    <row r="176" spans="2:2">
+    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B176" s="6"/>
     </row>
-    <row r="177" spans="2:2">
+    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B177" s="6"/>
     </row>
-    <row r="178" spans="2:2">
+    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B178" s="6"/>
     </row>
-    <row r="179" spans="2:2">
+    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B179" s="6"/>
     </row>
-    <row r="180" spans="2:2">
+    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B180" s="6"/>
     </row>
-    <row r="181" spans="2:2">
+    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B181" s="6"/>
     </row>
-    <row r="182" spans="2:2">
+    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B182" s="6"/>
     </row>
-    <row r="183" spans="2:2">
+    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B183" s="6"/>
     </row>
-    <row r="184" spans="2:2">
+    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B184" s="6"/>
     </row>
-    <row r="185" spans="2:2">
+    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B185" s="6"/>
     </row>
-    <row r="186" spans="2:2">
+    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B186" s="6"/>
     </row>
-    <row r="187" spans="2:2">
+    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B187" s="6"/>
     </row>
-    <row r="188" spans="2:2">
+    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B188" s="6"/>
     </row>
-    <row r="189" spans="2:2">
+    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B189" s="6"/>
     </row>
-    <row r="190" spans="2:2">
+    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B190" s="6"/>
     </row>
-    <row r="191" spans="2:2">
+    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B191" s="6"/>
     </row>
-    <row r="192" spans="2:2">
+    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B192" s="6"/>
     </row>
-    <row r="193" spans="2:2">
+    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B193" s="6"/>
     </row>
-    <row r="194" spans="2:2">
+    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B194" s="6"/>
     </row>
-    <row r="195" spans="2:2">
+    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B195" s="6"/>
     </row>
-    <row r="196" spans="2:2">
+    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B196" s="6"/>
     </row>
-    <row r="197" spans="2:2">
+    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B197" s="6"/>
     </row>
-    <row r="198" spans="2:2">
+    <row r="198" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B198" s="6"/>
     </row>
-    <row r="199" spans="2:2">
+    <row r="199" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B199" s="6"/>
     </row>
-    <row r="200" spans="2:2">
+    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B200" s="6"/>
     </row>
-    <row r="201" spans="2:2">
+    <row r="201" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B201" s="6"/>
     </row>
-    <row r="202" spans="2:2">
+    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B202" s="6"/>
     </row>
-    <row r="203" spans="2:2">
+    <row r="203" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B203" s="6"/>
     </row>
-    <row r="204" spans="2:2">
+    <row r="204" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B204" s="6"/>
     </row>
-    <row r="205" spans="2:2">
+    <row r="205" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B205" s="6"/>
     </row>
-    <row r="206" spans="2:2">
+    <row r="206" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B206" s="6"/>
     </row>
-    <row r="207" spans="2:2">
+    <row r="207" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B207" s="6"/>
     </row>
-    <row r="208" spans="2:2">
+    <row r="208" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B208" s="6"/>
     </row>
-    <row r="209" spans="2:2">
+    <row r="209" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B209" s="6"/>
     </row>
-    <row r="210" spans="2:2">
+    <row r="210" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B210" s="6"/>
     </row>
-    <row r="211" spans="2:2">
+    <row r="211" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B211" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated gifts and RSVPs
</commit_message>
<xml_diff>
--- a/Guest_List_Invited.xlsx
+++ b/Guest_List_Invited.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\logan\Documents\GitHub\Farrell_Garrett_Wedding\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D30D82-A36E-4C5D-9E27-898095D5A939}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="265">
   <si>
     <t xml:space="preserve">Priority </t>
   </si>
@@ -147,9 +141,6 @@
     <t xml:space="preserve">Kathy and Don </t>
   </si>
   <si>
-    <t>Brittany and Matt &amp; Family</t>
-  </si>
-  <si>
     <t>Brandon &amp; Guest</t>
   </si>
   <si>
@@ -792,9 +783,6 @@
     <t>Hellen Only</t>
   </si>
   <si>
-    <t xml:space="preserve">Is dating Sam </t>
-  </si>
-  <si>
     <t xml:space="preserve">Jane only </t>
   </si>
   <si>
@@ -814,16 +802,28 @@
   </si>
   <si>
     <t>chicken for both</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is "dating" Sam </t>
+  </si>
+  <si>
+    <t>Brittany and Matt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$40 for golf day/spa day </t>
+  </si>
+  <si>
+    <t>$100 for accomodations, hiking in the mountains</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1240,22 +1240,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC211"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P73" sqref="P73"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W114" sqref="W114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35.85546875" customWidth="1"/>
     <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
@@ -1280,17 +1280,17 @@
     <col min="27" max="27" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" ht="15" customHeight="1">
       <c r="A1" s="5">
         <v>4</v>
       </c>
       <c r="B1" s="15"/>
       <c r="D1" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E1" s="20"/>
       <c r="F1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G1">
         <f>SUM(G6:G11,G14:G41,G45:G50,G53:G59,G62:G85,G88:G113,G116:G124,G127:G129)</f>
@@ -1300,34 +1300,34 @@
       <c r="U1" s="10"/>
       <c r="V1" s="10"/>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29">
       <c r="A2" s="4">
         <v>3</v>
       </c>
       <c r="B2" s="6"/>
       <c r="D2" s="19" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E2" s="19"/>
       <c r="G2" s="19" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H2" s="19"/>
       <c r="I2" s="19"/>
       <c r="J2" s="11"/>
       <c r="K2" s="11"/>
       <c r="P2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="Q2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="R2" s="14">
         <f>D3+G3*(1+Z4/100)</f>
-        <v>147.05123214886862</v>
+        <v>146.27786723426857</v>
       </c>
       <c r="S2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="T2" s="10"/>
       <c r="U2" s="10"/>
@@ -1338,13 +1338,13 @@
         <v>28.53908325175902</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D3" s="19">
         <f>SUM(E6:E129)</f>
@@ -1353,29 +1353,29 @@
       <c r="E3" s="19"/>
       <c r="F3">
         <f>SUM(J6:J173)</f>
-        <v>131.19999999999999</v>
+        <v>130.69999999999999</v>
       </c>
       <c r="G3">
         <f>SUM(O6:O129)</f>
-        <v>59.199999999999974</v>
+        <v>58.699999999999974</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
       <c r="P3" s="12">
         <f>G3+D3</f>
-        <v>130.19999999999999</v>
+        <v>129.69999999999999</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="R3" s="14">
         <f>D3+G3*(1-Z4/100)</f>
-        <v>113.3487678511313</v>
+        <v>113.12213276573137</v>
       </c>
       <c r="S3" s="13">
         <f>SUM(X6:X129)/COUNT(X6:X11,X14:X41,X45:X50,X53:X59,X62:X85,X88:X113,X116:X124,X127:X129)</f>
-        <v>0.48623853211009177</v>
+        <v>0.49541284403669728</v>
       </c>
       <c r="T3" s="10"/>
       <c r="U3" s="10"/>
@@ -1384,10 +1384,10 @@
         <v>34</v>
       </c>
       <c r="Z3" s="10" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" s="10" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="10" customFormat="1" ht="31.5" customHeight="1">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -1396,37 +1396,37 @@
         <v>33</v>
       </c>
       <c r="D4" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="N4" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="L4" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>89</v>
-      </c>
       <c r="O4" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="P4" s="10" t="s">
         <v>2</v>
@@ -1435,29 +1435,29 @@
         <v>3</v>
       </c>
       <c r="T4" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="U4" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="U4" s="10" t="s">
+      <c r="V4" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="V4" s="10" t="s">
-        <v>126</v>
-      </c>
       <c r="W4" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="Y4" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Z4" s="10">
         <f>STDEV(Y6:Y129)</f>
-        <v>28.464919170386263</v>
+        <v>28.241681830099861</v>
       </c>
       <c r="AA4" s="10" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1517,13 +1517,13 @@
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="T6">
         <v>1</v>
       </c>
       <c r="U6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X6">
         <f t="shared" ref="X6:X11" si="1">IF(ISNUMBER(E6),1,0)</f>
@@ -1534,7 +1534,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1584,13 +1584,13 @@
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="T7">
         <v>1</v>
       </c>
       <c r="U7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X7">
         <f t="shared" si="1"/>
@@ -1601,7 +1601,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1651,13 +1651,13 @@
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="T8">
         <v>1</v>
       </c>
       <c r="U8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X8">
         <f t="shared" si="1"/>
@@ -1668,7 +1668,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1718,13 +1718,13 @@
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="T9">
         <v>1</v>
       </c>
       <c r="U9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X9">
         <f t="shared" si="1"/>
@@ -1735,7 +1735,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1785,13 +1785,13 @@
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="T10">
         <v>1</v>
       </c>
       <c r="U10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X10">
         <f t="shared" si="1"/>
@@ -1802,7 +1802,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>0</v>
       </c>
       <c r="P11" s="18" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="Q11" s="8"/>
       <c r="R11" s="8"/>
@@ -1860,7 +1860,7 @@
         <v>1</v>
       </c>
       <c r="U11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X11">
         <f t="shared" si="1"/>
@@ -1871,7 +1871,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29">
       <c r="B12" s="6"/>
       <c r="C12" s="1"/>
       <c r="D12">
@@ -1914,14 +1914,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="17"/>
       <c r="D13">
         <f>SUM(J14:J41)</f>
-        <v>24</v>
+        <v>23.5</v>
       </c>
       <c r="J13">
         <f t="shared" si="9"/>
@@ -1952,7 +1952,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
@@ -1999,13 +1999,13 @@
         <v>1</v>
       </c>
       <c r="P14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="T14">
         <v>1</v>
       </c>
       <c r="U14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X14">
         <f t="shared" ref="X14:X40" si="10">IF(ISNUMBER(E14),1,0)</f>
@@ -2016,7 +2016,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -2063,13 +2063,13 @@
         <v>1</v>
       </c>
       <c r="P15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="T15">
         <v>1</v>
       </c>
       <c r="U15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X15">
         <f t="shared" si="10"/>
@@ -2080,7 +2080,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
@@ -2127,7 +2127,7 @@
         <v>1</v>
       </c>
       <c r="P16" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q16" s="7"/>
       <c r="R16" s="7"/>
@@ -2136,7 +2136,7 @@
         <v>1</v>
       </c>
       <c r="U16" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X16">
         <f t="shared" si="10"/>
@@ -2147,7 +2147,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27">
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
@@ -2194,13 +2194,13 @@
         <v>0.5</v>
       </c>
       <c r="P17" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="T17">
         <v>1</v>
       </c>
       <c r="U17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X17">
         <f t="shared" si="10"/>
@@ -2211,7 +2211,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27">
       <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
@@ -2258,13 +2258,13 @@
         <v>1</v>
       </c>
       <c r="P18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="T18">
         <v>1</v>
       </c>
       <c r="U18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X18">
         <f t="shared" si="10"/>
@@ -2275,9 +2275,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27">
       <c r="A19" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B19" s="7">
         <v>12</v>
@@ -2322,7 +2322,7 @@
         <v>0.5</v>
       </c>
       <c r="P19" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="Q19" s="6"/>
       <c r="R19" s="6"/>
@@ -2331,7 +2331,7 @@
         <v>1</v>
       </c>
       <c r="U19" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X19">
         <f t="shared" si="10"/>
@@ -2342,7 +2342,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>0.5</v>
       </c>
       <c r="P20" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
@@ -2398,7 +2398,7 @@
         <v>1</v>
       </c>
       <c r="U20" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X20">
         <f t="shared" si="10"/>
@@ -2409,7 +2409,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27">
       <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
@@ -2456,13 +2456,13 @@
         <v>1</v>
       </c>
       <c r="P21" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="T21">
         <v>1</v>
       </c>
       <c r="U21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X21">
         <f t="shared" si="10"/>
@@ -2473,7 +2473,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27">
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
@@ -2520,13 +2520,13 @@
         <v>1</v>
       </c>
       <c r="P22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="T22">
         <v>1</v>
       </c>
       <c r="U22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X22">
         <f t="shared" si="10"/>
@@ -2537,9 +2537,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27">
       <c r="A23" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B23" s="7">
         <v>16</v>
@@ -2584,7 +2584,7 @@
         <v>0.5</v>
       </c>
       <c r="P23" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
@@ -2593,7 +2593,7 @@
         <v>1</v>
       </c>
       <c r="U23" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X23">
         <f t="shared" si="10"/>
@@ -2604,7 +2604,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27">
       <c r="A24" s="2" t="s">
         <v>17</v>
       </c>
@@ -2654,19 +2654,19 @@
         <v>0</v>
       </c>
       <c r="P24" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="S24" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="T24">
         <v>1</v>
       </c>
       <c r="U24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="W24" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="X24">
         <f t="shared" si="10"/>
@@ -2677,10 +2677,10 @@
         <v/>
       </c>
       <c r="AA24" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27">
       <c r="A25" s="2" t="s">
         <v>18</v>
       </c>
@@ -2730,16 +2730,16 @@
         <v>0</v>
       </c>
       <c r="P25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="T25">
         <v>1</v>
       </c>
       <c r="U25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="W25" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="X25">
         <f t="shared" si="10"/>
@@ -2750,10 +2750,10 @@
         <v/>
       </c>
       <c r="AA25" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27">
       <c r="A26" s="2" t="s">
         <v>19</v>
       </c>
@@ -2800,13 +2800,13 @@
         <v>0.5</v>
       </c>
       <c r="P26" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="T26">
         <v>1</v>
       </c>
       <c r="U26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X26">
         <f t="shared" si="10"/>
@@ -2817,7 +2817,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27">
       <c r="A27" s="2" t="s">
         <v>20</v>
       </c>
@@ -2867,13 +2867,13 @@
         <v>0</v>
       </c>
       <c r="P27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="T27">
         <v>1</v>
       </c>
       <c r="U27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X27">
         <f t="shared" si="10"/>
@@ -2884,7 +2884,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27">
       <c r="A28" s="2" t="s">
         <v>21</v>
       </c>
@@ -2934,13 +2934,13 @@
         <v>0</v>
       </c>
       <c r="P28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="T28">
         <v>1</v>
       </c>
       <c r="U28" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X28">
         <f t="shared" si="10"/>
@@ -2951,7 +2951,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27">
       <c r="A29" s="2" t="s">
         <v>22</v>
       </c>
@@ -3001,13 +3001,13 @@
         <v>0</v>
       </c>
       <c r="P29" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="T29">
         <v>1</v>
       </c>
       <c r="U29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X29">
         <f t="shared" si="10"/>
@@ -3018,7 +3018,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27">
       <c r="A30" s="2" t="s">
         <v>23</v>
       </c>
@@ -3065,13 +3065,13 @@
         <v>0.5</v>
       </c>
       <c r="P30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="T30">
         <v>1</v>
       </c>
       <c r="U30" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X30">
         <f t="shared" si="10"/>
@@ -3082,7 +3082,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27">
       <c r="A31" s="2" t="s">
         <v>24</v>
       </c>
@@ -3095,6 +3095,9 @@
       <c r="D31">
         <v>1</v>
       </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
       <c r="F31">
         <v>4</v>
       </c>
@@ -3106,19 +3109,19 @@
       </c>
       <c r="J31">
         <f t="shared" si="9"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="K31">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L31">
         <f t="shared" si="3"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="M31">
         <f t="shared" si="4"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="N31">
         <f t="shared" si="5"/>
@@ -3126,27 +3129,27 @@
       </c>
       <c r="O31">
         <f t="shared" si="6"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="P31" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="T31">
         <v>1</v>
       </c>
       <c r="U31" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X31">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="Y31">
+        <v>1</v>
+      </c>
+      <c r="Y31" t="str">
         <f t="shared" si="7"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:27">
       <c r="A32" s="2" t="s">
         <v>25</v>
       </c>
@@ -3193,13 +3196,13 @@
         <v>0.5</v>
       </c>
       <c r="P32" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="T32">
         <v>1</v>
       </c>
       <c r="U32" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X32">
         <f t="shared" si="10"/>
@@ -3210,7 +3213,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27">
       <c r="A33" s="2" t="s">
         <v>26</v>
       </c>
@@ -3257,13 +3260,13 @@
         <v>0.5</v>
       </c>
       <c r="P33" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="T33">
         <v>1</v>
       </c>
       <c r="U33" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X33">
         <f t="shared" si="10"/>
@@ -3274,7 +3277,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
@@ -3324,16 +3327,16 @@
         <v>0</v>
       </c>
       <c r="P34" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="T34">
         <v>1</v>
       </c>
       <c r="U34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="W34" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="X34">
         <f t="shared" si="10"/>
@@ -3344,10 +3347,10 @@
         <v/>
       </c>
       <c r="AA34" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
@@ -3394,13 +3397,13 @@
         <v>2</v>
       </c>
       <c r="P35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T35">
         <v>1</v>
       </c>
       <c r="U35" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X35">
         <f t="shared" si="10"/>
@@ -3411,9 +3414,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>40</v>
+    <row r="36" spans="1:27">
+      <c r="A36" t="s">
+        <v>262</v>
       </c>
       <c r="B36" s="7">
         <v>29</v>
@@ -3458,13 +3461,13 @@
         <v>1</v>
       </c>
       <c r="P36" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="T36">
         <v>1</v>
       </c>
       <c r="U36" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X36">
         <f t="shared" si="10"/>
@@ -3475,9 +3478,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27">
       <c r="A37" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B37" s="7">
         <v>30</v>
@@ -3522,13 +3525,13 @@
         <v>1</v>
       </c>
       <c r="P37" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T37">
         <v>1</v>
       </c>
       <c r="U37" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X37">
         <f t="shared" si="10"/>
@@ -3539,9 +3542,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27">
       <c r="A38" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B38" s="7">
         <v>31</v>
@@ -3589,16 +3592,16 @@
         <v>0</v>
       </c>
       <c r="P38" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="T38">
         <v>1</v>
       </c>
       <c r="U38" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="W38" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="X38">
         <f t="shared" si="10"/>
@@ -3609,12 +3612,12 @@
         <v/>
       </c>
       <c r="AA38" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27">
       <c r="A39" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B39" s="7">
         <v>32</v>
@@ -3662,13 +3665,13 @@
         <v>0</v>
       </c>
       <c r="P39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="T39">
         <v>1</v>
       </c>
       <c r="U39" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X39">
         <f t="shared" si="10"/>
@@ -3679,9 +3682,9 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27">
       <c r="A40" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B40" s="7">
         <v>33</v>
@@ -3729,16 +3732,16 @@
         <v>0</v>
       </c>
       <c r="P40" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="S40" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="T40">
         <v>1</v>
       </c>
       <c r="U40" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X40">
         <f t="shared" si="10"/>
@@ -3749,9 +3752,9 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27">
       <c r="A41" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B41" s="7">
         <v>34</v>
@@ -3796,13 +3799,13 @@
         <v>0.5</v>
       </c>
       <c r="P41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="T41">
         <v>1</v>
       </c>
       <c r="U41" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X41">
         <f>IF(ISNUMBER(E41),1,0)</f>
@@ -3813,7 +3816,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27">
       <c r="A42" s="2"/>
       <c r="B42" s="7"/>
       <c r="D42">
@@ -3849,7 +3852,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27">
       <c r="B43" s="6"/>
       <c r="C43" s="1"/>
       <c r="D43">
@@ -3885,7 +3888,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27">
       <c r="A44" s="1" t="s">
         <v>27</v>
       </c>
@@ -3923,7 +3926,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27">
       <c r="A45" t="s">
         <v>28</v>
       </c>
@@ -3973,19 +3976,19 @@
         <v>0</v>
       </c>
       <c r="P45" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="S45" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="T45">
         <v>1</v>
       </c>
       <c r="U45" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="W45" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="X45">
         <f t="shared" ref="X45:X50" si="11">IF(ISNUMBER(E45),1,0)</f>
@@ -3996,10 +3999,10 @@
         <v/>
       </c>
       <c r="AA45" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27">
       <c r="A46" t="s">
         <v>29</v>
       </c>
@@ -4046,13 +4049,13 @@
         <v>0.4</v>
       </c>
       <c r="P46" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T46">
         <v>1</v>
       </c>
       <c r="U46" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X46">
         <f t="shared" si="11"/>
@@ -4063,7 +4066,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27">
       <c r="A47" t="s">
         <v>30</v>
       </c>
@@ -4113,13 +4116,13 @@
         <v>0</v>
       </c>
       <c r="P47" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="T47">
         <v>1</v>
       </c>
       <c r="U47" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X47">
         <f t="shared" si="11"/>
@@ -4130,7 +4133,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27">
       <c r="A48" t="s">
         <v>31</v>
       </c>
@@ -4177,16 +4180,16 @@
         <v>0.2</v>
       </c>
       <c r="P48" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="S48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T48">
         <v>1</v>
       </c>
       <c r="U48" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X48">
         <f t="shared" si="11"/>
@@ -4197,7 +4200,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:29">
       <c r="A49" t="s">
         <v>32</v>
       </c>
@@ -4247,16 +4250,16 @@
         <v>0</v>
       </c>
       <c r="P49" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="S49" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T49">
         <v>1</v>
       </c>
       <c r="U49" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X49">
         <f t="shared" si="11"/>
@@ -4267,9 +4270,9 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:29">
       <c r="A50" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B50" s="6">
         <v>40</v>
@@ -4314,18 +4317,18 @@
         <v>0.5</v>
       </c>
       <c r="P50" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Q50" s="6"/>
       <c r="R50" s="6"/>
       <c r="S50" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="T50" s="6">
         <v>1</v>
       </c>
       <c r="U50" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X50">
         <f t="shared" si="11"/>
@@ -4339,7 +4342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:29">
       <c r="B51" s="6"/>
       <c r="J51">
         <f t="shared" si="9"/>
@@ -4370,9 +4373,9 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:29">
       <c r="A52" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B52" s="17"/>
       <c r="D52">
@@ -4408,9 +4411,9 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:29">
       <c r="A53" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B53" s="6">
         <v>41</v>
@@ -4458,7 +4461,7 @@
         <v>0</v>
       </c>
       <c r="P53" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Q53" s="6"/>
       <c r="R53" s="6"/>
@@ -4467,7 +4470,7 @@
         <v>1</v>
       </c>
       <c r="U53" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="V53" s="6"/>
       <c r="X53">
@@ -4479,9 +4482,9 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:29">
       <c r="A54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B54" s="6">
         <v>42</v>
@@ -4526,7 +4529,7 @@
         <v>2</v>
       </c>
       <c r="P54" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q54" s="6"/>
       <c r="R54" s="6"/>
@@ -4535,7 +4538,7 @@
         <v>1</v>
       </c>
       <c r="U54" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X54">
         <f t="shared" si="12"/>
@@ -4546,9 +4549,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:29">
       <c r="A55" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B55" s="6">
         <v>43</v>
@@ -4596,7 +4599,7 @@
         <v>0</v>
       </c>
       <c r="P55" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="Q55" s="6"/>
       <c r="R55" s="6"/>
@@ -4605,7 +4608,7 @@
         <v>1</v>
       </c>
       <c r="U55" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="V55" s="6"/>
       <c r="X55">
@@ -4617,9 +4620,9 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:29">
       <c r="A56" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B56" s="6">
         <v>44</v>
@@ -4667,13 +4670,13 @@
         <v>0</v>
       </c>
       <c r="P56" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="T56">
         <v>1</v>
       </c>
       <c r="U56" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X56">
         <f t="shared" si="12"/>
@@ -4684,9 +4687,9 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:29">
       <c r="A57" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B57" s="6">
         <v>45</v>
@@ -4734,16 +4737,16 @@
         <v>0</v>
       </c>
       <c r="P57" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="T57">
         <v>1</v>
       </c>
       <c r="U57" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="V57" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X57">
         <f t="shared" si="12"/>
@@ -4754,9 +4757,9 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:29">
       <c r="A58" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B58" s="6">
         <v>46</v>
@@ -4804,16 +4807,16 @@
         <v>0</v>
       </c>
       <c r="P58" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="S58" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="T58">
         <v>1</v>
       </c>
       <c r="U58" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X58">
         <f t="shared" si="12"/>
@@ -4824,9 +4827,9 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:29">
       <c r="A59" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B59" s="6">
         <v>47</v>
@@ -4874,13 +4877,13 @@
         <v>0</v>
       </c>
       <c r="P59" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="T59">
         <v>1</v>
       </c>
       <c r="U59" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X59">
         <f t="shared" si="12"/>
@@ -4891,7 +4894,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:29">
       <c r="B60" s="6"/>
       <c r="J60">
         <f t="shared" si="9"/>
@@ -4922,9 +4925,9 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:29">
       <c r="A61" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B61" s="17"/>
       <c r="D61">
@@ -4960,9 +4963,9 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:29">
       <c r="A62" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B62" s="6">
         <v>48</v>
@@ -5007,7 +5010,7 @@
         <v>1.8</v>
       </c>
       <c r="P62" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="Q62" s="6"/>
       <c r="R62" s="6"/>
@@ -5016,7 +5019,7 @@
         <v>1</v>
       </c>
       <c r="U62" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="V62" s="6"/>
       <c r="X62">
@@ -5028,9 +5031,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:29">
       <c r="A63" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B63" s="6">
         <v>49</v>
@@ -5075,7 +5078,7 @@
         <v>1.8</v>
       </c>
       <c r="P63" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q63" s="6"/>
       <c r="R63" s="6"/>
@@ -5084,7 +5087,7 @@
         <v>1</v>
       </c>
       <c r="U63" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="V63" s="6"/>
       <c r="X63">
@@ -5096,9 +5099,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:29">
       <c r="A64" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B64" s="6">
         <v>50</v>
@@ -5143,18 +5146,18 @@
         <v>0.9</v>
       </c>
       <c r="P64" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q64" s="6"/>
       <c r="R64" s="6"/>
       <c r="S64" s="6" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="T64" s="6">
         <v>1</v>
       </c>
       <c r="U64" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="V64" s="6"/>
       <c r="X64">
@@ -5166,9 +5169,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:25">
       <c r="A65" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B65" s="6">
         <v>51</v>
@@ -5213,7 +5216,7 @@
         <v>0.9</v>
       </c>
       <c r="P65" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="Q65" s="6"/>
       <c r="R65" s="6"/>
@@ -5222,7 +5225,7 @@
         <v>1</v>
       </c>
       <c r="U65" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="V65" s="6"/>
       <c r="X65">
@@ -5234,9 +5237,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:25">
       <c r="A66" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B66" s="6">
         <v>52</v>
@@ -5284,7 +5287,7 @@
         <v>0</v>
       </c>
       <c r="P66" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="Q66" s="6"/>
       <c r="R66" s="6"/>
@@ -5293,7 +5296,7 @@
         <v>1</v>
       </c>
       <c r="U66" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="V66" s="6"/>
       <c r="X66">
@@ -5305,9 +5308,9 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:25">
       <c r="A67" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B67" s="6">
         <v>53</v>
@@ -5340,18 +5343,18 @@
         <v>0</v>
       </c>
       <c r="P67" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Q67" s="6"/>
       <c r="R67" s="6"/>
       <c r="S67" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="T67" s="6">
         <v>1</v>
       </c>
       <c r="U67" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="V67" s="6"/>
       <c r="X67">
@@ -5363,9 +5366,9 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:25">
       <c r="A68" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B68" s="6">
         <v>54</v>
@@ -5410,7 +5413,7 @@
         <v>0.9</v>
       </c>
       <c r="P68" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q68" s="6"/>
       <c r="R68" s="6"/>
@@ -5419,7 +5422,7 @@
         <v>1</v>
       </c>
       <c r="U68" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="V68" s="6"/>
       <c r="X68">
@@ -5431,9 +5434,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:25">
       <c r="A69" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B69" s="6">
         <v>55</v>
@@ -5481,18 +5484,18 @@
         <v>0</v>
       </c>
       <c r="P69" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="Q69" s="6"/>
       <c r="R69" s="6"/>
       <c r="S69" s="6" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="T69" s="6">
         <v>1</v>
       </c>
       <c r="U69" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="V69" s="6"/>
       <c r="X69">
@@ -5504,9 +5507,9 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:25">
       <c r="A70" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B70" s="6">
         <v>56</v>
@@ -5554,7 +5557,7 @@
         <v>0</v>
       </c>
       <c r="P70" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q70" s="6"/>
       <c r="R70" s="6"/>
@@ -5563,7 +5566,7 @@
         <v>1</v>
       </c>
       <c r="U70" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="V70" s="6"/>
       <c r="X70">
@@ -5575,9 +5578,9 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:25">
       <c r="A71" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B71" s="6">
         <v>57</v>
@@ -5625,16 +5628,16 @@
         <v>0</v>
       </c>
       <c r="P71" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="T71">
         <v>1</v>
       </c>
       <c r="U71" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="V71" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X71">
         <f t="shared" si="13"/>
@@ -5645,9 +5648,9 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:25">
       <c r="A72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B72" s="6">
         <v>58</v>
@@ -5695,16 +5698,16 @@
         <v>0</v>
       </c>
       <c r="P72" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T72">
         <v>1</v>
       </c>
       <c r="U72" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="V72" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X72">
         <f t="shared" si="13"/>
@@ -5715,9 +5718,9 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:25">
       <c r="A73" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B73" s="6">
         <v>59</v>
@@ -5765,13 +5768,13 @@
         <v>0</v>
       </c>
       <c r="P73" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="T73">
         <v>1</v>
       </c>
       <c r="U73" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X73">
         <f t="shared" si="13"/>
@@ -5782,9 +5785,9 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:25">
       <c r="A74" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B74" s="6">
         <v>60</v>
@@ -5829,13 +5832,13 @@
         <v>0.9</v>
       </c>
       <c r="P74" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T74">
         <v>1</v>
       </c>
       <c r="U74" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X74">
         <f t="shared" si="13"/>
@@ -5846,9 +5849,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:25">
       <c r="A75" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B75" s="6">
         <v>61</v>
@@ -5893,13 +5896,13 @@
         <v>0.9</v>
       </c>
       <c r="P75" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="T75">
         <v>1</v>
       </c>
       <c r="U75" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X75">
         <f t="shared" si="13"/>
@@ -5910,9 +5913,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:25">
       <c r="A76" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B76" s="6">
         <v>62</v>
@@ -5960,16 +5963,16 @@
         <v>0</v>
       </c>
       <c r="P76" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="T76">
         <v>1</v>
       </c>
       <c r="U76" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="V76" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X76">
         <f t="shared" si="13"/>
@@ -5980,9 +5983,9 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:25">
       <c r="A77" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B77" s="6">
         <v>63</v>
@@ -6030,13 +6033,13 @@
         <v>0</v>
       </c>
       <c r="P77" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="T77">
         <v>1</v>
       </c>
       <c r="U77" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X77">
         <f t="shared" si="13"/>
@@ -6047,9 +6050,9 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:25">
       <c r="A78" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B78" s="6">
         <v>64</v>
@@ -6094,13 +6097,13 @@
         <v>0.9</v>
       </c>
       <c r="P78" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T78">
         <v>1</v>
       </c>
       <c r="U78" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X78">
         <f t="shared" si="13"/>
@@ -6111,9 +6114,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:25">
       <c r="A79" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B79" s="6">
         <v>65</v>
@@ -6161,13 +6164,13 @@
         <v>0</v>
       </c>
       <c r="P79" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="T79">
         <v>1</v>
       </c>
       <c r="U79" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X79">
         <f t="shared" si="13"/>
@@ -6178,9 +6181,9 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:25">
       <c r="A80" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B80" s="6">
         <v>66</v>
@@ -6225,13 +6228,13 @@
         <v>0.9</v>
       </c>
       <c r="P80" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="T80">
         <v>1</v>
       </c>
       <c r="U80" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X80">
         <f t="shared" si="13"/>
@@ -6242,9 +6245,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:27">
       <c r="A81" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B81" s="6">
         <v>67</v>
@@ -6292,13 +6295,13 @@
         <v>0</v>
       </c>
       <c r="P81" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="T81" s="6">
         <v>1</v>
       </c>
       <c r="U81" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X81">
         <f t="shared" si="13"/>
@@ -6309,9 +6312,9 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:27">
       <c r="A82" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B82" s="6">
         <v>68</v>
@@ -6356,13 +6359,13 @@
         <v>0.9</v>
       </c>
       <c r="P82" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="T82">
         <v>1</v>
       </c>
       <c r="U82" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X82">
         <f t="shared" si="13"/>
@@ -6373,9 +6376,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:27">
       <c r="A83" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B83" s="6">
         <v>69</v>
@@ -6420,7 +6423,7 @@
         <v>0.9</v>
       </c>
       <c r="P83" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Q83" s="6"/>
       <c r="R83" s="6"/>
@@ -6429,7 +6432,7 @@
         <v>1</v>
       </c>
       <c r="U83" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X83">
         <f t="shared" si="13"/>
@@ -6440,9 +6443,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:27">
       <c r="A84" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B84" s="6">
         <v>70</v>
@@ -6487,13 +6490,13 @@
         <v>0.5</v>
       </c>
       <c r="P84" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="T84">
         <v>1</v>
       </c>
       <c r="U84" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X84">
         <f t="shared" si="13"/>
@@ -6504,9 +6507,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:27">
       <c r="A85" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B85" s="6">
         <v>71</v>
@@ -6551,13 +6554,13 @@
         <v>1.8</v>
       </c>
       <c r="P85" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="T85">
         <v>1</v>
       </c>
       <c r="U85" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X85">
         <f t="shared" si="13"/>
@@ -6568,7 +6571,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:27">
       <c r="B86" s="6"/>
       <c r="J86">
         <f t="shared" si="20"/>
@@ -6599,9 +6602,9 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:27">
       <c r="A87" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B87" s="17"/>
       <c r="D87">
@@ -6637,9 +6640,9 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:27">
       <c r="A88" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B88" s="7">
         <v>72</v>
@@ -6687,13 +6690,13 @@
         <v>0</v>
       </c>
       <c r="P88" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="T88">
         <v>1</v>
       </c>
       <c r="U88" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X88">
         <f t="shared" ref="X88:X113" si="24">IF(ISNUMBER(E88),1,0)</f>
@@ -6704,9 +6707,9 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:27">
       <c r="A89" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B89" s="7">
         <v>73</v>
@@ -6754,13 +6757,13 @@
         <v>0</v>
       </c>
       <c r="P89" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="T89">
         <v>1</v>
       </c>
       <c r="U89" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X89">
         <f t="shared" si="24"/>
@@ -6771,9 +6774,9 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:27">
       <c r="A90" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B90" s="7">
         <v>74</v>
@@ -6818,13 +6821,13 @@
         <v>1.6</v>
       </c>
       <c r="P90" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="T90">
         <v>1</v>
       </c>
       <c r="U90" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X90">
         <f t="shared" si="24"/>
@@ -6835,9 +6838,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:27">
       <c r="A91" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B91" s="7">
         <v>75</v>
@@ -6885,13 +6888,13 @@
         <v>0</v>
       </c>
       <c r="P91" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="T91">
         <v>1</v>
       </c>
       <c r="U91" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X91">
         <f t="shared" si="24"/>
@@ -6902,9 +6905,9 @@
         <v/>
       </c>
     </row>
-    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:27">
       <c r="A92" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B92" s="7">
         <v>76</v>
@@ -6949,16 +6952,16 @@
         <v>1.6</v>
       </c>
       <c r="P92" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T92">
         <v>1</v>
       </c>
       <c r="U92" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="W92" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="X92">
         <f t="shared" si="24"/>
@@ -6969,12 +6972,12 @@
         <v>80</v>
       </c>
       <c r="AA92" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="93" spans="1:27">
       <c r="A93" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B93" s="7">
         <v>77</v>
@@ -7022,13 +7025,13 @@
         <v>0</v>
       </c>
       <c r="P93" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="T93">
         <v>1</v>
       </c>
       <c r="U93" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X93">
         <f t="shared" si="24"/>
@@ -7039,9 +7042,9 @@
         <v/>
       </c>
     </row>
-    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:27">
       <c r="A94" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B94" s="7">
         <v>78</v>
@@ -7089,13 +7092,13 @@
         <v>0</v>
       </c>
       <c r="P94" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="T94">
         <v>1</v>
       </c>
       <c r="U94" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X94">
         <f t="shared" si="24"/>
@@ -7106,9 +7109,9 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:27">
       <c r="A95" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B95" s="7">
         <v>79</v>
@@ -7156,13 +7159,13 @@
         <v>0</v>
       </c>
       <c r="P95" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="T95">
         <v>1</v>
       </c>
       <c r="U95" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X95">
         <f t="shared" si="24"/>
@@ -7173,9 +7176,9 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:27">
       <c r="A96" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B96" s="7">
         <v>80</v>
@@ -7220,13 +7223,13 @@
         <v>1</v>
       </c>
       <c r="P96" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="T96">
         <v>1</v>
       </c>
       <c r="U96" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X96">
         <f t="shared" si="24"/>
@@ -7237,9 +7240,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="97" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:27">
       <c r="A97" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B97" s="7">
         <v>81</v>
@@ -7284,13 +7287,13 @@
         <v>0.5</v>
       </c>
       <c r="P97" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="T97">
         <v>1</v>
       </c>
       <c r="U97" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X97">
         <f t="shared" si="24"/>
@@ -7301,9 +7304,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="98" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:27">
       <c r="A98" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B98" s="7">
         <v>82</v>
@@ -7351,13 +7354,13 @@
         <v>0</v>
       </c>
       <c r="P98" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="T98">
         <v>1</v>
       </c>
       <c r="U98" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X98">
         <f t="shared" si="24"/>
@@ -7368,9 +7371,9 @@
         <v/>
       </c>
     </row>
-    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:27">
       <c r="A99" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B99" s="7">
         <v>83</v>
@@ -7418,16 +7421,16 @@
         <v>0</v>
       </c>
       <c r="P99" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="T99">
         <v>1</v>
       </c>
       <c r="U99" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="W99" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="X99">
         <f t="shared" si="24"/>
@@ -7438,12 +7441,12 @@
         <v/>
       </c>
       <c r="AA99" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="100" spans="1:27">
       <c r="A100" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B100" s="7">
         <v>84</v>
@@ -7488,13 +7491,13 @@
         <v>0.9</v>
       </c>
       <c r="P100" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="T100">
         <v>1</v>
       </c>
       <c r="U100" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X100">
         <f t="shared" si="24"/>
@@ -7505,9 +7508,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:27">
       <c r="A101" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B101" s="7">
         <v>85</v>
@@ -7552,13 +7555,13 @@
         <v>0.8</v>
       </c>
       <c r="P101" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="T101">
         <v>1</v>
       </c>
       <c r="U101" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X101">
         <f t="shared" si="24"/>
@@ -7569,9 +7572,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="102" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:27">
       <c r="A102" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B102" s="7">
         <v>86</v>
@@ -7616,13 +7619,13 @@
         <v>1.6</v>
       </c>
       <c r="P102" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="T102">
         <v>1</v>
       </c>
       <c r="U102" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X102">
         <f t="shared" si="24"/>
@@ -7633,9 +7636,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="103" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:27">
       <c r="A103" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B103" s="7">
         <v>87</v>
@@ -7683,13 +7686,13 @@
         <v>0</v>
       </c>
       <c r="P103" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="T103">
         <v>1</v>
       </c>
       <c r="U103" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X103">
         <f t="shared" si="24"/>
@@ -7700,9 +7703,9 @@
         <v/>
       </c>
     </row>
-    <row r="104" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:27">
       <c r="A104" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B104" s="7">
         <v>88</v>
@@ -7738,16 +7741,16 @@
         <v>0</v>
       </c>
       <c r="P104" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="S104" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="T104">
         <v>1</v>
       </c>
       <c r="U104" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X104">
         <f t="shared" si="24"/>
@@ -7758,9 +7761,9 @@
         <v/>
       </c>
     </row>
-    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:27">
       <c r="A105" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B105" s="7">
         <v>89</v>
@@ -7793,13 +7796,13 @@
         <v>1.6</v>
       </c>
       <c r="P105" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="T105">
         <v>1</v>
       </c>
       <c r="U105" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X105">
         <f t="shared" si="24"/>
@@ -7810,9 +7813,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="106" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:27">
       <c r="A106" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B106" s="7">
         <v>90</v>
@@ -7848,13 +7851,13 @@
         <v>0</v>
       </c>
       <c r="P106" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="T106">
         <v>1</v>
       </c>
       <c r="U106" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X106">
         <f t="shared" si="24"/>
@@ -7865,9 +7868,9 @@
         <v/>
       </c>
     </row>
-    <row r="107" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:27">
       <c r="A107" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B107" s="7">
         <v>91</v>
@@ -7900,13 +7903,13 @@
         <v>1</v>
       </c>
       <c r="P107" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="T107">
         <v>1</v>
       </c>
       <c r="U107" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X107">
         <f t="shared" si="24"/>
@@ -7917,9 +7920,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="108" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:27">
       <c r="A108" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B108" s="7">
         <v>92</v>
@@ -7955,13 +7958,13 @@
         <v>0</v>
       </c>
       <c r="P108" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="T108">
         <v>1</v>
       </c>
       <c r="U108" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X108">
         <f t="shared" si="24"/>
@@ -7972,9 +7975,9 @@
         <v/>
       </c>
     </row>
-    <row r="109" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:27">
       <c r="A109" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B109" s="7">
         <v>93</v>
@@ -8010,13 +8013,16 @@
         <v>0</v>
       </c>
       <c r="P109" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="T109">
         <v>1</v>
       </c>
       <c r="U109" t="s">
-        <v>150</v>
+        <v>149</v>
+      </c>
+      <c r="W109" t="s">
+        <v>263</v>
       </c>
       <c r="X109">
         <f t="shared" si="24"/>
@@ -8026,10 +8032,13 @@
         <f t="shared" si="19"/>
         <v/>
       </c>
-    </row>
-    <row r="110" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA109" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="110" spans="1:27">
       <c r="A110" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B110" s="7">
         <v>94</v>
@@ -8077,13 +8086,13 @@
         <v>0</v>
       </c>
       <c r="P110" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="T110">
         <v>1</v>
       </c>
       <c r="U110" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X110">
         <f t="shared" si="24"/>
@@ -8094,9 +8103,9 @@
         <v/>
       </c>
     </row>
-    <row r="111" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:27">
       <c r="A111" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B111" s="7">
         <v>95</v>
@@ -8141,13 +8150,13 @@
         <v>1.6</v>
       </c>
       <c r="P111" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="T111">
         <v>1</v>
       </c>
       <c r="U111" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X111">
         <f t="shared" si="24"/>
@@ -8158,9 +8167,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="112" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:27">
       <c r="A112" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B112" s="7">
         <v>96</v>
@@ -8205,13 +8214,13 @@
         <v>1.6</v>
       </c>
       <c r="P112" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="T112">
         <v>1</v>
       </c>
       <c r="U112" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X112">
         <f t="shared" si="24"/>
@@ -8222,9 +8231,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="113" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:27">
       <c r="A113" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B113" s="7">
         <v>97</v>
@@ -8269,13 +8278,16 @@
         <v>0.8</v>
       </c>
       <c r="P113" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="T113">
         <v>1</v>
       </c>
       <c r="U113" t="s">
-        <v>150</v>
+        <v>149</v>
+      </c>
+      <c r="W113" t="s">
+        <v>264</v>
       </c>
       <c r="X113">
         <f t="shared" si="24"/>
@@ -8285,8 +8297,11 @@
         <f t="shared" si="19"/>
         <v>80</v>
       </c>
-    </row>
-    <row r="114" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA113" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="114" spans="1:27">
       <c r="B114" s="6"/>
       <c r="D114">
         <f t="shared" ref="D114:D115" si="29">IF(F114=4, 1,0)</f>
@@ -8321,9 +8336,9 @@
         <v/>
       </c>
     </row>
-    <row r="115" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:27">
       <c r="A115" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B115" s="17"/>
       <c r="D115">
@@ -8359,9 +8374,9 @@
         <v/>
       </c>
     </row>
-    <row r="116" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:27">
       <c r="A116" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B116" s="6">
         <v>98</v>
@@ -8406,13 +8421,13 @@
         <v>1</v>
       </c>
       <c r="P116" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="T116">
         <v>1</v>
       </c>
       <c r="U116" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X116">
         <f t="shared" ref="X116:X124" si="33">IF(ISNUMBER(E116),1,0)</f>
@@ -8423,9 +8438,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="117" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:27">
       <c r="A117" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B117" s="6">
         <v>99</v>
@@ -8470,13 +8485,13 @@
         <v>1.6</v>
       </c>
       <c r="P117" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="T117">
         <v>1</v>
       </c>
       <c r="U117" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X117">
         <f t="shared" si="33"/>
@@ -8487,9 +8502,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="118" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:27">
       <c r="A118" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B118" s="6">
         <v>100</v>
@@ -8534,13 +8549,13 @@
         <v>1.8</v>
       </c>
       <c r="P118" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="T118">
         <v>1</v>
       </c>
       <c r="U118" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X118">
         <f t="shared" si="33"/>
@@ -8551,9 +8566,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="119" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:27">
       <c r="A119" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B119" s="6">
         <v>101</v>
@@ -8598,13 +8613,13 @@
         <v>1.8</v>
       </c>
       <c r="P119" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="T119">
         <v>1</v>
       </c>
       <c r="U119" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X119">
         <f t="shared" si="33"/>
@@ -8615,9 +8630,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="120" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:27">
       <c r="A120" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B120" s="6">
         <v>102</v>
@@ -8662,13 +8677,13 @@
         <v>1.8</v>
       </c>
       <c r="P120" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="T120">
         <v>1</v>
       </c>
       <c r="U120" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X120">
         <f t="shared" si="33"/>
@@ -8679,9 +8694,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="121" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:27">
       <c r="A121" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B121" s="6">
         <v>103</v>
@@ -8726,13 +8741,13 @@
         <v>1.8</v>
       </c>
       <c r="P121" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="T121">
         <v>1</v>
       </c>
       <c r="U121" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X121">
         <f t="shared" si="33"/>
@@ -8743,9 +8758,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="122" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:27">
       <c r="A122" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B122" s="6">
         <v>104</v>
@@ -8790,13 +8805,13 @@
         <v>0.9</v>
       </c>
       <c r="P122" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="T122">
         <v>1</v>
       </c>
       <c r="U122" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X122">
         <f t="shared" si="33"/>
@@ -8807,9 +8822,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="123" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:27">
       <c r="A123" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B123" s="6">
         <v>105</v>
@@ -8854,13 +8869,13 @@
         <v>1.8</v>
       </c>
       <c r="P123" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="T123">
         <v>1</v>
       </c>
       <c r="U123" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X123">
         <f t="shared" si="33"/>
@@ -8871,9 +8886,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="124" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:27">
       <c r="A124" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B124" s="6">
         <v>106</v>
@@ -8921,13 +8936,13 @@
         <v>0</v>
       </c>
       <c r="S124" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="T124">
         <v>1</v>
       </c>
       <c r="U124" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X124">
         <f t="shared" si="33"/>
@@ -8938,7 +8953,7 @@
         <v/>
       </c>
     </row>
-    <row r="125" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:27">
       <c r="B125" s="6"/>
       <c r="J125">
         <f t="shared" si="20"/>
@@ -8957,9 +8972,9 @@
         <v/>
       </c>
     </row>
-    <row r="126" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:27">
       <c r="A126" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B126" s="17"/>
       <c r="J126">
@@ -8975,9 +8990,9 @@
         <v/>
       </c>
     </row>
-    <row r="127" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:27">
       <c r="A127" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B127" s="6"/>
       <c r="C127">
@@ -9012,9 +9027,9 @@
         <v/>
       </c>
     </row>
-    <row r="128" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:27">
       <c r="A128" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B128" s="6"/>
       <c r="C128">
@@ -9049,9 +9064,9 @@
         <v/>
       </c>
     </row>
-    <row r="129" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:25">
       <c r="A129" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B129" s="6"/>
       <c r="C129">
@@ -9086,9 +9101,9 @@
         <v/>
       </c>
     </row>
-    <row r="130" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:25">
       <c r="A130" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B130" s="6"/>
       <c r="C130">
@@ -9119,247 +9134,247 @@
         <v/>
       </c>
     </row>
-    <row r="131" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:25">
       <c r="B131" s="6"/>
     </row>
-    <row r="132" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:25">
       <c r="B132" s="6"/>
     </row>
-    <row r="133" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:25">
       <c r="B133" s="6"/>
     </row>
-    <row r="134" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:25">
       <c r="B134" s="6"/>
     </row>
-    <row r="135" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:25">
       <c r="B135" s="6"/>
     </row>
-    <row r="136" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:25">
       <c r="B136" s="6"/>
     </row>
-    <row r="137" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:25">
       <c r="B137" s="6"/>
     </row>
-    <row r="138" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:25">
       <c r="B138" s="6"/>
     </row>
-    <row r="139" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:25">
       <c r="B139" s="6"/>
     </row>
-    <row r="140" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:25">
       <c r="B140" s="6"/>
     </row>
-    <row r="141" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:25">
       <c r="B141" s="6"/>
     </row>
-    <row r="142" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:25">
       <c r="B142" s="6"/>
     </row>
-    <row r="143" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:25">
       <c r="B143" s="6"/>
     </row>
-    <row r="144" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:25">
       <c r="B144" s="6"/>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:2">
       <c r="B145" s="6"/>
     </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:2">
       <c r="B146" s="6"/>
     </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:2">
       <c r="B147" s="6"/>
     </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:2">
       <c r="B148" s="6"/>
     </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:2">
       <c r="B149" s="6"/>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:2">
       <c r="B150" s="6"/>
     </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:2">
       <c r="B151" s="6"/>
     </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:2">
       <c r="B152" s="6"/>
     </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:2">
       <c r="B153" s="6"/>
     </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:2">
       <c r="B154" s="6"/>
     </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:2">
       <c r="B155" s="6"/>
     </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:2">
       <c r="B156" s="6"/>
     </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:2">
       <c r="B157" s="6"/>
     </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:2">
       <c r="B158" s="6"/>
     </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:2">
       <c r="B159" s="6"/>
     </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:2">
       <c r="B160" s="6"/>
     </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:2">
       <c r="B161" s="6"/>
     </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:2">
       <c r="B162" s="6"/>
     </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:2">
       <c r="B163" s="6"/>
     </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:2">
       <c r="B164" s="6"/>
     </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:2">
       <c r="B165" s="6"/>
     </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:2">
       <c r="B166" s="6"/>
     </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:2">
       <c r="B167" s="6"/>
     </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:2">
       <c r="B168" s="6"/>
     </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:2">
       <c r="B169" s="6"/>
     </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:2">
       <c r="B170" s="6"/>
     </row>
-    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:2">
       <c r="B171" s="6"/>
     </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:2">
       <c r="B172" s="6"/>
     </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:2">
       <c r="B173" s="6"/>
     </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:2">
       <c r="B174" s="6"/>
     </row>
-    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:2">
       <c r="B175" s="6"/>
     </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:2">
       <c r="B176" s="6"/>
     </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:2">
       <c r="B177" s="6"/>
     </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:2">
       <c r="B178" s="6"/>
     </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:2">
       <c r="B179" s="6"/>
     </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:2">
       <c r="B180" s="6"/>
     </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:2">
       <c r="B181" s="6"/>
     </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:2">
       <c r="B182" s="6"/>
     </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:2">
       <c r="B183" s="6"/>
     </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:2">
       <c r="B184" s="6"/>
     </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:2">
       <c r="B185" s="6"/>
     </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:2">
       <c r="B186" s="6"/>
     </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:2">
       <c r="B187" s="6"/>
     </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:2">
       <c r="B188" s="6"/>
     </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:2">
       <c r="B189" s="6"/>
     </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:2">
       <c r="B190" s="6"/>
     </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:2">
       <c r="B191" s="6"/>
     </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:2">
       <c r="B192" s="6"/>
     </row>
-    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:2">
       <c r="B193" s="6"/>
     </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:2">
       <c r="B194" s="6"/>
     </row>
-    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:2">
       <c r="B195" s="6"/>
     </row>
-    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:2">
       <c r="B196" s="6"/>
     </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:2">
       <c r="B197" s="6"/>
     </row>
-    <row r="198" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:2">
       <c r="B198" s="6"/>
     </row>
-    <row r="199" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:2">
       <c r="B199" s="6"/>
     </row>
-    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:2">
       <c r="B200" s="6"/>
     </row>
-    <row r="201" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:2">
       <c r="B201" s="6"/>
     </row>
-    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:2">
       <c r="B202" s="6"/>
     </row>
-    <row r="203" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:2">
       <c r="B203" s="6"/>
     </row>
-    <row r="204" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:2">
       <c r="B204" s="6"/>
     </row>
-    <row r="205" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:2">
       <c r="B205" s="6"/>
     </row>
-    <row r="206" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:2">
       <c r="B206" s="6"/>
     </row>
-    <row r="207" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:2">
       <c r="B207" s="6"/>
     </row>
-    <row r="208" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:2">
       <c r="B208" s="6"/>
     </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:2">
       <c r="B209" s="6"/>
     </row>
-    <row r="210" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:2">
       <c r="B210" s="6"/>
     </row>
-    <row r="211" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:2">
       <c r="B211" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated RSVP for Kathy/Don
</commit_message>
<xml_diff>
--- a/Guest_List_Invited.xlsx
+++ b/Guest_List_Invited.xlsx
@@ -1252,7 +1252,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1263,8 +1263,8 @@
   <dimension ref="A1:AC212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S69" sqref="S69"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E109" sqref="E109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1336,7 +1336,7 @@
       </c>
       <c r="R2" s="14">
         <f>D3+G3*(1+Z4/100)</f>
-        <v>148.35491428715844</v>
+        <v>147.67689475048405</v>
       </c>
       <c r="S2" t="s">
         <v>215</v>
@@ -1360,7 +1360,7 @@
       </c>
       <c r="D3" s="19">
         <f>SUM(E6:E130)</f>
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3">
@@ -1369,7 +1369,7 @@
       </c>
       <c r="G3">
         <f>SUM(O6:O130)</f>
-        <v>57.199999999999974</v>
+        <v>55.199999999999974</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
@@ -1383,11 +1383,11 @@
       </c>
       <c r="R3" s="14">
         <f>D3+G3*(1-Z4/100)</f>
-        <v>116.04508571284151</v>
+        <v>116.7231052495159</v>
       </c>
       <c r="S3" s="13">
         <f>SUM(X6:X130)/COUNT(X6:X11,X14:X41,X45:X50,X53:X59,X62:X86,X89:X114,X117:X125,X128:X130)</f>
-        <v>0.51376146788990829</v>
+        <v>0.52293577981651373</v>
       </c>
       <c r="T3" s="10"/>
       <c r="U3" s="10"/>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="Z4" s="10">
         <f>STDEV(Y6:Y130)</f>
-        <v>28.242857145381937</v>
+        <v>28.037852808847969</v>
       </c>
       <c r="AA4" s="10" t="s">
         <v>241</v>
@@ -3375,6 +3375,9 @@
       <c r="D35">
         <v>1</v>
       </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
       <c r="F35">
         <v>4</v>
       </c>
@@ -3406,7 +3409,7 @@
       </c>
       <c r="O35">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P35" t="s">
         <v>94</v>
@@ -3419,11 +3422,11 @@
       </c>
       <c r="X35">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="Y35">
+        <v>1</v>
+      </c>
+      <c r="Y35" t="str">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v/>
       </c>
     </row>
     <row r="36" spans="1:27">

</xml_diff>

<commit_message>
Added Joe & Allison
</commit_message>
<xml_diff>
--- a/Guest_List_Invited.xlsx
+++ b/Guest_List_Invited.xlsx
@@ -1252,7 +1252,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1263,8 +1263,8 @@
   <dimension ref="A1:AC212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E76" sqref="E76"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1336,7 +1336,7 @@
       </c>
       <c r="R2" s="14">
         <f>D3+G3*(1+Z4/100)</f>
-        <v>147.52494331621301</v>
+        <v>149.21488217258093</v>
       </c>
       <c r="S2" t="s">
         <v>215</v>
@@ -1359,35 +1359,35 @@
         <v>85</v>
       </c>
       <c r="D3" s="19">
-        <f>SUM(E6:E130)</f>
-        <v>78</v>
+        <f>SUM(E6:E130)+2</f>
+        <v>82</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3">
         <f>SUM(J6:J174)</f>
-        <v>133.29999999999995</v>
+        <v>133.49999999999997</v>
       </c>
       <c r="G3">
         <f>SUM(O6:O130)</f>
-        <v>54.299999999999976</v>
+        <v>52.499999999999979</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
       <c r="P3" s="12">
         <f>G3+D3</f>
-        <v>132.29999999999998</v>
+        <v>134.49999999999997</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>219</v>
       </c>
       <c r="R3" s="14">
         <f>D3+G3*(1-Z4/100)</f>
-        <v>117.07505668378693</v>
+        <v>119.78511782741901</v>
       </c>
       <c r="S3" s="13">
         <f>SUM(X6:X130)/COUNT(X6:X11,X14:X41,X45:X50,X53:X59,X62:X86,X89:X114,X117:X125,X128:X130)</f>
-        <v>0.5321100917431193</v>
+        <v>0.54128440366972475</v>
       </c>
       <c r="T3" s="10"/>
       <c r="U3" s="10"/>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="Z4" s="10">
         <f>STDEV(Y6:Y130)</f>
-        <v>28.038569643117963</v>
+        <v>28.028346995392315</v>
       </c>
       <c r="AA4" s="10" t="s">
         <v>241</v>
@@ -4953,7 +4953,7 @@
       <c r="B61" s="17"/>
       <c r="D61">
         <f>SUM(J62:J85)</f>
-        <v>32.399999999999991</v>
+        <v>32.599999999999994</v>
       </c>
       <c r="J61">
         <f t="shared" si="9"/>
@@ -4997,6 +4997,9 @@
       <c r="D62">
         <v>1</v>
       </c>
+      <c r="E62">
+        <v>2</v>
+      </c>
       <c r="F62">
         <v>4</v>
       </c>
@@ -5008,19 +5011,19 @@
       </c>
       <c r="J62">
         <f t="shared" si="9"/>
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="K62">
         <f t="shared" si="2"/>
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="L62">
         <f t="shared" si="3"/>
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="M62">
         <f t="shared" si="4"/>
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="N62">
         <f t="shared" si="5"/>
@@ -5028,7 +5031,7 @@
       </c>
       <c r="O62">
         <f t="shared" si="6"/>
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="P62" s="6" t="s">
         <v>239</v>
@@ -5045,11 +5048,11 @@
       <c r="V62" s="6"/>
       <c r="X62">
         <f t="shared" ref="X62:X86" si="13">IF(ISNUMBER(E62),1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Y62">
+        <v>1</v>
+      </c>
+      <c r="Y62" t="str">
         <f t="shared" si="7"/>
-        <v>90</v>
+        <v/>
       </c>
     </row>
     <row r="63" spans="1:29">

</xml_diff>

<commit_message>
Updated RSVPs for Mi-Sun & Kyle
</commit_message>
<xml_diff>
--- a/Guest_List_Invited.xlsx
+++ b/Guest_List_Invited.xlsx
@@ -1252,7 +1252,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1263,8 +1263,8 @@
   <dimension ref="A1:AC212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <pane ySplit="4" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E112" sqref="E112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1336,7 +1336,7 @@
       </c>
       <c r="R2" s="14">
         <f>D3+G3*(1+Z4/100)</f>
-        <v>149.21488217258093</v>
+        <v>149.07716072514739</v>
       </c>
       <c r="S2" t="s">
         <v>215</v>
@@ -1360,34 +1360,34 @@
       </c>
       <c r="D3" s="19">
         <f>SUM(E6:E130)+2</f>
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3">
         <f>SUM(J6:J174)</f>
-        <v>133.49999999999997</v>
+        <v>133.99999999999997</v>
       </c>
       <c r="G3">
         <f>SUM(O6:O130)</f>
-        <v>52.499999999999979</v>
+        <v>49.999999999999979</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
       <c r="P3" s="12">
         <f>G3+D3</f>
-        <v>134.49999999999997</v>
+        <v>134.99999999999997</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>219</v>
       </c>
       <c r="R3" s="14">
         <f>D3+G3*(1-Z4/100)</f>
-        <v>119.78511782741901</v>
+        <v>120.92283927485258</v>
       </c>
       <c r="S3" s="13">
         <f>SUM(X6:X130)/COUNT(X6:X11,X14:X41,X45:X50,X53:X59,X62:X86,X89:X114,X117:X125,X128:X130)</f>
-        <v>0.54128440366972475</v>
+        <v>0.55963302752293576</v>
       </c>
       <c r="T3" s="10"/>
       <c r="U3" s="10"/>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="Z4" s="10">
         <f>STDEV(Y6:Y130)</f>
-        <v>28.028346995392315</v>
+        <v>28.154321450294809</v>
       </c>
       <c r="AA4" s="10" t="s">
         <v>241</v>
@@ -4953,7 +4953,7 @@
       <c r="B61" s="17"/>
       <c r="D61">
         <f>SUM(J62:J85)</f>
-        <v>32.599999999999994</v>
+        <v>32.699999999999996</v>
       </c>
       <c r="J61">
         <f t="shared" si="9"/>
@@ -5448,6 +5448,9 @@
       <c r="D69">
         <v>1</v>
       </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
       <c r="F69">
         <v>3</v>
       </c>
@@ -5459,15 +5462,15 @@
       </c>
       <c r="J69">
         <f t="shared" si="9"/>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="K69">
         <f t="shared" si="2"/>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="L69">
         <f t="shared" si="3"/>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="M69">
         <f t="shared" si="4"/>
@@ -5479,7 +5482,7 @@
       </c>
       <c r="O69">
         <f t="shared" si="6"/>
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="P69" s="6" t="s">
         <v>109</v>
@@ -5496,11 +5499,11 @@
       <c r="V69" s="6"/>
       <c r="X69">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="Y69">
+        <v>1</v>
+      </c>
+      <c r="Y69" t="str">
         <f t="shared" si="7"/>
-        <v>90</v>
+        <v/>
       </c>
     </row>
     <row r="70" spans="1:25">
@@ -8200,6 +8203,9 @@
       <c r="D112">
         <v>1</v>
       </c>
+      <c r="E112">
+        <v>2</v>
+      </c>
       <c r="F112">
         <v>3</v>
       </c>
@@ -8211,15 +8217,15 @@
       </c>
       <c r="J112">
         <f t="shared" si="20"/>
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="K112">
         <f t="shared" ref="K112:K114" si="26">IF(F112&gt;1,J112,0)</f>
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="L112">
         <f t="shared" ref="L112:L114" si="27">IF(F112&gt;2,J112,0)</f>
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="M112">
         <f t="shared" ref="M112:M114" si="28">IF(F112&gt;3,J112,0)</f>
@@ -8231,7 +8237,7 @@
       </c>
       <c r="O112">
         <f t="shared" si="14"/>
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="P112" t="s">
         <v>115</v>
@@ -8244,11 +8250,11 @@
       </c>
       <c r="X112">
         <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="Y112">
+        <v>1</v>
+      </c>
+      <c r="Y112" t="str">
         <f t="shared" si="19"/>
-        <v>80</v>
+        <v/>
       </c>
     </row>
     <row r="113" spans="1:27">

</xml_diff>

<commit_message>
Evan and Izzy Address updated
</commit_message>
<xml_diff>
--- a/Guest_List_Invited.xlsx
+++ b/Guest_List_Invited.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\logan\Documents\GitHub\Farrell_Garrett_Wedding\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C244C6FB-4F27-4365-9513-C24FC9665187}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="179017"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="270">
   <si>
     <t xml:space="preserve">Priority </t>
   </si>
@@ -826,16 +832,19 @@
   </si>
   <si>
     <t>Helen only</t>
+  </si>
+  <si>
+    <t>3040 Coreopsis Ct, Dickinson TX 77539</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1252,22 +1261,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E116" sqref="E116"/>
+      <pane ySplit="4" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S125" sqref="S125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.85546875" customWidth="1"/>
     <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
@@ -1292,7 +1301,7 @@
     <col min="27" max="27" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15" customHeight="1">
+    <row r="1" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5">
         <v>4</v>
       </c>
@@ -1312,7 +1321,7 @@
       <c r="U1" s="10"/>
       <c r="V1" s="10"/>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>3</v>
       </c>
@@ -1350,7 +1359,7 @@
         <v>28.469765066395961</v>
       </c>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1399,7 +1408,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="4" spans="1:29" s="10" customFormat="1" ht="31.5" customHeight="1">
+    <row r="4" spans="1:29" s="10" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -1469,7 +1478,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="5" spans="1:29">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1479,7 +1488,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1546,7 +1555,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1613,7 +1622,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1680,7 +1689,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:29">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1747,7 +1756,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:29">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1814,7 +1823,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:29">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -1883,7 +1892,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:29">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
       <c r="C12" s="1"/>
       <c r="D12">
@@ -1926,7 +1935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:29">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -1964,7 +1973,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:29">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
@@ -2028,7 +2037,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:29">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -2092,7 +2101,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:29">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
@@ -2159,7 +2168,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:27">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
@@ -2223,7 +2232,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:27">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
@@ -2287,7 +2296,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:27">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>186</v>
       </c>
@@ -2354,7 +2363,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:27">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -2421,7 +2430,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:27">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
@@ -2485,7 +2494,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:27">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
@@ -2549,7 +2558,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:27">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>228</v>
       </c>
@@ -2616,7 +2625,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:27">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>17</v>
       </c>
@@ -2692,7 +2701,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="25" spans="1:27">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>18</v>
       </c>
@@ -2765,7 +2774,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="26" spans="1:27">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>19</v>
       </c>
@@ -2829,7 +2838,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:27">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>20</v>
       </c>
@@ -2896,7 +2905,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:27">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>21</v>
       </c>
@@ -2963,7 +2972,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:27">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>22</v>
       </c>
@@ -3030,7 +3039,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:27">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>23</v>
       </c>
@@ -3094,7 +3103,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:27">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>24</v>
       </c>
@@ -3161,7 +3170,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:27">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>25</v>
       </c>
@@ -3225,7 +3234,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:27">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>26</v>
       </c>
@@ -3289,7 +3298,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:27">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
@@ -3362,7 +3371,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="35" spans="1:27">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
@@ -3429,7 +3438,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:27">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>260</v>
       </c>
@@ -3493,7 +3502,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:27">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>40</v>
       </c>
@@ -3557,7 +3566,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:27">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>41</v>
       </c>
@@ -3630,7 +3639,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="39" spans="1:27">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>42</v>
       </c>
@@ -3697,7 +3706,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:27">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>43</v>
       </c>
@@ -3767,7 +3776,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:27">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>98</v>
       </c>
@@ -3831,7 +3840,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:27">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="7"/>
       <c r="D42">
@@ -3867,7 +3876,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:27">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B43" s="6"/>
       <c r="C43" s="1"/>
       <c r="D43">
@@ -3903,7 +3912,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:27">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>27</v>
       </c>
@@ -3941,7 +3950,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:27">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>28</v>
       </c>
@@ -4017,7 +4026,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="46" spans="1:27">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>29</v>
       </c>
@@ -4081,7 +4090,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:27">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>30</v>
       </c>
@@ -4148,7 +4157,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:27">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>31</v>
       </c>
@@ -4215,7 +4224,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:29">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>32</v>
       </c>
@@ -4285,7 +4294,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:29">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>229</v>
       </c>
@@ -4360,7 +4369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:29">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B51" s="6"/>
       <c r="J51">
         <f t="shared" si="9"/>
@@ -4391,7 +4400,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:29">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>48</v>
       </c>
@@ -4429,7 +4438,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:29">
+    <row r="53" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>47</v>
       </c>
@@ -4500,7 +4509,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:29">
+    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>50</v>
       </c>
@@ -4567,7 +4576,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:29">
+    <row r="55" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>49</v>
       </c>
@@ -4638,7 +4647,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:29">
+    <row r="56" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>75</v>
       </c>
@@ -4711,7 +4720,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="57" spans="1:29">
+    <row r="57" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>51</v>
       </c>
@@ -4781,7 +4790,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:29">
+    <row r="58" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>52</v>
       </c>
@@ -4851,7 +4860,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:29">
+    <row r="59" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>53</v>
       </c>
@@ -4918,7 +4927,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:29">
+    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B60" s="6"/>
       <c r="J60">
         <f t="shared" si="9"/>
@@ -4949,7 +4958,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:29">
+    <row r="61" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>46</v>
       </c>
@@ -4987,7 +4996,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:29">
+    <row r="62" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>220</v>
       </c>
@@ -5058,7 +5067,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:29">
+    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>266</v>
       </c>
@@ -5103,7 +5112,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="64" spans="1:29">
+    <row r="64" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>54</v>
       </c>
@@ -5171,7 +5180,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="1:25">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>55</v>
       </c>
@@ -5241,7 +5250,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="66" spans="1:25">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>56</v>
       </c>
@@ -5309,7 +5318,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="67" spans="1:25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>165</v>
       </c>
@@ -5380,7 +5389,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:25">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>189</v>
       </c>
@@ -5438,7 +5447,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:25">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>57</v>
       </c>
@@ -5509,7 +5518,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:25">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>254</v>
       </c>
@@ -5582,7 +5591,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:25">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>58</v>
       </c>
@@ -5653,7 +5662,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:25">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>59</v>
       </c>
@@ -5723,7 +5732,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:25">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>60</v>
       </c>
@@ -5793,7 +5802,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:25">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>61</v>
       </c>
@@ -5860,7 +5869,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:25">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>62</v>
       </c>
@@ -5927,7 +5936,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:25">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>63</v>
       </c>
@@ -5991,7 +6000,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="77" spans="1:25">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>64</v>
       </c>
@@ -6061,7 +6070,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:25">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>164</v>
       </c>
@@ -6128,7 +6137,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:25">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>66</v>
       </c>
@@ -6192,7 +6201,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="80" spans="1:25">
+    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>125</v>
       </c>
@@ -6259,7 +6268,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:27">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>263</v>
       </c>
@@ -6326,7 +6335,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:27">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>65</v>
       </c>
@@ -6393,7 +6402,7 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:27">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>167</v>
       </c>
@@ -6457,7 +6466,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="84" spans="1:27">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>221</v>
       </c>
@@ -6527,7 +6536,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="1:27">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>247</v>
       </c>
@@ -6591,7 +6600,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="1:27">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>222</v>
       </c>
@@ -6655,7 +6664,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="87" spans="1:27">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B87" s="6"/>
       <c r="J87">
         <f t="shared" si="20"/>
@@ -6686,7 +6695,7 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="1:27">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>71</v>
       </c>
@@ -6724,7 +6733,7 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="1:27">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>78</v>
       </c>
@@ -6791,7 +6800,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="1:27">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>72</v>
       </c>
@@ -6858,7 +6867,7 @@
         <v/>
       </c>
     </row>
-    <row r="91" spans="1:27">
+    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>132</v>
       </c>
@@ -6931,7 +6940,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="92" spans="1:27">
+    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>73</v>
       </c>
@@ -6998,7 +7007,7 @@
         <v/>
       </c>
     </row>
-    <row r="93" spans="1:27">
+    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>74</v>
       </c>
@@ -7068,7 +7077,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="94" spans="1:27">
+    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>155</v>
       </c>
@@ -7135,7 +7144,7 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="1:27">
+    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>152</v>
       </c>
@@ -7202,7 +7211,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="1:27">
+    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>156</v>
       </c>
@@ -7269,7 +7278,7 @@
         <v/>
       </c>
     </row>
-    <row r="97" spans="1:27">
+    <row r="97" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>118</v>
       </c>
@@ -7333,7 +7342,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="98" spans="1:27">
+    <row r="98" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>133</v>
       </c>
@@ -7397,7 +7406,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="99" spans="1:27">
+    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>76</v>
       </c>
@@ -7464,7 +7473,7 @@
         <v/>
       </c>
     </row>
-    <row r="100" spans="1:27">
+    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>157</v>
       </c>
@@ -7537,7 +7546,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="101" spans="1:27">
+    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>145</v>
       </c>
@@ -7601,7 +7610,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="102" spans="1:27">
+    <row r="102" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>77</v>
       </c>
@@ -7665,7 +7674,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="103" spans="1:27">
+    <row r="103" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>149</v>
       </c>
@@ -7729,7 +7738,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="104" spans="1:27">
+    <row r="104" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>150</v>
       </c>
@@ -7796,7 +7805,7 @@
         <v/>
       </c>
     </row>
-    <row r="105" spans="1:27">
+    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>227</v>
       </c>
@@ -7854,7 +7863,7 @@
         <v/>
       </c>
     </row>
-    <row r="106" spans="1:27">
+    <row r="106" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>116</v>
       </c>
@@ -7906,7 +7915,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="107" spans="1:27">
+    <row r="107" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>158</v>
       </c>
@@ -7961,7 +7970,7 @@
         <v/>
       </c>
     </row>
-    <row r="108" spans="1:27">
+    <row r="108" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>159</v>
       </c>
@@ -8013,7 +8022,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="109" spans="1:27">
+    <row r="109" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>80</v>
       </c>
@@ -8068,7 +8077,7 @@
         <v/>
       </c>
     </row>
-    <row r="110" spans="1:27">
+    <row r="110" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>225</v>
       </c>
@@ -8129,7 +8138,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="111" spans="1:27">
+    <row r="111" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>224</v>
       </c>
@@ -8196,7 +8205,7 @@
         <v/>
       </c>
     </row>
-    <row r="112" spans="1:27">
+    <row r="112" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>226</v>
       </c>
@@ -8263,7 +8272,7 @@
         <v/>
       </c>
     </row>
-    <row r="113" spans="1:27">
+    <row r="113" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>79</v>
       </c>
@@ -8327,7 +8336,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="114" spans="1:27">
+    <row r="114" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>223</v>
       </c>
@@ -8397,7 +8406,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="115" spans="1:27">
+    <row r="115" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B115" s="6"/>
       <c r="D115">
         <f t="shared" ref="D115:D116" si="29">IF(F115=4, 1,0)</f>
@@ -8432,7 +8441,7 @@
         <v/>
       </c>
     </row>
-    <row r="116" spans="1:27">
+    <row r="116" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>81</v>
       </c>
@@ -8470,7 +8479,7 @@
         <v/>
       </c>
     </row>
-    <row r="117" spans="1:27">
+    <row r="117" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>230</v>
       </c>
@@ -8534,7 +8543,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="118" spans="1:27">
+    <row r="118" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>82</v>
       </c>
@@ -8598,7 +8607,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="119" spans="1:27">
+    <row r="119" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>231</v>
       </c>
@@ -8662,7 +8671,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="120" spans="1:27">
+    <row r="120" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>83</v>
       </c>
@@ -8726,7 +8735,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="121" spans="1:27">
+    <row r="121" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>84</v>
       </c>
@@ -8790,7 +8799,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="122" spans="1:27">
+    <row r="122" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>232</v>
       </c>
@@ -8854,7 +8863,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="123" spans="1:27">
+    <row r="123" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>233</v>
       </c>
@@ -8918,7 +8927,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="124" spans="1:27">
+    <row r="124" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>234</v>
       </c>
@@ -8982,7 +8991,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="125" spans="1:27">
+    <row r="125" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>235</v>
       </c>
@@ -9031,6 +9040,9 @@
         <f t="shared" si="34"/>
         <v>0</v>
       </c>
+      <c r="P125" t="s">
+        <v>269</v>
+      </c>
       <c r="S125" t="s">
         <v>258</v>
       </c>
@@ -9049,7 +9061,7 @@
         <v/>
       </c>
     </row>
-    <row r="126" spans="1:27">
+    <row r="126" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B126" s="6"/>
       <c r="J126">
         <f t="shared" si="20"/>
@@ -9068,7 +9080,7 @@
         <v/>
       </c>
     </row>
-    <row r="127" spans="1:27">
+    <row r="127" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>206</v>
       </c>
@@ -9086,7 +9098,7 @@
         <v/>
       </c>
     </row>
-    <row r="128" spans="1:27">
+    <row r="128" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>256</v>
       </c>
@@ -9123,7 +9135,7 @@
         <v/>
       </c>
     </row>
-    <row r="129" spans="1:25">
+    <row r="129" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>207</v>
       </c>
@@ -9160,7 +9172,7 @@
         <v/>
       </c>
     </row>
-    <row r="130" spans="1:25">
+    <row r="130" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>208</v>
       </c>
@@ -9197,7 +9209,7 @@
         <v/>
       </c>
     </row>
-    <row r="131" spans="1:25">
+    <row r="131" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>257</v>
       </c>
@@ -9230,247 +9242,247 @@
         <v/>
       </c>
     </row>
-    <row r="132" spans="1:25">
+    <row r="132" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B132" s="6"/>
     </row>
-    <row r="133" spans="1:25">
+    <row r="133" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B133" s="6"/>
     </row>
-    <row r="134" spans="1:25">
+    <row r="134" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B134" s="6"/>
     </row>
-    <row r="135" spans="1:25">
+    <row r="135" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B135" s="6"/>
     </row>
-    <row r="136" spans="1:25">
+    <row r="136" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B136" s="6"/>
     </row>
-    <row r="137" spans="1:25">
+    <row r="137" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B137" s="6"/>
     </row>
-    <row r="138" spans="1:25">
+    <row r="138" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B138" s="6"/>
     </row>
-    <row r="139" spans="1:25">
+    <row r="139" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B139" s="6"/>
     </row>
-    <row r="140" spans="1:25">
+    <row r="140" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B140" s="6"/>
     </row>
-    <row r="141" spans="1:25">
+    <row r="141" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B141" s="6"/>
     </row>
-    <row r="142" spans="1:25">
+    <row r="142" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B142" s="6"/>
     </row>
-    <row r="143" spans="1:25">
+    <row r="143" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B143" s="6"/>
     </row>
-    <row r="144" spans="1:25">
+    <row r="144" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B144" s="6"/>
     </row>
-    <row r="145" spans="2:2">
+    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B145" s="6"/>
     </row>
-    <row r="146" spans="2:2">
+    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B146" s="6"/>
     </row>
-    <row r="147" spans="2:2">
+    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B147" s="6"/>
     </row>
-    <row r="148" spans="2:2">
+    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B148" s="6"/>
     </row>
-    <row r="149" spans="2:2">
+    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B149" s="6"/>
     </row>
-    <row r="150" spans="2:2">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B150" s="6"/>
     </row>
-    <row r="151" spans="2:2">
+    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B151" s="6"/>
     </row>
-    <row r="152" spans="2:2">
+    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B152" s="6"/>
     </row>
-    <row r="153" spans="2:2">
+    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B153" s="6"/>
     </row>
-    <row r="154" spans="2:2">
+    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B154" s="6"/>
     </row>
-    <row r="155" spans="2:2">
+    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B155" s="6"/>
     </row>
-    <row r="156" spans="2:2">
+    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B156" s="6"/>
     </row>
-    <row r="157" spans="2:2">
+    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B157" s="6"/>
     </row>
-    <row r="158" spans="2:2">
+    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B158" s="6"/>
     </row>
-    <row r="159" spans="2:2">
+    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B159" s="6"/>
     </row>
-    <row r="160" spans="2:2">
+    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B160" s="6"/>
     </row>
-    <row r="161" spans="2:2">
+    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B161" s="6"/>
     </row>
-    <row r="162" spans="2:2">
+    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B162" s="6"/>
     </row>
-    <row r="163" spans="2:2">
+    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B163" s="6"/>
     </row>
-    <row r="164" spans="2:2">
+    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B164" s="6"/>
     </row>
-    <row r="165" spans="2:2">
+    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B165" s="6"/>
     </row>
-    <row r="166" spans="2:2">
+    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B166" s="6"/>
     </row>
-    <row r="167" spans="2:2">
+    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B167" s="6"/>
     </row>
-    <row r="168" spans="2:2">
+    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B168" s="6"/>
     </row>
-    <row r="169" spans="2:2">
+    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B169" s="6"/>
     </row>
-    <row r="170" spans="2:2">
+    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B170" s="6"/>
     </row>
-    <row r="171" spans="2:2">
+    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B171" s="6"/>
     </row>
-    <row r="172" spans="2:2">
+    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B172" s="6"/>
     </row>
-    <row r="173" spans="2:2">
+    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B173" s="6"/>
     </row>
-    <row r="174" spans="2:2">
+    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B174" s="6"/>
     </row>
-    <row r="175" spans="2:2">
+    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B175" s="6"/>
     </row>
-    <row r="176" spans="2:2">
+    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B176" s="6"/>
     </row>
-    <row r="177" spans="2:2">
+    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B177" s="6"/>
     </row>
-    <row r="178" spans="2:2">
+    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B178" s="6"/>
     </row>
-    <row r="179" spans="2:2">
+    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B179" s="6"/>
     </row>
-    <row r="180" spans="2:2">
+    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B180" s="6"/>
     </row>
-    <row r="181" spans="2:2">
+    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B181" s="6"/>
     </row>
-    <row r="182" spans="2:2">
+    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B182" s="6"/>
     </row>
-    <row r="183" spans="2:2">
+    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B183" s="6"/>
     </row>
-    <row r="184" spans="2:2">
+    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B184" s="6"/>
     </row>
-    <row r="185" spans="2:2">
+    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B185" s="6"/>
     </row>
-    <row r="186" spans="2:2">
+    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B186" s="6"/>
     </row>
-    <row r="187" spans="2:2">
+    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B187" s="6"/>
     </row>
-    <row r="188" spans="2:2">
+    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B188" s="6"/>
     </row>
-    <row r="189" spans="2:2">
+    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B189" s="6"/>
     </row>
-    <row r="190" spans="2:2">
+    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B190" s="6"/>
     </row>
-    <row r="191" spans="2:2">
+    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B191" s="6"/>
     </row>
-    <row r="192" spans="2:2">
+    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B192" s="6"/>
     </row>
-    <row r="193" spans="2:2">
+    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B193" s="6"/>
     </row>
-    <row r="194" spans="2:2">
+    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B194" s="6"/>
     </row>
-    <row r="195" spans="2:2">
+    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B195" s="6"/>
     </row>
-    <row r="196" spans="2:2">
+    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B196" s="6"/>
     </row>
-    <row r="197" spans="2:2">
+    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B197" s="6"/>
     </row>
-    <row r="198" spans="2:2">
+    <row r="198" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B198" s="6"/>
     </row>
-    <row r="199" spans="2:2">
+    <row r="199" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B199" s="6"/>
     </row>
-    <row r="200" spans="2:2">
+    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B200" s="6"/>
     </row>
-    <row r="201" spans="2:2">
+    <row r="201" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B201" s="6"/>
     </row>
-    <row r="202" spans="2:2">
+    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B202" s="6"/>
     </row>
-    <row r="203" spans="2:2">
+    <row r="203" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B203" s="6"/>
     </row>
-    <row r="204" spans="2:2">
+    <row r="204" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B204" s="6"/>
     </row>
-    <row r="205" spans="2:2">
+    <row r="205" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B205" s="6"/>
     </row>
-    <row r="206" spans="2:2">
+    <row r="206" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B206" s="6"/>
     </row>
-    <row r="207" spans="2:2">
+    <row r="207" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B207" s="6"/>
     </row>
-    <row r="208" spans="2:2">
+    <row r="208" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B208" s="6"/>
     </row>
-    <row r="209" spans="2:2">
+    <row r="209" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B209" s="6"/>
     </row>
-    <row r="210" spans="2:2">
+    <row r="210" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B210" s="6"/>
     </row>
-    <row r="211" spans="2:2">
+    <row r="211" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B211" s="6"/>
     </row>
-    <row r="212" spans="2:2">
+    <row r="212" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B212" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated with Mason's No
</commit_message>
<xml_diff>
--- a/Guest_List_Invited.xlsx
+++ b/Guest_List_Invited.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\logan\Documents\GitHub\Farrell_Garrett_Wedding\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{553660E8-0170-4DDE-A6BF-3E017AB1C6EC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="162913" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -834,11 +840,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1255,22 +1261,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E106" sqref="E106"/>
+      <pane ySplit="4" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E119" sqref="E119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.85546875" customWidth="1"/>
     <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
@@ -1295,7 +1301,7 @@
     <col min="27" max="27" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15" customHeight="1">
+    <row r="1" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5">
         <v>4</v>
       </c>
@@ -1315,7 +1321,7 @@
       <c r="U1" s="10"/>
       <c r="V1" s="10"/>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>3</v>
       </c>
@@ -1339,7 +1345,7 @@
       </c>
       <c r="R2" s="14">
         <f>D3+G3*(1+Z4/100)</f>
-        <v>147.37341204702642</v>
+        <v>145.39632067963103</v>
       </c>
       <c r="S2" t="s">
         <v>215</v>
@@ -1353,7 +1359,7 @@
         <v>28.469765066395961</v>
       </c>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1368,29 +1374,29 @@
       <c r="E3" s="19"/>
       <c r="F3">
         <f>SUM(J6:J174)</f>
-        <v>134.79999999999995</v>
+        <v>133.19999999999996</v>
       </c>
       <c r="G3">
         <f>SUM(O6:O130)</f>
-        <v>41.79999999999999</v>
+        <v>40.199999999999989</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
       <c r="P3" s="12">
         <f>G3+D3</f>
-        <v>135.79999999999998</v>
+        <v>134.19999999999999</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>219</v>
       </c>
       <c r="R3" s="14">
         <f>D3+G3*(1-Z4/100)</f>
-        <v>124.22658795297357</v>
+        <v>123.00367932036896</v>
       </c>
       <c r="S3" s="13">
         <f>SUM(X6:X130)/COUNT(X6:X11,X14:X41,X45:X50,X53:X59,X62:X86,X89:X114,X117:X125,X128:X130)</f>
-        <v>0.64220183486238536</v>
+        <v>0.65137614678899081</v>
       </c>
       <c r="T3" s="10"/>
       <c r="U3" s="10"/>
@@ -1402,7 +1408,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="4" spans="1:29" s="10" customFormat="1" ht="31.5" customHeight="1">
+    <row r="4" spans="1:29" s="10" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -1466,13 +1472,13 @@
       </c>
       <c r="Z4" s="10">
         <f>STDEV(Y6:Y130)</f>
-        <v>27.687588629249824</v>
+        <v>27.851543979181677</v>
       </c>
       <c r="AA4" s="10" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="5" spans="1:29">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1482,7 +1488,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1549,7 +1555,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1616,7 +1622,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1683,7 +1689,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:29">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1750,7 +1756,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:29">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1817,7 +1823,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:29">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -1886,7 +1892,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:29">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
       <c r="C12" s="1"/>
       <c r="D12">
@@ -1929,7 +1935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:29">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -1967,7 +1973,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:29">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
@@ -2031,7 +2037,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:29">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -2095,7 +2101,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:29">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
@@ -2162,7 +2168,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:27">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
@@ -2226,7 +2232,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:27">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
@@ -2290,7 +2296,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:27">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>186</v>
       </c>
@@ -2357,7 +2363,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:27">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -2424,7 +2430,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:27">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
@@ -2488,7 +2494,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:27">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
@@ -2552,7 +2558,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:27">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>228</v>
       </c>
@@ -2619,7 +2625,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:27">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>17</v>
       </c>
@@ -2695,7 +2701,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="25" spans="1:27">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>18</v>
       </c>
@@ -2768,7 +2774,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="26" spans="1:27">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>19</v>
       </c>
@@ -2832,7 +2838,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:27">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>20</v>
       </c>
@@ -2899,7 +2905,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:27">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>21</v>
       </c>
@@ -2966,7 +2972,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:27">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>22</v>
       </c>
@@ -3033,7 +3039,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:27">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>23</v>
       </c>
@@ -3097,7 +3103,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:27">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>24</v>
       </c>
@@ -3164,7 +3170,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:27">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>25</v>
       </c>
@@ -3228,7 +3234,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:27">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>26</v>
       </c>
@@ -3292,7 +3298,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:27">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
@@ -3365,7 +3371,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="35" spans="1:27">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
@@ -3432,7 +3438,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:27">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>260</v>
       </c>
@@ -3496,7 +3502,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:27">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>40</v>
       </c>
@@ -3563,7 +3569,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:27">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>41</v>
       </c>
@@ -3636,7 +3642,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="39" spans="1:27">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>42</v>
       </c>
@@ -3703,7 +3709,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:27">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>43</v>
       </c>
@@ -3773,7 +3779,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:27">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>98</v>
       </c>
@@ -3837,7 +3843,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:27">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="7"/>
       <c r="D42">
@@ -3873,7 +3879,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:27">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B43" s="6"/>
       <c r="C43" s="1"/>
       <c r="D43">
@@ -3909,7 +3915,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:27">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>27</v>
       </c>
@@ -3947,7 +3953,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:27">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>28</v>
       </c>
@@ -4023,7 +4029,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="46" spans="1:27">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>29</v>
       </c>
@@ -4087,7 +4093,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:27">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>30</v>
       </c>
@@ -4154,7 +4160,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:27">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>31</v>
       </c>
@@ -4221,7 +4227,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:29">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>32</v>
       </c>
@@ -4291,7 +4297,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:29">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>229</v>
       </c>
@@ -4366,7 +4372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:29">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B51" s="6"/>
       <c r="J51">
         <f t="shared" si="9"/>
@@ -4397,7 +4403,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:29">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>48</v>
       </c>
@@ -4435,7 +4441,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:29">
+    <row r="53" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>47</v>
       </c>
@@ -4506,7 +4512,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:29">
+    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>50</v>
       </c>
@@ -4573,7 +4579,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:29">
+    <row r="55" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>49</v>
       </c>
@@ -4644,7 +4650,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:29">
+    <row r="56" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>75</v>
       </c>
@@ -4717,7 +4723,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="57" spans="1:29">
+    <row r="57" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>51</v>
       </c>
@@ -4787,7 +4793,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:29">
+    <row r="58" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>52</v>
       </c>
@@ -4857,7 +4863,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:29">
+    <row r="59" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>53</v>
       </c>
@@ -4924,7 +4930,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:29">
+    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B60" s="6"/>
       <c r="J60">
         <f t="shared" si="9"/>
@@ -4955,7 +4961,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:29">
+    <row r="61" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>46</v>
       </c>
@@ -4993,7 +4999,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:29">
+    <row r="62" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>220</v>
       </c>
@@ -5064,7 +5070,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:29">
+    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>266</v>
       </c>
@@ -5109,7 +5115,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="64" spans="1:29">
+    <row r="64" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>54</v>
       </c>
@@ -5177,7 +5183,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="1:25">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>55</v>
       </c>
@@ -5247,7 +5253,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="66" spans="1:25">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>56</v>
       </c>
@@ -5315,7 +5321,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="67" spans="1:25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>165</v>
       </c>
@@ -5386,7 +5392,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:25">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>189</v>
       </c>
@@ -5444,7 +5450,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:25">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>57</v>
       </c>
@@ -5515,7 +5521,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:25">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>254</v>
       </c>
@@ -5588,7 +5594,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:25">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>58</v>
       </c>
@@ -5659,7 +5665,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:25">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>59</v>
       </c>
@@ -5729,7 +5735,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:25">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>60</v>
       </c>
@@ -5799,7 +5805,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:25">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>61</v>
       </c>
@@ -5866,7 +5872,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:25">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>62</v>
       </c>
@@ -5933,7 +5939,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:25">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>63</v>
       </c>
@@ -6000,7 +6006,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:25">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>64</v>
       </c>
@@ -6070,7 +6076,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:25">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>164</v>
       </c>
@@ -6137,7 +6143,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:25">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>66</v>
       </c>
@@ -6204,7 +6210,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="1:25">
+    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>125</v>
       </c>
@@ -6271,7 +6277,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:27">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>263</v>
       </c>
@@ -6338,7 +6344,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:27">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>65</v>
       </c>
@@ -6405,7 +6411,7 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:27">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>167</v>
       </c>
@@ -6472,7 +6478,7 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="1:27">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>221</v>
       </c>
@@ -6542,7 +6548,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="1:27">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>247</v>
       </c>
@@ -6609,7 +6615,7 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="1:27">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>222</v>
       </c>
@@ -6673,7 +6679,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="87" spans="1:27">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B87" s="6"/>
       <c r="J87">
         <f t="shared" si="20"/>
@@ -6704,7 +6710,7 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="1:27">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>71</v>
       </c>
@@ -6742,7 +6748,7 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="1:27">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>78</v>
       </c>
@@ -6809,7 +6815,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="1:27">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>72</v>
       </c>
@@ -6876,7 +6882,7 @@
         <v/>
       </c>
     </row>
-    <row r="91" spans="1:27">
+    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>132</v>
       </c>
@@ -6949,7 +6955,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="92" spans="1:27">
+    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>73</v>
       </c>
@@ -7016,7 +7022,7 @@
         <v/>
       </c>
     </row>
-    <row r="93" spans="1:27">
+    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>74</v>
       </c>
@@ -7086,7 +7092,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="94" spans="1:27">
+    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>155</v>
       </c>
@@ -7153,7 +7159,7 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="1:27">
+    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>152</v>
       </c>
@@ -7220,7 +7226,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="1:27">
+    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>156</v>
       </c>
@@ -7287,7 +7293,7 @@
         <v/>
       </c>
     </row>
-    <row r="97" spans="1:27">
+    <row r="97" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>118</v>
       </c>
@@ -7351,7 +7357,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="98" spans="1:27">
+    <row r="98" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>133</v>
       </c>
@@ -7415,7 +7421,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="99" spans="1:27">
+    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>76</v>
       </c>
@@ -7482,7 +7488,7 @@
         <v/>
       </c>
     </row>
-    <row r="100" spans="1:27">
+    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>157</v>
       </c>
@@ -7555,7 +7561,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="101" spans="1:27">
+    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>145</v>
       </c>
@@ -7619,7 +7625,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="102" spans="1:27">
+    <row r="102" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>77</v>
       </c>
@@ -7683,7 +7689,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="103" spans="1:27">
+    <row r="103" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>149</v>
       </c>
@@ -7747,7 +7753,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="104" spans="1:27">
+    <row r="104" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>150</v>
       </c>
@@ -7814,7 +7820,7 @@
         <v/>
       </c>
     </row>
-    <row r="105" spans="1:27">
+    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>227</v>
       </c>
@@ -7872,7 +7878,7 @@
         <v/>
       </c>
     </row>
-    <row r="106" spans="1:27">
+    <row r="106" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>116</v>
       </c>
@@ -7924,7 +7930,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="107" spans="1:27">
+    <row r="107" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>158</v>
       </c>
@@ -7979,7 +7985,7 @@
         <v/>
       </c>
     </row>
-    <row r="108" spans="1:27">
+    <row r="108" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>159</v>
       </c>
@@ -8034,7 +8040,7 @@
         <v/>
       </c>
     </row>
-    <row r="109" spans="1:27">
+    <row r="109" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>80</v>
       </c>
@@ -8089,7 +8095,7 @@
         <v/>
       </c>
     </row>
-    <row r="110" spans="1:27">
+    <row r="110" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>225</v>
       </c>
@@ -8150,7 +8156,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="111" spans="1:27">
+    <row r="111" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>224</v>
       </c>
@@ -8217,7 +8223,7 @@
         <v/>
       </c>
     </row>
-    <row r="112" spans="1:27">
+    <row r="112" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>226</v>
       </c>
@@ -8284,7 +8290,7 @@
         <v/>
       </c>
     </row>
-    <row r="113" spans="1:27">
+    <row r="113" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>79</v>
       </c>
@@ -8351,7 +8357,7 @@
         <v/>
       </c>
     </row>
-    <row r="114" spans="1:27">
+    <row r="114" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>223</v>
       </c>
@@ -8421,7 +8427,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="115" spans="1:27">
+    <row r="115" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B115" s="6"/>
       <c r="D115">
         <f t="shared" ref="D115:D116" si="29">IF(F115=4, 1,0)</f>
@@ -8456,7 +8462,7 @@
         <v/>
       </c>
     </row>
-    <row r="116" spans="1:27">
+    <row r="116" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>81</v>
       </c>
@@ -8494,7 +8500,7 @@
         <v/>
       </c>
     </row>
-    <row r="117" spans="1:27">
+    <row r="117" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>230</v>
       </c>
@@ -8558,7 +8564,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="118" spans="1:27">
+    <row r="118" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>82</v>
       </c>
@@ -8571,6 +8577,9 @@
       <c r="D118">
         <v>1</v>
       </c>
+      <c r="E118">
+        <v>0</v>
+      </c>
       <c r="F118">
         <v>4</v>
       </c>
@@ -8582,19 +8591,19 @@
       </c>
       <c r="J118">
         <f t="shared" si="20"/>
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="K118">
         <f t="shared" si="30"/>
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="L118">
         <f t="shared" si="31"/>
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="M118">
         <f t="shared" si="32"/>
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="N118">
         <f t="shared" si="25"/>
@@ -8602,7 +8611,7 @@
       </c>
       <c r="O118">
         <f t="shared" si="14"/>
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="P118" t="s">
         <v>138</v>
@@ -8615,14 +8624,14 @@
       </c>
       <c r="X118">
         <f t="shared" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="Y118">
+        <v>1</v>
+      </c>
+      <c r="Y118" t="str">
         <f t="shared" si="19"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="119" spans="1:27">
+        <v/>
+      </c>
+    </row>
+    <row r="119" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>231</v>
       </c>
@@ -8686,7 +8695,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="120" spans="1:27">
+    <row r="120" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>83</v>
       </c>
@@ -8750,7 +8759,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="121" spans="1:27">
+    <row r="121" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>84</v>
       </c>
@@ -8814,7 +8823,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="122" spans="1:27">
+    <row r="122" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>232</v>
       </c>
@@ -8878,7 +8887,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="123" spans="1:27">
+    <row r="123" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>233</v>
       </c>
@@ -8942,7 +8951,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="124" spans="1:27">
+    <row r="124" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>234</v>
       </c>
@@ -9006,7 +9015,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="125" spans="1:27">
+    <row r="125" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>235</v>
       </c>
@@ -9076,7 +9085,7 @@
         <v/>
       </c>
     </row>
-    <row r="126" spans="1:27">
+    <row r="126" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B126" s="6"/>
       <c r="J126">
         <f t="shared" si="20"/>
@@ -9095,7 +9104,7 @@
         <v/>
       </c>
     </row>
-    <row r="127" spans="1:27">
+    <row r="127" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>206</v>
       </c>
@@ -9113,7 +9122,7 @@
         <v/>
       </c>
     </row>
-    <row r="128" spans="1:27">
+    <row r="128" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>256</v>
       </c>
@@ -9150,7 +9159,7 @@
         <v/>
       </c>
     </row>
-    <row r="129" spans="1:25">
+    <row r="129" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>207</v>
       </c>
@@ -9187,7 +9196,7 @@
         <v/>
       </c>
     </row>
-    <row r="130" spans="1:25">
+    <row r="130" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>208</v>
       </c>
@@ -9224,7 +9233,7 @@
         <v/>
       </c>
     </row>
-    <row r="131" spans="1:25">
+    <row r="131" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>257</v>
       </c>
@@ -9257,247 +9266,247 @@
         <v/>
       </c>
     </row>
-    <row r="132" spans="1:25">
+    <row r="132" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B132" s="6"/>
     </row>
-    <row r="133" spans="1:25">
+    <row r="133" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B133" s="6"/>
     </row>
-    <row r="134" spans="1:25">
+    <row r="134" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B134" s="6"/>
     </row>
-    <row r="135" spans="1:25">
+    <row r="135" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B135" s="6"/>
     </row>
-    <row r="136" spans="1:25">
+    <row r="136" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B136" s="6"/>
     </row>
-    <row r="137" spans="1:25">
+    <row r="137" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B137" s="6"/>
     </row>
-    <row r="138" spans="1:25">
+    <row r="138" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B138" s="6"/>
     </row>
-    <row r="139" spans="1:25">
+    <row r="139" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B139" s="6"/>
     </row>
-    <row r="140" spans="1:25">
+    <row r="140" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B140" s="6"/>
     </row>
-    <row r="141" spans="1:25">
+    <row r="141" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B141" s="6"/>
     </row>
-    <row r="142" spans="1:25">
+    <row r="142" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B142" s="6"/>
     </row>
-    <row r="143" spans="1:25">
+    <row r="143" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B143" s="6"/>
     </row>
-    <row r="144" spans="1:25">
+    <row r="144" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B144" s="6"/>
     </row>
-    <row r="145" spans="2:2">
+    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B145" s="6"/>
     </row>
-    <row r="146" spans="2:2">
+    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B146" s="6"/>
     </row>
-    <row r="147" spans="2:2">
+    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B147" s="6"/>
     </row>
-    <row r="148" spans="2:2">
+    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B148" s="6"/>
     </row>
-    <row r="149" spans="2:2">
+    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B149" s="6"/>
     </row>
-    <row r="150" spans="2:2">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B150" s="6"/>
     </row>
-    <row r="151" spans="2:2">
+    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B151" s="6"/>
     </row>
-    <row r="152" spans="2:2">
+    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B152" s="6"/>
     </row>
-    <row r="153" spans="2:2">
+    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B153" s="6"/>
     </row>
-    <row r="154" spans="2:2">
+    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B154" s="6"/>
     </row>
-    <row r="155" spans="2:2">
+    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B155" s="6"/>
     </row>
-    <row r="156" spans="2:2">
+    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B156" s="6"/>
     </row>
-    <row r="157" spans="2:2">
+    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B157" s="6"/>
     </row>
-    <row r="158" spans="2:2">
+    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B158" s="6"/>
     </row>
-    <row r="159" spans="2:2">
+    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B159" s="6"/>
     </row>
-    <row r="160" spans="2:2">
+    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B160" s="6"/>
     </row>
-    <row r="161" spans="2:2">
+    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B161" s="6"/>
     </row>
-    <row r="162" spans="2:2">
+    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B162" s="6"/>
     </row>
-    <row r="163" spans="2:2">
+    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B163" s="6"/>
     </row>
-    <row r="164" spans="2:2">
+    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B164" s="6"/>
     </row>
-    <row r="165" spans="2:2">
+    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B165" s="6"/>
     </row>
-    <row r="166" spans="2:2">
+    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B166" s="6"/>
     </row>
-    <row r="167" spans="2:2">
+    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B167" s="6"/>
     </row>
-    <row r="168" spans="2:2">
+    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B168" s="6"/>
     </row>
-    <row r="169" spans="2:2">
+    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B169" s="6"/>
     </row>
-    <row r="170" spans="2:2">
+    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B170" s="6"/>
     </row>
-    <row r="171" spans="2:2">
+    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B171" s="6"/>
     </row>
-    <row r="172" spans="2:2">
+    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B172" s="6"/>
     </row>
-    <row r="173" spans="2:2">
+    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B173" s="6"/>
     </row>
-    <row r="174" spans="2:2">
+    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B174" s="6"/>
     </row>
-    <row r="175" spans="2:2">
+    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B175" s="6"/>
     </row>
-    <row r="176" spans="2:2">
+    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B176" s="6"/>
     </row>
-    <row r="177" spans="2:2">
+    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B177" s="6"/>
     </row>
-    <row r="178" spans="2:2">
+    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B178" s="6"/>
     </row>
-    <row r="179" spans="2:2">
+    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B179" s="6"/>
     </row>
-    <row r="180" spans="2:2">
+    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B180" s="6"/>
     </row>
-    <row r="181" spans="2:2">
+    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B181" s="6"/>
     </row>
-    <row r="182" spans="2:2">
+    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B182" s="6"/>
     </row>
-    <row r="183" spans="2:2">
+    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B183" s="6"/>
     </row>
-    <row r="184" spans="2:2">
+    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B184" s="6"/>
     </row>
-    <row r="185" spans="2:2">
+    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B185" s="6"/>
     </row>
-    <row r="186" spans="2:2">
+    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B186" s="6"/>
     </row>
-    <row r="187" spans="2:2">
+    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B187" s="6"/>
     </row>
-    <row r="188" spans="2:2">
+    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B188" s="6"/>
     </row>
-    <row r="189" spans="2:2">
+    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B189" s="6"/>
     </row>
-    <row r="190" spans="2:2">
+    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B190" s="6"/>
     </row>
-    <row r="191" spans="2:2">
+    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B191" s="6"/>
     </row>
-    <row r="192" spans="2:2">
+    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B192" s="6"/>
     </row>
-    <row r="193" spans="2:2">
+    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B193" s="6"/>
     </row>
-    <row r="194" spans="2:2">
+    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B194" s="6"/>
     </row>
-    <row r="195" spans="2:2">
+    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B195" s="6"/>
     </row>
-    <row r="196" spans="2:2">
+    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B196" s="6"/>
     </row>
-    <row r="197" spans="2:2">
+    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B197" s="6"/>
     </row>
-    <row r="198" spans="2:2">
+    <row r="198" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B198" s="6"/>
     </row>
-    <row r="199" spans="2:2">
+    <row r="199" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B199" s="6"/>
     </row>
-    <row r="200" spans="2:2">
+    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B200" s="6"/>
     </row>
-    <row r="201" spans="2:2">
+    <row r="201" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B201" s="6"/>
     </row>
-    <row r="202" spans="2:2">
+    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B202" s="6"/>
     </row>
-    <row r="203" spans="2:2">
+    <row r="203" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B203" s="6"/>
     </row>
-    <row r="204" spans="2:2">
+    <row r="204" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B204" s="6"/>
     </row>
-    <row r="205" spans="2:2">
+    <row r="205" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B205" s="6"/>
     </row>
-    <row r="206" spans="2:2">
+    <row r="206" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B206" s="6"/>
     </row>
-    <row r="207" spans="2:2">
+    <row r="207" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B207" s="6"/>
     </row>
-    <row r="208" spans="2:2">
+    <row r="208" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B208" s="6"/>
     </row>
-    <row r="209" spans="2:2">
+    <row r="209" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B209" s="6"/>
     </row>
-    <row r="210" spans="2:2">
+    <row r="210" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B210" s="6"/>
     </row>
-    <row r="211" spans="2:2">
+    <row r="211" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B211" s="6"/>
     </row>
-    <row r="212" spans="2:2">
+    <row r="212" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B212" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated with rehearsal folks
</commit_message>
<xml_diff>
--- a/Guest_List_Invited.xlsx
+++ b/Guest_List_Invited.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\logan\Documents\GitHub\Farrell_Garrett_Wedding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{CE49E238-B826-4629-B345-2419F25DC4BF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{E0B3B818-8ED6-4CC9-8C9A-A4C54C51A1D5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="291">
   <si>
     <t xml:space="preserve">Priority </t>
   </si>
@@ -838,6 +838,66 @@
   </si>
   <si>
     <t>Ask about Food</t>
+  </si>
+  <si>
+    <t>Alex Farrell</t>
+  </si>
+  <si>
+    <t>Cory Brewer and Katie Schott</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bill O'Neil and Megan </t>
+  </si>
+  <si>
+    <t>Amanda Wenger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Courtney </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lisa </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laura </t>
+  </si>
+  <si>
+    <t>Mom and Dad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deb and Mark Garrett </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Janet and Tom Nugent </t>
+  </si>
+  <si>
+    <t>Grandma Donahou</t>
+  </si>
+  <si>
+    <t>Father Phil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seth and Allison Saldivar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kirstyn and James </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethan and Ashley </t>
+  </si>
+  <si>
+    <t>Kelsi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rehearsal Attendance </t>
+  </si>
+  <si>
+    <t>Num</t>
+  </si>
+  <si>
+    <t>Need to send</t>
+  </si>
+  <si>
+    <t>Krista and Logan</t>
   </si>
 </sst>
 </file>
@@ -1275,8 +1335,8 @@
   <dimension ref="A1:AC212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1:E1"/>
+      <pane ySplit="4" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q152" sqref="Q152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9299,81 +9359,169 @@
     </row>
     <row r="135" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B135" s="6"/>
+      <c r="P135" t="s">
+        <v>287</v>
+      </c>
+      <c r="Q135" t="s">
+        <v>288</v>
+      </c>
+      <c r="R135">
+        <f>SUM(Q136:Q160)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="136" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B136" s="6"/>
+      <c r="P136" t="s">
+        <v>290</v>
+      </c>
+      <c r="Q136">
+        <v>2</v>
+      </c>
     </row>
     <row r="137" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B137" s="6"/>
+      <c r="P137" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="138" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B138" s="6"/>
+      <c r="P138" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="139" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B139" s="6"/>
+      <c r="P139" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q139">
+        <v>2</v>
+      </c>
     </row>
     <row r="140" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B140" s="6"/>
+      <c r="P140" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="141" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B141" s="6"/>
+      <c r="P141" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="142" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B142" s="6"/>
+      <c r="P142" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="143" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B143" s="6"/>
     </row>
     <row r="144" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B144" s="6"/>
-    </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="P144" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="145" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B145" s="6"/>
-    </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="P145" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="146" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B146" s="6"/>
-    </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="P146" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="147" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B147" s="6"/>
-    </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="P147" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="148" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B148" s="6"/>
-    </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="P148" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="149" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B149" s="6"/>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B150" s="6"/>
-    </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="P150" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q150">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="151" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B151" s="6"/>
-    </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="P151" t="s">
+        <v>279</v>
+      </c>
+      <c r="Q151">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B152" s="6"/>
-    </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="P152" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="153" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B153" s="6"/>
-    </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="P153" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="154" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B154" s="6"/>
     </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B155" s="6"/>
-    </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="P155" t="s">
+        <v>282</v>
+      </c>
+      <c r="Q155" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="156" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B156" s="6"/>
-    </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="P156" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="157" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B157" s="6"/>
     </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B158" s="6"/>
-    </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="P158" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="159" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B159" s="6"/>
-    </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="P159" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="160" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B160" s="6"/>
+      <c r="P160" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="161" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B161" s="6"/>

</xml_diff>

<commit_message>
Updated RSVPs and some gift information
</commit_message>
<xml_diff>
--- a/Guest_List_Invited.xlsx
+++ b/Guest_List_Invited.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\logan\Documents\GitHub\Farrell_Garrett_Wedding\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{E0B3B818-8ED6-4CC9-8C9A-A4C54C51A1D5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="294">
   <si>
     <t xml:space="preserve">Priority </t>
   </si>
@@ -192,9 +186,6 @@
     <t>Ethan Miller and Ashley Marvel</t>
   </si>
   <si>
-    <t xml:space="preserve">Kayse Chen </t>
-  </si>
-  <si>
     <t>Cam Ebner</t>
   </si>
   <si>
@@ -804,9 +795,6 @@
     <t>chicken for both</t>
   </si>
   <si>
-    <t xml:space="preserve">Is "dating" Sam </t>
-  </si>
-  <si>
     <t>Brittany and Matt</t>
   </si>
   <si>
@@ -816,9 +804,6 @@
     <t>$100 for accomodations, hiking in the mountains</t>
   </si>
   <si>
-    <t>Andrea Parker &amp; Laurence Finn</t>
-  </si>
-  <si>
     <t>$150 for zip-lining</t>
   </si>
   <si>
@@ -837,9 +822,6 @@
     <t>3040 Coreopsis Ct, Dickinson TX 77539</t>
   </si>
   <si>
-    <t>Ask about Food</t>
-  </si>
-  <si>
     <t>Alex Farrell</t>
   </si>
   <si>
@@ -898,16 +880,38 @@
   </si>
   <si>
     <t>Krista and Logan</t>
+  </si>
+  <si>
+    <t>Andrea Parker</t>
+  </si>
+  <si>
+    <t>Pork</t>
+  </si>
+  <si>
+    <t>Ask about Food, didn't RSVP, but Deb says she's a NO</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>$100 for flights</t>
+  </si>
+  <si>
+    <t>Kayse Chen and Sam Stephens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sam would like a vegetarian meal </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -995,7 +999,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1031,6 +1035,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1324,22 +1329,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q152" sqref="Q152"/>
+      <pane ySplit="4" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35.85546875" customWidth="1"/>
     <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
@@ -1364,17 +1369,17 @@
     <col min="27" max="27" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" ht="15" customHeight="1">
       <c r="A1" s="5">
         <v>4</v>
       </c>
       <c r="B1" s="15"/>
       <c r="D1" s="20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E1" s="20"/>
       <c r="F1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G1">
         <f>SUM(G6:G11,G14:G41,G45:G50,G53:G59,G62:G86,G89:G114,G117:G125,G128:G130)</f>
@@ -1384,34 +1389,34 @@
       <c r="U1" s="10"/>
       <c r="V1" s="10"/>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29">
       <c r="A2" s="4">
         <v>3</v>
       </c>
       <c r="B2" s="6"/>
       <c r="D2" s="19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E2" s="19"/>
       <c r="G2" s="19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H2" s="19"/>
       <c r="I2" s="19"/>
       <c r="J2" s="11"/>
       <c r="K2" s="11"/>
       <c r="P2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Q2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="R2" s="14">
         <f>D3+G3*(1+Z4/100)</f>
-        <v>142.44116984738247</v>
+        <v>132.89972893137681</v>
       </c>
       <c r="S2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="T2" s="10"/>
       <c r="U2" s="10"/>
@@ -1422,44 +1427,44 @@
         <v>28.469765066395961</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D3" s="19">
         <f>SUM(E6:E130)+2</f>
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3">
         <f>SUM(J6:J174)</f>
-        <v>132.09999999999997</v>
+        <v>125.89999999999998</v>
       </c>
       <c r="G3">
         <f>SUM(O6:O130)</f>
-        <v>37.1</v>
+        <v>24.900000000000006</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
       <c r="P3" s="12">
         <f>G3+D3</f>
-        <v>133.1</v>
+        <v>126.9</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="R3" s="14">
         <f>D3+G3*(1-Z4/100)</f>
-        <v>123.75883015261755</v>
+        <v>120.90027106862318</v>
       </c>
       <c r="S3" s="13">
         <f>SUM(X6:X130)/COUNT(X6:X11,X14:X41,X45:X50,X53:X59,X62:X86,X89:X114,X117:X125,X128:X130)</f>
-        <v>0.68807339449541283</v>
+        <v>0.77064220183486243</v>
       </c>
       <c r="T3" s="10"/>
       <c r="U3" s="10"/>
@@ -1468,10 +1473,10 @@
         <v>34</v>
       </c>
       <c r="Z3" s="10" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" s="10" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="10" customFormat="1" ht="31.5" customHeight="1">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -1480,37 +1485,37 @@
         <v>33</v>
       </c>
       <c r="D4" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="N4" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="L4" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>87</v>
-      </c>
       <c r="O4" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="P4" s="10" t="s">
         <v>2</v>
@@ -1519,29 +1524,29 @@
         <v>3</v>
       </c>
       <c r="T4" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="U4" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="U4" s="10" t="s">
+      <c r="V4" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="V4" s="10" t="s">
-        <v>124</v>
-      </c>
       <c r="W4" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="Y4" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="Z4" s="10">
         <f>STDEV(Y6:Y130)</f>
-        <v>25.178355383780186</v>
+        <v>24.095296913159906</v>
       </c>
       <c r="AA4" s="10" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1551,7 +1556,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1601,13 +1606,13 @@
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="T6">
         <v>1</v>
       </c>
       <c r="U6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X6">
         <f t="shared" ref="X6:X11" si="1">IF(ISNUMBER(E6),1,0)</f>
@@ -1618,7 +1623,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1668,13 +1673,13 @@
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T7">
         <v>1</v>
       </c>
       <c r="U7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X7">
         <f t="shared" si="1"/>
@@ -1685,7 +1690,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1735,13 +1740,13 @@
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="T8">
         <v>1</v>
       </c>
       <c r="U8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X8">
         <f t="shared" si="1"/>
@@ -1752,7 +1757,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1802,13 +1807,13 @@
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="T9">
         <v>1</v>
       </c>
       <c r="U9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X9">
         <f t="shared" si="1"/>
@@ -1819,7 +1824,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1869,13 +1874,13 @@
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="T10">
         <v>1</v>
       </c>
       <c r="U10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X10">
         <f t="shared" si="1"/>
@@ -1886,7 +1891,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -1936,7 +1941,7 @@
         <v>0</v>
       </c>
       <c r="P11" s="18" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="Q11" s="8"/>
       <c r="R11" s="8"/>
@@ -1944,7 +1949,7 @@
         <v>1</v>
       </c>
       <c r="U11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X11">
         <f t="shared" si="1"/>
@@ -1955,7 +1960,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29">
       <c r="B12" s="6"/>
       <c r="C12" s="1"/>
       <c r="D12">
@@ -1998,14 +2003,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="17"/>
       <c r="D13">
         <f>SUM(J14:J41)</f>
-        <v>23</v>
+        <v>22.5</v>
       </c>
       <c r="J13">
         <f t="shared" si="9"/>
@@ -2036,7 +2041,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
@@ -2083,13 +2088,13 @@
         <v>1</v>
       </c>
       <c r="P14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="T14">
         <v>1</v>
       </c>
       <c r="U14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X14">
         <f t="shared" ref="X14:X40" si="10">IF(ISNUMBER(E14),1,0)</f>
@@ -2100,7 +2105,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -2147,13 +2152,13 @@
         <v>1</v>
       </c>
       <c r="P15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="T15">
         <v>1</v>
       </c>
       <c r="U15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X15">
         <f t="shared" si="10"/>
@@ -2164,7 +2169,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
@@ -2211,7 +2216,7 @@
         <v>1</v>
       </c>
       <c r="P16" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q16" s="7"/>
       <c r="R16" s="7"/>
@@ -2220,7 +2225,7 @@
         <v>1</v>
       </c>
       <c r="U16" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X16">
         <f t="shared" si="10"/>
@@ -2231,7 +2236,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29">
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
@@ -2278,13 +2283,13 @@
         <v>0.5</v>
       </c>
       <c r="P17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="T17">
         <v>1</v>
       </c>
       <c r="U17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X17">
         <f t="shared" si="10"/>
@@ -2299,7 +2304,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29">
       <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
@@ -2346,13 +2351,13 @@
         <v>1</v>
       </c>
       <c r="P18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="T18">
         <v>1</v>
       </c>
       <c r="U18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X18">
         <f t="shared" si="10"/>
@@ -2363,9 +2368,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29">
       <c r="A19" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B19" s="7">
         <v>12</v>
@@ -2410,7 +2415,7 @@
         <v>0.5</v>
       </c>
       <c r="P19" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="Q19" s="6"/>
       <c r="R19" s="6"/>
@@ -2419,7 +2424,7 @@
         <v>1</v>
       </c>
       <c r="U19" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X19">
         <f t="shared" si="10"/>
@@ -2430,7 +2435,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -2477,7 +2482,7 @@
         <v>0.5</v>
       </c>
       <c r="P20" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
@@ -2486,7 +2491,7 @@
         <v>1</v>
       </c>
       <c r="U20" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X20">
         <f t="shared" si="10"/>
@@ -2497,7 +2502,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29">
       <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
@@ -2544,13 +2549,13 @@
         <v>1</v>
       </c>
       <c r="P21" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="T21">
         <v>1</v>
       </c>
       <c r="U21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X21">
         <f t="shared" si="10"/>
@@ -2561,7 +2566,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29">
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
@@ -2608,13 +2613,13 @@
         <v>1</v>
       </c>
       <c r="P22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T22">
         <v>1</v>
       </c>
       <c r="U22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X22">
         <f t="shared" si="10"/>
@@ -2625,9 +2630,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29">
       <c r="A23" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B23" s="7">
         <v>16</v>
@@ -2672,7 +2677,7 @@
         <v>0.5</v>
       </c>
       <c r="P23" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
@@ -2681,7 +2686,7 @@
         <v>1</v>
       </c>
       <c r="U23" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X23">
         <f t="shared" si="10"/>
@@ -2692,7 +2697,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29">
       <c r="A24" s="2" t="s">
         <v>17</v>
       </c>
@@ -2742,19 +2747,19 @@
         <v>0</v>
       </c>
       <c r="P24" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="S24" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="T24">
         <v>1</v>
       </c>
       <c r="U24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="W24" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="X24">
         <f t="shared" si="10"/>
@@ -2765,10 +2770,10 @@
         <v/>
       </c>
       <c r="AA24" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29">
       <c r="A25" s="2" t="s">
         <v>18</v>
       </c>
@@ -2818,16 +2823,16 @@
         <v>0</v>
       </c>
       <c r="P25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="T25">
         <v>1</v>
       </c>
       <c r="U25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="W25" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="X25">
         <f t="shared" si="10"/>
@@ -2838,10 +2843,10 @@
         <v/>
       </c>
       <c r="AA25" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29">
       <c r="A26" s="2" t="s">
         <v>19</v>
       </c>
@@ -2891,13 +2896,13 @@
         <v>0</v>
       </c>
       <c r="P26" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="T26">
         <v>1</v>
       </c>
       <c r="U26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X26">
         <f t="shared" si="10"/>
@@ -2908,7 +2913,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:29">
       <c r="A27" s="2" t="s">
         <v>20</v>
       </c>
@@ -2958,13 +2963,13 @@
         <v>0</v>
       </c>
       <c r="P27" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="T27">
         <v>1</v>
       </c>
       <c r="U27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X27">
         <f t="shared" si="10"/>
@@ -2975,7 +2980,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:29">
       <c r="A28" s="2" t="s">
         <v>21</v>
       </c>
@@ -3025,13 +3030,13 @@
         <v>0</v>
       </c>
       <c r="P28" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T28">
         <v>1</v>
       </c>
       <c r="U28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X28">
         <f t="shared" si="10"/>
@@ -3042,7 +3047,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:29">
       <c r="A29" s="2" t="s">
         <v>22</v>
       </c>
@@ -3092,13 +3097,13 @@
         <v>0</v>
       </c>
       <c r="P29" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="T29">
         <v>1</v>
       </c>
       <c r="U29" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X29">
         <f t="shared" si="10"/>
@@ -3109,7 +3114,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:29">
       <c r="A30" s="2" t="s">
         <v>23</v>
       </c>
@@ -3156,13 +3161,13 @@
         <v>0.5</v>
       </c>
       <c r="P30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="T30">
         <v>1</v>
       </c>
       <c r="U30" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X30">
         <f t="shared" si="10"/>
@@ -3173,7 +3178,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:29">
       <c r="A31" s="2" t="s">
         <v>24</v>
       </c>
@@ -3223,13 +3228,13 @@
         <v>0</v>
       </c>
       <c r="P31" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="T31">
         <v>1</v>
       </c>
       <c r="U31" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X31">
         <f t="shared" si="10"/>
@@ -3240,7 +3245,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:29">
       <c r="A32" s="2" t="s">
         <v>25</v>
       </c>
@@ -3287,13 +3292,13 @@
         <v>0.5</v>
       </c>
       <c r="P32" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="T32">
         <v>1</v>
       </c>
       <c r="U32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X32">
         <f t="shared" si="10"/>
@@ -3304,7 +3309,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27">
       <c r="A33" s="2" t="s">
         <v>26</v>
       </c>
@@ -3351,13 +3356,13 @@
         <v>0.5</v>
       </c>
       <c r="P33" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="T33">
         <v>1</v>
       </c>
       <c r="U33" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X33">
         <f t="shared" si="10"/>
@@ -3368,7 +3373,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
@@ -3418,16 +3423,16 @@
         <v>0</v>
       </c>
       <c r="P34" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="T34">
         <v>1</v>
       </c>
       <c r="U34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="W34" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="X34">
         <f t="shared" si="10"/>
@@ -3438,10 +3443,10 @@
         <v/>
       </c>
       <c r="AA34" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
@@ -3491,13 +3496,13 @@
         <v>0</v>
       </c>
       <c r="P35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="T35">
         <v>1</v>
       </c>
       <c r="U35" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X35">
         <f t="shared" si="10"/>
@@ -3508,9 +3513,9 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27">
       <c r="A36" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B36" s="7">
         <v>29</v>
@@ -3555,13 +3560,13 @@
         <v>1</v>
       </c>
       <c r="P36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="T36">
         <v>1</v>
       </c>
       <c r="U36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X36">
         <f t="shared" si="10"/>
@@ -3572,7 +3577,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27">
       <c r="A37" s="2" t="s">
         <v>40</v>
       </c>
@@ -3622,13 +3627,13 @@
         <v>0</v>
       </c>
       <c r="P37" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="T37">
         <v>1</v>
       </c>
       <c r="U37" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X37">
         <f t="shared" si="10"/>
@@ -3639,7 +3644,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27">
       <c r="A38" s="2" t="s">
         <v>41</v>
       </c>
@@ -3689,16 +3694,16 @@
         <v>0</v>
       </c>
       <c r="P38" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="T38">
         <v>1</v>
       </c>
       <c r="U38" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="W38" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="X38">
         <f t="shared" si="10"/>
@@ -3709,10 +3714,10 @@
         <v/>
       </c>
       <c r="AA38" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27">
       <c r="A39" s="2" t="s">
         <v>42</v>
       </c>
@@ -3762,13 +3767,13 @@
         <v>0</v>
       </c>
       <c r="P39" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="T39">
         <v>1</v>
       </c>
       <c r="U39" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X39">
         <f t="shared" si="10"/>
@@ -3779,7 +3784,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27">
       <c r="A40" s="2" t="s">
         <v>43</v>
       </c>
@@ -3829,16 +3834,16 @@
         <v>0</v>
       </c>
       <c r="P40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="S40" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="T40">
         <v>1</v>
       </c>
       <c r="U40" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X40">
         <f t="shared" si="10"/>
@@ -3849,9 +3854,9 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27">
       <c r="A41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B41" s="7">
         <v>34</v>
@@ -3862,6 +3867,9 @@
       <c r="D41">
         <v>1</v>
       </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
       <c r="F41">
         <v>4</v>
       </c>
@@ -3873,19 +3881,19 @@
       </c>
       <c r="J41">
         <f t="shared" si="9"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="K41">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L41">
         <f t="shared" si="3"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="M41">
         <f t="shared" si="4"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="N41">
         <f t="shared" si="5"/>
@@ -3893,30 +3901,30 @@
       </c>
       <c r="O41">
         <f t="shared" si="6"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="P41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S41" t="s">
-        <v>270</v>
+        <v>289</v>
       </c>
       <c r="T41">
         <v>1</v>
       </c>
       <c r="U41" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X41">
         <f>IF(ISNUMBER(E41),1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Y41">
+        <v>1</v>
+      </c>
+      <c r="Y41" t="str">
         <f t="shared" si="7"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:27">
       <c r="A42" s="2"/>
       <c r="B42" s="7"/>
       <c r="D42">
@@ -3952,7 +3960,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27">
       <c r="B43" s="6"/>
       <c r="C43" s="1"/>
       <c r="D43">
@@ -3988,7 +3996,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27">
       <c r="A44" s="1" t="s">
         <v>27</v>
       </c>
@@ -4026,7 +4034,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27">
       <c r="A45" t="s">
         <v>28</v>
       </c>
@@ -4076,19 +4084,19 @@
         <v>0</v>
       </c>
       <c r="P45" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="S45" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="T45">
         <v>1</v>
       </c>
       <c r="U45" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="W45" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="X45">
         <f t="shared" ref="X45:X50" si="11">IF(ISNUMBER(E45),1,0)</f>
@@ -4099,10 +4107,10 @@
         <v/>
       </c>
       <c r="AA45" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27">
       <c r="A46" t="s">
         <v>29</v>
       </c>
@@ -4152,13 +4160,13 @@
         <v>0</v>
       </c>
       <c r="P46" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="T46">
         <v>1</v>
       </c>
       <c r="U46" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X46">
         <f t="shared" si="11"/>
@@ -4169,7 +4177,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27">
       <c r="A47" t="s">
         <v>30</v>
       </c>
@@ -4219,13 +4227,13 @@
         <v>0</v>
       </c>
       <c r="P47" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="T47">
         <v>1</v>
       </c>
       <c r="U47" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X47">
         <f t="shared" si="11"/>
@@ -4236,7 +4244,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27">
       <c r="A48" t="s">
         <v>31</v>
       </c>
@@ -4286,7 +4294,7 @@
         <v>0</v>
       </c>
       <c r="P48" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="S48" t="s">
         <v>44</v>
@@ -4295,7 +4303,7 @@
         <v>1</v>
       </c>
       <c r="U48" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X48">
         <f t="shared" si="11"/>
@@ -4306,7 +4314,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:29">
       <c r="A49" t="s">
         <v>32</v>
       </c>
@@ -4356,7 +4364,7 @@
         <v>0</v>
       </c>
       <c r="P49" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="S49" t="s">
         <v>44</v>
@@ -4365,7 +4373,7 @@
         <v>1</v>
       </c>
       <c r="U49" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X49">
         <f t="shared" si="11"/>
@@ -4376,9 +4384,9 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:29">
       <c r="A50" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B50" s="6">
         <v>40</v>
@@ -4426,7 +4434,7 @@
         <v>0</v>
       </c>
       <c r="P50" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q50" s="6"/>
       <c r="R50" s="6"/>
@@ -4437,7 +4445,7 @@
         <v>1</v>
       </c>
       <c r="U50" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X50">
         <f t="shared" si="11"/>
@@ -4451,7 +4459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:29">
       <c r="B51" s="6"/>
       <c r="J51">
         <f t="shared" si="9"/>
@@ -4482,7 +4490,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:29">
       <c r="A52" s="1" t="s">
         <v>48</v>
       </c>
@@ -4520,7 +4528,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:29">
       <c r="A53" t="s">
         <v>47</v>
       </c>
@@ -4570,7 +4578,7 @@
         <v>0</v>
       </c>
       <c r="P53" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="Q53" s="6"/>
       <c r="R53" s="6"/>
@@ -4579,7 +4587,7 @@
         <v>1</v>
       </c>
       <c r="U53" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="V53" s="6"/>
       <c r="X53">
@@ -4591,7 +4599,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:29">
       <c r="A54" t="s">
         <v>50</v>
       </c>
@@ -4641,7 +4649,7 @@
         <v>0</v>
       </c>
       <c r="P54" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q54" s="6"/>
       <c r="R54" s="6"/>
@@ -4650,7 +4658,7 @@
         <v>1</v>
       </c>
       <c r="U54" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X54">
         <f t="shared" si="12"/>
@@ -4661,7 +4669,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:29">
       <c r="A55" t="s">
         <v>49</v>
       </c>
@@ -4711,7 +4719,7 @@
         <v>0</v>
       </c>
       <c r="P55" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Q55" s="6"/>
       <c r="R55" s="6"/>
@@ -4720,7 +4728,7 @@
         <v>1</v>
       </c>
       <c r="U55" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="V55" s="6"/>
       <c r="X55">
@@ -4732,9 +4740,9 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:29">
       <c r="A56" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B56" s="6">
         <v>44</v>
@@ -4782,16 +4790,16 @@
         <v>0</v>
       </c>
       <c r="P56" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="T56">
         <v>1</v>
       </c>
       <c r="U56" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="W56" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="X56">
         <f t="shared" si="12"/>
@@ -4802,10 +4810,10 @@
         <v/>
       </c>
       <c r="AA56" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="57" spans="1:29">
       <c r="A57" t="s">
         <v>51</v>
       </c>
@@ -4855,16 +4863,16 @@
         <v>0</v>
       </c>
       <c r="P57" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T57">
         <v>1</v>
       </c>
       <c r="U57" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="V57" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X57">
         <f t="shared" si="12"/>
@@ -4875,7 +4883,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:29">
       <c r="A58" t="s">
         <v>52</v>
       </c>
@@ -4925,16 +4933,16 @@
         <v>0</v>
       </c>
       <c r="P58" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="S58" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="T58">
         <v>1</v>
       </c>
       <c r="U58" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X58">
         <f t="shared" si="12"/>
@@ -4945,7 +4953,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:29">
       <c r="A59" t="s">
         <v>53</v>
       </c>
@@ -4995,13 +5003,13 @@
         <v>0</v>
       </c>
       <c r="P59" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="T59">
         <v>1</v>
       </c>
       <c r="U59" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X59">
         <f t="shared" si="12"/>
@@ -5012,7 +5020,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:29">
       <c r="B60" s="6"/>
       <c r="J60">
         <f t="shared" si="9"/>
@@ -5043,14 +5051,14 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:29">
       <c r="A61" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B61" s="17"/>
       <c r="D61">
         <f>SUM(J62:J85)</f>
-        <v>32.6</v>
+        <v>33</v>
       </c>
       <c r="J61">
         <f t="shared" si="9"/>
@@ -5081,9 +5089,9 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:29">
       <c r="A62" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B62" s="6">
         <v>48</v>
@@ -5131,7 +5139,7 @@
         <v>0</v>
       </c>
       <c r="P62" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="Q62" s="6"/>
       <c r="R62" s="6"/>
@@ -5140,7 +5148,7 @@
         <v>1</v>
       </c>
       <c r="U62" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="V62" s="6"/>
       <c r="X62">
@@ -5152,9 +5160,9 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:29">
       <c r="A63" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B63" s="6">
         <v>48.5</v>
@@ -5165,6 +5173,9 @@
       <c r="D63">
         <v>2</v>
       </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
       <c r="G63">
         <v>2</v>
       </c>
@@ -5181,10 +5192,10 @@
       </c>
       <c r="O63">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P63" s="6" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="Q63" s="6"/>
       <c r="R63" s="6"/>
@@ -5192,12 +5203,18 @@
       <c r="T63" s="6"/>
       <c r="U63" s="6"/>
       <c r="V63" s="6"/>
-      <c r="Y63">
+      <c r="W63" t="s">
+        <v>262</v>
+      </c>
+      <c r="Y63" t="str">
         <f t="shared" si="7"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+      <c r="AA63" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="64" spans="1:29">
       <c r="A64" t="s">
         <v>54</v>
       </c>
@@ -5210,6 +5227,9 @@
       <c r="D64">
         <v>1</v>
       </c>
+      <c r="E64">
+        <v>2</v>
+      </c>
       <c r="F64">
         <v>4</v>
       </c>
@@ -5221,19 +5241,19 @@
       </c>
       <c r="J64">
         <f t="shared" si="9"/>
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="K64">
         <f t="shared" si="2"/>
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="L64">
         <f t="shared" si="3"/>
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="M64">
         <f t="shared" si="4"/>
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="N64">
         <f t="shared" si="5"/>
@@ -5241,10 +5261,10 @@
       </c>
       <c r="O64">
         <f t="shared" si="6"/>
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="P64" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q64" s="6"/>
       <c r="R64" s="6"/>
@@ -5253,21 +5273,21 @@
         <v>1</v>
       </c>
       <c r="U64" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="V64" s="6"/>
       <c r="X64">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="Y64">
+        <v>1</v>
+      </c>
+      <c r="Y64" t="str">
         <f t="shared" si="7"/>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:27">
       <c r="A65" t="s">
-        <v>55</v>
+        <v>292</v>
       </c>
       <c r="B65" s="6">
         <v>50</v>
@@ -5278,6 +5298,9 @@
       <c r="D65">
         <v>1</v>
       </c>
+      <c r="E65">
+        <v>2</v>
+      </c>
       <c r="F65">
         <v>3</v>
       </c>
@@ -5289,15 +5312,15 @@
       </c>
       <c r="J65">
         <f t="shared" si="9"/>
-        <v>0.9</v>
+        <v>2</v>
       </c>
       <c r="K65">
         <f t="shared" si="2"/>
-        <v>0.9</v>
+        <v>2</v>
       </c>
       <c r="L65">
         <f t="shared" si="3"/>
-        <v>0.9</v>
+        <v>2</v>
       </c>
       <c r="M65">
         <f t="shared" si="4"/>
@@ -5309,35 +5332,35 @@
       </c>
       <c r="O65">
         <f t="shared" si="6"/>
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="P65" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q65" s="6"/>
       <c r="R65" s="6"/>
       <c r="S65" s="6" t="s">
-        <v>259</v>
+        <v>293</v>
       </c>
       <c r="T65" s="6">
         <v>1</v>
       </c>
       <c r="U65" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="V65" s="6"/>
       <c r="X65">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="Y65">
+        <v>1</v>
+      </c>
+      <c r="Y65" t="str">
         <f t="shared" si="7"/>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="1:27">
       <c r="A66" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B66" s="6">
         <v>51</v>
@@ -5348,6 +5371,9 @@
       <c r="D66">
         <v>1</v>
       </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
       <c r="F66">
         <v>3</v>
       </c>
@@ -5359,15 +5385,15 @@
       </c>
       <c r="J66">
         <f t="shared" si="9"/>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="K66">
         <f t="shared" si="2"/>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="L66">
         <f t="shared" si="3"/>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="M66">
         <f t="shared" si="4"/>
@@ -5379,10 +5405,10 @@
       </c>
       <c r="O66">
         <f t="shared" si="6"/>
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="P66" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Q66" s="6"/>
       <c r="R66" s="6"/>
@@ -5391,21 +5417,21 @@
         <v>1</v>
       </c>
       <c r="U66" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="V66" s="6"/>
       <c r="X66">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="Y66">
+        <v>1</v>
+      </c>
+      <c r="Y66" t="str">
         <f t="shared" si="7"/>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="1:27">
       <c r="A67" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B67" s="6">
         <v>52</v>
@@ -5453,7 +5479,7 @@
         <v>0</v>
       </c>
       <c r="P67" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q67" s="6"/>
       <c r="R67" s="6"/>
@@ -5462,7 +5488,7 @@
         <v>1</v>
       </c>
       <c r="U67" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="V67" s="6"/>
       <c r="X67">
@@ -5474,9 +5500,9 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:27">
       <c r="A68" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B68" s="6">
         <v>53</v>
@@ -5509,20 +5535,23 @@
         <v>0</v>
       </c>
       <c r="P68" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="Q68" s="6"/>
       <c r="R68" s="6"/>
       <c r="S68" s="6" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="T68" s="6">
         <v>1</v>
       </c>
       <c r="U68" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="V68" s="6"/>
+      <c r="W68" t="s">
+        <v>259</v>
+      </c>
       <c r="X68">
         <f t="shared" si="13"/>
         <v>1</v>
@@ -5531,10 +5560,13 @@
         <f t="shared" si="7"/>
         <v/>
       </c>
-    </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA68" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="69" spans="1:27">
       <c r="A69" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B69" s="6">
         <v>54</v>
@@ -5582,7 +5614,7 @@
         <v>0</v>
       </c>
       <c r="P69" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Q69" s="6"/>
       <c r="R69" s="6"/>
@@ -5591,7 +5623,7 @@
         <v>1</v>
       </c>
       <c r="U69" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="V69" s="6"/>
       <c r="X69">
@@ -5603,9 +5635,9 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:27">
       <c r="A70" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B70" s="6">
         <v>55</v>
@@ -5653,18 +5685,18 @@
         <v>0</v>
       </c>
       <c r="P70" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Q70" s="6"/>
       <c r="R70" s="6"/>
       <c r="S70" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="T70" s="6">
         <v>1</v>
       </c>
       <c r="U70" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="V70" s="6"/>
       <c r="X70">
@@ -5676,9 +5708,9 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:27">
       <c r="A71" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B71" s="6">
         <v>56</v>
@@ -5726,7 +5758,7 @@
         <v>0</v>
       </c>
       <c r="P71" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="Q71" s="6"/>
       <c r="R71" s="6"/>
@@ -5735,7 +5767,7 @@
         <v>1</v>
       </c>
       <c r="U71" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="V71" s="6"/>
       <c r="X71">
@@ -5747,9 +5779,9 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:27">
       <c r="A72" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B72" s="6">
         <v>57</v>
@@ -5797,16 +5829,16 @@
         <v>0</v>
       </c>
       <c r="P72" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="T72">
         <v>1</v>
       </c>
       <c r="U72" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="V72" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X72">
         <f t="shared" si="13"/>
@@ -5817,9 +5849,9 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:27">
       <c r="A73" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B73" s="6">
         <v>58</v>
@@ -5867,16 +5899,16 @@
         <v>0</v>
       </c>
       <c r="P73" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="T73">
         <v>1</v>
       </c>
       <c r="U73" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="V73" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X73">
         <f t="shared" si="13"/>
@@ -5887,9 +5919,9 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:27">
       <c r="A74" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B74" s="6">
         <v>59</v>
@@ -5937,13 +5969,13 @@
         <v>0</v>
       </c>
       <c r="P74" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T74">
         <v>1</v>
       </c>
       <c r="U74" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X74">
         <f t="shared" si="13"/>
@@ -5954,9 +5986,9 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:27">
       <c r="A75" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B75" s="6">
         <v>60</v>
@@ -6004,13 +6036,13 @@
         <v>0</v>
       </c>
       <c r="P75" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="T75">
         <v>1</v>
       </c>
       <c r="U75" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X75">
         <f t="shared" si="13"/>
@@ -6021,9 +6053,9 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:27">
       <c r="A76" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B76" s="6">
         <v>61</v>
@@ -6071,13 +6103,13 @@
         <v>0</v>
       </c>
       <c r="P76" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="T76">
         <v>1</v>
       </c>
       <c r="U76" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X76">
         <f t="shared" si="13"/>
@@ -6088,9 +6120,9 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:27">
       <c r="A77" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B77" s="6">
         <v>62</v>
@@ -6138,16 +6170,16 @@
         <v>0</v>
       </c>
       <c r="P77" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="T77">
         <v>1</v>
       </c>
       <c r="U77" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="V77" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X77">
         <f t="shared" si="13"/>
@@ -6158,9 +6190,9 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:27">
       <c r="A78" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B78" s="6">
         <v>63</v>
@@ -6208,13 +6240,13 @@
         <v>0</v>
       </c>
       <c r="P78" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="T78">
         <v>1</v>
       </c>
       <c r="U78" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X78">
         <f t="shared" si="13"/>
@@ -6225,9 +6257,9 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:27">
       <c r="A79" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B79" s="6">
         <v>64</v>
@@ -6275,13 +6307,13 @@
         <v>0</v>
       </c>
       <c r="P79" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="T79">
         <v>1</v>
       </c>
       <c r="U79" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X79">
         <f t="shared" si="13"/>
@@ -6292,9 +6324,9 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:27">
       <c r="A80" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B80" s="6">
         <v>65</v>
@@ -6342,13 +6374,13 @@
         <v>0</v>
       </c>
       <c r="P80" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="T80">
         <v>1</v>
       </c>
       <c r="U80" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X80">
         <f t="shared" si="13"/>
@@ -6359,9 +6391,9 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:27">
       <c r="A81" t="s">
-        <v>263</v>
+        <v>287</v>
       </c>
       <c r="B81" s="6">
         <v>66</v>
@@ -6373,7 +6405,7 @@
         <v>1</v>
       </c>
       <c r="E81">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F81">
         <v>4</v>
@@ -6386,19 +6418,19 @@
       </c>
       <c r="J81">
         <f t="shared" si="20"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K81">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L81">
         <f t="shared" si="16"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M81">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N81">
         <f t="shared" si="18"/>
@@ -6409,13 +6441,13 @@
         <v>0</v>
       </c>
       <c r="P81" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="T81">
         <v>1</v>
       </c>
       <c r="U81" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X81">
         <f t="shared" si="13"/>
@@ -6426,9 +6458,9 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:27">
       <c r="A82" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B82" s="6">
         <v>67</v>
@@ -6476,13 +6508,13 @@
         <v>0</v>
       </c>
       <c r="P82" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T82" s="6">
         <v>1</v>
       </c>
       <c r="U82" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X82">
         <f t="shared" si="13"/>
@@ -6493,9 +6525,9 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:27">
       <c r="A83" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B83" s="6">
         <v>68</v>
@@ -6543,13 +6575,13 @@
         <v>0</v>
       </c>
       <c r="P83" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="T83">
         <v>1</v>
       </c>
       <c r="U83" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X83">
         <f t="shared" si="13"/>
@@ -6560,9 +6592,9 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:27">
       <c r="A84" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B84" s="6">
         <v>69</v>
@@ -6610,7 +6642,7 @@
         <v>0</v>
       </c>
       <c r="P84" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="Q84" s="6"/>
       <c r="R84" s="6"/>
@@ -6619,7 +6651,7 @@
         <v>1</v>
       </c>
       <c r="U84" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X84">
         <f t="shared" si="13"/>
@@ -6630,9 +6662,9 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:27">
       <c r="A85" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B85" s="6">
         <v>70</v>
@@ -6680,13 +6712,13 @@
         <v>0</v>
       </c>
       <c r="P85" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="T85">
         <v>1</v>
       </c>
       <c r="U85" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X85">
         <f t="shared" si="13"/>
@@ -6697,9 +6729,9 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:27">
       <c r="A86" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B86" s="6">
         <v>71</v>
@@ -6744,13 +6776,13 @@
         <v>1.8</v>
       </c>
       <c r="P86" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="T86">
         <v>1</v>
       </c>
       <c r="U86" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X86">
         <f t="shared" si="13"/>
@@ -6761,7 +6793,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:27">
       <c r="B87" s="6"/>
       <c r="J87">
         <f t="shared" si="20"/>
@@ -6792,14 +6824,14 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:27">
       <c r="A88" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B88" s="17"/>
       <c r="D88">
         <f>SUM(J89:J103)</f>
-        <v>21.400000000000002</v>
+        <v>20.6</v>
       </c>
       <c r="J88">
         <f t="shared" si="20"/>
@@ -6830,9 +6862,9 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:27">
       <c r="A89" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B89" s="7">
         <v>72</v>
@@ -6880,13 +6912,13 @@
         <v>0</v>
       </c>
       <c r="P89" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="T89">
         <v>1</v>
       </c>
       <c r="U89" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X89">
         <f t="shared" ref="X89:X114" si="24">IF(ISNUMBER(E89),1,0)</f>
@@ -6897,9 +6929,9 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:27">
       <c r="A90" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B90" s="7">
         <v>73</v>
@@ -6947,13 +6979,13 @@
         <v>0</v>
       </c>
       <c r="P90" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="T90">
         <v>1</v>
       </c>
       <c r="U90" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X90">
         <f t="shared" si="24"/>
@@ -6964,9 +6996,9 @@
         <v/>
       </c>
     </row>
-    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:27">
       <c r="A91" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B91" s="7">
         <v>74</v>
@@ -7014,16 +7046,16 @@
         <v>0</v>
       </c>
       <c r="P91" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="T91">
         <v>1</v>
       </c>
       <c r="U91" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="W91" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="X91">
         <f t="shared" si="24"/>
@@ -7034,12 +7066,12 @@
         <v/>
       </c>
       <c r="AA91" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="92" spans="1:27">
       <c r="A92" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B92" s="7">
         <v>75</v>
@@ -7087,13 +7119,13 @@
         <v>0</v>
       </c>
       <c r="P92" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="T92">
         <v>1</v>
       </c>
       <c r="U92" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X92">
         <f t="shared" si="24"/>
@@ -7104,9 +7136,9 @@
         <v/>
       </c>
     </row>
-    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:27">
       <c r="A93" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B93" s="7">
         <v>76</v>
@@ -7151,16 +7183,16 @@
         <v>1.6</v>
       </c>
       <c r="P93" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="T93">
         <v>1</v>
       </c>
       <c r="U93" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="W93" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="X93">
         <f t="shared" si="24"/>
@@ -7171,12 +7203,12 @@
         <v>80</v>
       </c>
       <c r="AA93" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="94" spans="1:27">
       <c r="A94" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B94" s="7">
         <v>77</v>
@@ -7224,13 +7256,13 @@
         <v>0</v>
       </c>
       <c r="P94" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="T94">
         <v>1</v>
       </c>
       <c r="U94" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X94">
         <f t="shared" si="24"/>
@@ -7241,9 +7273,9 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:27">
       <c r="A95" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B95" s="7">
         <v>78</v>
@@ -7291,13 +7323,13 @@
         <v>0</v>
       </c>
       <c r="P95" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="T95">
         <v>1</v>
       </c>
       <c r="U95" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X95">
         <f t="shared" si="24"/>
@@ -7308,9 +7340,9 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:27">
       <c r="A96" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B96" s="7">
         <v>79</v>
@@ -7358,13 +7390,13 @@
         <v>0</v>
       </c>
       <c r="P96" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="T96">
         <v>1</v>
       </c>
       <c r="U96" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X96">
         <f t="shared" si="24"/>
@@ -7375,9 +7407,9 @@
         <v/>
       </c>
     </row>
-    <row r="97" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:27">
       <c r="A97" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B97" s="7">
         <v>80</v>
@@ -7422,13 +7454,13 @@
         <v>1</v>
       </c>
       <c r="P97" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="T97">
         <v>1</v>
       </c>
       <c r="U97" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X97">
         <f t="shared" si="24"/>
@@ -7439,9 +7471,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="98" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:27">
       <c r="A98" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B98" s="7">
         <v>81</v>
@@ -7486,13 +7518,13 @@
         <v>0.5</v>
       </c>
       <c r="P98" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="T98">
         <v>1</v>
       </c>
       <c r="U98" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X98">
         <f t="shared" si="24"/>
@@ -7503,9 +7535,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:27">
       <c r="A99" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B99" s="7">
         <v>82</v>
@@ -7553,13 +7585,13 @@
         <v>0</v>
       </c>
       <c r="P99" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="T99">
         <v>1</v>
       </c>
       <c r="U99" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X99">
         <f t="shared" si="24"/>
@@ -7570,9 +7602,9 @@
         <v/>
       </c>
     </row>
-    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:27">
       <c r="A100" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B100" s="7">
         <v>83</v>
@@ -7620,16 +7652,16 @@
         <v>0</v>
       </c>
       <c r="P100" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="T100">
         <v>1</v>
       </c>
       <c r="U100" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="W100" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="X100">
         <f t="shared" si="24"/>
@@ -7640,12 +7672,12 @@
         <v/>
       </c>
       <c r="AA100" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="101" spans="1:27">
       <c r="A101" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B101" s="7">
         <v>84</v>
@@ -7690,13 +7722,13 @@
         <v>0.9</v>
       </c>
       <c r="P101" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="T101">
         <v>1</v>
       </c>
       <c r="U101" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X101">
         <f t="shared" si="24"/>
@@ -7707,9 +7739,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="102" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:27">
       <c r="A102" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B102" s="7">
         <v>85</v>
@@ -7720,6 +7752,9 @@
       <c r="D102">
         <v>1</v>
       </c>
+      <c r="E102">
+        <v>0</v>
+      </c>
       <c r="F102">
         <v>3</v>
       </c>
@@ -7731,15 +7766,15 @@
       </c>
       <c r="J102">
         <f t="shared" si="20"/>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="K102">
         <f t="shared" si="21"/>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="L102">
         <f t="shared" si="22"/>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="M102">
         <f t="shared" si="23"/>
@@ -7751,29 +7786,29 @@
       </c>
       <c r="O102">
         <f t="shared" si="14"/>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="P102" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="T102">
         <v>1</v>
       </c>
       <c r="U102" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X102">
         <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="Y102">
+        <v>1</v>
+      </c>
+      <c r="Y102" t="str">
         <f t="shared" si="19"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="103" spans="1:27" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="103" spans="1:27">
       <c r="A103" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B103" s="7">
         <v>86</v>
@@ -7818,13 +7853,13 @@
         <v>1.6</v>
       </c>
       <c r="P103" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="T103">
         <v>1</v>
       </c>
       <c r="U103" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X103">
         <f t="shared" si="24"/>
@@ -7835,9 +7870,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="104" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:27">
       <c r="A104" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B104" s="7">
         <v>87</v>
@@ -7885,13 +7920,16 @@
         <v>0</v>
       </c>
       <c r="P104" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="T104">
         <v>1</v>
       </c>
       <c r="U104" t="s">
-        <v>148</v>
+        <v>147</v>
+      </c>
+      <c r="W104" s="21" t="s">
+        <v>262</v>
       </c>
       <c r="X104">
         <f t="shared" si="24"/>
@@ -7901,10 +7939,13 @@
         <f t="shared" si="19"/>
         <v/>
       </c>
-    </row>
-    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA104" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="105" spans="1:27">
       <c r="A105" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B105" s="7">
         <v>88</v>
@@ -7940,16 +7981,16 @@
         <v>0</v>
       </c>
       <c r="P105" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="S105" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="T105">
         <v>1</v>
       </c>
       <c r="U105" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X105">
         <f t="shared" si="24"/>
@@ -7960,9 +8001,9 @@
         <v/>
       </c>
     </row>
-    <row r="106" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:27">
       <c r="A106" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B106" s="7">
         <v>89</v>
@@ -7995,13 +8036,13 @@
         <v>1.6</v>
       </c>
       <c r="P106" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="T106">
         <v>1</v>
       </c>
       <c r="U106" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X106">
         <f t="shared" si="24"/>
@@ -8012,9 +8053,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="107" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:27">
       <c r="A107" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B107" s="7">
         <v>90</v>
@@ -8050,13 +8091,13 @@
         <v>0</v>
       </c>
       <c r="P107" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="T107">
         <v>1</v>
       </c>
       <c r="U107" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X107">
         <f t="shared" si="24"/>
@@ -8067,9 +8108,9 @@
         <v/>
       </c>
     </row>
-    <row r="108" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:27">
       <c r="A108" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B108" s="7">
         <v>91</v>
@@ -8105,13 +8146,13 @@
         <v>0</v>
       </c>
       <c r="P108" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T108">
         <v>1</v>
       </c>
       <c r="U108" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X108">
         <f t="shared" si="24"/>
@@ -8122,9 +8163,9 @@
         <v/>
       </c>
     </row>
-    <row r="109" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:27">
       <c r="A109" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B109" s="7">
         <v>92</v>
@@ -8160,13 +8201,13 @@
         <v>0</v>
       </c>
       <c r="P109" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="T109">
         <v>1</v>
       </c>
       <c r="U109" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X109">
         <f t="shared" si="24"/>
@@ -8177,9 +8218,9 @@
         <v/>
       </c>
     </row>
-    <row r="110" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:27">
       <c r="A110" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B110" s="7">
         <v>93</v>
@@ -8215,16 +8256,16 @@
         <v>0</v>
       </c>
       <c r="P110" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="T110">
         <v>1</v>
       </c>
       <c r="U110" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="W110" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="X110">
         <f t="shared" si="24"/>
@@ -8235,12 +8276,12 @@
         <v/>
       </c>
       <c r="AA110" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="111" spans="1:27" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="111" spans="1:27">
       <c r="A111" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B111" s="7">
         <v>94</v>
@@ -8288,13 +8329,13 @@
         <v>0</v>
       </c>
       <c r="P111" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="T111">
         <v>1</v>
       </c>
       <c r="U111" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X111">
         <f t="shared" si="24"/>
@@ -8305,9 +8346,9 @@
         <v/>
       </c>
     </row>
-    <row r="112" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:27">
       <c r="A112" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B112" s="7">
         <v>95</v>
@@ -8355,13 +8396,13 @@
         <v>0</v>
       </c>
       <c r="P112" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="T112">
         <v>1</v>
       </c>
       <c r="U112" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X112">
         <f t="shared" si="24"/>
@@ -8372,9 +8413,9 @@
         <v/>
       </c>
     </row>
-    <row r="113" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:27">
       <c r="A113" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B113" s="7">
         <v>96</v>
@@ -8422,13 +8463,13 @@
         <v>0</v>
       </c>
       <c r="P113" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="T113">
         <v>1</v>
       </c>
       <c r="U113" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X113">
         <f t="shared" si="24"/>
@@ -8439,9 +8480,9 @@
         <v/>
       </c>
     </row>
-    <row r="114" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:27">
       <c r="A114" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B114" s="7">
         <v>97</v>
@@ -8486,16 +8527,16 @@
         <v>0.8</v>
       </c>
       <c r="P114" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="T114">
         <v>1</v>
       </c>
       <c r="U114" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="W114" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="X114">
         <f t="shared" si="24"/>
@@ -8506,10 +8547,10 @@
         <v>80</v>
       </c>
       <c r="AA114" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="115" spans="1:27" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="115" spans="1:27">
       <c r="B115" s="6"/>
       <c r="D115">
         <f t="shared" ref="D115:D116" si="29">IF(F115=4, 1,0)</f>
@@ -8544,9 +8585,9 @@
         <v/>
       </c>
     </row>
-    <row r="116" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:27">
       <c r="A116" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B116" s="17"/>
       <c r="D116">
@@ -8582,9 +8623,9 @@
         <v/>
       </c>
     </row>
-    <row r="117" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:27">
       <c r="A117" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B117" s="6">
         <v>98</v>
@@ -8629,13 +8670,13 @@
         <v>1</v>
       </c>
       <c r="P117" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="T117">
         <v>1</v>
       </c>
       <c r="U117" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X117">
         <f t="shared" ref="X117:X125" si="33">IF(ISNUMBER(E117),1,0)</f>
@@ -8646,9 +8687,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="118" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:27">
       <c r="A118" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B118" s="6">
         <v>99</v>
@@ -8696,13 +8737,13 @@
         <v>0</v>
       </c>
       <c r="P118" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="T118">
         <v>1</v>
       </c>
       <c r="U118" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X118">
         <f t="shared" si="33"/>
@@ -8713,9 +8754,9 @@
         <v/>
       </c>
     </row>
-    <row r="119" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:27">
       <c r="A119" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B119" s="6">
         <v>100</v>
@@ -8726,6 +8767,9 @@
       <c r="D119">
         <v>1</v>
       </c>
+      <c r="E119">
+        <v>0</v>
+      </c>
       <c r="F119">
         <v>4</v>
       </c>
@@ -8737,19 +8781,19 @@
       </c>
       <c r="J119">
         <f t="shared" si="20"/>
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="K119">
         <f t="shared" si="30"/>
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="L119">
         <f t="shared" si="31"/>
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="M119">
         <f t="shared" si="32"/>
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="N119">
         <f t="shared" si="25"/>
@@ -8757,29 +8801,29 @@
       </c>
       <c r="O119">
         <f t="shared" si="14"/>
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="P119" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="T119">
         <v>1</v>
       </c>
       <c r="U119" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X119">
         <f t="shared" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="Y119">
+        <v>1</v>
+      </c>
+      <c r="Y119" t="str">
         <f t="shared" si="19"/>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="120" spans="1:27" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="120" spans="1:27">
       <c r="A120" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B120" s="6">
         <v>101</v>
@@ -8790,6 +8834,9 @@
       <c r="D120">
         <v>1</v>
       </c>
+      <c r="E120">
+        <v>0</v>
+      </c>
       <c r="F120">
         <v>4</v>
       </c>
@@ -8801,19 +8848,19 @@
       </c>
       <c r="J120">
         <f t="shared" si="20"/>
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="K120">
         <f t="shared" si="30"/>
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="L120">
         <f t="shared" si="31"/>
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="M120">
         <f t="shared" si="32"/>
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="N120">
         <f t="shared" si="25"/>
@@ -8821,29 +8868,29 @@
       </c>
       <c r="O120">
         <f t="shared" si="14"/>
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="P120" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="T120">
         <v>1</v>
       </c>
       <c r="U120" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X120">
         <f t="shared" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="Y120">
+        <v>1</v>
+      </c>
+      <c r="Y120" t="str">
         <f t="shared" si="19"/>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="121" spans="1:27" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="121" spans="1:27">
       <c r="A121" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B121" s="6">
         <v>102</v>
@@ -8888,13 +8935,13 @@
         <v>1.8</v>
       </c>
       <c r="P121" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="T121">
         <v>1</v>
       </c>
       <c r="U121" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X121">
         <f t="shared" si="33"/>
@@ -8905,9 +8952,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="122" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:27">
       <c r="A122" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B122" s="6">
         <v>103</v>
@@ -8952,13 +8999,13 @@
         <v>1.8</v>
       </c>
       <c r="P122" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="T122">
         <v>1</v>
       </c>
       <c r="U122" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X122">
         <f t="shared" si="33"/>
@@ -8969,9 +9016,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="123" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:27">
       <c r="A123" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B123" s="6">
         <v>104</v>
@@ -8982,6 +9029,9 @@
       <c r="D123">
         <v>1</v>
       </c>
+      <c r="E123">
+        <v>1</v>
+      </c>
       <c r="F123">
         <v>2</v>
       </c>
@@ -8993,11 +9043,11 @@
       </c>
       <c r="J123">
         <f t="shared" si="20"/>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="K123">
         <f t="shared" si="30"/>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="L123">
         <f t="shared" si="31"/>
@@ -9013,29 +9063,32 @@
       </c>
       <c r="O123">
         <f t="shared" ref="O123:O131" si="34">IF(ISNUMBER(E123), 0, J123)</f>
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="P123" t="s">
-        <v>237</v>
+        <v>236</v>
+      </c>
+      <c r="S123" t="s">
+        <v>288</v>
       </c>
       <c r="T123">
         <v>1</v>
       </c>
       <c r="U123" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X123">
         <f t="shared" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="Y123">
+        <v>1</v>
+      </c>
+      <c r="Y123" t="str">
         <f t="shared" si="19"/>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="124" spans="1:27" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="124" spans="1:27">
       <c r="A124" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B124" s="6">
         <v>105</v>
@@ -9046,6 +9099,9 @@
       <c r="D124">
         <v>1</v>
       </c>
+      <c r="E124">
+        <v>0</v>
+      </c>
       <c r="F124">
         <v>4</v>
       </c>
@@ -9057,19 +9113,19 @@
       </c>
       <c r="J124">
         <f t="shared" si="20"/>
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="K124">
         <f t="shared" si="30"/>
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="L124">
         <f t="shared" si="31"/>
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="M124">
         <f t="shared" si="32"/>
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="N124">
         <f t="shared" si="25"/>
@@ -9077,29 +9133,35 @@
       </c>
       <c r="O124">
         <f t="shared" si="34"/>
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="P124" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="T124">
         <v>1</v>
       </c>
       <c r="U124" t="s">
-        <v>148</v>
+        <v>147</v>
+      </c>
+      <c r="W124" t="s">
+        <v>291</v>
       </c>
       <c r="X124">
         <f t="shared" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="Y124">
+        <v>1</v>
+      </c>
+      <c r="Y124" t="str">
         <f t="shared" si="19"/>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="125" spans="1:27" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+      <c r="AA124" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="125" spans="1:27">
       <c r="A125" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B125" s="6">
         <v>106</v>
@@ -9147,16 +9209,16 @@
         <v>0</v>
       </c>
       <c r="P125" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="S125" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="T125">
         <v>1</v>
       </c>
       <c r="U125" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X125">
         <f t="shared" si="33"/>
@@ -9167,7 +9229,7 @@
         <v/>
       </c>
     </row>
-    <row r="126" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:27">
       <c r="B126" s="6"/>
       <c r="J126">
         <f t="shared" si="20"/>
@@ -9186,9 +9248,9 @@
         <v/>
       </c>
     </row>
-    <row r="127" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:27">
       <c r="A127" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B127" s="17"/>
       <c r="J127">
@@ -9204,9 +9266,9 @@
         <v/>
       </c>
     </row>
-    <row r="128" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:27">
       <c r="A128" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B128" s="6"/>
       <c r="C128">
@@ -9241,9 +9303,9 @@
         <v/>
       </c>
     </row>
-    <row r="129" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:25">
       <c r="A129" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B129" s="6"/>
       <c r="C129">
@@ -9278,9 +9340,9 @@
         <v/>
       </c>
     </row>
-    <row r="130" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:25">
       <c r="A130" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B130" s="6"/>
       <c r="C130">
@@ -9315,9 +9377,9 @@
         <v/>
       </c>
     </row>
-    <row r="131" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:25">
       <c r="A131" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B131" s="6"/>
       <c r="C131">
@@ -9348,335 +9410,335 @@
         <v/>
       </c>
     </row>
-    <row r="132" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:25">
       <c r="B132" s="6"/>
     </row>
-    <row r="133" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:25">
       <c r="B133" s="6"/>
     </row>
-    <row r="134" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:25">
       <c r="B134" s="6"/>
     </row>
-    <row r="135" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:25">
       <c r="B135" s="6"/>
       <c r="P135" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="Q135" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="R135">
         <f>SUM(Q136:Q160)</f>
         <v>8</v>
       </c>
     </row>
-    <row r="136" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:25">
       <c r="B136" s="6"/>
       <c r="P136" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="Q136">
         <v>2</v>
       </c>
     </row>
-    <row r="137" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:25">
       <c r="B137" s="6"/>
       <c r="P137" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="138" spans="1:25" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="138" spans="1:25">
       <c r="B138" s="6"/>
       <c r="P138" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="139" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:25">
       <c r="B139" s="6"/>
       <c r="P139" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="Q139">
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:25">
       <c r="B140" s="6"/>
       <c r="P140" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="141" spans="1:25" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="141" spans="1:25">
       <c r="B141" s="6"/>
       <c r="P141" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="142" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:25">
       <c r="B142" s="6"/>
       <c r="P142" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="143" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:25">
       <c r="B143" s="6"/>
     </row>
-    <row r="144" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:25">
       <c r="B144" s="6"/>
       <c r="P144" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="145" spans="2:17" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="145" spans="2:17">
       <c r="B145" s="6"/>
       <c r="P145" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="146" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:17">
       <c r="B146" s="6"/>
       <c r="P146" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="147" spans="2:17" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="147" spans="2:17">
       <c r="B147" s="6"/>
       <c r="P147" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="148" spans="2:17" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="148" spans="2:17">
       <c r="B148" s="6"/>
       <c r="P148" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="149" spans="2:17" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="149" spans="2:17">
       <c r="B149" s="6"/>
     </row>
-    <row r="150" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:17">
       <c r="B150" s="6"/>
       <c r="P150" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="Q150">
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:17">
       <c r="B151" s="6"/>
       <c r="P151" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="Q151">
         <v>2</v>
       </c>
     </row>
-    <row r="152" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:17">
       <c r="B152" s="6"/>
       <c r="P152" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="153" spans="2:17" x14ac:dyDescent="0.25">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="153" spans="2:17">
       <c r="B153" s="6"/>
       <c r="P153" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="154" spans="2:17" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="154" spans="2:17">
       <c r="B154" s="6"/>
     </row>
-    <row r="155" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:17">
       <c r="B155" s="6"/>
       <c r="P155" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="Q155" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="156" spans="2:17" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="156" spans="2:17">
       <c r="B156" s="6"/>
       <c r="P156" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="157" spans="2:17" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="157" spans="2:17">
       <c r="B157" s="6"/>
     </row>
-    <row r="158" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:17">
       <c r="B158" s="6"/>
       <c r="P158" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="159" spans="2:17" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="159" spans="2:17">
       <c r="B159" s="6"/>
       <c r="P159" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="160" spans="2:17" x14ac:dyDescent="0.25">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="160" spans="2:17">
       <c r="B160" s="6"/>
       <c r="P160" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="161" spans="2:2">
       <c r="B161" s="6"/>
     </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:2">
       <c r="B162" s="6"/>
     </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:2">
       <c r="B163" s="6"/>
     </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:2">
       <c r="B164" s="6"/>
     </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:2">
       <c r="B165" s="6"/>
     </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:2">
       <c r="B166" s="6"/>
     </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:2">
       <c r="B167" s="6"/>
     </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:2">
       <c r="B168" s="6"/>
     </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:2">
       <c r="B169" s="6"/>
     </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:2">
       <c r="B170" s="6"/>
     </row>
-    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:2">
       <c r="B171" s="6"/>
     </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:2">
       <c r="B172" s="6"/>
     </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:2">
       <c r="B173" s="6"/>
     </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:2">
       <c r="B174" s="6"/>
     </row>
-    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:2">
       <c r="B175" s="6"/>
     </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:2">
       <c r="B176" s="6"/>
     </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:2">
       <c r="B177" s="6"/>
     </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:2">
       <c r="B178" s="6"/>
     </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:2">
       <c r="B179" s="6"/>
     </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:2">
       <c r="B180" s="6"/>
     </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:2">
       <c r="B181" s="6"/>
     </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:2">
       <c r="B182" s="6"/>
     </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:2">
       <c r="B183" s="6"/>
     </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:2">
       <c r="B184" s="6"/>
     </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:2">
       <c r="B185" s="6"/>
     </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:2">
       <c r="B186" s="6"/>
     </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:2">
       <c r="B187" s="6"/>
     </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:2">
       <c r="B188" s="6"/>
     </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:2">
       <c r="B189" s="6"/>
     </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:2">
       <c r="B190" s="6"/>
     </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:2">
       <c r="B191" s="6"/>
     </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:2">
       <c r="B192" s="6"/>
     </row>
-    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:2">
       <c r="B193" s="6"/>
     </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:2">
       <c r="B194" s="6"/>
     </row>
-    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:2">
       <c r="B195" s="6"/>
     </row>
-    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:2">
       <c r="B196" s="6"/>
     </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:2">
       <c r="B197" s="6"/>
     </row>
-    <row r="198" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:2">
       <c r="B198" s="6"/>
     </row>
-    <row r="199" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:2">
       <c r="B199" s="6"/>
     </row>
-    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:2">
       <c r="B200" s="6"/>
     </row>
-    <row r="201" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:2">
       <c r="B201" s="6"/>
     </row>
-    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:2">
       <c r="B202" s="6"/>
     </row>
-    <row r="203" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:2">
       <c r="B203" s="6"/>
     </row>
-    <row r="204" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:2">
       <c r="B204" s="6"/>
     </row>
-    <row r="205" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:2">
       <c r="B205" s="6"/>
     </row>
-    <row r="206" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:2">
       <c r="B206" s="6"/>
     </row>
-    <row r="207" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:2">
       <c r="B207" s="6"/>
     </row>
-    <row r="208" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:2">
       <c r="B208" s="6"/>
     </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:2">
       <c r="B209" s="6"/>
     </row>
-    <row r="210" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:2">
       <c r="B210" s="6"/>
     </row>
-    <row r="211" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:2">
       <c r="B211" s="6"/>
     </row>
-    <row r="212" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:2">
       <c r="B212" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated RSVP for Brett and Scott
</commit_message>
<xml_diff>
--- a/Guest_List_Invited.xlsx
+++ b/Guest_List_Invited.xlsx
@@ -1329,7 +1329,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1340,8 +1340,8 @@
   <dimension ref="A1:AC212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
+      <pane ySplit="4" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E112" sqref="E112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1413,7 +1413,7 @@
       </c>
       <c r="R2" s="14">
         <f>D3+G3*(1+Z4/100)</f>
-        <v>131.77875473217645</v>
+        <v>130.46671162099287</v>
       </c>
       <c r="S2" t="s">
         <v>214</v>
@@ -1437,34 +1437,34 @@
       </c>
       <c r="D3" s="20">
         <f>SUM(E6:E130)+2</f>
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E3" s="20"/>
       <c r="F3">
         <f>SUM(J6:J174)</f>
-        <v>124.89999999999998</v>
+        <v>124.19999999999997</v>
       </c>
       <c r="G3">
         <f>SUM(O6:O130)</f>
-        <v>23.900000000000006</v>
+        <v>22.200000000000003</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
       <c r="P3" s="12">
         <f>G3+D3</f>
-        <v>125.9</v>
+        <v>125.2</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>218</v>
       </c>
       <c r="R3" s="14">
         <f>D3+G3*(1-Z4/100)</f>
-        <v>120.02124526782356</v>
+        <v>119.93328837900714</v>
       </c>
       <c r="S3" s="13">
         <f>SUM(X6:X130)/COUNT(X6:X11,X14:X41,X45:X50,X53:X59,X62:X86,X89:X114,X117:X125,X128:X130)</f>
-        <v>0.77981651376146788</v>
+        <v>0.79816513761467889</v>
       </c>
       <c r="T3" s="10"/>
       <c r="U3" s="10"/>
@@ -1540,7 +1540,7 @@
       </c>
       <c r="Z4" s="10">
         <f>STDEV(Y6:Y130)</f>
-        <v>24.597300134629482</v>
+        <v>23.723926220688586</v>
       </c>
       <c r="AA4" s="10" t="s">
         <v>240</v>
@@ -6834,7 +6834,7 @@
       <c r="B88" s="17"/>
       <c r="D88">
         <f>SUM(J89:J103)</f>
-        <v>20.6</v>
+        <v>20.700000000000003</v>
       </c>
       <c r="J88">
         <f t="shared" si="20"/>
@@ -7691,6 +7691,9 @@
       <c r="D101">
         <v>1</v>
       </c>
+      <c r="E101">
+        <v>1</v>
+      </c>
       <c r="F101">
         <v>2</v>
       </c>
@@ -7702,11 +7705,11 @@
       </c>
       <c r="J101">
         <f t="shared" si="20"/>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="K101">
         <f t="shared" si="21"/>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="L101">
         <f t="shared" si="22"/>
@@ -7722,7 +7725,7 @@
       </c>
       <c r="O101">
         <f t="shared" si="14"/>
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="P101" t="s">
         <v>145</v>
@@ -7735,11 +7738,11 @@
       </c>
       <c r="X101">
         <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="Y101">
+        <v>1</v>
+      </c>
+      <c r="Y101" t="str">
         <f t="shared" si="19"/>
-        <v>90</v>
+        <v/>
       </c>
     </row>
     <row r="102" spans="1:27">
@@ -8496,6 +8499,9 @@
       <c r="D114">
         <v>1</v>
       </c>
+      <c r="E114">
+        <v>0</v>
+      </c>
       <c r="F114">
         <v>3</v>
       </c>
@@ -8507,15 +8513,15 @@
       </c>
       <c r="J114">
         <f t="shared" si="20"/>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="K114">
         <f t="shared" si="26"/>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="L114">
         <f t="shared" si="27"/>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="M114">
         <f t="shared" si="28"/>
@@ -8527,7 +8533,7 @@
       </c>
       <c r="O114">
         <f t="shared" si="14"/>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="P114" t="s">
         <v>160</v>
@@ -8543,11 +8549,11 @@
       </c>
       <c r="X114">
         <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="Y114">
+        <v>1</v>
+      </c>
+      <c r="Y114" t="str">
         <f t="shared" si="19"/>
-        <v>80</v>
+        <v/>
       </c>
       <c r="AA114" t="s">
         <v>243</v>

</xml_diff>

<commit_message>
Updated RSVP and thank yous
</commit_message>
<xml_diff>
--- a/Guest_List_Invited.xlsx
+++ b/Guest_List_Invited.xlsx
@@ -1338,7 +1338,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1349,8 +1349,8 @@
   <dimension ref="A1:AC212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E48" sqref="E48"/>
+      <pane ySplit="4" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E99" sqref="E99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1422,7 +1422,7 @@
       </c>
       <c r="R2" s="14">
         <f>D3+G3*(1+Z4/100)</f>
-        <v>121.81658213822109</v>
+        <v>121.30899116788952</v>
       </c>
       <c r="S2" t="s">
         <v>214</v>
@@ -1451,29 +1451,29 @@
       <c r="E3" s="20"/>
       <c r="F3">
         <f>SUM(J6:J174)</f>
-        <v>117.39999999999999</v>
+        <v>116.89999999999999</v>
       </c>
       <c r="G3">
         <f>SUM(O6:O130)</f>
-        <v>11.4</v>
+        <v>10.9</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
       <c r="P3" s="12">
         <f>G3+D3</f>
-        <v>119.4</v>
+        <v>118.9</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>218</v>
       </c>
       <c r="R3" s="14">
         <f>D3+G3*(1-Z4/100)</f>
-        <v>116.9834178617789</v>
+        <v>116.49100883211048</v>
       </c>
       <c r="S3" s="13">
         <f>SUM(X6:X130)/COUNT(X6:X11,X14:X41,X45:X50,X53:X59,X62:X86,X89:X114,X117:X125,X128:X130)</f>
-        <v>0.88073394495412849</v>
+        <v>0.88990825688073394</v>
       </c>
       <c r="T3" s="10"/>
       <c r="U3" s="10"/>
@@ -1549,7 +1549,7 @@
       </c>
       <c r="Z4" s="10">
         <f>STDEV(Y6:Y130)</f>
-        <v>21.198088931763973</v>
+        <v>22.100836402656117</v>
       </c>
       <c r="AA4" s="10" t="s">
         <v>240</v>
@@ -6864,7 +6864,7 @@
       <c r="B88" s="17"/>
       <c r="D88">
         <f>SUM(J89:J103)</f>
-        <v>19.100000000000001</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="J88">
         <f t="shared" si="20"/>
@@ -7520,6 +7520,9 @@
       <c r="D98">
         <v>1</v>
       </c>
+      <c r="E98">
+        <v>0</v>
+      </c>
       <c r="F98">
         <v>2</v>
       </c>
@@ -7531,11 +7534,11 @@
       </c>
       <c r="J98">
         <f t="shared" si="20"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="K98">
         <f t="shared" si="21"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L98">
         <f t="shared" si="22"/>
@@ -7551,7 +7554,7 @@
       </c>
       <c r="O98">
         <f t="shared" si="14"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="P98" t="s">
         <v>133</v>
@@ -7564,11 +7567,11 @@
       </c>
       <c r="X98">
         <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="Y98">
+        <v>1</v>
+      </c>
+      <c r="Y98" t="str">
         <f t="shared" si="19"/>
-        <v>50</v>
+        <v/>
       </c>
     </row>
     <row r="99" spans="1:27">
@@ -7982,7 +7985,7 @@
         <v/>
       </c>
       <c r="AA104" t="s">
-        <v>290</v>
+        <v>243</v>
       </c>
     </row>
     <row r="105" spans="1:27">

</xml_diff>

<commit_message>
Updated RSVPs and Gifts
</commit_message>
<xml_diff>
--- a/Guest_List_Invited.xlsx
+++ b/Guest_List_Invited.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="299">
   <si>
     <t xml:space="preserve">Priority </t>
   </si>
@@ -910,6 +910,12 @@
   </si>
   <si>
     <t>Electric kettle</t>
+  </si>
+  <si>
+    <t>Will be at wedding but not at reception</t>
+  </si>
+  <si>
+    <t>$25 for hotel on honeymoon</t>
   </si>
 </sst>
 </file>
@@ -1338,7 +1344,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1348,9 +1354,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC212"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E99" sqref="E99"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA123" sqref="AA123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1422,7 +1428,7 @@
       </c>
       <c r="R2" s="14">
         <f>D3+G3*(1+Z4/100)</f>
-        <v>121.30899116788952</v>
+        <v>119.04894379103355</v>
       </c>
       <c r="S2" t="s">
         <v>214</v>
@@ -1446,34 +1452,34 @@
       </c>
       <c r="D3" s="20">
         <f>SUM(E6:E132)</f>
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="E3" s="20"/>
       <c r="F3">
         <f>SUM(J6:J174)</f>
-        <v>116.89999999999999</v>
+        <v>116.5</v>
       </c>
       <c r="G3">
         <f>SUM(O6:O130)</f>
-        <v>10.9</v>
+        <v>4.5</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
       <c r="P3" s="12">
         <f>G3+D3</f>
-        <v>118.9</v>
+        <v>118.5</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>218</v>
       </c>
       <c r="R3" s="14">
         <f>D3+G3*(1-Z4/100)</f>
-        <v>116.49100883211048</v>
+        <v>117.95105620896645</v>
       </c>
       <c r="S3" s="13">
         <f>SUM(X6:X130)/COUNT(X6:X11,X14:X41,X45:X50,X53:X59,X62:X86,X89:X114,X117:X125,X128:X130)</f>
-        <v>0.88990825688073394</v>
+        <v>0.93577981651376152</v>
       </c>
       <c r="T3" s="10"/>
       <c r="U3" s="10"/>
@@ -1549,7 +1555,7 @@
       </c>
       <c r="Z4" s="10">
         <f>STDEV(Y6:Y130)</f>
-        <v>22.100836402656117</v>
+        <v>12.198750911856667</v>
       </c>
       <c r="AA4" s="10" t="s">
         <v>240</v>
@@ -1960,6 +1966,9 @@
       <c r="U11" t="s">
         <v>147</v>
       </c>
+      <c r="W11" t="s">
+        <v>298</v>
+      </c>
       <c r="X11">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -1967,6 +1976,9 @@
       <c r="Y11" t="str">
         <f t="shared" si="7"/>
         <v/>
+      </c>
+      <c r="AA11" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="12" spans="1:29">
@@ -2063,6 +2075,9 @@
       <c r="D14">
         <v>1</v>
       </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
       <c r="F14">
         <v>4</v>
       </c>
@@ -2074,19 +2089,19 @@
       </c>
       <c r="J14">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L14">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M14">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N14">
         <f t="shared" si="5"/>
@@ -2094,7 +2109,7 @@
       </c>
       <c r="O14">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P14" t="s">
         <v>170</v>
@@ -2107,11 +2122,11 @@
       </c>
       <c r="X14">
         <f t="shared" ref="X14:X40" si="10">IF(ISNUMBER(E14),1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Y14">
+        <v>1</v>
+      </c>
+      <c r="Y14" t="str">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:29">
@@ -2127,6 +2142,9 @@
       <c r="D15">
         <v>1</v>
       </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
       <c r="F15">
         <v>4</v>
       </c>
@@ -2138,19 +2156,19 @@
       </c>
       <c r="J15">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M15">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N15">
         <f t="shared" si="5"/>
@@ -2158,7 +2176,7 @@
       </c>
       <c r="O15">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P15" t="s">
         <v>141</v>
@@ -2171,11 +2189,11 @@
       </c>
       <c r="X15">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="Y15">
+        <v>1</v>
+      </c>
+      <c r="Y15" t="str">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v/>
       </c>
     </row>
     <row r="16" spans="1:29">
@@ -6864,7 +6882,7 @@
       <c r="B88" s="17"/>
       <c r="D88">
         <f>SUM(J89:J103)</f>
-        <v>18.600000000000001</v>
+        <v>19</v>
       </c>
       <c r="J88">
         <f t="shared" si="20"/>
@@ -7182,6 +7200,9 @@
       <c r="D93">
         <v>1</v>
       </c>
+      <c r="E93">
+        <v>2</v>
+      </c>
       <c r="F93">
         <v>4</v>
       </c>
@@ -7193,19 +7214,19 @@
       </c>
       <c r="J93">
         <f t="shared" si="20"/>
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="K93">
         <f t="shared" si="21"/>
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="L93">
         <f t="shared" si="22"/>
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="M93">
         <f t="shared" si="23"/>
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="N93">
         <f t="shared" si="18"/>
@@ -7213,7 +7234,7 @@
       </c>
       <c r="O93">
         <f t="shared" si="14"/>
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="P93" t="s">
         <v>138</v>
@@ -7229,11 +7250,11 @@
       </c>
       <c r="X93">
         <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="Y93">
+        <v>1</v>
+      </c>
+      <c r="Y93" t="str">
         <f t="shared" si="19"/>
-        <v>80</v>
+        <v/>
       </c>
       <c r="AA93" t="s">
         <v>243</v>
@@ -8690,6 +8711,9 @@
       <c r="D117">
         <v>1</v>
       </c>
+      <c r="E117">
+        <v>0</v>
+      </c>
       <c r="F117">
         <v>4</v>
       </c>
@@ -8701,19 +8725,19 @@
       </c>
       <c r="J117">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K117">
         <f t="shared" si="30"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L117">
         <f t="shared" si="31"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M117">
         <f t="shared" si="32"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N117">
         <f t="shared" si="25"/>
@@ -8721,11 +8745,14 @@
       </c>
       <c r="O117">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P117" t="s">
         <v>198</v>
       </c>
+      <c r="S117" t="s">
+        <v>297</v>
+      </c>
       <c r="T117">
         <v>1</v>
       </c>
@@ -8734,11 +8761,11 @@
       </c>
       <c r="X117">
         <f t="shared" ref="X117:X125" si="33">IF(ISNUMBER(E117),1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Y117">
+        <v>1</v>
+      </c>
+      <c r="Y117" t="str">
         <f t="shared" si="19"/>
-        <v>50</v>
+        <v/>
       </c>
     </row>
     <row r="118" spans="1:27">
@@ -8955,6 +8982,9 @@
       <c r="D121">
         <v>1</v>
       </c>
+      <c r="E121">
+        <v>2</v>
+      </c>
       <c r="F121">
         <v>4</v>
       </c>
@@ -8966,19 +8996,19 @@
       </c>
       <c r="J121">
         <f t="shared" si="20"/>
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="K121">
         <f t="shared" si="30"/>
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="L121">
         <f t="shared" si="31"/>
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="M121">
         <f t="shared" si="32"/>
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="N121">
         <f t="shared" si="25"/>
@@ -8986,7 +9016,7 @@
       </c>
       <c r="O121">
         <f t="shared" si="14"/>
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="P121" t="s">
         <v>201</v>
@@ -8999,11 +9029,11 @@
       </c>
       <c r="X121">
         <f t="shared" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="Y121">
+        <v>1</v>
+      </c>
+      <c r="Y121" t="str">
         <f t="shared" si="19"/>
-        <v>90</v>
+        <v/>
       </c>
     </row>
     <row r="122" spans="1:27">

</xml_diff>

<commit_message>
Updated Thank You notes
</commit_message>
<xml_diff>
--- a/Guest_List_Invited.xlsx
+++ b/Guest_List_Invited.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\logan\Documents\GitHub\Farrell_Garrett_Wedding\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C7A1CFAB-BA44-432A-9C44-81201C681FD1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="312">
   <si>
     <t xml:space="preserve">Priority </t>
   </si>
@@ -955,17 +949,23 @@
   </si>
   <si>
     <t>Pat</t>
+  </si>
+  <si>
+    <t>3 plates</t>
+  </si>
+  <si>
+    <t>$60 for airline miles</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1383,22 +1383,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AD212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q142" sqref="Q142"/>
+      <pane ySplit="4" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W84" sqref="W84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35.85546875" customWidth="1"/>
     <col min="2" max="2" width="4" hidden="1" customWidth="1"/>
@@ -1424,7 +1424,7 @@
     <col min="27" max="27" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" ht="15" customHeight="1">
       <c r="A1" s="5">
         <v>4</v>
       </c>
@@ -1444,7 +1444,7 @@
       <c r="U1" s="10"/>
       <c r="V1" s="10"/>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30">
       <c r="A2" s="4">
         <v>3</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="4" spans="1:30" s="10" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" s="10" customFormat="1" ht="31.5" customHeight="1">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -1605,7 +1605,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1619,7 +1619,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1753,7 +1753,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1963,7 +1963,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30">
       <c r="B12" s="6"/>
       <c r="C12" s="1"/>
       <c r="D12">
@@ -2080,7 +2080,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27">
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27">
       <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27">
       <c r="A19" s="2" t="s">
         <v>184</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27">
       <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
@@ -2676,7 +2676,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27">
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27">
       <c r="A23" s="2" t="s">
         <v>226</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27">
       <c r="A24" s="2" t="s">
         <v>17</v>
       </c>
@@ -2889,7 +2889,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27">
       <c r="A25" s="2" t="s">
         <v>18</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27">
       <c r="A26" s="2" t="s">
         <v>19</v>
       </c>
@@ -3029,7 +3029,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27">
       <c r="A27" s="2" t="s">
         <v>20</v>
       </c>
@@ -3096,7 +3096,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27">
       <c r="A28" s="2" t="s">
         <v>21</v>
       </c>
@@ -3163,7 +3163,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27">
       <c r="A29" s="2" t="s">
         <v>22</v>
       </c>
@@ -3230,7 +3230,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27">
       <c r="A30" s="2" t="s">
         <v>23</v>
       </c>
@@ -3297,7 +3297,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27">
       <c r="A31" s="2" t="s">
         <v>24</v>
       </c>
@@ -3370,7 +3370,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27">
       <c r="A32" s="2" t="s">
         <v>25</v>
       </c>
@@ -3437,7 +3437,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27">
       <c r="A33" s="2" t="s">
         <v>26</v>
       </c>
@@ -3504,7 +3504,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
@@ -3577,7 +3577,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
@@ -3644,7 +3644,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27">
       <c r="A36" t="s">
         <v>257</v>
       </c>
@@ -3711,7 +3711,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27">
       <c r="A37" s="2" t="s">
         <v>40</v>
       </c>
@@ -3778,7 +3778,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27">
       <c r="A38" s="2" t="s">
         <v>41</v>
       </c>
@@ -3851,7 +3851,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27">
       <c r="A39" s="2" t="s">
         <v>42</v>
       </c>
@@ -3918,7 +3918,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27">
       <c r="A40" s="2" t="s">
         <v>43</v>
       </c>
@@ -3979,6 +3979,9 @@
       <c r="U40" t="s">
         <v>146</v>
       </c>
+      <c r="W40" t="s">
+        <v>310</v>
+      </c>
       <c r="X40">
         <f t="shared" si="10"/>
         <v>1</v>
@@ -3987,8 +3990,11 @@
         <f t="shared" si="7"/>
         <v/>
       </c>
-    </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA40" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27">
       <c r="A41" t="s">
         <v>96</v>
       </c>
@@ -4058,7 +4064,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27">
       <c r="A42" s="2"/>
       <c r="B42" s="7"/>
       <c r="D42">
@@ -4094,7 +4100,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27">
       <c r="B43" s="6"/>
       <c r="C43" s="1"/>
       <c r="D43">
@@ -4130,7 +4136,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27">
       <c r="A44" s="1" t="s">
         <v>27</v>
       </c>
@@ -4172,7 +4178,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27">
       <c r="A45" t="s">
         <v>28</v>
       </c>
@@ -4248,7 +4254,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27">
       <c r="A46" t="s">
         <v>29</v>
       </c>
@@ -4315,7 +4321,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27">
       <c r="A47" t="s">
         <v>30</v>
       </c>
@@ -4382,7 +4388,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27">
       <c r="A48" t="s">
         <v>31</v>
       </c>
@@ -4452,7 +4458,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:29">
       <c r="A49" t="s">
         <v>32</v>
       </c>
@@ -4522,7 +4528,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:29">
       <c r="A50" t="s">
         <v>227</v>
       </c>
@@ -4597,7 +4603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:29">
       <c r="B51" s="6"/>
       <c r="J51">
         <f t="shared" si="9"/>
@@ -4628,7 +4634,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:29">
       <c r="A52" s="1" t="s">
         <v>48</v>
       </c>
@@ -4670,7 +4676,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:29">
       <c r="A53" t="s">
         <v>47</v>
       </c>
@@ -4741,7 +4747,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:29">
       <c r="A54" t="s">
         <v>307</v>
       </c>
@@ -4811,7 +4817,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:29">
       <c r="A55" t="s">
         <v>49</v>
       </c>
@@ -4882,7 +4888,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:29">
       <c r="A56" t="s">
         <v>73</v>
       </c>
@@ -4955,7 +4961,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:29">
       <c r="A57" t="s">
         <v>50</v>
       </c>
@@ -5025,7 +5031,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:29">
       <c r="A58" t="s">
         <v>51</v>
       </c>
@@ -5095,7 +5101,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:29">
       <c r="A59" t="s">
         <v>52</v>
       </c>
@@ -5162,7 +5168,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:29">
       <c r="B60" s="6"/>
       <c r="J60">
         <f t="shared" si="9"/>
@@ -5193,7 +5199,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:29">
       <c r="A61" s="1" t="s">
         <v>46</v>
       </c>
@@ -5235,7 +5241,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:29">
       <c r="A62" t="s">
         <v>218</v>
       </c>
@@ -5306,7 +5312,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:29">
       <c r="A63" t="s">
         <v>262</v>
       </c>
@@ -5360,7 +5366,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:29">
       <c r="A64" t="s">
         <v>53</v>
       </c>
@@ -5431,7 +5437,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:27">
       <c r="A65" t="s">
         <v>290</v>
       </c>
@@ -5504,7 +5510,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:27">
       <c r="A66" t="s">
         <v>54</v>
       </c>
@@ -5575,7 +5581,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:27">
       <c r="A67" t="s">
         <v>163</v>
       </c>
@@ -5646,7 +5652,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:27">
       <c r="A68" t="s">
         <v>187</v>
       </c>
@@ -5710,7 +5716,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="69" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:27">
       <c r="A69" t="s">
         <v>55</v>
       </c>
@@ -5781,7 +5787,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:27">
       <c r="A70" t="s">
         <v>252</v>
       </c>
@@ -5854,7 +5860,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:27">
       <c r="A71" t="s">
         <v>56</v>
       </c>
@@ -5925,7 +5931,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:27">
       <c r="A72" t="s">
         <v>57</v>
       </c>
@@ -5995,7 +6001,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:27">
       <c r="A73" t="s">
         <v>58</v>
       </c>
@@ -6065,7 +6071,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:27">
       <c r="A74" t="s">
         <v>59</v>
       </c>
@@ -6132,7 +6138,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:27">
       <c r="A75" t="s">
         <v>60</v>
       </c>
@@ -6190,6 +6196,9 @@
       <c r="U75" t="s">
         <v>146</v>
       </c>
+      <c r="W75" t="s">
+        <v>258</v>
+      </c>
       <c r="X75">
         <f t="shared" si="13"/>
         <v>1</v>
@@ -6198,8 +6207,11 @@
         <f t="shared" si="19"/>
         <v/>
       </c>
-    </row>
-    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA75" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="76" spans="1:27">
       <c r="A76" t="s">
         <v>61</v>
       </c>
@@ -6272,7 +6284,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:27">
       <c r="A77" t="s">
         <v>62</v>
       </c>
@@ -6342,7 +6354,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:27">
       <c r="A78" t="s">
         <v>162</v>
       </c>
@@ -6409,7 +6421,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:27">
       <c r="A79" t="s">
         <v>64</v>
       </c>
@@ -6476,7 +6488,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:27">
       <c r="A80" t="s">
         <v>123</v>
       </c>
@@ -6543,7 +6555,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:27">
       <c r="A81" t="s">
         <v>285</v>
       </c>
@@ -6610,7 +6622,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:27">
       <c r="A82" t="s">
         <v>63</v>
       </c>
@@ -6677,7 +6689,7 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:27">
       <c r="A83" t="s">
         <v>165</v>
       </c>
@@ -6735,6 +6747,9 @@
       <c r="U83" t="s">
         <v>146</v>
       </c>
+      <c r="W83" t="s">
+        <v>311</v>
+      </c>
       <c r="X83">
         <f t="shared" si="13"/>
         <v>1</v>
@@ -6743,8 +6758,11 @@
         <f t="shared" si="19"/>
         <v/>
       </c>
-    </row>
-    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA83" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="84" spans="1:27">
       <c r="A84" t="s">
         <v>219</v>
       </c>
@@ -6814,7 +6832,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:27">
       <c r="A85" t="s">
         <v>245</v>
       </c>
@@ -6881,7 +6899,7 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:27">
       <c r="A86" t="s">
         <v>220</v>
       </c>
@@ -6948,7 +6966,7 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:27">
       <c r="B87" s="6"/>
       <c r="J87">
         <f t="shared" si="20"/>
@@ -6979,7 +6997,7 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:27">
       <c r="A88" s="1" t="s">
         <v>69</v>
       </c>
@@ -7021,7 +7039,7 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:27">
       <c r="A89" s="2" t="s">
         <v>76</v>
       </c>
@@ -7088,7 +7106,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:27">
       <c r="A90" t="s">
         <v>70</v>
       </c>
@@ -7155,7 +7173,7 @@
         <v/>
       </c>
     </row>
-    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:27">
       <c r="A91" t="s">
         <v>130</v>
       </c>
@@ -7228,7 +7246,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:27">
       <c r="A92" t="s">
         <v>71</v>
       </c>
@@ -7295,7 +7313,7 @@
         <v/>
       </c>
     </row>
-    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:27">
       <c r="A93" t="s">
         <v>72</v>
       </c>
@@ -7368,7 +7386,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:27">
       <c r="A94" t="s">
         <v>153</v>
       </c>
@@ -7435,7 +7453,7 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:27">
       <c r="A95" t="s">
         <v>150</v>
       </c>
@@ -7502,7 +7520,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:27">
       <c r="A96" t="s">
         <v>154</v>
       </c>
@@ -7569,7 +7587,7 @@
         <v/>
       </c>
     </row>
-    <row r="97" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:27">
       <c r="A97" t="s">
         <v>116</v>
       </c>
@@ -7636,7 +7654,7 @@
         <v/>
       </c>
     </row>
-    <row r="98" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:27">
       <c r="A98" t="s">
         <v>131</v>
       </c>
@@ -7703,7 +7721,7 @@
         <v/>
       </c>
     </row>
-    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:27">
       <c r="A99" t="s">
         <v>74</v>
       </c>
@@ -7770,7 +7788,7 @@
         <v/>
       </c>
     </row>
-    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:27">
       <c r="A100" t="s">
         <v>155</v>
       </c>
@@ -7843,7 +7861,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:27">
       <c r="A101" t="s">
         <v>143</v>
       </c>
@@ -7910,7 +7928,7 @@
         <v/>
       </c>
     </row>
-    <row r="102" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:27">
       <c r="A102" t="s">
         <v>75</v>
       </c>
@@ -7983,7 +8001,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="103" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:27">
       <c r="A103" t="s">
         <v>147</v>
       </c>
@@ -8053,7 +8071,7 @@
         <v/>
       </c>
     </row>
-    <row r="104" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:27">
       <c r="A104" t="s">
         <v>148</v>
       </c>
@@ -8126,7 +8144,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:27">
       <c r="A105" t="s">
         <v>225</v>
       </c>
@@ -8184,7 +8202,7 @@
         <v/>
       </c>
     </row>
-    <row r="106" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:27">
       <c r="A106" t="s">
         <v>114</v>
       </c>
@@ -8242,7 +8260,7 @@
         <v/>
       </c>
     </row>
-    <row r="107" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:27">
       <c r="A107" t="s">
         <v>156</v>
       </c>
@@ -8297,7 +8315,7 @@
         <v/>
       </c>
     </row>
-    <row r="108" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:27">
       <c r="A108" t="s">
         <v>157</v>
       </c>
@@ -8352,7 +8370,7 @@
         <v/>
       </c>
     </row>
-    <row r="109" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:27">
       <c r="A109" t="s">
         <v>78</v>
       </c>
@@ -8407,7 +8425,7 @@
         <v/>
       </c>
     </row>
-    <row r="110" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:27">
       <c r="A110" t="s">
         <v>223</v>
       </c>
@@ -8468,7 +8486,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="111" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:27">
       <c r="A111" t="s">
         <v>222</v>
       </c>
@@ -8535,7 +8553,7 @@
         <v/>
       </c>
     </row>
-    <row r="112" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:27">
       <c r="A112" t="s">
         <v>224</v>
       </c>
@@ -8602,7 +8620,7 @@
         <v/>
       </c>
     </row>
-    <row r="113" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:27">
       <c r="A113" t="s">
         <v>77</v>
       </c>
@@ -8669,7 +8687,7 @@
         <v/>
       </c>
     </row>
-    <row r="114" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:27">
       <c r="A114" t="s">
         <v>221</v>
       </c>
@@ -8742,7 +8760,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="115" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:27">
       <c r="B115" s="6"/>
       <c r="D115">
         <f t="shared" ref="D115:D116" si="29">IF(F115=4, 1,0)</f>
@@ -8777,7 +8795,7 @@
         <v/>
       </c>
     </row>
-    <row r="116" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:27">
       <c r="A116" s="1" t="s">
         <v>79</v>
       </c>
@@ -8819,7 +8837,7 @@
         <v/>
       </c>
     </row>
-    <row r="117" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:27">
       <c r="A117" t="s">
         <v>228</v>
       </c>
@@ -8889,7 +8907,7 @@
         <v/>
       </c>
     </row>
-    <row r="118" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:27">
       <c r="A118" t="s">
         <v>80</v>
       </c>
@@ -8956,7 +8974,7 @@
         <v/>
       </c>
     </row>
-    <row r="119" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:27">
       <c r="A119" t="s">
         <v>229</v>
       </c>
@@ -9023,7 +9041,7 @@
         <v/>
       </c>
     </row>
-    <row r="120" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:27">
       <c r="A120" t="s">
         <v>81</v>
       </c>
@@ -9090,7 +9108,7 @@
         <v/>
       </c>
     </row>
-    <row r="121" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:27">
       <c r="A121" t="s">
         <v>82</v>
       </c>
@@ -9157,7 +9175,7 @@
         <v/>
       </c>
     </row>
-    <row r="122" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:27">
       <c r="A122" t="s">
         <v>230</v>
       </c>
@@ -9227,7 +9245,7 @@
         <v/>
       </c>
     </row>
-    <row r="123" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:27">
       <c r="A123" t="s">
         <v>231</v>
       </c>
@@ -9297,7 +9315,7 @@
         <v/>
       </c>
     </row>
-    <row r="124" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:27">
       <c r="A124" t="s">
         <v>232</v>
       </c>
@@ -9370,7 +9388,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="125" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:27">
       <c r="A125" t="s">
         <v>233</v>
       </c>
@@ -9440,7 +9458,7 @@
         <v/>
       </c>
     </row>
-    <row r="126" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:27">
       <c r="B126" s="6"/>
       <c r="J126">
         <f t="shared" si="20"/>
@@ -9459,7 +9477,7 @@
         <v/>
       </c>
     </row>
-    <row r="127" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:27">
       <c r="A127" s="1" t="s">
         <v>204</v>
       </c>
@@ -9481,7 +9499,7 @@
         <v/>
       </c>
     </row>
-    <row r="128" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:27">
       <c r="A128" t="s">
         <v>254</v>
       </c>
@@ -9518,7 +9536,7 @@
         <v/>
       </c>
     </row>
-    <row r="129" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:25">
       <c r="A129" t="s">
         <v>205</v>
       </c>
@@ -9555,7 +9573,7 @@
         <v/>
       </c>
     </row>
-    <row r="130" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:25">
       <c r="A130" t="s">
         <v>206</v>
       </c>
@@ -9592,7 +9610,7 @@
         <v/>
       </c>
     </row>
-    <row r="131" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:25">
       <c r="A131" t="s">
         <v>255</v>
       </c>
@@ -9625,7 +9643,7 @@
         <v/>
       </c>
     </row>
-    <row r="132" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:25">
       <c r="A132" t="s">
         <v>293</v>
       </c>
@@ -9634,13 +9652,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:25">
       <c r="B133" s="6"/>
     </row>
-    <row r="134" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:25">
       <c r="B134" s="6"/>
     </row>
-    <row r="135" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:25">
       <c r="B135" s="6"/>
       <c r="P135" t="s">
         <v>282</v>
@@ -9653,7 +9671,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="136" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:25">
       <c r="B136" s="6"/>
       <c r="P136" t="s">
         <v>284</v>
@@ -9662,7 +9680,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="137" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:25">
       <c r="B137" s="6"/>
       <c r="P137" t="s">
         <v>266</v>
@@ -9671,7 +9689,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:25">
       <c r="B138" s="6"/>
       <c r="P138" t="s">
         <v>47</v>
@@ -9680,7 +9698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:25">
       <c r="B139" s="6"/>
       <c r="P139" t="s">
         <v>267</v>
@@ -9689,7 +9707,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:25">
       <c r="B140" s="6"/>
       <c r="P140" t="s">
         <v>268</v>
@@ -9698,7 +9716,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:25">
       <c r="B141" s="6"/>
       <c r="P141" t="s">
         <v>49</v>
@@ -9707,7 +9725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:25">
       <c r="B142" s="6"/>
       <c r="P142" t="s">
         <v>7</v>
@@ -9716,10 +9734,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:25">
       <c r="B143" s="6"/>
     </row>
-    <row r="144" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:25">
       <c r="B144" s="6"/>
       <c r="P144" t="s">
         <v>269</v>
@@ -9728,7 +9746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:23">
       <c r="B145" s="6"/>
       <c r="P145" t="s">
         <v>51</v>
@@ -9737,7 +9755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:23">
       <c r="B146" s="6"/>
       <c r="P146" t="s">
         <v>270</v>
@@ -9749,7 +9767,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="147" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:23">
       <c r="B147" s="6"/>
       <c r="P147" t="s">
         <v>271</v>
@@ -9758,7 +9776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:23">
       <c r="B148" s="6"/>
       <c r="P148" t="s">
         <v>272</v>
@@ -9767,10 +9785,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:23">
       <c r="B149" s="6"/>
     </row>
-    <row r="150" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:23">
       <c r="B150" s="6"/>
       <c r="P150" t="s">
         <v>273</v>
@@ -9779,7 +9797,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:23">
       <c r="B151" s="6"/>
       <c r="P151" t="s">
         <v>274</v>
@@ -9788,7 +9806,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="152" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:23">
       <c r="B152" s="6"/>
       <c r="P152" t="s">
         <v>275</v>
@@ -9797,7 +9815,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="153" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:23">
       <c r="B153" s="6"/>
       <c r="P153" t="s">
         <v>276</v>
@@ -9806,10 +9824,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:23">
       <c r="B154" s="6"/>
     </row>
-    <row r="155" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:23">
       <c r="B155" s="6"/>
       <c r="P155" t="s">
         <v>277</v>
@@ -9818,7 +9836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:23">
       <c r="B156" s="6"/>
       <c r="P156" t="s">
         <v>278</v>
@@ -9827,10 +9845,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="157" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:23">
       <c r="B157" s="6"/>
     </row>
-    <row r="158" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:23">
       <c r="B158" s="6"/>
       <c r="P158" t="s">
         <v>279</v>
@@ -9839,19 +9857,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:23">
       <c r="B159" s="6"/>
       <c r="P159" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="160" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:23">
       <c r="B160" s="6"/>
       <c r="P160" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="161" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:17">
       <c r="B161" s="6"/>
       <c r="P161" t="s">
         <v>309</v>
@@ -9860,157 +9878,157 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:17">
       <c r="B162" s="6"/>
     </row>
-    <row r="163" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:17">
       <c r="B163" s="6"/>
     </row>
-    <row r="164" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:17">
       <c r="B164" s="6"/>
     </row>
-    <row r="165" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:17">
       <c r="B165" s="6"/>
     </row>
-    <row r="166" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:17">
       <c r="B166" s="6"/>
     </row>
-    <row r="167" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:17">
       <c r="B167" s="6"/>
     </row>
-    <row r="168" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:17">
       <c r="B168" s="6"/>
     </row>
-    <row r="169" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:17">
       <c r="B169" s="6"/>
     </row>
-    <row r="170" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:17">
       <c r="B170" s="6"/>
     </row>
-    <row r="171" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:17">
       <c r="B171" s="6"/>
     </row>
-    <row r="172" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:17">
       <c r="B172" s="6"/>
     </row>
-    <row r="173" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:17">
       <c r="B173" s="6"/>
     </row>
-    <row r="174" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:17">
       <c r="B174" s="6"/>
     </row>
-    <row r="175" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:17">
       <c r="B175" s="6"/>
     </row>
-    <row r="176" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:17">
       <c r="B176" s="6"/>
     </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:2">
       <c r="B177" s="6"/>
     </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:2">
       <c r="B178" s="6"/>
     </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:2">
       <c r="B179" s="6"/>
     </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:2">
       <c r="B180" s="6"/>
     </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:2">
       <c r="B181" s="6"/>
     </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:2">
       <c r="B182" s="6"/>
     </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:2">
       <c r="B183" s="6"/>
     </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:2">
       <c r="B184" s="6"/>
     </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:2">
       <c r="B185" s="6"/>
     </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:2">
       <c r="B186" s="6"/>
     </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:2">
       <c r="B187" s="6"/>
     </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:2">
       <c r="B188" s="6"/>
     </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:2">
       <c r="B189" s="6"/>
     </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:2">
       <c r="B190" s="6"/>
     </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:2">
       <c r="B191" s="6"/>
     </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:2">
       <c r="B192" s="6"/>
     </row>
-    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:2">
       <c r="B193" s="6"/>
     </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:2">
       <c r="B194" s="6"/>
     </row>
-    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:2">
       <c r="B195" s="6"/>
     </row>
-    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:2">
       <c r="B196" s="6"/>
     </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:2">
       <c r="B197" s="6"/>
     </row>
-    <row r="198" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:2">
       <c r="B198" s="6"/>
     </row>
-    <row r="199" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:2">
       <c r="B199" s="6"/>
     </row>
-    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:2">
       <c r="B200" s="6"/>
     </row>
-    <row r="201" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:2">
       <c r="B201" s="6"/>
     </row>
-    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:2">
       <c r="B202" s="6"/>
     </row>
-    <row r="203" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:2">
       <c r="B203" s="6"/>
     </row>
-    <row r="204" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:2">
       <c r="B204" s="6"/>
     </row>
-    <row r="205" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:2">
       <c r="B205" s="6"/>
     </row>
-    <row r="206" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:2">
       <c r="B206" s="6"/>
     </row>
-    <row r="207" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:2">
       <c r="B207" s="6"/>
     </row>
-    <row r="208" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:2">
       <c r="B208" s="6"/>
     </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:2">
       <c r="B209" s="6"/>
     </row>
-    <row r="210" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:2">
       <c r="B210" s="6"/>
     </row>
-    <row r="211" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:2">
       <c r="B211" s="6"/>
     </row>
-    <row r="212" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:2">
       <c r="B212" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added tab for table assignments
</commit_message>
<xml_diff>
--- a/Guest_List_Invited.xlsx
+++ b/Guest_List_Invited.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Table #" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="332">
   <si>
     <t xml:space="preserve">Priority </t>
   </si>
@@ -955,6 +956,66 @@
   </si>
   <si>
     <t>$60 for airline miles</t>
+  </si>
+  <si>
+    <t>Table 1</t>
+  </si>
+  <si>
+    <t>Ms. Lisa Garrett</t>
+  </si>
+  <si>
+    <t>Ms. Laura Garrett</t>
+  </si>
+  <si>
+    <t>Ms. Amanda Wenger</t>
+  </si>
+  <si>
+    <t>Ms. Sarah Mesrobian</t>
+  </si>
+  <si>
+    <t>Mr. Kelly Mann</t>
+  </si>
+  <si>
+    <t>Mr. Eric Davis</t>
+  </si>
+  <si>
+    <t>Mr. Alexander Farrell</t>
+  </si>
+  <si>
+    <t>Total - 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table 2 </t>
+  </si>
+  <si>
+    <t>Total - 8</t>
+  </si>
+  <si>
+    <t>Veggie?</t>
+  </si>
+  <si>
+    <t>Mr. Cory Brewer</t>
+  </si>
+  <si>
+    <t>Mrs. Katie Brewer</t>
+  </si>
+  <si>
+    <t>Mrs. Courtney Gorbandt</t>
+  </si>
+  <si>
+    <t>Mr. John Gorbandt IV</t>
+  </si>
+  <si>
+    <t>Mrs. Jennifer Walker</t>
+  </si>
+  <si>
+    <t>Mr. Brian Walker</t>
+  </si>
+  <si>
+    <t>Mr. William O'Neill</t>
+  </si>
+  <si>
+    <t>Ms. Megan Smith</t>
   </si>
 </sst>
 </file>
@@ -1383,7 +1444,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1393,7 +1454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AD212"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="W84" sqref="W84"/>
     </sheetView>
@@ -10049,4 +10110,117 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>321</v>
+      </c>
+      <c r="B10" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="8" t="s">
+        <v>331</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated table numbers + veggie meals
</commit_message>
<xml_diff>
--- a/Guest_List_Invited.xlsx
+++ b/Guest_List_Invited.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="439">
   <si>
     <t xml:space="preserve">Priority </t>
   </si>
@@ -982,18 +982,9 @@
     <t>Mr. Alexander Farrell</t>
   </si>
   <si>
-    <t>Total - 7</t>
-  </si>
-  <si>
     <t xml:space="preserve">Table 2 </t>
   </si>
   <si>
-    <t>Total - 8</t>
-  </si>
-  <si>
-    <t>Veggie?</t>
-  </si>
-  <si>
     <t>Mr. Cory Brewer</t>
   </si>
   <si>
@@ -1016,6 +1007,336 @@
   </si>
   <si>
     <t>Ms. Megan Smith</t>
+  </si>
+  <si>
+    <t>Table 3</t>
+  </si>
+  <si>
+    <t>Mrs. Lannie Bluethmann</t>
+  </si>
+  <si>
+    <t>Mr. Bill Bluethmann</t>
+  </si>
+  <si>
+    <t>Mr. Parker Francis</t>
+  </si>
+  <si>
+    <t>Ms. Isabelle Edhlund</t>
+  </si>
+  <si>
+    <t>Mrs. Kris Pettinger</t>
+  </si>
+  <si>
+    <t>Vegetarian</t>
+  </si>
+  <si>
+    <t>Mr. Ross Pettinger</t>
+  </si>
+  <si>
+    <t>Mr. Evan Laske</t>
+  </si>
+  <si>
+    <t>Table 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kris </t>
+  </si>
+  <si>
+    <t>Mr. Zachary Farrell</t>
+  </si>
+  <si>
+    <t>Mr. David Farrell</t>
+  </si>
+  <si>
+    <t>Guest</t>
+  </si>
+  <si>
+    <t>Mr. Jeff Garrett</t>
+  </si>
+  <si>
+    <t>Mrs. Linda Garrett</t>
+  </si>
+  <si>
+    <t>Mr. Michael Garrett</t>
+  </si>
+  <si>
+    <t>Mr. Mark Garrett</t>
+  </si>
+  <si>
+    <t>Mrs. Deborah Garrett</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table 5 </t>
+  </si>
+  <si>
+    <t>Mr. Brandon Hatfield</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mrs. Kathy Hatfield </t>
+  </si>
+  <si>
+    <t>Mr. Don Hatfield</t>
+  </si>
+  <si>
+    <t>Mr. Tom Nugent</t>
+  </si>
+  <si>
+    <t>Mrs. Janet Nugent</t>
+  </si>
+  <si>
+    <t>Mrs. Gwen Donahue</t>
+  </si>
+  <si>
+    <t>Fr. Phil Lloyd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr. Seth Saldivar </t>
+  </si>
+  <si>
+    <t>Mrs. Allison Saldivar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table 6 </t>
+  </si>
+  <si>
+    <t>Mr. Joseph Farrell</t>
+  </si>
+  <si>
+    <t>Mrs. Suzanne Farrell</t>
+  </si>
+  <si>
+    <t>Mr. Doug Klumpe</t>
+  </si>
+  <si>
+    <t>Mrs. Angie Klumpe</t>
+  </si>
+  <si>
+    <t>Mrs. Lavon Sigler</t>
+  </si>
+  <si>
+    <t>Mrs. Jane Myers</t>
+  </si>
+  <si>
+    <t>Mr. John Sigler</t>
+  </si>
+  <si>
+    <t>Mrs. Diana Sigler</t>
+  </si>
+  <si>
+    <t>Table 7</t>
+  </si>
+  <si>
+    <t>Ms. Katelyn Dvorsky</t>
+  </si>
+  <si>
+    <t>Ms. Sarah Luna</t>
+  </si>
+  <si>
+    <t>Mr. Lucas Kinion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr. Matthew Honeychuck </t>
+  </si>
+  <si>
+    <t>Ms. Sarah Gonzaga</t>
+  </si>
+  <si>
+    <t>Ms. Ami Yang</t>
+  </si>
+  <si>
+    <t>Mr. Brian Killeen</t>
+  </si>
+  <si>
+    <t>Mr. Brent Davis</t>
+  </si>
+  <si>
+    <t>Mrs. Kristine Davis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table 8 </t>
+  </si>
+  <si>
+    <t>Ms. Lauren Cooper</t>
+  </si>
+  <si>
+    <t>Mr. Ronak Dave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr. James Reil </t>
+  </si>
+  <si>
+    <t>Ms. Kirstyn Johnson</t>
+  </si>
+  <si>
+    <t>Mr. Gary Jordan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. Liz RotiRoti </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. Fiona Turett </t>
+  </si>
+  <si>
+    <t>Ms. Andrea Parker</t>
+  </si>
+  <si>
+    <t>Ms. Kelsi Redfearn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. Kristen Breitenbach </t>
+  </si>
+  <si>
+    <t>Low Sodium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table 9 </t>
+  </si>
+  <si>
+    <t>Mr. Joel Pullen</t>
+  </si>
+  <si>
+    <t>Ms. Jennifer Gaffney</t>
+  </si>
+  <si>
+    <t>Mr. Ethan Gastineau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr. Kyle Scherer </t>
+  </si>
+  <si>
+    <t>Mr. Jared Willits</t>
+  </si>
+  <si>
+    <t>Mrs. Allison Willits</t>
+  </si>
+  <si>
+    <t>Ms. Lindsey Stiffler</t>
+  </si>
+  <si>
+    <t>Ms. Christine Schmitz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table 10 </t>
+  </si>
+  <si>
+    <t>Ms. Melissa Hastert</t>
+  </si>
+  <si>
+    <t>Mr. Michael Bellinghausen</t>
+  </si>
+  <si>
+    <t>Ms. Tori Pedrotty</t>
+  </si>
+  <si>
+    <t>Mr. Benjamin Booher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. Ginina Vittuci </t>
+  </si>
+  <si>
+    <t>Ms. Mallory Daly</t>
+  </si>
+  <si>
+    <t>Mr. Joshua Nation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table 11 </t>
+  </si>
+  <si>
+    <t>Ms. Anna Podobas</t>
+  </si>
+  <si>
+    <t>Mr. Cesar Roca</t>
+  </si>
+  <si>
+    <t>Mr. Ethan Miller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. Ashley Marvel </t>
+  </si>
+  <si>
+    <t>Mr. Kayse Chen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. Samatha Stephens </t>
+  </si>
+  <si>
+    <t>Mr. Cam Ebner</t>
+  </si>
+  <si>
+    <t>Mr. Michael Haluska</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. Kelly Regimbal </t>
+  </si>
+  <si>
+    <t>Table 12</t>
+  </si>
+  <si>
+    <t>Mr. Zachary Palfenier</t>
+  </si>
+  <si>
+    <t>Ms. Claire Chavez</t>
+  </si>
+  <si>
+    <t>Mr. Patrick Murphy</t>
+  </si>
+  <si>
+    <t>Ms. Margaret Lees</t>
+  </si>
+  <si>
+    <t>Mr. Christopher Naranjo</t>
+  </si>
+  <si>
+    <t>Ms. Helen Xu</t>
+  </si>
+  <si>
+    <t>Mrs. Allison Vander Heyden</t>
+  </si>
+  <si>
+    <t>Mr. Joseph Vander Heyden</t>
+  </si>
+  <si>
+    <t>Ms. Mi-Sun Bae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table 13 </t>
+  </si>
+  <si>
+    <t>Mrs. Bobbi Ensinger</t>
+  </si>
+  <si>
+    <t>Mr. Kevin Ensinger</t>
+  </si>
+  <si>
+    <t>Mr. Brett Zimmerman</t>
+  </si>
+  <si>
+    <t>Mr. Michael Jerman</t>
+  </si>
+  <si>
+    <t>Mr. Drew Stephens</t>
+  </si>
+  <si>
+    <t>Ms. Amanda Mueller</t>
+  </si>
+  <si>
+    <t>Mr. Christopher Blount (CB)</t>
+  </si>
+  <si>
+    <t>Mrs. Kaylea Blount</t>
+  </si>
+  <si>
+    <t>Mrs. Shannon Happ</t>
+  </si>
+  <si>
+    <t>Mr. Peter Happ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total # of chairs: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total # of veggie meals: </t>
   </si>
 </sst>
 </file>
@@ -1444,7 +1765,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1454,9 +1775,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AD212"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W84" sqref="W84"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AD11" sqref="AD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2395,6 +2716,9 @@
         <f t="shared" si="7"/>
         <v/>
       </c>
+      <c r="AD16" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="17" spans="1:27">
       <c r="A17" s="2" t="s">
@@ -10114,109 +10438,745 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:E134"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>312</v>
       </c>
-      <c r="B1" t="s">
-        <v>320</v>
-      </c>
-      <c r="C1" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="B1">
+        <v>7</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="E5" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="E6">
+        <f>B1+B10+B20+B29+B39+B50+B60+B71+B83+B93+B102+B113+B124</f>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="E8" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="E9">
+        <f>C1+C10+C20+C39+C50+C60+C71+C83+C93+C102+C113+C124</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
+        <v>320</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
         <v>321</v>
       </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
+    <row r="18" spans="1:3">
+      <c r="A18" s="8" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
+      <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="8" t="s">
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
         <v>331</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>333</v>
+      </c>
+      <c r="C24" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>334</v>
+      </c>
+      <c r="C25" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>338</v>
+      </c>
+      <c r="B29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>348</v>
+      </c>
+      <c r="B39">
+        <v>9</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>358</v>
+      </c>
+      <c r="B50">
+        <v>8</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>367</v>
+      </c>
+      <c r="B60">
+        <v>9</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>377</v>
+      </c>
+      <c r="B71">
+        <v>10</v>
+      </c>
+      <c r="C71">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>379</v>
+      </c>
+      <c r="C73" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>383</v>
+      </c>
+      <c r="C77" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>384</v>
+      </c>
+      <c r="C78" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
+        <v>389</v>
+      </c>
+      <c r="B83">
+        <v>8</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
+        <v>398</v>
+      </c>
+      <c r="B93">
+        <v>7</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="8" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" t="s">
+        <v>406</v>
+      </c>
+      <c r="B102">
+        <v>9</v>
+      </c>
+      <c r="C102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" t="s">
+        <v>412</v>
+      </c>
+      <c r="C108" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" t="s">
+        <v>416</v>
+      </c>
+      <c r="B113">
+        <v>9</v>
+      </c>
+      <c r="C113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" t="s">
+        <v>426</v>
+      </c>
+      <c r="B124">
+        <v>10</v>
+      </c>
+      <c r="C124">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" t="s">
+        <v>433</v>
+      </c>
+      <c r="C131" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" t="s">
+        <v>435</v>
+      </c>
+      <c r="C133" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" t="s">
+        <v>436</v>
+      </c>
+      <c r="C134" t="s">
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected angie to angela
</commit_message>
<xml_diff>
--- a/Guest_List_Invited.xlsx
+++ b/Guest_List_Invited.xlsx
@@ -1,18 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\logan\Documents\GitHub\Farrell_Garrett_Wedding\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A9D817F5-8971-476A-8591-B493535F3057}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Table #" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="162913" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -1015,9 +1021,6 @@
     <t>Mrs. Lannie Bluethmann</t>
   </si>
   <si>
-    <t>Mr. Bill Bluethmann</t>
-  </si>
-  <si>
     <t>Mr. Parker Francis</t>
   </si>
   <si>
@@ -1108,9 +1111,6 @@
     <t>Mr. Doug Klumpe</t>
   </si>
   <si>
-    <t>Mrs. Angie Klumpe</t>
-  </si>
-  <si>
     <t>Mrs. Lavon Sigler</t>
   </si>
   <si>
@@ -1337,17 +1337,23 @@
   </si>
   <si>
     <t xml:space="preserve">Total # of veggie meals: </t>
+  </si>
+  <si>
+    <t>Mr. William Bluethmann</t>
+  </si>
+  <si>
+    <t>Mrs. Angela Klumpe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1765,14 +1771,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD212"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
@@ -1780,7 +1786,7 @@
       <selection pane="bottomLeft" activeCell="AD11" sqref="AD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.85546875" customWidth="1"/>
     <col min="2" max="2" width="4" hidden="1" customWidth="1"/>
@@ -1806,7 +1812,7 @@
     <col min="27" max="27" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15" customHeight="1">
+    <row r="1" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5">
         <v>4</v>
       </c>
@@ -1826,7 +1832,7 @@
       <c r="U1" s="10"/>
       <c r="V1" s="10"/>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>3</v>
       </c>
@@ -1868,7 +1874,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1917,7 +1923,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="4" spans="1:30" s="10" customFormat="1" ht="31.5" customHeight="1">
+    <row r="4" spans="1:30" s="10" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -1987,7 +1993,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -2001,7 +2007,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2068,7 +2074,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:30">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2135,7 +2141,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2205,7 +2211,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -2275,7 +2281,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -2345,7 +2351,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -2423,7 +2429,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:30">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
       <c r="C12" s="1"/>
       <c r="D12">
@@ -2462,7 +2468,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="13" spans="1:30">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -2507,7 +2513,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="14" spans="1:30">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
@@ -2577,7 +2583,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="15" spans="1:30">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -2647,7 +2653,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="16" spans="1:30">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
@@ -2717,10 +2723,10 @@
         <v/>
       </c>
       <c r="AD16" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="17" spans="1:27">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
@@ -2787,7 +2793,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:27">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
@@ -2854,7 +2860,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:27">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>184</v>
       </c>
@@ -2924,7 +2930,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:27">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -2994,7 +3000,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:27">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
@@ -3061,7 +3067,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:27">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
@@ -3128,7 +3134,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:27">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>226</v>
       </c>
@@ -3198,7 +3204,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:27">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>17</v>
       </c>
@@ -3274,7 +3280,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="25" spans="1:27">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>18</v>
       </c>
@@ -3347,7 +3353,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="26" spans="1:27">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>19</v>
       </c>
@@ -3414,7 +3420,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:27">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>20</v>
       </c>
@@ -3481,7 +3487,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:27">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>21</v>
       </c>
@@ -3548,7 +3554,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:27">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>22</v>
       </c>
@@ -3615,7 +3621,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:27">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>23</v>
       </c>
@@ -3682,7 +3688,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:27">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>24</v>
       </c>
@@ -3755,7 +3761,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="32" spans="1:27">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>25</v>
       </c>
@@ -3822,7 +3828,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:27">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>26</v>
       </c>
@@ -3889,7 +3895,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:27">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
@@ -3962,7 +3968,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="35" spans="1:27">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
@@ -4029,7 +4035,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:27">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>257</v>
       </c>
@@ -4096,7 +4102,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:27">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>40</v>
       </c>
@@ -4163,7 +4169,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:27">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>41</v>
       </c>
@@ -4236,7 +4242,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="39" spans="1:27">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>42</v>
       </c>
@@ -4303,7 +4309,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:27">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>43</v>
       </c>
@@ -4379,7 +4385,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="41" spans="1:27">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>96</v>
       </c>
@@ -4449,7 +4455,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:27">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="7"/>
       <c r="D42">
@@ -4485,7 +4491,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:27">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B43" s="6"/>
       <c r="C43" s="1"/>
       <c r="D43">
@@ -4521,7 +4527,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:27">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>27</v>
       </c>
@@ -4563,7 +4569,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:27">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>28</v>
       </c>
@@ -4639,7 +4645,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="46" spans="1:27">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>29</v>
       </c>
@@ -4706,7 +4712,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:27">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>30</v>
       </c>
@@ -4773,7 +4779,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:27">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>31</v>
       </c>
@@ -4843,7 +4849,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:29">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>32</v>
       </c>
@@ -4913,7 +4919,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:29">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>227</v>
       </c>
@@ -4988,7 +4994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:29">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B51" s="6"/>
       <c r="J51">
         <f t="shared" si="9"/>
@@ -5019,7 +5025,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:29">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>48</v>
       </c>
@@ -5061,7 +5067,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:29">
+    <row r="53" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>47</v>
       </c>
@@ -5132,7 +5138,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:29">
+    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>307</v>
       </c>
@@ -5202,7 +5208,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:29">
+    <row r="55" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>49</v>
       </c>
@@ -5273,7 +5279,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:29">
+    <row r="56" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>73</v>
       </c>
@@ -5346,7 +5352,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="57" spans="1:29">
+    <row r="57" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>50</v>
       </c>
@@ -5416,7 +5422,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:29">
+    <row r="58" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>51</v>
       </c>
@@ -5486,7 +5492,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:29">
+    <row r="59" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>52</v>
       </c>
@@ -5553,7 +5559,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:29">
+    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B60" s="6"/>
       <c r="J60">
         <f t="shared" si="9"/>
@@ -5584,7 +5590,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:29">
+    <row r="61" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>46</v>
       </c>
@@ -5626,7 +5632,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:29">
+    <row r="62" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>218</v>
       </c>
@@ -5697,7 +5703,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:29">
+    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>262</v>
       </c>
@@ -5751,7 +5757,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="64" spans="1:29">
+    <row r="64" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>53</v>
       </c>
@@ -5822,7 +5828,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:27">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>290</v>
       </c>
@@ -5895,7 +5901,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:27">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>54</v>
       </c>
@@ -5966,7 +5972,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:27">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>163</v>
       </c>
@@ -6037,7 +6043,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:27">
+    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>187</v>
       </c>
@@ -6101,7 +6107,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="69" spans="1:27">
+    <row r="69" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>55</v>
       </c>
@@ -6172,7 +6178,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:27">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>252</v>
       </c>
@@ -6245,7 +6251,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:27">
+    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>56</v>
       </c>
@@ -6316,7 +6322,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:27">
+    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>57</v>
       </c>
@@ -6386,7 +6392,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:27">
+    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>58</v>
       </c>
@@ -6456,7 +6462,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:27">
+    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>59</v>
       </c>
@@ -6523,7 +6529,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:27">
+    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>60</v>
       </c>
@@ -6596,7 +6602,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="76" spans="1:27">
+    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>61</v>
       </c>
@@ -6669,7 +6675,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="77" spans="1:27">
+    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>62</v>
       </c>
@@ -6739,7 +6745,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:27">
+    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>162</v>
       </c>
@@ -6806,7 +6812,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:27">
+    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>64</v>
       </c>
@@ -6873,7 +6879,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="1:27">
+    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>123</v>
       </c>
@@ -6940,7 +6946,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:27">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>285</v>
       </c>
@@ -7007,7 +7013,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:27">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>63</v>
       </c>
@@ -7074,7 +7080,7 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:27">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>165</v>
       </c>
@@ -7147,7 +7153,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="84" spans="1:27">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>219</v>
       </c>
@@ -7217,7 +7223,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="1:27">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>245</v>
       </c>
@@ -7284,7 +7290,7 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="1:27">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>220</v>
       </c>
@@ -7351,7 +7357,7 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="1:27">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B87" s="6"/>
       <c r="J87">
         <f t="shared" si="20"/>
@@ -7382,7 +7388,7 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="1:27">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>69</v>
       </c>
@@ -7424,7 +7430,7 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="1:27">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>76</v>
       </c>
@@ -7491,7 +7497,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="1:27">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>70</v>
       </c>
@@ -7558,7 +7564,7 @@
         <v/>
       </c>
     </row>
-    <row r="91" spans="1:27">
+    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>130</v>
       </c>
@@ -7631,7 +7637,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="92" spans="1:27">
+    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>71</v>
       </c>
@@ -7698,7 +7704,7 @@
         <v/>
       </c>
     </row>
-    <row r="93" spans="1:27">
+    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>72</v>
       </c>
@@ -7771,7 +7777,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="94" spans="1:27">
+    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>153</v>
       </c>
@@ -7838,7 +7844,7 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="1:27">
+    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>150</v>
       </c>
@@ -7905,7 +7911,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="1:27">
+    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>154</v>
       </c>
@@ -7972,7 +7978,7 @@
         <v/>
       </c>
     </row>
-    <row r="97" spans="1:27">
+    <row r="97" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>116</v>
       </c>
@@ -8039,7 +8045,7 @@
         <v/>
       </c>
     </row>
-    <row r="98" spans="1:27">
+    <row r="98" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>131</v>
       </c>
@@ -8106,7 +8112,7 @@
         <v/>
       </c>
     </row>
-    <row r="99" spans="1:27">
+    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>74</v>
       </c>
@@ -8173,7 +8179,7 @@
         <v/>
       </c>
     </row>
-    <row r="100" spans="1:27">
+    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>155</v>
       </c>
@@ -8246,7 +8252,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="101" spans="1:27">
+    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>143</v>
       </c>
@@ -8313,7 +8319,7 @@
         <v/>
       </c>
     </row>
-    <row r="102" spans="1:27">
+    <row r="102" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>75</v>
       </c>
@@ -8386,7 +8392,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="103" spans="1:27">
+    <row r="103" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>147</v>
       </c>
@@ -8456,7 +8462,7 @@
         <v/>
       </c>
     </row>
-    <row r="104" spans="1:27">
+    <row r="104" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>148</v>
       </c>
@@ -8529,7 +8535,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="105" spans="1:27">
+    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>225</v>
       </c>
@@ -8587,7 +8593,7 @@
         <v/>
       </c>
     </row>
-    <row r="106" spans="1:27">
+    <row r="106" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>114</v>
       </c>
@@ -8645,7 +8651,7 @@
         <v/>
       </c>
     </row>
-    <row r="107" spans="1:27">
+    <row r="107" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>156</v>
       </c>
@@ -8700,7 +8706,7 @@
         <v/>
       </c>
     </row>
-    <row r="108" spans="1:27">
+    <row r="108" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>157</v>
       </c>
@@ -8755,7 +8761,7 @@
         <v/>
       </c>
     </row>
-    <row r="109" spans="1:27">
+    <row r="109" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>78</v>
       </c>
@@ -8810,7 +8816,7 @@
         <v/>
       </c>
     </row>
-    <row r="110" spans="1:27">
+    <row r="110" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>223</v>
       </c>
@@ -8871,7 +8877,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="111" spans="1:27">
+    <row r="111" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>222</v>
       </c>
@@ -8938,7 +8944,7 @@
         <v/>
       </c>
     </row>
-    <row r="112" spans="1:27">
+    <row r="112" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>224</v>
       </c>
@@ -9005,7 +9011,7 @@
         <v/>
       </c>
     </row>
-    <row r="113" spans="1:27">
+    <row r="113" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>77</v>
       </c>
@@ -9072,7 +9078,7 @@
         <v/>
       </c>
     </row>
-    <row r="114" spans="1:27">
+    <row r="114" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>221</v>
       </c>
@@ -9145,7 +9151,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="115" spans="1:27">
+    <row r="115" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B115" s="6"/>
       <c r="D115">
         <f t="shared" ref="D115:D116" si="29">IF(F115=4, 1,0)</f>
@@ -9180,7 +9186,7 @@
         <v/>
       </c>
     </row>
-    <row r="116" spans="1:27">
+    <row r="116" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>79</v>
       </c>
@@ -9222,7 +9228,7 @@
         <v/>
       </c>
     </row>
-    <row r="117" spans="1:27">
+    <row r="117" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>228</v>
       </c>
@@ -9292,7 +9298,7 @@
         <v/>
       </c>
     </row>
-    <row r="118" spans="1:27">
+    <row r="118" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>80</v>
       </c>
@@ -9359,7 +9365,7 @@
         <v/>
       </c>
     </row>
-    <row r="119" spans="1:27">
+    <row r="119" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>229</v>
       </c>
@@ -9426,7 +9432,7 @@
         <v/>
       </c>
     </row>
-    <row r="120" spans="1:27">
+    <row r="120" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>81</v>
       </c>
@@ -9493,7 +9499,7 @@
         <v/>
       </c>
     </row>
-    <row r="121" spans="1:27">
+    <row r="121" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>82</v>
       </c>
@@ -9560,7 +9566,7 @@
         <v/>
       </c>
     </row>
-    <row r="122" spans="1:27">
+    <row r="122" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>230</v>
       </c>
@@ -9630,7 +9636,7 @@
         <v/>
       </c>
     </row>
-    <row r="123" spans="1:27">
+    <row r="123" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>231</v>
       </c>
@@ -9700,7 +9706,7 @@
         <v/>
       </c>
     </row>
-    <row r="124" spans="1:27">
+    <row r="124" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>232</v>
       </c>
@@ -9773,7 +9779,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="125" spans="1:27">
+    <row r="125" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>233</v>
       </c>
@@ -9843,7 +9849,7 @@
         <v/>
       </c>
     </row>
-    <row r="126" spans="1:27">
+    <row r="126" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B126" s="6"/>
       <c r="J126">
         <f t="shared" si="20"/>
@@ -9862,7 +9868,7 @@
         <v/>
       </c>
     </row>
-    <row r="127" spans="1:27">
+    <row r="127" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>204</v>
       </c>
@@ -9884,7 +9890,7 @@
         <v/>
       </c>
     </row>
-    <row r="128" spans="1:27">
+    <row r="128" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>254</v>
       </c>
@@ -9921,7 +9927,7 @@
         <v/>
       </c>
     </row>
-    <row r="129" spans="1:25">
+    <row r="129" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>205</v>
       </c>
@@ -9958,7 +9964,7 @@
         <v/>
       </c>
     </row>
-    <row r="130" spans="1:25">
+    <row r="130" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>206</v>
       </c>
@@ -9995,7 +10001,7 @@
         <v/>
       </c>
     </row>
-    <row r="131" spans="1:25">
+    <row r="131" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>255</v>
       </c>
@@ -10028,7 +10034,7 @@
         <v/>
       </c>
     </row>
-    <row r="132" spans="1:25">
+    <row r="132" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>293</v>
       </c>
@@ -10037,13 +10043,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:25">
+    <row r="133" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B133" s="6"/>
     </row>
-    <row r="134" spans="1:25">
+    <row r="134" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B134" s="6"/>
     </row>
-    <row r="135" spans="1:25">
+    <row r="135" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B135" s="6"/>
       <c r="P135" t="s">
         <v>282</v>
@@ -10056,7 +10062,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="136" spans="1:25">
+    <row r="136" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B136" s="6"/>
       <c r="P136" t="s">
         <v>284</v>
@@ -10065,7 +10071,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="137" spans="1:25">
+    <row r="137" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B137" s="6"/>
       <c r="P137" t="s">
         <v>266</v>
@@ -10074,7 +10080,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="1:25">
+    <row r="138" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B138" s="6"/>
       <c r="P138" t="s">
         <v>47</v>
@@ -10083,7 +10089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:25">
+    <row r="139" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B139" s="6"/>
       <c r="P139" t="s">
         <v>267</v>
@@ -10092,7 +10098,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="1:25">
+    <row r="140" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B140" s="6"/>
       <c r="P140" t="s">
         <v>268</v>
@@ -10101,7 +10107,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="1:25">
+    <row r="141" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B141" s="6"/>
       <c r="P141" t="s">
         <v>49</v>
@@ -10110,7 +10116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:25">
+    <row r="142" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B142" s="6"/>
       <c r="P142" t="s">
         <v>7</v>
@@ -10119,10 +10125,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="1:25">
+    <row r="143" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B143" s="6"/>
     </row>
-    <row r="144" spans="1:25">
+    <row r="144" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B144" s="6"/>
       <c r="P144" t="s">
         <v>269</v>
@@ -10131,7 +10137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="2:23">
+    <row r="145" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B145" s="6"/>
       <c r="P145" t="s">
         <v>51</v>
@@ -10140,7 +10146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="2:23">
+    <row r="146" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B146" s="6"/>
       <c r="P146" t="s">
         <v>270</v>
@@ -10152,7 +10158,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="147" spans="2:23">
+    <row r="147" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B147" s="6"/>
       <c r="P147" t="s">
         <v>271</v>
@@ -10161,7 +10167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="2:23">
+    <row r="148" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B148" s="6"/>
       <c r="P148" t="s">
         <v>272</v>
@@ -10170,10 +10176,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="2:23">
+    <row r="149" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B149" s="6"/>
     </row>
-    <row r="150" spans="2:23">
+    <row r="150" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B150" s="6"/>
       <c r="P150" t="s">
         <v>273</v>
@@ -10182,7 +10188,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="2:23">
+    <row r="151" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B151" s="6"/>
       <c r="P151" t="s">
         <v>274</v>
@@ -10191,7 +10197,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="152" spans="2:23">
+    <row r="152" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B152" s="6"/>
       <c r="P152" t="s">
         <v>275</v>
@@ -10200,7 +10206,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="153" spans="2:23">
+    <row r="153" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B153" s="6"/>
       <c r="P153" t="s">
         <v>276</v>
@@ -10209,10 +10215,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="2:23">
+    <row r="154" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B154" s="6"/>
     </row>
-    <row r="155" spans="2:23">
+    <row r="155" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B155" s="6"/>
       <c r="P155" t="s">
         <v>277</v>
@@ -10221,7 +10227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="2:23">
+    <row r="156" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B156" s="6"/>
       <c r="P156" t="s">
         <v>278</v>
@@ -10230,10 +10236,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="157" spans="2:23">
+    <row r="157" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B157" s="6"/>
     </row>
-    <row r="158" spans="2:23">
+    <row r="158" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B158" s="6"/>
       <c r="P158" t="s">
         <v>279</v>
@@ -10242,19 +10248,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="2:23">
+    <row r="159" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B159" s="6"/>
       <c r="P159" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="160" spans="2:23">
+    <row r="160" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B160" s="6"/>
       <c r="P160" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="161" spans="2:17">
+    <row r="161" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B161" s="6"/>
       <c r="P161" t="s">
         <v>309</v>
@@ -10263,157 +10269,157 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="2:17">
+    <row r="162" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B162" s="6"/>
     </row>
-    <row r="163" spans="2:17">
+    <row r="163" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B163" s="6"/>
     </row>
-    <row r="164" spans="2:17">
+    <row r="164" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B164" s="6"/>
     </row>
-    <row r="165" spans="2:17">
+    <row r="165" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B165" s="6"/>
     </row>
-    <row r="166" spans="2:17">
+    <row r="166" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B166" s="6"/>
     </row>
-    <row r="167" spans="2:17">
+    <row r="167" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B167" s="6"/>
     </row>
-    <row r="168" spans="2:17">
+    <row r="168" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B168" s="6"/>
     </row>
-    <row r="169" spans="2:17">
+    <row r="169" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B169" s="6"/>
     </row>
-    <row r="170" spans="2:17">
+    <row r="170" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B170" s="6"/>
     </row>
-    <row r="171" spans="2:17">
+    <row r="171" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B171" s="6"/>
     </row>
-    <row r="172" spans="2:17">
+    <row r="172" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B172" s="6"/>
     </row>
-    <row r="173" spans="2:17">
+    <row r="173" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B173" s="6"/>
     </row>
-    <row r="174" spans="2:17">
+    <row r="174" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B174" s="6"/>
     </row>
-    <row r="175" spans="2:17">
+    <row r="175" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B175" s="6"/>
     </row>
-    <row r="176" spans="2:17">
+    <row r="176" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B176" s="6"/>
     </row>
-    <row r="177" spans="2:2">
+    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B177" s="6"/>
     </row>
-    <row r="178" spans="2:2">
+    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B178" s="6"/>
     </row>
-    <row r="179" spans="2:2">
+    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B179" s="6"/>
     </row>
-    <row r="180" spans="2:2">
+    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B180" s="6"/>
     </row>
-    <row r="181" spans="2:2">
+    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B181" s="6"/>
     </row>
-    <row r="182" spans="2:2">
+    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B182" s="6"/>
     </row>
-    <row r="183" spans="2:2">
+    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B183" s="6"/>
     </row>
-    <row r="184" spans="2:2">
+    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B184" s="6"/>
     </row>
-    <row r="185" spans="2:2">
+    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B185" s="6"/>
     </row>
-    <row r="186" spans="2:2">
+    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B186" s="6"/>
     </row>
-    <row r="187" spans="2:2">
+    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B187" s="6"/>
     </row>
-    <row r="188" spans="2:2">
+    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B188" s="6"/>
     </row>
-    <row r="189" spans="2:2">
+    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B189" s="6"/>
     </row>
-    <row r="190" spans="2:2">
+    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B190" s="6"/>
     </row>
-    <row r="191" spans="2:2">
+    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B191" s="6"/>
     </row>
-    <row r="192" spans="2:2">
+    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B192" s="6"/>
     </row>
-    <row r="193" spans="2:2">
+    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B193" s="6"/>
     </row>
-    <row r="194" spans="2:2">
+    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B194" s="6"/>
     </row>
-    <row r="195" spans="2:2">
+    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B195" s="6"/>
     </row>
-    <row r="196" spans="2:2">
+    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B196" s="6"/>
     </row>
-    <row r="197" spans="2:2">
+    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B197" s="6"/>
     </row>
-    <row r="198" spans="2:2">
+    <row r="198" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B198" s="6"/>
     </row>
-    <row r="199" spans="2:2">
+    <row r="199" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B199" s="6"/>
     </row>
-    <row r="200" spans="2:2">
+    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B200" s="6"/>
     </row>
-    <row r="201" spans="2:2">
+    <row r="201" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B201" s="6"/>
     </row>
-    <row r="202" spans="2:2">
+    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B202" s="6"/>
     </row>
-    <row r="203" spans="2:2">
+    <row r="203" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B203" s="6"/>
     </row>
-    <row r="204" spans="2:2">
+    <row r="204" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B204" s="6"/>
     </row>
-    <row r="205" spans="2:2">
+    <row r="205" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B205" s="6"/>
     </row>
-    <row r="206" spans="2:2">
+    <row r="206" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B206" s="6"/>
     </row>
-    <row r="207" spans="2:2">
+    <row r="207" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B207" s="6"/>
     </row>
-    <row r="208" spans="2:2">
+    <row r="208" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B208" s="6"/>
     </row>
-    <row r="209" spans="2:2">
+    <row r="209" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B209" s="6"/>
     </row>
-    <row r="210" spans="2:2">
+    <row r="210" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B210" s="6"/>
     </row>
-    <row r="211" spans="2:2">
+    <row r="211" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B211" s="6"/>
     </row>
-    <row r="212" spans="2:2">
+    <row r="212" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B212" s="6"/>
     </row>
   </sheetData>
@@ -10437,21 +10443,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>312</v>
       </c>
@@ -10462,30 +10468,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>316</v>
       </c>
       <c r="E5" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>317</v>
       </c>
@@ -10494,26 +10500,26 @@
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>319</v>
       </c>
       <c r="E8" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E9">
         <f>C1+C10+C20+C39+C50+C60+C71+C83+C93+C102+C113+C124</f>
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>320</v>
       </c>
@@ -10524,47 +10530,47 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>329</v>
       </c>
@@ -10575,98 +10581,98 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
+      <c r="C24" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>333</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>334</v>
-      </c>
-      <c r="C25" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>337</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
-        <v>338</v>
       </c>
       <c r="B29">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>347</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" t="s">
-        <v>348</v>
       </c>
       <c r="B39">
         <v>9</v>
@@ -10675,54 +10681,54 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
-      <c r="A41" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
-      <c r="A42" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
-      <c r="A43" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
-      <c r="A44" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
-      <c r="A45" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
-      <c r="A46" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
-      <c r="A47" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
-      <c r="A48" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>357</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" t="s">
-        <v>358</v>
       </c>
       <c r="B50">
         <v>8</v>
@@ -10731,49 +10737,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
-      <c r="A52" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
-      <c r="A53" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
-      <c r="A54" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
-      <c r="A55" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
-      <c r="A56" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
-      <c r="A57" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>365</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" t="s">
-        <v>367</v>
       </c>
       <c r="B60">
         <v>9</v>
@@ -10782,54 +10788,54 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
-      <c r="A62" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
-      <c r="A63" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
-      <c r="A64" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
-      <c r="A65" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
-      <c r="A66" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
-      <c r="A67" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
-      <c r="A68" t="s">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>375</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" t="s">
-        <v>377</v>
       </c>
       <c r="B71">
         <v>10</v>
@@ -10838,68 +10844,68 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C73" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
-      <c r="A75" t="s">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>381</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77" t="s">
-        <v>383</v>
       </c>
       <c r="C77" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>382</v>
+      </c>
+      <c r="C78" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>384</v>
       </c>
-      <c r="C78" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" t="s">
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
-      <c r="A80" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" t="s">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>387</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83" t="s">
-        <v>389</v>
       </c>
       <c r="B83">
         <v>8</v>
@@ -10908,49 +10914,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
-      <c r="A85" t="s">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
-      <c r="A86" t="s">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
-      <c r="A87" t="s">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
-      <c r="A88" t="s">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
-      <c r="A89" t="s">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
-      <c r="A90" t="s">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>396</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3">
-      <c r="A91" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3">
-      <c r="A93" t="s">
-        <v>398</v>
       </c>
       <c r="B93">
         <v>7</v>
@@ -10959,44 +10965,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="8" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
-      <c r="A95" t="s">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
-      <c r="A96" s="8" t="s">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
-      <c r="A97" t="s">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
-      <c r="A98" t="s">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
-      <c r="A99" t="s">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>404</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3">
-      <c r="A100" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3">
-      <c r="A102" t="s">
-        <v>406</v>
       </c>
       <c r="B102">
         <v>9</v>
@@ -11005,57 +11011,57 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
-      <c r="A104" t="s">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
-      <c r="A105" t="s">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
-      <c r="A106" t="s">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>410</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3">
-      <c r="A107" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3">
-      <c r="A108" t="s">
-        <v>412</v>
       </c>
       <c r="C108" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
-      <c r="A110" t="s">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>414</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3">
-      <c r="A111" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3">
-      <c r="A113" t="s">
-        <v>416</v>
       </c>
       <c r="B113">
         <v>9</v>
@@ -11064,54 +11070,54 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="115" spans="1:3">
-      <c r="A115" t="s">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="116" spans="1:3">
-      <c r="A116" t="s">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="117" spans="1:3">
-      <c r="A117" t="s">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="118" spans="1:3">
-      <c r="A118" t="s">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="119" spans="1:3">
-      <c r="A119" t="s">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="120" spans="1:3">
-      <c r="A120" t="s">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="121" spans="1:3">
-      <c r="A121" t="s">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>424</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3">
-      <c r="A122" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3">
-      <c r="A124" t="s">
-        <v>426</v>
       </c>
       <c r="B124">
         <v>10</v>
@@ -11120,60 +11126,60 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="126" spans="1:3">
-      <c r="A126" t="s">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="127" spans="1:3">
-      <c r="A127" t="s">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="128" spans="1:3">
-      <c r="A128" t="s">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="129" spans="1:3">
-      <c r="A129" t="s">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
         <v>431</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3">
-      <c r="A130" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3">
-      <c r="A131" t="s">
-        <v>433</v>
       </c>
       <c r="C131" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="132" spans="1:3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C133" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="134" spans="1:3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C134" t="s">
         <v>242</v>

</xml_diff>

<commit_message>
updated with thank yous
</commit_message>
<xml_diff>
--- a/Guest_List_Invited.xlsx
+++ b/Guest_List_Invited.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\logan\Documents\GitHub\Farrell_Garrett_Wedding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AAD4E4-713D-432D-8EEC-DFF8F51D09AD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43105037-3FEF-4D60-BF1A-E097BAF603B8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="457">
   <si>
     <t xml:space="preserve">Priority </t>
   </si>
@@ -916,9 +916,6 @@
     <t>Will be at wedding but not at reception</t>
   </si>
   <si>
-    <t>$25 for hotel on honeymoon</t>
-  </si>
-  <si>
     <t>Comferter and sheets</t>
   </si>
   <si>
@@ -1351,12 +1348,6 @@
     <t>Target gift card $15</t>
   </si>
   <si>
-    <t xml:space="preserve">no </t>
-  </si>
-  <si>
-    <t>9 small plates</t>
-  </si>
-  <si>
     <t xml:space="preserve">check to make sure there was nothing else </t>
   </si>
   <si>
@@ -1372,10 +1363,40 @@
     <t>songs of solomon sign</t>
   </si>
   <si>
-    <t xml:space="preserve">bathroom can and toothbrush holder </t>
-  </si>
-  <si>
     <t>bunches of plates and mugs</t>
+  </si>
+  <si>
+    <t>$50 for accomodations</t>
+  </si>
+  <si>
+    <t>$100 for accomodations (also from Brian)</t>
+  </si>
+  <si>
+    <t>$150 for accomodations</t>
+  </si>
+  <si>
+    <t>$200 for spa day/golf</t>
+  </si>
+  <si>
+    <t>$80 for golf/spa day</t>
+  </si>
+  <si>
+    <t>bathroom can and toothbrush holder, $40 for spa day</t>
+  </si>
+  <si>
+    <t>$100 for accomodations</t>
+  </si>
+  <si>
+    <t>$100 for hotel, golf/spa, flight, plus extra</t>
+  </si>
+  <si>
+    <t>$50 for hotel on honeymoon ($25 for bridal shower, $25 for wedding)</t>
+  </si>
+  <si>
+    <t>2 sets of silverware</t>
+  </si>
+  <si>
+    <t>9 small plates, 3 rice bowls</t>
   </si>
 </sst>
 </file>
@@ -1474,7 +1495,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1504,12 +1525,17 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1814,9 +1840,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD212"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W50" sqref="W50"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I77" sqref="I77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1839,7 +1865,7 @@
     <col min="20" max="20" width="10.85546875" hidden="1" customWidth="1"/>
     <col min="21" max="21" width="11" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="11.85546875" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="24.140625" customWidth="1"/>
+    <col min="23" max="23" width="44.7109375" style="12" bestFit="1" customWidth="1"/>
     <col min="24" max="25" width="0" hidden="1" customWidth="1"/>
     <col min="26" max="26" width="13.85546875" hidden="1" customWidth="1"/>
     <col min="27" max="27" width="10" bestFit="1" customWidth="1"/>
@@ -1850,10 +1876,10 @@
         <v>4</v>
       </c>
       <c r="B1" s="15"/>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="21"/>
+      <c r="E1" s="20"/>
       <c r="F1" t="s">
         <v>68</v>
       </c>
@@ -1870,15 +1896,15 @@
         <v>3</v>
       </c>
       <c r="B2" s="6"/>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="19" t="s">
         <v>207</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="G2" s="20" t="s">
+      <c r="E2" s="19"/>
+      <c r="G2" s="19" t="s">
         <v>208</v>
       </c>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
       <c r="J2" s="11"/>
       <c r="K2" s="11"/>
       <c r="P2" t="s">
@@ -1915,11 +1941,11 @@
       <c r="C3" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="20">
+      <c r="D3" s="19">
         <f>SUM(E6:E132)-E13-E44-E52-E61-E88-E116-E127</f>
         <v>114</v>
       </c>
-      <c r="E3" s="20"/>
+      <c r="E3" s="19"/>
       <c r="F3">
         <f>SUM(J6:J174)</f>
         <v>217</v>
@@ -2012,7 +2038,7 @@
       <c r="V4" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="W4" s="10" t="s">
+      <c r="W4" s="21" t="s">
         <v>238</v>
       </c>
       <c r="Y4" s="10" t="s">
@@ -2232,6 +2258,9 @@
       <c r="U8" t="s">
         <v>146</v>
       </c>
+      <c r="W8" s="12" t="s">
+        <v>455</v>
+      </c>
       <c r="X8">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2240,8 +2269,11 @@
         <f t="shared" si="7"/>
         <v/>
       </c>
+      <c r="AA8" t="s">
+        <v>438</v>
+      </c>
       <c r="AD8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
@@ -2311,7 +2343,7 @@
         <v/>
       </c>
       <c r="AD9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
@@ -2381,7 +2413,7 @@
         <v/>
       </c>
       <c r="AD10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
@@ -2444,8 +2476,8 @@
       <c r="U11" t="s">
         <v>146</v>
       </c>
-      <c r="W11" t="s">
-        <v>296</v>
+      <c r="W11" s="12" t="s">
+        <v>454</v>
       </c>
       <c r="X11">
         <f t="shared" si="1"/>
@@ -2498,7 +2530,7 @@
         <v/>
       </c>
       <c r="AD12" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
@@ -2543,7 +2575,7 @@
         <v/>
       </c>
       <c r="AD13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
@@ -2604,7 +2636,7 @@
       <c r="U14" t="s">
         <v>146</v>
       </c>
-      <c r="W14" s="19">
+      <c r="W14" s="22">
         <v>100</v>
       </c>
       <c r="X14">
@@ -2616,10 +2648,10 @@
         <v/>
       </c>
       <c r="AA14" t="s">
-        <v>439</v>
+        <v>248</v>
       </c>
       <c r="AD14" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
@@ -2689,7 +2721,7 @@
         <v/>
       </c>
       <c r="AD15" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
@@ -2762,7 +2794,7 @@
         <v/>
       </c>
       <c r="AD16" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
@@ -3304,7 +3336,7 @@
       <c r="U24" t="s">
         <v>146</v>
       </c>
-      <c r="W24" s="19">
+      <c r="W24" s="22">
         <v>50</v>
       </c>
       <c r="X24">
@@ -3316,7 +3348,7 @@
         <v/>
       </c>
       <c r="AA24" t="s">
-        <v>439</v>
+        <v>248</v>
       </c>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
@@ -3377,7 +3409,7 @@
       <c r="U25" t="s">
         <v>146</v>
       </c>
-      <c r="W25" t="s">
+      <c r="W25" s="12" t="s">
         <v>247</v>
       </c>
       <c r="X25">
@@ -3785,8 +3817,8 @@
       <c r="U31" t="s">
         <v>146</v>
       </c>
-      <c r="W31" t="s">
-        <v>298</v>
+      <c r="W31" s="12" t="s">
+        <v>297</v>
       </c>
       <c r="X31">
         <f t="shared" si="10"/>
@@ -3992,7 +4024,7 @@
       <c r="U34" t="s">
         <v>146</v>
       </c>
-      <c r="W34" t="s">
+      <c r="W34" s="12" t="s">
         <v>243</v>
       </c>
       <c r="X34">
@@ -4065,8 +4097,8 @@
       <c r="U35" t="s">
         <v>146</v>
       </c>
-      <c r="W35" t="s">
-        <v>446</v>
+      <c r="W35" s="12" t="s">
+        <v>443</v>
       </c>
       <c r="X35">
         <f t="shared" si="10"/>
@@ -4269,7 +4301,7 @@
       <c r="U38" t="s">
         <v>146</v>
       </c>
-      <c r="W38" t="s">
+      <c r="W38" s="12" t="s">
         <v>244</v>
       </c>
       <c r="X38">
@@ -4342,8 +4374,8 @@
       <c r="U39" t="s">
         <v>146</v>
       </c>
-      <c r="W39" t="s">
-        <v>442</v>
+      <c r="W39" s="12" t="s">
+        <v>456</v>
       </c>
       <c r="X39">
         <f t="shared" si="10"/>
@@ -4354,10 +4386,10 @@
         <v/>
       </c>
       <c r="AA39" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="AB39" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.25">
@@ -4421,8 +4453,8 @@
       <c r="U40" t="s">
         <v>146</v>
       </c>
-      <c r="W40" t="s">
-        <v>310</v>
+      <c r="W40" s="12" t="s">
+        <v>309</v>
       </c>
       <c r="X40">
         <f t="shared" si="10"/>
@@ -4496,6 +4528,9 @@
       </c>
       <c r="U41" t="s">
         <v>146</v>
+      </c>
+      <c r="W41" s="22">
+        <v>50</v>
       </c>
       <c r="X41">
         <f>IF(ISNUMBER(E41),1,0)</f>
@@ -4681,7 +4716,7 @@
       <c r="U45" t="s">
         <v>146</v>
       </c>
-      <c r="W45" t="s">
+      <c r="W45" s="12" t="s">
         <v>246</v>
       </c>
       <c r="X45">
@@ -4961,8 +4996,8 @@
       <c r="U49" t="s">
         <v>146</v>
       </c>
-      <c r="W49" t="s">
-        <v>449</v>
+      <c r="W49" s="12" t="s">
+        <v>445</v>
       </c>
       <c r="X49">
         <f t="shared" si="11"/>
@@ -4973,7 +5008,7 @@
         <v/>
       </c>
       <c r="AA49" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="50" spans="1:29" x14ac:dyDescent="0.25">
@@ -5039,7 +5074,7 @@
       <c r="U50" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="W50" s="19">
+      <c r="W50" s="22">
         <v>100</v>
       </c>
       <c r="X50">
@@ -5051,7 +5086,7 @@
         <v/>
       </c>
       <c r="AA50" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="AC50">
         <v>1</v>
@@ -5203,7 +5238,7 @@
     </row>
     <row r="54" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B54" s="6">
         <v>42</v>
@@ -5262,7 +5297,7 @@
       <c r="U54" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="W54" s="19">
+      <c r="W54" s="22">
         <v>50</v>
       </c>
       <c r="X54">
@@ -5274,7 +5309,7 @@
         <v/>
       </c>
       <c r="AA54" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="55" spans="1:29" x14ac:dyDescent="0.25">
@@ -5406,7 +5441,7 @@
       <c r="U56" t="s">
         <v>146</v>
       </c>
-      <c r="W56" t="s">
+      <c r="W56" s="12" t="s">
         <v>260</v>
       </c>
       <c r="X56">
@@ -5763,7 +5798,7 @@
         <v>146</v>
       </c>
       <c r="V62" s="6"/>
-      <c r="W62" s="19">
+      <c r="W62" s="22">
         <v>100</v>
       </c>
       <c r="X62">
@@ -5775,7 +5810,7 @@
         <v/>
       </c>
       <c r="AA62" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="63" spans="1:29" x14ac:dyDescent="0.25">
@@ -5821,7 +5856,7 @@
       <c r="T63" s="6"/>
       <c r="U63" s="6"/>
       <c r="V63" s="6"/>
-      <c r="W63" t="s">
+      <c r="W63" s="12" t="s">
         <v>261</v>
       </c>
       <c r="Y63" t="str">
@@ -6109,7 +6144,7 @@
         <v>146</v>
       </c>
       <c r="V67" s="6"/>
-      <c r="W67" s="19">
+      <c r="W67" s="22">
         <v>100</v>
       </c>
       <c r="X67">
@@ -6121,7 +6156,7 @@
         <v/>
       </c>
       <c r="AA67" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="68" spans="1:27" x14ac:dyDescent="0.25">
@@ -6173,7 +6208,7 @@
         <v>146</v>
       </c>
       <c r="V68" s="6"/>
-      <c r="W68" t="s">
+      <c r="W68" s="12" t="s">
         <v>258</v>
       </c>
       <c r="X68">
@@ -6394,7 +6429,7 @@
         <v>146</v>
       </c>
       <c r="V71" s="6"/>
-      <c r="W71" s="19">
+      <c r="W71" s="22">
         <v>150</v>
       </c>
       <c r="X71">
@@ -6406,7 +6441,7 @@
         <v/>
       </c>
       <c r="AA71" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="72" spans="1:27" x14ac:dyDescent="0.25">
@@ -6470,6 +6505,9 @@
       <c r="V72" t="s">
         <v>146</v>
       </c>
+      <c r="W72" s="12" t="s">
+        <v>446</v>
+      </c>
       <c r="X72">
         <f t="shared" si="13"/>
         <v>1</v>
@@ -6477,6 +6515,9 @@
       <c r="Y72" t="str">
         <f t="shared" si="19"/>
         <v/>
+      </c>
+      <c r="AA72" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="73" spans="1:27" x14ac:dyDescent="0.25">
@@ -6607,7 +6648,7 @@
       <c r="U74" t="s">
         <v>146</v>
       </c>
-      <c r="W74" s="19">
+      <c r="W74" s="22">
         <v>100</v>
       </c>
       <c r="X74">
@@ -6619,7 +6660,7 @@
         <v/>
       </c>
       <c r="AA74" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="75" spans="1:27" x14ac:dyDescent="0.25">
@@ -6680,7 +6721,7 @@
       <c r="U75" t="s">
         <v>146</v>
       </c>
-      <c r="W75" t="s">
+      <c r="W75" s="12" t="s">
         <v>258</v>
       </c>
       <c r="X75">
@@ -6753,7 +6794,7 @@
       <c r="U76" t="s">
         <v>146</v>
       </c>
-      <c r="W76" t="s">
+      <c r="W76" s="12" t="s">
         <v>294</v>
       </c>
       <c r="X76">
@@ -6829,7 +6870,7 @@
       <c r="V77" t="s">
         <v>146</v>
       </c>
-      <c r="W77" s="19">
+      <c r="W77" s="22">
         <v>50</v>
       </c>
       <c r="X77">
@@ -6841,7 +6882,7 @@
         <v/>
       </c>
       <c r="AA77" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="78" spans="1:27" x14ac:dyDescent="0.25">
@@ -6969,6 +7010,9 @@
       <c r="U79" t="s">
         <v>146</v>
       </c>
+      <c r="W79" s="12" t="s">
+        <v>452</v>
+      </c>
       <c r="X79">
         <f t="shared" si="13"/>
         <v>1</v>
@@ -6976,6 +7020,9 @@
       <c r="Y79" t="str">
         <f t="shared" si="19"/>
         <v/>
+      </c>
+      <c r="AA79" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="80" spans="1:27" x14ac:dyDescent="0.25">
@@ -7103,8 +7150,8 @@
       <c r="U81" t="s">
         <v>146</v>
       </c>
-      <c r="W81" t="s">
-        <v>440</v>
+      <c r="W81" s="12" t="s">
+        <v>439</v>
       </c>
       <c r="X81">
         <f t="shared" si="13"/>
@@ -7115,7 +7162,7 @@
         <v/>
       </c>
       <c r="AA81" t="s">
-        <v>441</v>
+        <v>242</v>
       </c>
     </row>
     <row r="82" spans="1:27" x14ac:dyDescent="0.25">
@@ -7176,6 +7223,9 @@
       <c r="U82" s="6" t="s">
         <v>146</v>
       </c>
+      <c r="W82" s="12" t="s">
+        <v>447</v>
+      </c>
       <c r="X82">
         <f t="shared" si="13"/>
         <v>1</v>
@@ -7183,6 +7233,9 @@
       <c r="Y82" t="str">
         <f t="shared" si="19"/>
         <v/>
+      </c>
+      <c r="AA82" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="83" spans="1:27" x14ac:dyDescent="0.25">
@@ -7243,8 +7296,8 @@
       <c r="U83" t="s">
         <v>146</v>
       </c>
-      <c r="W83" t="s">
-        <v>311</v>
+      <c r="W83" s="12" t="s">
+        <v>310</v>
       </c>
       <c r="X83">
         <f t="shared" si="13"/>
@@ -7319,8 +7372,8 @@
       <c r="U84" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="W84" t="s">
-        <v>444</v>
+      <c r="W84" s="12" t="s">
+        <v>441</v>
       </c>
       <c r="X84">
         <f t="shared" si="13"/>
@@ -7331,7 +7384,7 @@
         <v/>
       </c>
       <c r="AA84" t="s">
-        <v>439</v>
+        <v>248</v>
       </c>
     </row>
     <row r="85" spans="1:27" x14ac:dyDescent="0.25">
@@ -7459,6 +7512,9 @@
       <c r="U86" t="s">
         <v>146</v>
       </c>
+      <c r="W86" s="12" t="s">
+        <v>446</v>
+      </c>
       <c r="X86">
         <f t="shared" si="13"/>
         <v>1</v>
@@ -7466,6 +7522,9 @@
       <c r="Y86" t="str">
         <f t="shared" si="19"/>
         <v/>
+      </c>
+      <c r="AA86" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="87" spans="1:27" x14ac:dyDescent="0.25">
@@ -7599,6 +7658,9 @@
       <c r="U89" t="s">
         <v>146</v>
       </c>
+      <c r="W89" s="22">
+        <v>150</v>
+      </c>
       <c r="X89">
         <f t="shared" ref="X89:X114" si="24">IF(ISNUMBER(E89),1,0)</f>
         <v>1</v>
@@ -7606,6 +7668,9 @@
       <c r="Y89" t="str">
         <f t="shared" si="19"/>
         <v/>
+      </c>
+      <c r="AA89" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="90" spans="1:27" x14ac:dyDescent="0.25">
@@ -7666,6 +7731,9 @@
       <c r="U90" t="s">
         <v>146</v>
       </c>
+      <c r="W90" s="12" t="s">
+        <v>450</v>
+      </c>
       <c r="X90">
         <f t="shared" si="24"/>
         <v>1</v>
@@ -7673,6 +7741,9 @@
       <c r="Y90" t="str">
         <f t="shared" si="19"/>
         <v/>
+      </c>
+      <c r="AA90" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="91" spans="1:27" x14ac:dyDescent="0.25">
@@ -7733,7 +7804,7 @@
       <c r="U91" t="s">
         <v>146</v>
       </c>
-      <c r="W91" t="s">
+      <c r="W91" s="12" t="s">
         <v>261</v>
       </c>
       <c r="X91">
@@ -7806,7 +7877,7 @@
       <c r="U92" t="s">
         <v>146</v>
       </c>
-      <c r="W92" s="19">
+      <c r="W92" s="22">
         <v>100</v>
       </c>
       <c r="X92">
@@ -7818,7 +7889,7 @@
         <v/>
       </c>
       <c r="AA92" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="93" spans="1:27" x14ac:dyDescent="0.25">
@@ -7879,7 +7950,7 @@
       <c r="U93" t="s">
         <v>146</v>
       </c>
-      <c r="W93" t="s">
+      <c r="W93" s="12" t="s">
         <v>241</v>
       </c>
       <c r="X93">
@@ -7952,6 +8023,9 @@
       <c r="U94" t="s">
         <v>146</v>
       </c>
+      <c r="W94" s="12" t="s">
+        <v>448</v>
+      </c>
       <c r="X94">
         <f t="shared" si="24"/>
         <v>1</v>
@@ -7959,6 +8033,9 @@
       <c r="Y94" t="str">
         <f t="shared" si="19"/>
         <v/>
+      </c>
+      <c r="AA94" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="95" spans="1:27" x14ac:dyDescent="0.25">
@@ -8086,6 +8163,9 @@
       <c r="U96" t="s">
         <v>146</v>
       </c>
+      <c r="W96" s="12" t="s">
+        <v>289</v>
+      </c>
       <c r="X96">
         <f t="shared" si="24"/>
         <v>1</v>
@@ -8093,6 +8173,9 @@
       <c r="Y96" t="str">
         <f t="shared" si="19"/>
         <v/>
+      </c>
+      <c r="AA96" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="97" spans="1:27" x14ac:dyDescent="0.25">
@@ -8287,8 +8370,8 @@
       <c r="U99" t="s">
         <v>146</v>
       </c>
-      <c r="W99" t="s">
-        <v>448</v>
+      <c r="W99" s="12" t="s">
+        <v>451</v>
       </c>
       <c r="X99">
         <f t="shared" si="24"/>
@@ -8299,7 +8382,7 @@
         <v/>
       </c>
       <c r="AA99" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="100" spans="1:27" x14ac:dyDescent="0.25">
@@ -8360,7 +8443,7 @@
       <c r="U100" t="s">
         <v>146</v>
       </c>
-      <c r="W100" t="s">
+      <c r="W100" s="12" t="s">
         <v>251</v>
       </c>
       <c r="X100">
@@ -8433,8 +8516,8 @@
       <c r="U101" t="s">
         <v>146</v>
       </c>
-      <c r="W101" t="s">
-        <v>445</v>
+      <c r="W101" s="12" t="s">
+        <v>442</v>
       </c>
       <c r="X101">
         <f t="shared" si="24"/>
@@ -8445,7 +8528,7 @@
         <v/>
       </c>
       <c r="AA101" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="102" spans="1:27" x14ac:dyDescent="0.25">
@@ -8506,8 +8589,8 @@
       <c r="U102" t="s">
         <v>146</v>
       </c>
-      <c r="W102" t="s">
-        <v>297</v>
+      <c r="W102" s="12" t="s">
+        <v>296</v>
       </c>
       <c r="X102">
         <f t="shared" si="24"/>
@@ -8579,8 +8662,8 @@
       <c r="U103" t="s">
         <v>146</v>
       </c>
-      <c r="W103" t="s">
-        <v>299</v>
+      <c r="W103" s="12" t="s">
+        <v>298</v>
       </c>
       <c r="X103">
         <f t="shared" si="24"/>
@@ -8649,7 +8732,7 @@
       <c r="U104" t="s">
         <v>146</v>
       </c>
-      <c r="W104" s="19" t="s">
+      <c r="W104" s="22" t="s">
         <v>261</v>
       </c>
       <c r="X104">
@@ -8713,6 +8796,9 @@
       <c r="U105" t="s">
         <v>146</v>
       </c>
+      <c r="W105" s="12" t="s">
+        <v>453</v>
+      </c>
       <c r="X105">
         <f t="shared" si="24"/>
         <v>1</v>
@@ -8720,6 +8806,9 @@
       <c r="Y105" t="str">
         <f t="shared" si="19"/>
         <v/>
+      </c>
+      <c r="AA105" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="106" spans="1:27" x14ac:dyDescent="0.25">
@@ -8936,7 +9025,7 @@
       <c r="U109" t="s">
         <v>146</v>
       </c>
-      <c r="W109" s="19">
+      <c r="W109" s="22">
         <v>30</v>
       </c>
       <c r="X109">
@@ -8948,7 +9037,7 @@
         <v/>
       </c>
       <c r="AA109" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="110" spans="1:27" x14ac:dyDescent="0.25">
@@ -8997,7 +9086,7 @@
       <c r="U110" t="s">
         <v>146</v>
       </c>
-      <c r="W110" t="s">
+      <c r="W110" s="12" t="s">
         <v>258</v>
       </c>
       <c r="X110">
@@ -9070,8 +9159,8 @@
       <c r="U111" t="s">
         <v>146</v>
       </c>
-      <c r="W111" t="s">
-        <v>447</v>
+      <c r="W111" s="12" t="s">
+        <v>444</v>
       </c>
       <c r="X111">
         <f t="shared" si="24"/>
@@ -9082,7 +9171,7 @@
         <v/>
       </c>
       <c r="AA111" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="112" spans="1:27" x14ac:dyDescent="0.25">
@@ -9143,7 +9232,7 @@
       <c r="U112" t="s">
         <v>146</v>
       </c>
-      <c r="W112" s="19">
+      <c r="W112" s="22">
         <v>45</v>
       </c>
       <c r="X112">
@@ -9155,7 +9244,7 @@
         <v/>
       </c>
       <c r="AA112" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="113" spans="1:27" x14ac:dyDescent="0.25">
@@ -9216,6 +9305,9 @@
       <c r="U113" t="s">
         <v>146</v>
       </c>
+      <c r="W113" s="12" t="s">
+        <v>449</v>
+      </c>
       <c r="X113">
         <f t="shared" si="24"/>
         <v>1</v>
@@ -9223,6 +9315,9 @@
       <c r="Y113" t="str">
         <f t="shared" si="19"/>
         <v/>
+      </c>
+      <c r="AA113" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="114" spans="1:27" x14ac:dyDescent="0.25">
@@ -9283,7 +9378,7 @@
       <c r="U114" t="s">
         <v>146</v>
       </c>
-      <c r="W114" t="s">
+      <c r="W114" s="12" t="s">
         <v>259</v>
       </c>
       <c r="X114">
@@ -9637,6 +9732,9 @@
       <c r="U120" t="s">
         <v>146</v>
       </c>
+      <c r="W120" s="12" t="s">
+        <v>450</v>
+      </c>
       <c r="X120">
         <f t="shared" si="33"/>
         <v>1</v>
@@ -9644,6 +9742,9 @@
       <c r="Y120" t="str">
         <f t="shared" si="19"/>
         <v/>
+      </c>
+      <c r="AA120" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="121" spans="1:27" x14ac:dyDescent="0.25">
@@ -9704,7 +9805,7 @@
       <c r="U121" t="s">
         <v>146</v>
       </c>
-      <c r="W121" s="19">
+      <c r="W121" s="22">
         <v>250</v>
       </c>
       <c r="X121">
@@ -9716,7 +9817,7 @@
         <v/>
       </c>
       <c r="AA121" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="122" spans="1:27" x14ac:dyDescent="0.25">
@@ -9777,8 +9878,8 @@
       <c r="U122" t="s">
         <v>146</v>
       </c>
-      <c r="W122" t="s">
-        <v>299</v>
+      <c r="W122" s="12" t="s">
+        <v>298</v>
       </c>
       <c r="X122">
         <f t="shared" si="33"/>
@@ -9917,7 +10018,7 @@
       <c r="U124" t="s">
         <v>146</v>
       </c>
-      <c r="W124" t="s">
+      <c r="W124" s="12" t="s">
         <v>289</v>
       </c>
       <c r="X124">
@@ -9993,6 +10094,9 @@
       <c r="U125" t="s">
         <v>146</v>
       </c>
+      <c r="W125" s="12" t="s">
+        <v>289</v>
+      </c>
       <c r="X125">
         <f t="shared" si="33"/>
         <v>1</v>
@@ -10000,6 +10104,9 @@
       <c r="Y125" t="str">
         <f t="shared" si="19"/>
         <v/>
+      </c>
+      <c r="AA125" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="126" spans="1:27" x14ac:dyDescent="0.25">
@@ -10307,8 +10414,8 @@
       <c r="Q146">
         <v>2</v>
       </c>
-      <c r="W146" t="s">
-        <v>308</v>
+      <c r="W146" s="12" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="147" spans="2:23" x14ac:dyDescent="0.25">
@@ -10422,7 +10529,7 @@
     <row r="161" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B161" s="6"/>
       <c r="P161" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="Q161">
         <v>1</v>
@@ -10605,7 +10712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E134"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
@@ -10618,7 +10725,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B1">
         <v>7</v>
@@ -10629,30 +10736,30 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E6">
         <f>B1+B10+B20+B29+B39+B50+B60+B71+B83+B93+B102+B113+B124</f>
@@ -10661,15 +10768,15 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E8" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -10680,7 +10787,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B10">
         <v>8</v>
@@ -10691,47 +10798,47 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B20">
         <v>7</v>
@@ -10742,48 +10849,48 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C24" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>332</v>
+      </c>
+      <c r="C25" t="s">
         <v>333</v>
-      </c>
-      <c r="C25" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B29">
         <v>8</v>
@@ -10791,47 +10898,47 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B39">
         <v>9</v>
@@ -10842,52 +10949,52 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B50">
         <v>8</v>
@@ -10898,47 +11005,47 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B60">
         <v>9</v>
@@ -10949,52 +11056,52 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B71">
         <v>10</v>
@@ -11005,12 +11112,12 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C73" t="s">
         <v>242</v>
@@ -11018,22 +11125,22 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C77" t="s">
         <v>242</v>
@@ -11041,30 +11148,30 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C78" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B83">
         <v>8</v>
@@ -11075,47 +11182,47 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B93">
         <v>7</v>
@@ -11126,42 +11233,42 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B102">
         <v>9</v>
@@ -11172,32 +11279,32 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C108" t="s">
         <v>242</v>
@@ -11205,22 +11312,22 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B113">
         <v>9</v>
@@ -11231,52 +11338,52 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B124">
         <v>10</v>
@@ -11287,37 +11394,37 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C131" t="s">
         <v>242</v>
@@ -11325,12 +11432,12 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C133" t="s">
         <v>242</v>
@@ -11338,7 +11445,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C134" t="s">
         <v>242</v>

</xml_diff>

<commit_message>
Updated thank you notes sent
</commit_message>
<xml_diff>
--- a/Guest_List_Invited.xlsx
+++ b/Guest_List_Invited.xlsx
@@ -1,24 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\logan\Documents\GitHub\Farrell_Garrett_Wedding\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43105037-3FEF-4D60-BF1A-E097BAF603B8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Table #" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="458">
   <si>
     <t xml:space="preserve">Priority </t>
   </si>
@@ -1397,17 +1391,20 @@
   </si>
   <si>
     <t>9 small plates, 3 rice bowls</t>
+  </si>
+  <si>
+    <t>Honeyfund…</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1526,16 +1523,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1830,22 +1827,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AD212"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I77" sqref="I77"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA106" sqref="AA106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35.85546875" customWidth="1"/>
     <col min="2" max="2" width="4" hidden="1" customWidth="1"/>
@@ -1871,15 +1868,15 @@
     <col min="27" max="27" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" ht="15" customHeight="1">
       <c r="A1" s="5">
         <v>4</v>
       </c>
       <c r="B1" s="15"/>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="20"/>
+      <c r="E1" s="22"/>
       <c r="F1" t="s">
         <v>68</v>
       </c>
@@ -1891,20 +1888,20 @@
       <c r="U1" s="10"/>
       <c r="V1" s="10"/>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30">
       <c r="A2" s="4">
         <v>3</v>
       </c>
       <c r="B2" s="6"/>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="G2" s="19" t="s">
+      <c r="E2" s="21"/>
+      <c r="G2" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
       <c r="J2" s="11"/>
       <c r="K2" s="11"/>
       <c r="P2" t="s">
@@ -1933,7 +1930,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1941,11 +1938,11 @@
       <c r="C3" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="21">
         <f>SUM(E6:E132)-E13-E44-E52-E61-E88-E116-E127</f>
         <v>114</v>
       </c>
-      <c r="E3" s="19"/>
+      <c r="E3" s="21"/>
       <c r="F3">
         <f>SUM(J6:J174)</f>
         <v>217</v>
@@ -1982,7 +1979,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="4" spans="1:30" s="10" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" s="10" customFormat="1" ht="31.5" customHeight="1">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -2038,7 +2035,7 @@
       <c r="V4" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="W4" s="21" t="s">
+      <c r="W4" s="19" t="s">
         <v>238</v>
       </c>
       <c r="Y4" s="10" t="s">
@@ -2052,7 +2049,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -2066,7 +2063,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2133,7 +2130,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2200,7 +2197,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2276,7 +2273,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -2346,7 +2343,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -2416,7 +2413,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -2494,7 +2491,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30">
       <c r="B12" s="6"/>
       <c r="C12" s="1"/>
       <c r="D12">
@@ -2533,7 +2530,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -2578,7 +2575,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
@@ -2636,7 +2633,7 @@
       <c r="U14" t="s">
         <v>146</v>
       </c>
-      <c r="W14" s="22">
+      <c r="W14" s="20">
         <v>100</v>
       </c>
       <c r="X14">
@@ -2654,7 +2651,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -2724,7 +2721,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
@@ -2797,7 +2794,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27">
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
@@ -2864,7 +2861,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27">
       <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
@@ -2931,7 +2928,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27">
       <c r="A19" s="2" t="s">
         <v>184</v>
       </c>
@@ -3001,7 +2998,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -3071,7 +3068,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27">
       <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
@@ -3138,7 +3135,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27">
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
@@ -3205,7 +3202,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27">
       <c r="A23" s="2" t="s">
         <v>226</v>
       </c>
@@ -3275,7 +3272,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27">
       <c r="A24" s="2" t="s">
         <v>17</v>
       </c>
@@ -3336,7 +3333,7 @@
       <c r="U24" t="s">
         <v>146</v>
       </c>
-      <c r="W24" s="22">
+      <c r="W24" s="20">
         <v>50</v>
       </c>
       <c r="X24">
@@ -3351,7 +3348,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27">
       <c r="A25" s="2" t="s">
         <v>18</v>
       </c>
@@ -3424,7 +3421,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27">
       <c r="A26" s="2" t="s">
         <v>19</v>
       </c>
@@ -3491,7 +3488,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27">
       <c r="A27" s="2" t="s">
         <v>20</v>
       </c>
@@ -3558,7 +3555,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27">
       <c r="A28" s="2" t="s">
         <v>21</v>
       </c>
@@ -3625,7 +3622,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27">
       <c r="A29" s="2" t="s">
         <v>22</v>
       </c>
@@ -3692,7 +3689,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27">
       <c r="A30" s="2" t="s">
         <v>23</v>
       </c>
@@ -3759,7 +3756,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27">
       <c r="A31" s="2" t="s">
         <v>24</v>
       </c>
@@ -3832,7 +3829,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27">
       <c r="A32" s="2" t="s">
         <v>25</v>
       </c>
@@ -3899,7 +3896,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28">
       <c r="A33" s="2" t="s">
         <v>26</v>
       </c>
@@ -3966,7 +3963,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
@@ -4039,7 +4036,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
@@ -4109,7 +4106,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28">
       <c r="A36" t="s">
         <v>257</v>
       </c>
@@ -4176,7 +4173,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28">
       <c r="A37" s="2" t="s">
         <v>40</v>
       </c>
@@ -4243,7 +4240,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28">
       <c r="A38" s="2" t="s">
         <v>41</v>
       </c>
@@ -4316,7 +4313,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28">
       <c r="A39" s="2" t="s">
         <v>42</v>
       </c>
@@ -4392,7 +4389,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28">
       <c r="A40" s="2" t="s">
         <v>43</v>
       </c>
@@ -4468,7 +4465,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28">
       <c r="A41" t="s">
         <v>96</v>
       </c>
@@ -4529,7 +4526,7 @@
       <c r="U41" t="s">
         <v>146</v>
       </c>
-      <c r="W41" s="22">
+      <c r="W41" s="20">
         <v>50</v>
       </c>
       <c r="X41">
@@ -4541,7 +4538,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28">
       <c r="A42" s="2"/>
       <c r="B42" s="7"/>
       <c r="D42">
@@ -4577,7 +4574,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28">
       <c r="B43" s="6"/>
       <c r="C43" s="1"/>
       <c r="D43">
@@ -4613,7 +4610,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28">
       <c r="A44" s="1" t="s">
         <v>27</v>
       </c>
@@ -4655,7 +4652,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28">
       <c r="A45" t="s">
         <v>28</v>
       </c>
@@ -4731,7 +4728,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28">
       <c r="A46" t="s">
         <v>29</v>
       </c>
@@ -4798,7 +4795,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28">
       <c r="A47" t="s">
         <v>30</v>
       </c>
@@ -4865,7 +4862,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28">
       <c r="A48" t="s">
         <v>31</v>
       </c>
@@ -4935,7 +4932,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:29">
       <c r="A49" t="s">
         <v>32</v>
       </c>
@@ -5011,7 +5008,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:29">
       <c r="A50" t="s">
         <v>227</v>
       </c>
@@ -5074,7 +5071,7 @@
       <c r="U50" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="W50" s="22">
+      <c r="W50" s="20">
         <v>100</v>
       </c>
       <c r="X50">
@@ -5092,7 +5089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:29">
       <c r="B51" s="6"/>
       <c r="J51">
         <f t="shared" si="9"/>
@@ -5123,7 +5120,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:29">
       <c r="A52" s="1" t="s">
         <v>48</v>
       </c>
@@ -5165,7 +5162,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:29">
       <c r="A53" t="s">
         <v>47</v>
       </c>
@@ -5236,7 +5233,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:29">
       <c r="A54" t="s">
         <v>306</v>
       </c>
@@ -5297,7 +5294,7 @@
       <c r="U54" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="W54" s="22">
+      <c r="W54" s="20">
         <v>50</v>
       </c>
       <c r="X54">
@@ -5312,7 +5309,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:29">
       <c r="A55" t="s">
         <v>49</v>
       </c>
@@ -5383,7 +5380,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:29">
       <c r="A56" t="s">
         <v>73</v>
       </c>
@@ -5456,7 +5453,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:29">
       <c r="A57" t="s">
         <v>50</v>
       </c>
@@ -5526,7 +5523,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:29">
       <c r="A58" t="s">
         <v>51</v>
       </c>
@@ -5596,7 +5593,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:29">
       <c r="A59" t="s">
         <v>52</v>
       </c>
@@ -5663,7 +5660,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:29">
       <c r="B60" s="6"/>
       <c r="J60">
         <f t="shared" si="9"/>
@@ -5694,7 +5691,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:29">
       <c r="A61" s="1" t="s">
         <v>46</v>
       </c>
@@ -5736,7 +5733,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:29">
       <c r="A62" t="s">
         <v>218</v>
       </c>
@@ -5798,7 +5795,7 @@
         <v>146</v>
       </c>
       <c r="V62" s="6"/>
-      <c r="W62" s="22">
+      <c r="W62" s="20">
         <v>100</v>
       </c>
       <c r="X62">
@@ -5813,7 +5810,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:29">
       <c r="A63" t="s">
         <v>262</v>
       </c>
@@ -5867,7 +5864,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:29">
       <c r="A64" t="s">
         <v>53</v>
       </c>
@@ -5938,7 +5935,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:27">
       <c r="A65" t="s">
         <v>290</v>
       </c>
@@ -6011,7 +6008,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:27">
       <c r="A66" t="s">
         <v>54</v>
       </c>
@@ -6082,7 +6079,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:27">
       <c r="A67" t="s">
         <v>163</v>
       </c>
@@ -6144,7 +6141,7 @@
         <v>146</v>
       </c>
       <c r="V67" s="6"/>
-      <c r="W67" s="22">
+      <c r="W67" s="20">
         <v>100</v>
       </c>
       <c r="X67">
@@ -6159,7 +6156,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:27">
       <c r="A68" t="s">
         <v>187</v>
       </c>
@@ -6223,7 +6220,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="69" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:27">
       <c r="A69" t="s">
         <v>55</v>
       </c>
@@ -6285,6 +6282,9 @@
         <v>146</v>
       </c>
       <c r="V69" s="6"/>
+      <c r="W69" s="12" t="s">
+        <v>457</v>
+      </c>
       <c r="X69">
         <f t="shared" si="13"/>
         <v>1</v>
@@ -6294,7 +6294,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:27">
       <c r="A70" t="s">
         <v>252</v>
       </c>
@@ -6367,7 +6367,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:27">
       <c r="A71" t="s">
         <v>56</v>
       </c>
@@ -6429,7 +6429,7 @@
         <v>146</v>
       </c>
       <c r="V71" s="6"/>
-      <c r="W71" s="22">
+      <c r="W71" s="20">
         <v>150</v>
       </c>
       <c r="X71">
@@ -6444,7 +6444,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:27">
       <c r="A72" t="s">
         <v>57</v>
       </c>
@@ -6520,7 +6520,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:27">
       <c r="A73" t="s">
         <v>58</v>
       </c>
@@ -6590,7 +6590,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:27">
       <c r="A74" t="s">
         <v>59</v>
       </c>
@@ -6648,7 +6648,7 @@
       <c r="U74" t="s">
         <v>146</v>
       </c>
-      <c r="W74" s="22">
+      <c r="W74" s="20">
         <v>100</v>
       </c>
       <c r="X74">
@@ -6663,7 +6663,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:27">
       <c r="A75" t="s">
         <v>60</v>
       </c>
@@ -6736,7 +6736,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:27">
       <c r="A76" t="s">
         <v>61</v>
       </c>
@@ -6809,7 +6809,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:27">
       <c r="A77" t="s">
         <v>62</v>
       </c>
@@ -6870,7 +6870,7 @@
       <c r="V77" t="s">
         <v>146</v>
       </c>
-      <c r="W77" s="22">
+      <c r="W77" s="20">
         <v>50</v>
       </c>
       <c r="X77">
@@ -6885,7 +6885,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:27">
       <c r="A78" t="s">
         <v>162</v>
       </c>
@@ -6952,7 +6952,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:27">
       <c r="A79" t="s">
         <v>64</v>
       </c>
@@ -7022,10 +7022,10 @@
         <v/>
       </c>
       <c r="AA79" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="80" spans="1:27">
       <c r="A80" t="s">
         <v>123</v>
       </c>
@@ -7092,7 +7092,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:27">
       <c r="A81" t="s">
         <v>285</v>
       </c>
@@ -7165,7 +7165,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:27">
       <c r="A82" t="s">
         <v>63</v>
       </c>
@@ -7238,7 +7238,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:27">
       <c r="A83" t="s">
         <v>165</v>
       </c>
@@ -7311,7 +7311,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:27">
       <c r="A84" t="s">
         <v>219</v>
       </c>
@@ -7384,10 +7384,10 @@
         <v/>
       </c>
       <c r="AA84" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="85" spans="1:27">
       <c r="A85" t="s">
         <v>245</v>
       </c>
@@ -7454,7 +7454,7 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:27">
       <c r="A86" t="s">
         <v>220</v>
       </c>
@@ -7524,10 +7524,10 @@
         <v/>
       </c>
       <c r="AA86" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="87" spans="1:27">
       <c r="B87" s="6"/>
       <c r="J87">
         <f t="shared" si="20"/>
@@ -7558,7 +7558,7 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:27">
       <c r="A88" s="1" t="s">
         <v>69</v>
       </c>
@@ -7600,7 +7600,7 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:27">
       <c r="A89" s="2" t="s">
         <v>76</v>
       </c>
@@ -7658,7 +7658,7 @@
       <c r="U89" t="s">
         <v>146</v>
       </c>
-      <c r="W89" s="22">
+      <c r="W89" s="20">
         <v>150</v>
       </c>
       <c r="X89">
@@ -7673,7 +7673,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:27">
       <c r="A90" t="s">
         <v>70</v>
       </c>
@@ -7746,7 +7746,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:27">
       <c r="A91" t="s">
         <v>130</v>
       </c>
@@ -7819,7 +7819,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:27">
       <c r="A92" t="s">
         <v>71</v>
       </c>
@@ -7877,7 +7877,7 @@
       <c r="U92" t="s">
         <v>146</v>
       </c>
-      <c r="W92" s="22">
+      <c r="W92" s="20">
         <v>100</v>
       </c>
       <c r="X92">
@@ -7892,7 +7892,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:27">
       <c r="A93" t="s">
         <v>72</v>
       </c>
@@ -7965,7 +7965,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:27">
       <c r="A94" t="s">
         <v>153</v>
       </c>
@@ -8038,7 +8038,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:27">
       <c r="A95" t="s">
         <v>150</v>
       </c>
@@ -8105,7 +8105,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:27">
       <c r="A96" t="s">
         <v>154</v>
       </c>
@@ -8178,7 +8178,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="97" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:27">
       <c r="A97" t="s">
         <v>116</v>
       </c>
@@ -8245,7 +8245,7 @@
         <v/>
       </c>
     </row>
-    <row r="98" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:27">
       <c r="A98" t="s">
         <v>131</v>
       </c>
@@ -8312,7 +8312,7 @@
         <v/>
       </c>
     </row>
-    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:27">
       <c r="A99" t="s">
         <v>74</v>
       </c>
@@ -8385,7 +8385,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:27">
       <c r="A100" t="s">
         <v>155</v>
       </c>
@@ -8458,7 +8458,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:27">
       <c r="A101" t="s">
         <v>143</v>
       </c>
@@ -8531,7 +8531,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="102" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:27">
       <c r="A102" t="s">
         <v>75</v>
       </c>
@@ -8604,7 +8604,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="103" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:27">
       <c r="A103" t="s">
         <v>147</v>
       </c>
@@ -8674,7 +8674,7 @@
         <v/>
       </c>
     </row>
-    <row r="104" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:27">
       <c r="A104" t="s">
         <v>148</v>
       </c>
@@ -8732,7 +8732,7 @@
       <c r="U104" t="s">
         <v>146</v>
       </c>
-      <c r="W104" s="22" t="s">
+      <c r="W104" s="20" t="s">
         <v>261</v>
       </c>
       <c r="X104">
@@ -8747,7 +8747,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:27">
       <c r="A105" t="s">
         <v>225</v>
       </c>
@@ -8808,10 +8808,10 @@
         <v/>
       </c>
       <c r="AA105" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="106" spans="1:27" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="106" spans="1:27">
       <c r="A106" t="s">
         <v>114</v>
       </c>
@@ -8869,7 +8869,7 @@
         <v/>
       </c>
     </row>
-    <row r="107" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:27">
       <c r="A107" t="s">
         <v>156</v>
       </c>
@@ -8924,7 +8924,7 @@
         <v/>
       </c>
     </row>
-    <row r="108" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:27">
       <c r="A108" t="s">
         <v>157</v>
       </c>
@@ -8979,7 +8979,7 @@
         <v/>
       </c>
     </row>
-    <row r="109" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:27">
       <c r="A109" t="s">
         <v>78</v>
       </c>
@@ -9025,7 +9025,7 @@
       <c r="U109" t="s">
         <v>146</v>
       </c>
-      <c r="W109" s="22">
+      <c r="W109" s="20">
         <v>30</v>
       </c>
       <c r="X109">
@@ -9040,7 +9040,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="110" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:27">
       <c r="A110" t="s">
         <v>223</v>
       </c>
@@ -9101,7 +9101,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="111" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:27">
       <c r="A111" t="s">
         <v>222</v>
       </c>
@@ -9174,7 +9174,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="112" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:27">
       <c r="A112" t="s">
         <v>224</v>
       </c>
@@ -9232,7 +9232,7 @@
       <c r="U112" t="s">
         <v>146</v>
       </c>
-      <c r="W112" s="22">
+      <c r="W112" s="20">
         <v>45</v>
       </c>
       <c r="X112">
@@ -9244,10 +9244,10 @@
         <v/>
       </c>
       <c r="AA112" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="113" spans="1:27" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="113" spans="1:27">
       <c r="A113" t="s">
         <v>77</v>
       </c>
@@ -9320,7 +9320,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="114" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:27">
       <c r="A114" t="s">
         <v>221</v>
       </c>
@@ -9393,7 +9393,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="115" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:27">
       <c r="B115" s="6"/>
       <c r="D115">
         <f t="shared" ref="D115:D116" si="29">IF(F115=4, 1,0)</f>
@@ -9428,7 +9428,7 @@
         <v/>
       </c>
     </row>
-    <row r="116" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:27">
       <c r="A116" s="1" t="s">
         <v>79</v>
       </c>
@@ -9470,7 +9470,7 @@
         <v/>
       </c>
     </row>
-    <row r="117" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:27">
       <c r="A117" t="s">
         <v>228</v>
       </c>
@@ -9540,7 +9540,7 @@
         <v/>
       </c>
     </row>
-    <row r="118" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:27">
       <c r="A118" t="s">
         <v>80</v>
       </c>
@@ -9607,7 +9607,7 @@
         <v/>
       </c>
     </row>
-    <row r="119" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:27">
       <c r="A119" t="s">
         <v>229</v>
       </c>
@@ -9674,7 +9674,7 @@
         <v/>
       </c>
     </row>
-    <row r="120" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:27">
       <c r="A120" t="s">
         <v>81</v>
       </c>
@@ -9747,7 +9747,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="121" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:27">
       <c r="A121" t="s">
         <v>82</v>
       </c>
@@ -9805,7 +9805,7 @@
       <c r="U121" t="s">
         <v>146</v>
       </c>
-      <c r="W121" s="22">
+      <c r="W121" s="20">
         <v>250</v>
       </c>
       <c r="X121">
@@ -9820,7 +9820,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="122" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:27">
       <c r="A122" t="s">
         <v>230</v>
       </c>
@@ -9890,7 +9890,7 @@
         <v/>
       </c>
     </row>
-    <row r="123" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:27">
       <c r="A123" t="s">
         <v>231</v>
       </c>
@@ -9960,7 +9960,7 @@
         <v/>
       </c>
     </row>
-    <row r="124" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:27">
       <c r="A124" t="s">
         <v>232</v>
       </c>
@@ -10033,7 +10033,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="125" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:27">
       <c r="A125" t="s">
         <v>233</v>
       </c>
@@ -10109,7 +10109,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="126" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:27">
       <c r="B126" s="6"/>
       <c r="J126">
         <f t="shared" si="20"/>
@@ -10128,7 +10128,7 @@
         <v/>
       </c>
     </row>
-    <row r="127" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:27">
       <c r="A127" s="1" t="s">
         <v>204</v>
       </c>
@@ -10150,7 +10150,7 @@
         <v/>
       </c>
     </row>
-    <row r="128" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:27">
       <c r="A128" t="s">
         <v>254</v>
       </c>
@@ -10187,7 +10187,7 @@
         <v/>
       </c>
     </row>
-    <row r="129" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:25">
       <c r="A129" t="s">
         <v>205</v>
       </c>
@@ -10224,7 +10224,7 @@
         <v/>
       </c>
     </row>
-    <row r="130" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:25">
       <c r="A130" t="s">
         <v>206</v>
       </c>
@@ -10261,7 +10261,7 @@
         <v/>
       </c>
     </row>
-    <row r="131" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:25">
       <c r="A131" t="s">
         <v>255</v>
       </c>
@@ -10294,7 +10294,7 @@
         <v/>
       </c>
     </row>
-    <row r="132" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:25">
       <c r="A132" t="s">
         <v>293</v>
       </c>
@@ -10303,13 +10303,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:25">
       <c r="B133" s="6"/>
     </row>
-    <row r="134" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:25">
       <c r="B134" s="6"/>
     </row>
-    <row r="135" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:25">
       <c r="B135" s="6"/>
       <c r="P135" t="s">
         <v>282</v>
@@ -10322,7 +10322,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="136" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:25">
       <c r="B136" s="6"/>
       <c r="P136" t="s">
         <v>284</v>
@@ -10331,7 +10331,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="137" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:25">
       <c r="B137" s="6"/>
       <c r="P137" t="s">
         <v>266</v>
@@ -10340,7 +10340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:25">
       <c r="B138" s="6"/>
       <c r="P138" t="s">
         <v>47</v>
@@ -10349,7 +10349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:25">
       <c r="B139" s="6"/>
       <c r="P139" t="s">
         <v>267</v>
@@ -10358,7 +10358,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:25">
       <c r="B140" s="6"/>
       <c r="P140" t="s">
         <v>268</v>
@@ -10367,7 +10367,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:25">
       <c r="B141" s="6"/>
       <c r="P141" t="s">
         <v>49</v>
@@ -10376,7 +10376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:25">
       <c r="B142" s="6"/>
       <c r="P142" t="s">
         <v>7</v>
@@ -10385,10 +10385,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:25">
       <c r="B143" s="6"/>
     </row>
-    <row r="144" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:25">
       <c r="B144" s="6"/>
       <c r="P144" t="s">
         <v>269</v>
@@ -10397,7 +10397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:23">
       <c r="B145" s="6"/>
       <c r="P145" t="s">
         <v>51</v>
@@ -10406,7 +10406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:23">
       <c r="B146" s="6"/>
       <c r="P146" t="s">
         <v>270</v>
@@ -10418,7 +10418,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="147" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:23">
       <c r="B147" s="6"/>
       <c r="P147" t="s">
         <v>271</v>
@@ -10427,7 +10427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:23">
       <c r="B148" s="6"/>
       <c r="P148" t="s">
         <v>272</v>
@@ -10436,10 +10436,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:23">
       <c r="B149" s="6"/>
     </row>
-    <row r="150" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:23">
       <c r="B150" s="6"/>
       <c r="P150" t="s">
         <v>273</v>
@@ -10448,7 +10448,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:23">
       <c r="B151" s="6"/>
       <c r="P151" t="s">
         <v>274</v>
@@ -10457,7 +10457,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="152" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:23">
       <c r="B152" s="6"/>
       <c r="P152" t="s">
         <v>275</v>
@@ -10466,7 +10466,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="153" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:23">
       <c r="B153" s="6"/>
       <c r="P153" t="s">
         <v>276</v>
@@ -10475,10 +10475,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:23">
       <c r="B154" s="6"/>
     </row>
-    <row r="155" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:23">
       <c r="B155" s="6"/>
       <c r="P155" t="s">
         <v>277</v>
@@ -10487,7 +10487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:23">
       <c r="B156" s="6"/>
       <c r="P156" t="s">
         <v>278</v>
@@ -10496,10 +10496,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="157" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:23">
       <c r="B157" s="6"/>
     </row>
-    <row r="158" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:23">
       <c r="B158" s="6"/>
       <c r="P158" t="s">
         <v>279</v>
@@ -10508,7 +10508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:23">
       <c r="B159" s="6"/>
       <c r="P159" t="s">
         <v>281</v>
@@ -10517,7 +10517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:23">
       <c r="B160" s="6"/>
       <c r="P160" t="s">
         <v>280</v>
@@ -10526,7 +10526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:17">
       <c r="B161" s="6"/>
       <c r="P161" t="s">
         <v>308</v>
@@ -10535,157 +10535,157 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:17">
       <c r="B162" s="6"/>
     </row>
-    <row r="163" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:17">
       <c r="B163" s="6"/>
     </row>
-    <row r="164" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:17">
       <c r="B164" s="6"/>
     </row>
-    <row r="165" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:17">
       <c r="B165" s="6"/>
     </row>
-    <row r="166" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:17">
       <c r="B166" s="6"/>
     </row>
-    <row r="167" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:17">
       <c r="B167" s="6"/>
     </row>
-    <row r="168" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:17">
       <c r="B168" s="6"/>
     </row>
-    <row r="169" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:17">
       <c r="B169" s="6"/>
     </row>
-    <row r="170" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:17">
       <c r="B170" s="6"/>
     </row>
-    <row r="171" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:17">
       <c r="B171" s="6"/>
     </row>
-    <row r="172" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:17">
       <c r="B172" s="6"/>
     </row>
-    <row r="173" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:17">
       <c r="B173" s="6"/>
     </row>
-    <row r="174" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:17">
       <c r="B174" s="6"/>
     </row>
-    <row r="175" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:17">
       <c r="B175" s="6"/>
     </row>
-    <row r="176" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:17">
       <c r="B176" s="6"/>
     </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:2">
       <c r="B177" s="6"/>
     </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:2">
       <c r="B178" s="6"/>
     </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:2">
       <c r="B179" s="6"/>
     </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:2">
       <c r="B180" s="6"/>
     </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:2">
       <c r="B181" s="6"/>
     </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:2">
       <c r="B182" s="6"/>
     </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:2">
       <c r="B183" s="6"/>
     </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:2">
       <c r="B184" s="6"/>
     </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:2">
       <c r="B185" s="6"/>
     </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:2">
       <c r="B186" s="6"/>
     </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:2">
       <c r="B187" s="6"/>
     </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:2">
       <c r="B188" s="6"/>
     </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:2">
       <c r="B189" s="6"/>
     </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:2">
       <c r="B190" s="6"/>
     </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:2">
       <c r="B191" s="6"/>
     </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:2">
       <c r="B192" s="6"/>
     </row>
-    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:2">
       <c r="B193" s="6"/>
     </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:2">
       <c r="B194" s="6"/>
     </row>
-    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:2">
       <c r="B195" s="6"/>
     </row>
-    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:2">
       <c r="B196" s="6"/>
     </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:2">
       <c r="B197" s="6"/>
     </row>
-    <row r="198" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:2">
       <c r="B198" s="6"/>
     </row>
-    <row r="199" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:2">
       <c r="B199" s="6"/>
     </row>
-    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:2">
       <c r="B200" s="6"/>
     </row>
-    <row r="201" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:2">
       <c r="B201" s="6"/>
     </row>
-    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:2">
       <c r="B202" s="6"/>
     </row>
-    <row r="203" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:2">
       <c r="B203" s="6"/>
     </row>
-    <row r="204" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:2">
       <c r="B204" s="6"/>
     </row>
-    <row r="205" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:2">
       <c r="B205" s="6"/>
     </row>
-    <row r="206" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:2">
       <c r="B206" s="6"/>
     </row>
-    <row r="207" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:2">
       <c r="B207" s="6"/>
     </row>
-    <row r="208" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:2">
       <c r="B208" s="6"/>
     </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:2">
       <c r="B209" s="6"/>
     </row>
-    <row r="210" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:2">
       <c r="B210" s="6"/>
     </row>
-    <row r="211" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:2">
       <c r="B211" s="6"/>
     </row>
-    <row r="212" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:2">
       <c r="B212" s="6"/>
     </row>
   </sheetData>
@@ -10709,21 +10709,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E134"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>311</v>
       </c>
@@ -10734,22 +10734,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>315</v>
       </c>
@@ -10757,7 +10757,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>316</v>
       </c>
@@ -10766,12 +10766,12 @@
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>318</v>
       </c>
@@ -10779,13 +10779,13 @@
         <v>433</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="E9">
         <f>C1+C10+C20+C39+C50+C60+C71+C83+C93+C102+C113+C124</f>
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>319</v>
       </c>
@@ -10796,47 +10796,47 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="8" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>328</v>
       </c>
@@ -10847,22 +10847,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>331</v>
       </c>
@@ -10870,7 +10870,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>332</v>
       </c>
@@ -10878,17 +10878,17 @@
         <v>333</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>336</v>
       </c>
@@ -10896,47 +10896,47 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>345</v>
       </c>
@@ -10947,52 +10947,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3">
       <c r="A45" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3">
       <c r="A47" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
         <v>355</v>
       </c>
@@ -11003,47 +11003,47 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3">
       <c r="A52" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3">
       <c r="A53" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3">
       <c r="A54" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3">
       <c r="A55" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3">
       <c r="A56" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3">
       <c r="A57" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3">
       <c r="A58" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3">
       <c r="A60" t="s">
         <v>363</v>
       </c>
@@ -11054,52 +11054,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3">
       <c r="A61" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3">
       <c r="A62" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3">
       <c r="A63" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3">
       <c r="A64" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3">
       <c r="A65" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3">
       <c r="A66" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3">
       <c r="A67" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3">
       <c r="A68" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3">
       <c r="A69" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3">
       <c r="A71" t="s">
         <v>373</v>
       </c>
@@ -11110,12 +11110,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3">
       <c r="A72" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3">
       <c r="A73" t="s">
         <v>375</v>
       </c>
@@ -11123,22 +11123,22 @@
         <v>242</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3">
       <c r="A74" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3">
       <c r="A75" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3">
       <c r="A76" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3">
       <c r="A77" t="s">
         <v>436</v>
       </c>
@@ -11146,7 +11146,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3">
       <c r="A78" t="s">
         <v>379</v>
       </c>
@@ -11154,22 +11154,22 @@
         <v>383</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3">
       <c r="A79" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3">
       <c r="A80" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3">
       <c r="A81" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3">
       <c r="A83" t="s">
         <v>384</v>
       </c>
@@ -11180,47 +11180,47 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3">
       <c r="A84" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3">
       <c r="A85" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3">
       <c r="A86" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3">
       <c r="A87" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3">
       <c r="A88" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3">
       <c r="A89" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3">
       <c r="A90" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3">
       <c r="A91" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3">
       <c r="A93" t="s">
         <v>393</v>
       </c>
@@ -11231,42 +11231,42 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3">
       <c r="A94" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3">
       <c r="A95" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3">
       <c r="A96" s="8" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3">
       <c r="A97" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3">
       <c r="A98" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3">
       <c r="A99" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3">
       <c r="A100" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3">
       <c r="A102" t="s">
         <v>401</v>
       </c>
@@ -11277,32 +11277,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3">
       <c r="A103" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3">
       <c r="A104" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3">
       <c r="A105" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3">
       <c r="A106" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3">
       <c r="A107" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3">
       <c r="A108" t="s">
         <v>407</v>
       </c>
@@ -11310,22 +11310,22 @@
         <v>242</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3">
       <c r="A109" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3">
       <c r="A110" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3">
       <c r="A111" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3">
       <c r="A113" t="s">
         <v>411</v>
       </c>
@@ -11336,52 +11336,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3">
       <c r="A114" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3">
       <c r="A115" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3">
       <c r="A116" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3">
       <c r="A117" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3">
       <c r="A118" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3">
       <c r="A119" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3">
       <c r="A120" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3">
       <c r="A121" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3">
       <c r="A122" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3">
       <c r="A124" t="s">
         <v>421</v>
       </c>
@@ -11392,37 +11392,37 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3">
       <c r="A125" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3">
       <c r="A126" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3">
       <c r="A127" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3">
       <c r="A128" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3">
       <c r="A129" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3">
       <c r="A130" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3">
       <c r="A131" t="s">
         <v>428</v>
       </c>
@@ -11430,12 +11430,12 @@
         <v>242</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3">
       <c r="A132" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3">
       <c r="A133" t="s">
         <v>430</v>
       </c>
@@ -11443,7 +11443,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3">
       <c r="A134" t="s">
         <v>431</v>
       </c>

</xml_diff>

<commit_message>
Updated thank you note section
</commit_message>
<xml_diff>
--- a/Guest_List_Invited.xlsx
+++ b/Guest_List_Invited.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="461">
   <si>
     <t xml:space="preserve">Priority </t>
   </si>
@@ -886,9 +886,6 @@
     <t>Ask about Food, didn't RSVP, but Deb says she's a NO</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>$100 for flights</t>
   </si>
   <si>
@@ -1336,9 +1333,6 @@
     <t>Ms. Diane Levesque (David Guest)</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>Target gift card $15</t>
   </si>
   <si>
@@ -1397,6 +1391,18 @@
   </si>
   <si>
     <t>Super nice blanket</t>
+  </si>
+  <si>
+    <t>Got hotel room so ours was comped</t>
+  </si>
+  <si>
+    <t>Thank you for Victoria Secret gift card</t>
+  </si>
+  <si>
+    <t>What did they give? Did we write them already?</t>
+  </si>
+  <si>
+    <t>$100 for accomodations (also from Ami)</t>
   </si>
 </sst>
 </file>
@@ -1495,7 +1501,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1536,6 +1542,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1830,7 +1839,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1840,9 +1849,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AD212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W65" sqref="W65"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA42" sqref="AA42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1850,18 +1859,17 @@
     <col min="1" max="1" width="35.85546875" customWidth="1"/>
     <col min="2" max="2" width="4" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="6.85546875" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="8" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="8" customWidth="1"/>
-    <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
+    <col min="4" max="5" width="8" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="0" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" hidden="1" customWidth="1"/>
     <col min="11" max="14" width="9.140625" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="2.5703125" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="35.5703125" customWidth="1"/>
     <col min="17" max="17" width="12.85546875" customWidth="1"/>
-    <col min="18" max="18" width="7.85546875" customWidth="1"/>
-    <col min="19" max="19" width="15.140625" customWidth="1"/>
+    <col min="18" max="18" width="7.85546875" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="15.140625" hidden="1" customWidth="1"/>
     <col min="20" max="20" width="10.85546875" hidden="1" customWidth="1"/>
     <col min="21" max="21" width="11" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="11.85546875" hidden="1" customWidth="1"/>
@@ -2259,7 +2267,7 @@
         <v>146</v>
       </c>
       <c r="W8" s="12" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="X8">
         <f t="shared" si="1"/>
@@ -2270,10 +2278,10 @@
         <v/>
       </c>
       <c r="AA8" t="s">
-        <v>438</v>
+        <v>242</v>
       </c>
       <c r="AD8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="9" spans="1:30">
@@ -2343,7 +2351,7 @@
         <v/>
       </c>
       <c r="AD9" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="10" spans="1:30">
@@ -2413,7 +2421,7 @@
         <v/>
       </c>
       <c r="AD10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="11" spans="1:30">
@@ -2477,7 +2485,7 @@
         <v>146</v>
       </c>
       <c r="W11" s="12" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="X11">
         <f t="shared" si="1"/>
@@ -2488,7 +2496,7 @@
         <v/>
       </c>
       <c r="AA11" t="s">
-        <v>288</v>
+        <v>242</v>
       </c>
       <c r="AD11" t="s">
         <v>60</v>
@@ -2530,7 +2538,7 @@
         <v/>
       </c>
       <c r="AD12" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="13" spans="1:30">
@@ -2575,7 +2583,7 @@
         <v/>
       </c>
       <c r="AD13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="14" spans="1:30">
@@ -2648,10 +2656,10 @@
         <v/>
       </c>
       <c r="AA14" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="AD14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="15" spans="1:30">
@@ -2721,7 +2729,7 @@
         <v/>
       </c>
       <c r="AD15" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="16" spans="1:30">
@@ -2794,7 +2802,7 @@
         <v/>
       </c>
       <c r="AD16" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="17" spans="1:27">
@@ -3348,7 +3356,7 @@
         <v/>
       </c>
       <c r="AA24" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="25" spans="1:27">
@@ -3421,7 +3429,7 @@
         <v/>
       </c>
       <c r="AA25" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="26" spans="1:27">
@@ -3818,7 +3826,7 @@
         <v>146</v>
       </c>
       <c r="W31" s="12" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="X31">
         <f t="shared" si="10"/>
@@ -4098,7 +4106,7 @@
         <v>146</v>
       </c>
       <c r="W35" s="12" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="X35">
         <f t="shared" si="10"/>
@@ -4107,6 +4115,12 @@
       <c r="Y35" t="str">
         <f t="shared" si="7"/>
         <v/>
+      </c>
+      <c r="AA35" t="s">
+        <v>242</v>
+      </c>
+      <c r="AB35" s="8" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="36" spans="1:28">
@@ -4375,7 +4389,7 @@
         <v>146</v>
       </c>
       <c r="W39" s="12" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="X39">
         <f t="shared" si="10"/>
@@ -4386,10 +4400,10 @@
         <v/>
       </c>
       <c r="AA39" t="s">
+        <v>242</v>
+      </c>
+      <c r="AB39" t="s">
         <v>438</v>
-      </c>
-      <c r="AB39" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="40" spans="1:28">
@@ -4454,7 +4468,7 @@
         <v>146</v>
       </c>
       <c r="W40" s="12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="X40">
         <f t="shared" si="10"/>
@@ -4539,6 +4553,9 @@
       <c r="Y41" t="str">
         <f t="shared" si="7"/>
         <v/>
+      </c>
+      <c r="AA41" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="42" spans="1:28">
@@ -4997,7 +5014,7 @@
         <v>146</v>
       </c>
       <c r="W49" s="12" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="X49">
         <f t="shared" si="11"/>
@@ -5008,7 +5025,7 @@
         <v/>
       </c>
       <c r="AA49" t="s">
-        <v>438</v>
+        <v>242</v>
       </c>
     </row>
     <row r="50" spans="1:29">
@@ -5086,7 +5103,7 @@
         <v/>
       </c>
       <c r="AA50" t="s">
-        <v>438</v>
+        <v>242</v>
       </c>
       <c r="AC50">
         <v>1</v>
@@ -5238,7 +5255,7 @@
     </row>
     <row r="54" spans="1:29">
       <c r="A54" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B54" s="6">
         <v>42</v>
@@ -5309,7 +5326,7 @@
         <v/>
       </c>
       <c r="AA54" t="s">
-        <v>438</v>
+        <v>242</v>
       </c>
     </row>
     <row r="55" spans="1:29">
@@ -5374,6 +5391,9 @@
         <v>146</v>
       </c>
       <c r="V55" s="6"/>
+      <c r="W55" s="12" t="s">
+        <v>457</v>
+      </c>
       <c r="X55">
         <f t="shared" si="12"/>
         <v>1</v>
@@ -5381,6 +5401,9 @@
       <c r="Y55" t="str">
         <f t="shared" si="7"/>
         <v/>
+      </c>
+      <c r="AA55" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="56" spans="1:29">
@@ -5810,7 +5833,7 @@
         <v/>
       </c>
       <c r="AA62" t="s">
-        <v>438</v>
+        <v>242</v>
       </c>
     </row>
     <row r="63" spans="1:29">
@@ -5930,7 +5953,7 @@
       </c>
       <c r="V64" s="6"/>
       <c r="W64" s="12" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="X64">
         <f t="shared" si="13"/>
@@ -5941,12 +5964,12 @@
         <v/>
       </c>
       <c r="AA64" t="s">
-        <v>438</v>
+        <v>242</v>
       </c>
     </row>
     <row r="65" spans="1:27">
       <c r="A65" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B65" s="6">
         <v>50</v>
@@ -5999,7 +6022,7 @@
       <c r="Q65" s="6"/>
       <c r="R65" s="6"/>
       <c r="S65" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="T65" s="6">
         <v>1</v>
@@ -6162,7 +6185,7 @@
         <v/>
       </c>
       <c r="AA67" t="s">
-        <v>438</v>
+        <v>242</v>
       </c>
     </row>
     <row r="68" spans="1:27">
@@ -6292,7 +6315,7 @@
       </c>
       <c r="V69" s="6"/>
       <c r="W69" s="12" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="X69">
         <f t="shared" si="13"/>
@@ -6450,7 +6473,7 @@
         <v/>
       </c>
       <c r="AA71" t="s">
-        <v>438</v>
+        <v>242</v>
       </c>
     </row>
     <row r="72" spans="1:27">
@@ -6515,7 +6538,7 @@
         <v>146</v>
       </c>
       <c r="W72" s="12" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="X72">
         <f t="shared" si="13"/>
@@ -6526,7 +6549,7 @@
         <v/>
       </c>
       <c r="AA72" t="s">
-        <v>438</v>
+        <v>242</v>
       </c>
     </row>
     <row r="73" spans="1:27">
@@ -6669,7 +6692,7 @@
         <v/>
       </c>
       <c r="AA74" t="s">
-        <v>438</v>
+        <v>242</v>
       </c>
     </row>
     <row r="75" spans="1:27">
@@ -6804,7 +6827,7 @@
         <v>146</v>
       </c>
       <c r="W76" s="12" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="X76">
         <f t="shared" si="13"/>
@@ -6891,7 +6914,7 @@
         <v/>
       </c>
       <c r="AA77" t="s">
-        <v>438</v>
+        <v>242</v>
       </c>
     </row>
     <row r="78" spans="1:27">
@@ -6952,6 +6975,9 @@
       <c r="U78" t="s">
         <v>146</v>
       </c>
+      <c r="W78" s="12" t="s">
+        <v>460</v>
+      </c>
       <c r="X78">
         <f t="shared" si="13"/>
         <v>1</v>
@@ -6959,6 +6985,9 @@
       <c r="Y78" t="str">
         <f t="shared" si="19"/>
         <v/>
+      </c>
+      <c r="AA78" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="79" spans="1:27">
@@ -7020,7 +7049,7 @@
         <v>146</v>
       </c>
       <c r="W79" s="12" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="X79">
         <f t="shared" si="13"/>
@@ -7160,7 +7189,7 @@
         <v>146</v>
       </c>
       <c r="W81" s="12" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="X81">
         <f t="shared" si="13"/>
@@ -7233,7 +7262,7 @@
         <v>146</v>
       </c>
       <c r="W82" s="12" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="X82">
         <f t="shared" si="13"/>
@@ -7244,7 +7273,7 @@
         <v/>
       </c>
       <c r="AA82" t="s">
-        <v>438</v>
+        <v>242</v>
       </c>
     </row>
     <row r="83" spans="1:27">
@@ -7306,7 +7335,7 @@
         <v>146</v>
       </c>
       <c r="W83" s="12" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="X83">
         <f t="shared" si="13"/>
@@ -7382,7 +7411,7 @@
         <v>146</v>
       </c>
       <c r="W84" s="12" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="X84">
         <f t="shared" si="13"/>
@@ -7522,7 +7551,7 @@
         <v>146</v>
       </c>
       <c r="W86" s="12" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="X86">
         <f t="shared" si="13"/>
@@ -7679,7 +7708,7 @@
         <v/>
       </c>
       <c r="AA89" t="s">
-        <v>438</v>
+        <v>242</v>
       </c>
     </row>
     <row r="90" spans="1:27">
@@ -7741,7 +7770,7 @@
         <v>146</v>
       </c>
       <c r="W90" s="12" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="X90">
         <f t="shared" si="24"/>
@@ -7752,7 +7781,7 @@
         <v/>
       </c>
       <c r="AA90" t="s">
-        <v>438</v>
+        <v>242</v>
       </c>
     </row>
     <row r="91" spans="1:27">
@@ -7898,7 +7927,7 @@
         <v/>
       </c>
       <c r="AA92" t="s">
-        <v>438</v>
+        <v>242</v>
       </c>
     </row>
     <row r="93" spans="1:27">
@@ -8033,7 +8062,7 @@
         <v>146</v>
       </c>
       <c r="W94" s="12" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="X94">
         <f t="shared" si="24"/>
@@ -8044,7 +8073,7 @@
         <v/>
       </c>
       <c r="AA94" t="s">
-        <v>438</v>
+        <v>242</v>
       </c>
     </row>
     <row r="95" spans="1:27">
@@ -8105,6 +8134,9 @@
       <c r="U95" t="s">
         <v>146</v>
       </c>
+      <c r="W95" s="23" t="s">
+        <v>459</v>
+      </c>
       <c r="X95">
         <f t="shared" si="24"/>
         <v>1</v>
@@ -8173,7 +8205,7 @@
         <v>146</v>
       </c>
       <c r="W96" s="12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="X96">
         <f t="shared" si="24"/>
@@ -8184,7 +8216,7 @@
         <v/>
       </c>
       <c r="AA96" t="s">
-        <v>438</v>
+        <v>242</v>
       </c>
     </row>
     <row r="97" spans="1:27">
@@ -8380,7 +8412,7 @@
         <v>146</v>
       </c>
       <c r="W99" s="12" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="X99">
         <f t="shared" si="24"/>
@@ -8391,7 +8423,7 @@
         <v/>
       </c>
       <c r="AA99" t="s">
-        <v>438</v>
+        <v>242</v>
       </c>
     </row>
     <row r="100" spans="1:27">
@@ -8526,7 +8558,7 @@
         <v>146</v>
       </c>
       <c r="W101" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="X101">
         <f t="shared" si="24"/>
@@ -8537,7 +8569,7 @@
         <v/>
       </c>
       <c r="AA101" t="s">
-        <v>438</v>
+        <v>242</v>
       </c>
     </row>
     <row r="102" spans="1:27">
@@ -8599,7 +8631,7 @@
         <v>146</v>
       </c>
       <c r="W102" s="12" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="X102">
         <f t="shared" si="24"/>
@@ -8672,7 +8704,7 @@
         <v>146</v>
       </c>
       <c r="W103" s="12" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="X103">
         <f t="shared" si="24"/>
@@ -8681,6 +8713,9 @@
       <c r="Y103" t="str">
         <f t="shared" si="19"/>
         <v/>
+      </c>
+      <c r="AA103" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="104" spans="1:27">
@@ -8806,7 +8841,7 @@
         <v>146</v>
       </c>
       <c r="W105" s="12" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="X105">
         <f t="shared" si="24"/>
@@ -8861,7 +8896,7 @@
         <v>119</v>
       </c>
       <c r="S106" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="T106">
         <v>1</v>
@@ -9046,7 +9081,7 @@
         <v/>
       </c>
       <c r="AA109" t="s">
-        <v>438</v>
+        <v>242</v>
       </c>
     </row>
     <row r="110" spans="1:27">
@@ -9169,7 +9204,7 @@
         <v>146</v>
       </c>
       <c r="W111" s="12" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="X111">
         <f t="shared" si="24"/>
@@ -9180,7 +9215,7 @@
         <v/>
       </c>
       <c r="AA111" t="s">
-        <v>438</v>
+        <v>242</v>
       </c>
     </row>
     <row r="112" spans="1:27">
@@ -9315,7 +9350,7 @@
         <v>146</v>
       </c>
       <c r="W113" s="12" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="X113">
         <f t="shared" si="24"/>
@@ -9326,7 +9361,7 @@
         <v/>
       </c>
       <c r="AA113" t="s">
-        <v>438</v>
+        <v>242</v>
       </c>
     </row>
     <row r="114" spans="1:27">
@@ -9532,7 +9567,7 @@
         <v>197</v>
       </c>
       <c r="S117" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="T117">
         <v>1</v>
@@ -9742,7 +9777,7 @@
         <v>146</v>
       </c>
       <c r="W120" s="12" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="X120">
         <f t="shared" si="33"/>
@@ -9753,7 +9788,7 @@
         <v/>
       </c>
       <c r="AA120" t="s">
-        <v>438</v>
+        <v>242</v>
       </c>
     </row>
     <row r="121" spans="1:27">
@@ -9826,7 +9861,7 @@
         <v/>
       </c>
       <c r="AA121" t="s">
-        <v>438</v>
+        <v>242</v>
       </c>
     </row>
     <row r="122" spans="1:27">
@@ -9888,7 +9923,7 @@
         <v>146</v>
       </c>
       <c r="W122" s="12" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="X122">
         <f t="shared" si="33"/>
@@ -9897,6 +9932,9 @@
       <c r="Y122" t="str">
         <f t="shared" si="19"/>
         <v/>
+      </c>
+      <c r="AA122" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="123" spans="1:27">
@@ -10028,7 +10066,7 @@
         <v>146</v>
       </c>
       <c r="W124" s="12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="X124">
         <f t="shared" si="33"/>
@@ -10104,7 +10142,7 @@
         <v>146</v>
       </c>
       <c r="W125" s="12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="X125">
         <f t="shared" si="33"/>
@@ -10115,7 +10153,7 @@
         <v/>
       </c>
       <c r="AA125" t="s">
-        <v>438</v>
+        <v>242</v>
       </c>
     </row>
     <row r="126" spans="1:27">
@@ -10305,7 +10343,7 @@
     </row>
     <row r="132" spans="1:25">
       <c r="A132" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B132" s="6"/>
       <c r="E132">
@@ -10424,7 +10462,7 @@
         <v>2</v>
       </c>
       <c r="W146" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="147" spans="2:23">
@@ -10538,7 +10576,7 @@
     <row r="161" spans="2:17">
       <c r="B161" s="6"/>
       <c r="P161" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="Q161">
         <v>1</v>
@@ -10734,7 +10772,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B1">
         <v>7</v>
@@ -10745,30 +10783,30 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E6">
         <f>B1+B10+B20+B29+B39+B50+B60+B71+B83+B93+B102+B113+B124</f>
@@ -10777,15 +10815,15 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E8" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -10796,7 +10834,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B10">
         <v>8</v>
@@ -10807,47 +10845,47 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B20">
         <v>7</v>
@@ -10858,48 +10896,48 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C24" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
+        <v>331</v>
+      </c>
+      <c r="C25" t="s">
         <v>332</v>
-      </c>
-      <c r="C25" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B29">
         <v>8</v>
@@ -10907,47 +10945,47 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B39">
         <v>9</v>
@@ -10958,52 +10996,52 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B50">
         <v>8</v>
@@ -11014,47 +11052,47 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B60">
         <v>9</v>
@@ -11065,52 +11103,52 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B71">
         <v>10</v>
@@ -11121,12 +11159,12 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C73" t="s">
         <v>242</v>
@@ -11134,22 +11172,22 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C77" t="s">
         <v>242</v>
@@ -11157,30 +11195,30 @@
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C78" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B83">
         <v>8</v>
@@ -11191,47 +11229,47 @@
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B93">
         <v>7</v>
@@ -11242,42 +11280,42 @@
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B102">
         <v>9</v>
@@ -11288,32 +11326,32 @@
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C108" t="s">
         <v>242</v>
@@ -11321,22 +11359,22 @@
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B113">
         <v>9</v>
@@ -11347,52 +11385,52 @@
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B124">
         <v>10</v>
@@ -11403,37 +11441,37 @@
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C131" t="s">
         <v>242</v>
@@ -11441,12 +11479,12 @@
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C133" t="s">
         <v>242</v>
@@ -11454,7 +11492,7 @@
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C134" t="s">
         <v>242</v>

</xml_diff>